<commit_message>
functions in separate folder + small adjustments
</commit_message>
<xml_diff>
--- a/data/SDK.xlsx
+++ b/data/SDK.xlsx
@@ -5545,8 +5545,8 @@
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5582,207 +5582,159 @@
     </row>
     <row r="2" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="2" t="n">
-        <v>3</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" s="4" t="n">
-        <v>6</v>
-      </c>
+      <c r="F2" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
-        <v>29</v>
-      </c>
+      <c r="A3" s="5"/>
       <c r="B3" s="6"/>
       <c r="C3" s="7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="7" t="n">
-        <v>4</v>
-      </c>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="10"/>
       <c r="D4" s="8"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="8" t="n">
+      <c r="F4" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="H4" s="9"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="9" t="n">
+        <v>9</v>
+      </c>
       <c r="I4" s="10" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="n">
         <v>5</v>
       </c>
+      <c r="B5" s="3"/>
       <c r="C5" s="4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="F5" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="G5" s="2" t="n">
+      <c r="E5" s="3"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="10" t="n">
         <v>9</v>
-      </c>
-      <c r="H5" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="I5" s="4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="B6" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="C6" s="7" t="n">
-        <v>29</v>
-      </c>
-      <c r="D6" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="E6" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="F6" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="G6" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="H6" s="6" t="n">
-        <v>7</v>
-      </c>
-      <c r="I6" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="B7" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="10" t="n">
-        <v>7</v>
-      </c>
-      <c r="D7" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="E7" s="9" t="n">
-        <v>69</v>
-      </c>
-      <c r="F7" s="10" t="n">
-        <v>69</v>
-      </c>
-      <c r="G7" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="H7" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="I7" s="10" t="n">
-        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="2" t="n">
+        <v>2</v>
+      </c>
       <c r="E8" s="3"/>
       <c r="F8" s="4"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="3" t="n">
+      <c r="H8" s="3"/>
+      <c r="I8" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="I8" s="4" t="n">
-        <v>9</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B9" s="6"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="6" t="n">
+        <v>6</v>
+      </c>
       <c r="C9" s="7"/>
-      <c r="D9" s="5" t="n">
-        <v>5</v>
-      </c>
+      <c r="D9" s="5"/>
       <c r="E9" s="6" t="n">
         <v>8</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="D10" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="H9" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="I9" s="7" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B10" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="8"/>
       <c r="E10" s="9"/>
-      <c r="F10" s="10" t="n">
-        <v>4</v>
-      </c>
+      <c r="F10" s="10"/>
       <c r="G10" s="8"/>
       <c r="H10" s="9"/>
       <c r="I10" s="10" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5886,7 +5838,7 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -6770,7 +6722,7 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -7525,7 +7477,7 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -8408,7 +8360,7 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K27" activeCellId="0" sqref="K27"/>
     </sheetView>
   </sheetViews>
@@ -9291,7 +9243,7 @@
   </sheetPr>
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -10034,7 +9986,7 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -10283,7 +10235,7 @@
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G44" activeCellId="0" sqref="G44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
improved function in separate dir
</commit_message>
<xml_diff>
--- a/data/SDK.xlsx
+++ b/data/SDK.xlsx
@@ -5545,8 +5545,8 @@
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5586,8 +5586,12 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
+      <c r="D2" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>12</v>
+      </c>
       <c r="F2" s="4" t="n">
         <v>4</v>
       </c>
@@ -5603,11 +5607,15 @@
       <c r="C3" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="D3" s="5"/>
+      <c r="D3" s="5" t="n">
+        <v>7</v>
+      </c>
       <c r="E3" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="7" t="n">
+        <v>6</v>
+      </c>
       <c r="G3" s="5"/>
       <c r="H3" s="6" t="n">
         <v>1</v>
@@ -5620,8 +5628,12 @@
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="10"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
+      <c r="D4" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="9" t="n">
+        <v>12</v>
+      </c>
       <c r="F4" s="10" t="n">
         <v>5</v>
       </c>
@@ -5704,7 +5716,9 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
+      <c r="A9" s="5" t="n">
+        <v>2</v>
+      </c>
       <c r="B9" s="6" t="n">
         <v>6</v>
       </c>
@@ -5718,7 +5732,9 @@
         <v>9</v>
       </c>
       <c r="H9" s="6"/>
-      <c r="I9" s="7"/>
+      <c r="I9" s="7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="8"/>
@@ -5731,7 +5747,9 @@
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="10"/>
-      <c r="G10" s="8"/>
+      <c r="G10" s="8" t="n">
+        <v>8</v>
+      </c>
       <c r="H10" s="9"/>
       <c r="I10" s="10" t="n">
         <v>2</v>
@@ -5838,7 +5856,7 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -6722,7 +6740,7 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -7477,7 +7495,7 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -8360,7 +8378,7 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K27" activeCellId="0" sqref="K27"/>
     </sheetView>
   </sheetViews>
@@ -9243,7 +9261,7 @@
   </sheetPr>
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -9986,7 +10004,7 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -10235,7 +10253,7 @@
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G44" activeCellId="0" sqref="G44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
deleted column header in excel sheet
</commit_message>
<xml_diff>
--- a/data/SDK.xlsx
+++ b/data/SDK.xlsx
@@ -27,34 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t xml:space="preserve">cell / #</t>
   </si>
@@ -497,10 +470,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -535,6 +504,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -5543,300 +5516,358 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="D2" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H2" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="I2" s="6" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B3" s="8" t="n">
+        <v>9</v>
+      </c>
+      <c r="C3" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G3" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="D4" s="1" t="n">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+      <c r="E4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="2" t="n">
+      <c r="H4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="F2" s="4" t="n">
+      <c r="B5" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="I5" s="6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="B6" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="G6" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="n">
+      <c r="H6" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="I6" s="9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="F7" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="I8" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="E3" s="6" t="n">
+    </row>
+    <row r="9" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="D9" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="E9" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="F3" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="8" t="n">
+      <c r="F9" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="G9" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="E4" s="9" t="n">
-        <v>12</v>
-      </c>
-      <c r="F4" s="10" t="n">
+      <c r="H9" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9" t="n">
-        <v>9</v>
-      </c>
-      <c r="I4" s="10" t="n">
+      <c r="I9" s="9" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="6" t="n">
-        <v>8</v>
-      </c>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="G7" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="10" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="4" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6" t="n">
-        <v>8</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10" t="n">
-        <v>7</v>
-      </c>
-      <c r="D10" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="8" t="n">
-        <v>8</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="10" t="n">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="A2:A10">
+  <conditionalFormatting sqref="A1:A9">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A1:I1">
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C9">
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A2:I2">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C10">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:I3">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:I4">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:C6">
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:I5">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5:C7">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B9">
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C3">
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:I6">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B10">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:C4">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7:C9">
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:I7">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8:C10">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:I8">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:I9">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10:I10">
     <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:F4">
+  <conditionalFormatting sqref="D1:F3">
     <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D1:D9">
     <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:F7">
+  <conditionalFormatting sqref="D4:F6">
     <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:F10">
+  <conditionalFormatting sqref="D7:F9">
     <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E10">
+  <conditionalFormatting sqref="E1:E9">
     <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F10">
+  <conditionalFormatting sqref="F1:F9">
     <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:I4">
+  <conditionalFormatting sqref="G1:I3">
     <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G1:G9">
     <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5:I7">
+  <conditionalFormatting sqref="G4:I6">
     <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8:I10">
+  <conditionalFormatting sqref="G7:I9">
     <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H10">
+  <conditionalFormatting sqref="H1:H9">
     <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I10">
+  <conditionalFormatting sqref="I1:I9">
     <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5856,486 +5887,486 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="1" width="7.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="6.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="12" style="1" width="8.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="1.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="10" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="6.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="12" style="10" width="8.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="10" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="10" width="3.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="2" t="n">
+      <c r="B1" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="n">
+      <c r="C1" s="2" t="n">
         <v>4789</v>
       </c>
-      <c r="D1" s="4" t="n">
+      <c r="D1" s="3" t="n">
         <v>289</v>
       </c>
-      <c r="E1" s="2" t="n">
+      <c r="E1" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="n">
+      <c r="F1" s="2" t="n">
         <v>479</v>
       </c>
-      <c r="G1" s="4" t="n">
+      <c r="G1" s="3" t="n">
         <v>289</v>
       </c>
-      <c r="H1" s="2" t="n">
+      <c r="H1" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="I1" s="3" t="n">
+      <c r="I1" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="J1" s="4" t="n">
+      <c r="J1" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="6"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="C2" s="6" t="n">
+      <c r="C2" s="5" t="n">
         <v>3789</v>
       </c>
-      <c r="D2" s="7" t="n">
+      <c r="D2" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="E2" s="5" t="n">
+      <c r="E2" s="4" t="n">
         <v>279</v>
       </c>
-      <c r="F2" s="6" t="n">
+      <c r="F2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="7" t="n">
+      <c r="G2" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="H2" s="5" t="n">
+      <c r="H2" s="4" t="n">
         <v>378</v>
       </c>
-      <c r="I2" s="6" t="n">
+      <c r="I2" s="5" t="n">
         <v>389</v>
       </c>
-      <c r="J2" s="7" t="n">
+      <c r="J2" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="6"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="8" t="n">
+      <c r="B3" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="n">
+      <c r="C3" s="8" t="n">
         <v>34789</v>
       </c>
-      <c r="D3" s="10" t="n">
+      <c r="D3" s="9" t="n">
         <v>389</v>
       </c>
-      <c r="E3" s="8" t="n">
+      <c r="E3" s="7" t="n">
         <v>679</v>
       </c>
-      <c r="F3" s="9" t="n">
+      <c r="F3" s="8" t="n">
         <v>34679</v>
       </c>
-      <c r="G3" s="10" t="n">
+      <c r="G3" s="9" t="n">
         <v>689</v>
       </c>
-      <c r="H3" s="8" t="n">
+      <c r="H3" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="I3" s="9" t="n">
+      <c r="I3" s="8" t="n">
         <v>389</v>
       </c>
-      <c r="J3" s="10" t="n">
+      <c r="J3" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="6"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="G4" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="H4" s="2" t="n">
+      <c r="H4" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I4" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="J4" s="4" t="n">
+      <c r="J4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="6"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="C5" s="6" t="n">
+      <c r="C5" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="6" t="n">
         <v>29</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="G5" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="H5" s="5" t="n">
+      <c r="H5" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="I5" s="6" t="n">
+      <c r="I5" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="J5" s="7" t="n">
+      <c r="J5" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="6"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="8" t="n">
+      <c r="B6" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="9" t="n">
+      <c r="C6" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="10" t="n">
+      <c r="D6" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="E6" s="8" t="n">
+      <c r="E6" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="F6" s="9" t="n">
+      <c r="F6" s="8" t="n">
         <v>69</v>
       </c>
-      <c r="G6" s="10" t="n">
+      <c r="G6" s="9" t="n">
         <v>69</v>
       </c>
-      <c r="H6" s="8" t="n">
+      <c r="H6" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="I6" s="9" t="n">
+      <c r="I6" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="J6" s="10" t="n">
+      <c r="J6" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="L6" s="8"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="6"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="D7" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="G7" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="H7" s="2" t="n">
+      <c r="H7" s="1" t="n">
         <v>138</v>
       </c>
-      <c r="I7" s="3" t="n">
+      <c r="I7" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="J7" s="4" t="n">
+      <c r="J7" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="6"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5" t="n">
+      <c r="B8" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="C8" s="6" t="n">
+      <c r="C8" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="D8" s="6" t="n">
         <v>139</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F8" s="6" t="n">
+      <c r="F8" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="G8" s="7" t="n">
+      <c r="G8" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="H8" s="5" t="n">
+      <c r="H8" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="I8" s="6" t="n">
+      <c r="I8" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="J8" s="7" t="n">
+      <c r="J8" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="6"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="8" t="n">
+      <c r="B9" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="C9" s="9" t="n">
+      <c r="C9" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="D9" s="10" t="n">
+      <c r="D9" s="9" t="n">
         <v>1389</v>
       </c>
-      <c r="E9" s="8" t="n">
+      <c r="E9" s="7" t="n">
         <v>69</v>
       </c>
-      <c r="F9" s="9" t="n">
+      <c r="F9" s="8" t="n">
         <v>369</v>
       </c>
-      <c r="G9" s="10" t="n">
+      <c r="G9" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="H9" s="8" t="n">
+      <c r="H9" s="7" t="n">
         <v>138</v>
       </c>
-      <c r="I9" s="9" t="n">
+      <c r="I9" s="8" t="n">
         <v>38</v>
       </c>
-      <c r="J9" s="10" t="n">
+      <c r="J9" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="L9" s="8"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="6"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="11"/>
-      <c r="F10" s="6"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="12"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="4"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="7"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="10"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="4"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="7"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="10"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="4"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="7"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="10"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="13" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C22" s="13" t="n">
         <v>1</v>
@@ -6740,399 +6771,399 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="1" width="7.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="6.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="1.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="10" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="6.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="10" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="10" width="3.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="2" t="n">
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3" t="n">
+      <c r="F1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="J1" s="4" t="n">
+      <c r="J1" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="6"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="5" t="n">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="F2" s="6" t="n">
+      <c r="F2" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="5" t="n">
+      <c r="G2" s="6"/>
+      <c r="H2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="I2" s="6" t="n">
+      <c r="I2" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="8" t="n">
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="9" t="n">
+      <c r="F3" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="8" t="n">
+      <c r="G3" s="9"/>
+      <c r="H3" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="I3" s="9" t="n">
+      <c r="I3" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="J3" s="10" t="n">
+      <c r="J3" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="6"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4" t="n">
+      <c r="B4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3" t="n">
+      <c r="E4" s="1"/>
+      <c r="F4" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="2" t="n">
+      <c r="G4" s="3"/>
+      <c r="H4" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="6"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="3"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6" t="n">
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="5" t="n">
+      <c r="G5" s="6"/>
+      <c r="H5" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="7" t="n">
+      <c r="I5" s="5"/>
+      <c r="J5" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="6"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10" t="n">
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="8" t="n">
+      <c r="E6" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="F6" s="9" t="n">
+      <c r="F6" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="8" t="n">
+      <c r="G6" s="9"/>
+      <c r="H6" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="10"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="6"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="9"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="D7" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3" t="n">
+      <c r="E7" s="1"/>
+      <c r="F7" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="G7" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="4"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="6"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="3"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5"/>
-      <c r="C8" s="6" t="n">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="D8" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6" t="n">
+      <c r="E8" s="4"/>
+      <c r="F8" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="G8" s="7" t="n">
+      <c r="G8" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="6" t="n">
+      <c r="H8" s="4"/>
+      <c r="I8" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="J8" s="7" t="n">
+      <c r="J8" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="6"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="8" t="n">
+      <c r="B9" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10" t="n">
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="H9" s="8" t="n">
+      <c r="H9" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="I9" s="9" t="n">
+      <c r="I9" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="6"/>
+      <c r="J9" s="9"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="11"/>
-      <c r="F10" s="6"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="12"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="4"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="7"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="10"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="4"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="7"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="10"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="4"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="7"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="10"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="13" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C22" s="13" t="n">
         <v>1</v>
@@ -7495,485 +7526,485 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="1" width="7.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="6.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="1.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="10" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="6.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="10" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="10" width="3.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="2" t="n">
+      <c r="B1" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C1" s="3" t="n">
+      <c r="C1" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="n">
+      <c r="D1" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="n">
+      <c r="E1" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="n">
+      <c r="F1" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G1" s="4" t="n">
+      <c r="G1" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="H1" s="2" t="n">
+      <c r="H1" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="n">
+      <c r="I1" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="J1" s="4" t="n">
+      <c r="J1" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="6"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="C2" s="6" t="n">
+      <c r="C2" s="5" t="n">
         <v>1467</v>
       </c>
-      <c r="D2" s="7" t="n">
+      <c r="D2" s="6" t="n">
         <v>1467</v>
       </c>
-      <c r="E2" s="5" t="n">
+      <c r="E2" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="F2" s="6" t="n">
+      <c r="F2" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G2" s="7" t="n">
+      <c r="G2" s="6" t="n">
         <v>25</v>
       </c>
-      <c r="H2" s="5" t="n">
+      <c r="H2" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="I2" s="6" t="n">
+      <c r="I2" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="J2" s="7" t="n">
+      <c r="J2" s="6" t="n">
         <v>178</v>
       </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="6"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="8" t="n">
+      <c r="B3" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="C3" s="9" t="n">
+      <c r="C3" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="D3" s="10" t="n">
+      <c r="D3" s="9" t="n">
         <v>178</v>
       </c>
-      <c r="E3" s="8" t="n">
+      <c r="E3" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="F3" s="9" t="n">
+      <c r="F3" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="G3" s="10" t="n">
+      <c r="G3" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="H3" s="8" t="n">
+      <c r="H3" s="7" t="n">
         <v>17</v>
       </c>
-      <c r="I3" s="9" t="n">
+      <c r="I3" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="J3" s="10" t="n">
+      <c r="J3" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="6"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="2" t="n">
         <v>134</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="G4" s="3" t="n">
         <v>123</v>
       </c>
-      <c r="H4" s="2" t="n">
+      <c r="H4" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I4" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="J4" s="4" t="n">
+      <c r="J4" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="6"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="n">
+      <c r="C5" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="G5" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="H5" s="5" t="n">
+      <c r="H5" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="I5" s="6" t="n">
+      <c r="I5" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="J5" s="7" t="n">
+      <c r="J5" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="6"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="8" t="n">
+      <c r="B6" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="C6" s="9" t="n">
+      <c r="C6" s="8" t="n">
         <v>13</v>
       </c>
-      <c r="D6" s="10" t="n">
+      <c r="D6" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="E6" s="8" t="n">
+      <c r="E6" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="F6" s="9" t="n">
+      <c r="F6" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="G6" s="10" t="n">
+      <c r="G6" s="9" t="n">
         <v>13</v>
       </c>
-      <c r="H6" s="8" t="n">
+      <c r="H6" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="I6" s="9" t="n">
+      <c r="I6" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="J6" s="10" t="n">
+      <c r="J6" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="L6" s="8"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="6"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="D7" s="3" t="n">
         <v>68</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="G7" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="H7" s="2" t="n">
+      <c r="H7" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="I7" s="3" t="n">
+      <c r="I7" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="J7" s="4" t="n">
+      <c r="J7" s="3" t="n">
         <v>68</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="6"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5" t="n">
+      <c r="B8" s="4" t="n">
         <v>148</v>
       </c>
-      <c r="C8" s="6" t="n">
+      <c r="C8" s="5" t="n">
         <v>1467</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="D8" s="6" t="n">
         <v>14678</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="F8" s="6" t="n">
+      <c r="F8" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G8" s="7" t="n">
+      <c r="G8" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="H8" s="5" t="n">
+      <c r="H8" s="4" t="n">
         <v>1357</v>
       </c>
-      <c r="I8" s="6" t="n">
+      <c r="I8" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="J8" s="7" t="n">
+      <c r="J8" s="6" t="n">
         <v>13678</v>
       </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="6"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="8" t="n">
+      <c r="B9" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="9" t="n">
+      <c r="C9" s="8" t="n">
         <v>17</v>
       </c>
-      <c r="D9" s="10" t="n">
+      <c r="D9" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="E9" s="8" t="n">
+      <c r="E9" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="F9" s="9" t="n">
+      <c r="F9" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="G9" s="10" t="n">
+      <c r="G9" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="H9" s="8" t="n">
+      <c r="H9" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="I9" s="9" t="n">
+      <c r="I9" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="J9" s="10" t="n">
+      <c r="J9" s="9" t="n">
         <v>17</v>
       </c>
-      <c r="L9" s="8"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="6"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="11"/>
-      <c r="F10" s="6"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="12"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="4"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="7"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="10"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="4"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="7"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="10"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="4"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="7"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="10"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="13" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C22" s="13" t="n">
         <v>1</v>
@@ -8378,485 +8409,485 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K27" activeCellId="0" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="1" width="7.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="6.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="1.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="10" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="6.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="10" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="10" width="3.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="2" t="n">
+      <c r="B1" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="n">
+      <c r="C1" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="n">
+      <c r="D1" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="E1" s="2" t="n">
+      <c r="E1" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="F1" s="3" t="n">
+      <c r="F1" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="G1" s="4" t="n">
+      <c r="G1" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="H1" s="2" t="n">
+      <c r="H1" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="I1" s="3" t="n">
+      <c r="I1" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="J1" s="4" t="n">
+      <c r="J1" s="3" t="n">
         <v>49</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="6"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="4" t="n">
         <v>458</v>
       </c>
-      <c r="C2" s="6" t="n">
+      <c r="C2" s="5" t="n">
         <v>45</v>
       </c>
-      <c r="D2" s="7" t="n">
+      <c r="D2" s="6" t="n">
         <v>458</v>
       </c>
-      <c r="E2" s="5" t="n">
+      <c r="E2" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="F2" s="6" t="n">
+      <c r="F2" s="5" t="n">
         <v>67</v>
       </c>
-      <c r="G2" s="7" t="n">
+      <c r="G2" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="H2" s="5" t="n">
+      <c r="H2" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="I2" s="6" t="n">
+      <c r="I2" s="5" t="n">
         <v>67</v>
       </c>
-      <c r="J2" s="7" t="n">
+      <c r="J2" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="6"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="8" t="n">
+      <c r="B3" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="C3" s="9" t="n">
+      <c r="C3" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="D3" s="10" t="n">
+      <c r="D3" s="9" t="n">
         <v>19</v>
       </c>
-      <c r="E3" s="8" t="n">
+      <c r="E3" s="7" t="n">
         <v>14</v>
       </c>
-      <c r="F3" s="9" t="n">
+      <c r="F3" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="10" t="n">
+      <c r="G3" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="H3" s="8" t="n">
+      <c r="H3" s="7" t="n">
         <v>49</v>
       </c>
-      <c r="I3" s="9" t="n">
+      <c r="I3" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="J3" s="10" t="n">
+      <c r="J3" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="6"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="2" t="n">
         <v>1456</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="3" t="n">
         <v>3456</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="2" t="n">
         <v>145</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="G4" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="H4" s="2" t="n">
+      <c r="H4" s="1" t="n">
         <v>1346</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I4" s="2" t="n">
         <v>46</v>
       </c>
-      <c r="J4" s="4" t="n">
+      <c r="J4" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="6"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="4" t="n">
         <v>348</v>
       </c>
-      <c r="C5" s="6" t="n">
+      <c r="C5" s="5" t="n">
         <v>146</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="G5" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="H5" s="5" t="n">
+      <c r="H5" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="I5" s="6" t="n">
+      <c r="I5" s="5" t="n">
         <v>468</v>
       </c>
-      <c r="J5" s="7" t="n">
+      <c r="J5" s="6" t="n">
         <v>34</v>
       </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="6"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="8" t="n">
+      <c r="B6" s="7" t="n">
         <v>458</v>
       </c>
-      <c r="C6" s="9" t="n">
+      <c r="C6" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="D6" s="10" t="n">
+      <c r="D6" s="9" t="n">
         <v>458</v>
       </c>
-      <c r="E6" s="8" t="n">
+      <c r="E6" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="F6" s="9" t="n">
+      <c r="F6" s="8" t="n">
         <v>145</v>
       </c>
-      <c r="G6" s="10" t="n">
+      <c r="G6" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="H6" s="8" t="n">
+      <c r="H6" s="7" t="n">
         <v>149</v>
       </c>
-      <c r="I6" s="9" t="n">
+      <c r="I6" s="8" t="n">
         <v>489</v>
       </c>
-      <c r="J6" s="10" t="n">
+      <c r="J6" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="L6" s="8"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="6"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="1" t="n">
         <v>3457</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="D7" s="3" t="n">
         <v>345</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="G7" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H7" s="2" t="n">
+      <c r="H7" s="1" t="n">
         <v>347</v>
       </c>
-      <c r="I7" s="3" t="n">
+      <c r="I7" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="J7" s="4" t="n">
+      <c r="J7" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="6"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5" t="n">
+      <c r="B8" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="6" t="n">
+      <c r="C8" s="5" t="n">
         <v>46</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="D8" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F8" s="6" t="n">
+      <c r="F8" s="5" t="n">
         <v>367</v>
       </c>
-      <c r="G8" s="7" t="n">
+      <c r="G8" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="H8" s="5" t="n">
+      <c r="H8" s="4" t="n">
         <v>3479</v>
       </c>
-      <c r="I8" s="6" t="n">
+      <c r="I8" s="5" t="n">
         <v>479</v>
       </c>
-      <c r="J8" s="7" t="n">
+      <c r="J8" s="6" t="n">
         <v>349</v>
       </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="6"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="8" t="n">
+      <c r="B9" s="7" t="n">
         <v>347</v>
       </c>
-      <c r="C9" s="9" t="n">
+      <c r="C9" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="D9" s="10" t="n">
+      <c r="D9" s="9" t="n">
         <v>346</v>
       </c>
-      <c r="E9" s="8" t="n">
+      <c r="E9" s="7" t="n">
         <v>1467</v>
       </c>
-      <c r="F9" s="9" t="n">
+      <c r="F9" s="8" t="n">
         <v>367</v>
       </c>
-      <c r="G9" s="10" t="n">
+      <c r="G9" s="9" t="n">
         <v>14</v>
       </c>
-      <c r="H9" s="8" t="n">
+      <c r="H9" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="I9" s="9" t="n">
+      <c r="I9" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="J9" s="10" t="n">
+      <c r="J9" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="L9" s="8"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="6"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="11"/>
-      <c r="F10" s="6"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="12"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="4"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="7"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="10"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="4"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="7"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="10"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="4"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="7"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="10"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="13" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C22" s="13" t="n">
         <v>1</v>
@@ -9261,75 +9292,75 @@
   </sheetPr>
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="1" width="7.64"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="20" min="12" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="8.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="10" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="20" min="12" style="10" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="2" t="n">
+      <c r="B1" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="2" t="n">
+      <c r="C1" s="2"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3" t="n">
+      <c r="F1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="J1" s="4" t="n">
+      <c r="J1" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="1" t="s">
-        <v>10</v>
+      <c r="L1" s="1"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="10" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7" t="n">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6" t="n">
+      <c r="E2" s="4"/>
+      <c r="F2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="7" t="n">
+      <c r="G2" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="7"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="7"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="6"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="6"/>
       <c r="U2" s="13" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="V2" s="13" t="n">
         <v>1</v>
@@ -9348,30 +9379,30 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="8" t="n">
+      <c r="B3" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="8" t="n">
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10" t="n">
+      <c r="I3" s="8"/>
+      <c r="J3" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="10"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="9"/>
       <c r="U3" s="13" t="n">
         <v>15</v>
       </c>
@@ -9388,34 +9419,34 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2"/>
-      <c r="C4" s="3" t="n">
+      <c r="B4" s="1"/>
+      <c r="C4" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4" t="n">
+      <c r="E4" s="1"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="3" t="n">
+      <c r="H4" s="1"/>
+      <c r="I4" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="J4" s="4" t="n">
+      <c r="J4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="4"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="3"/>
       <c r="U4" s="13" t="n">
         <v>35</v>
       </c>
@@ -9432,46 +9463,46 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="10" t="n">
         <v>12489</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="6" t="n">
+      <c r="B5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="6" t="n">
+      <c r="D5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="G5" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="6" t="n">
+      <c r="H5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="J5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="7"/>
+      <c r="J5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="6"/>
       <c r="U5" s="13" t="n">
         <v>45</v>
       </c>
@@ -9490,36 +9521,36 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="8" t="n">
+      <c r="B6" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="9" t="n">
+      <c r="C6" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="10" t="n">
+      <c r="D6" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="E6" s="8" t="n">
+      <c r="E6" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="8" t="n">
+      <c r="F6" s="8"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="I6" s="9" t="n">
+      <c r="I6" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="10"/>
+      <c r="J6" s="9"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="9"/>
       <c r="U6" s="13" t="n">
         <v>75</v>
       </c>
@@ -9538,30 +9569,30 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4" t="n">
+      <c r="C7" s="2"/>
+      <c r="D7" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="4" t="n">
+      <c r="E7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="4"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="3"/>
       <c r="U7" s="13" t="n">
         <v>95</v>
       </c>
@@ -9578,170 +9609,170 @@
       <c r="Z7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="5" t="n">
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F8" s="6" t="n">
+      <c r="F8" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="5" t="n">
+      <c r="G8" s="6"/>
+      <c r="H8" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="7"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="7"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="6"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="8" t="n">
+      <c r="B9" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="C9" s="9" t="n">
+      <c r="C9" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10" t="n">
+      <c r="D9" s="9"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="10" t="n">
+      <c r="H9" s="7"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="L9" s="8"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="10"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="17"/>
-      <c r="F10" s="6"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="7"/>
+      <c r="F10" s="5"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="4"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="7"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="10"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="4"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="7"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="10"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="4"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="7"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="10"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B10">
@@ -10004,32 +10035,32 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="1" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="10" width="7.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="4"/>
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5"/>
+      <c r="A2" s="4"/>
       <c r="B2" s="18"/>
       <c r="C2" s="19"/>
       <c r="D2" s="20"/>
-      <c r="E2" s="6"/>
+      <c r="E2" s="5"/>
       <c r="F2" s="21" t="n">
         <v>8</v>
       </c>
@@ -10037,29 +10068,29 @@
       <c r="H2" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="I2" s="7"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="24"/>
-      <c r="C3" s="10"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="25" t="n">
         <v>5</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="8"/>
       <c r="F3" s="26"/>
-      <c r="G3" s="8"/>
+      <c r="G3" s="7"/>
       <c r="H3" s="27"/>
-      <c r="I3" s="10" t="n">
+      <c r="I3" s="9" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
+      <c r="A4" s="1"/>
       <c r="B4" s="28"/>
       <c r="C4" s="29"/>
       <c r="D4" s="30"/>
-      <c r="E4" s="3"/>
+      <c r="E4" s="2"/>
       <c r="F4" s="31" t="n">
         <v>4</v>
       </c>
@@ -10067,57 +10098,57 @@
       <c r="H4" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="I4" s="4"/>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="7"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="34"/>
       <c r="C6" s="35"/>
       <c r="D6" s="36" t="n">
         <v>7</v>
       </c>
-      <c r="E6" s="9"/>
+      <c r="E6" s="8"/>
       <c r="F6" s="37"/>
       <c r="G6" s="38"/>
       <c r="H6" s="39"/>
-      <c r="I6" s="10"/>
+      <c r="I6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
+      <c r="A7" s="1"/>
       <c r="B7" s="40" t="n">
         <v>8</v>
       </c>
-      <c r="C7" s="4" t="n">
+      <c r="C7" s="3" t="n">
         <v>5</v>
       </c>
       <c r="D7" s="41"/>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="2" t="n">
         <v>4</v>
       </c>
       <c r="F7" s="42"/>
-      <c r="G7" s="2"/>
+      <c r="G7" s="1"/>
       <c r="H7" s="43"/>
-      <c r="I7" s="4"/>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
+      <c r="A8" s="4"/>
       <c r="B8" s="44"/>
       <c r="C8" s="45" t="n">
         <v>9</v>
       </c>
       <c r="D8" s="46"/>
-      <c r="E8" s="6" t="n">
+      <c r="E8" s="5" t="n">
         <v>1</v>
       </c>
       <c r="F8" s="47"/>
@@ -10125,22 +10156,22 @@
       <c r="H8" s="49" t="n">
         <v>7</v>
       </c>
-      <c r="I8" s="7"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="10" t="n">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9" t="n">
+      <c r="G9" s="7"/>
+      <c r="H9" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="I9" s="10"/>
+      <c r="I9" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A9">
@@ -10253,46 +10284,46 @@
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G44" activeCellId="0" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="4.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14"/>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
+      <c r="D2" s="10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14"/>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
+      <c r="D3" s="10" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>21</v>
+      <c r="B5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10302,11 +10333,11 @@
       <c r="A7" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>23</v>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10316,11 +10347,11 @@
       <c r="A9" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>25</v>
+      <c r="B9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10330,11 +10361,11 @@
       <c r="A11" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>27</v>
+      <c r="B11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
two branches to look at error in scanning
</commit_message>
<xml_diff>
--- a/data/SDK.xlsx
+++ b/data/SDK.xlsx
@@ -5518,271 +5518,251 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="C1" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3" t="n">
-        <v>5</v>
-      </c>
       <c r="D1" s="1" t="n">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="E1" s="2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F1" s="3" t="n">
         <v>9</v>
       </c>
       <c r="G1" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H1" s="2" t="n">
-        <v>6</v>
+        <v>258</v>
       </c>
       <c r="I1" s="3" t="n">
-        <v>3</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="C2" s="6" t="n">
+        <v>358</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>358</v>
+      </c>
+      <c r="H2" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="C2" s="6" t="n">
+      <c r="I2" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" s="5" t="n">
+      <c r="D3" s="7" t="n">
+        <v>38</v>
+      </c>
+      <c r="E3" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="G2" s="4" t="n">
+      <c r="F3" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="H2" s="5" t="n">
+      <c r="G3" s="7"/>
+      <c r="H3" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="I2" s="6" t="n">
+      <c r="I3" s="9" t="n">
         <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="B3" s="8" t="n">
-        <v>9</v>
-      </c>
-      <c r="C3" s="9" t="n">
-        <v>3</v>
-      </c>
-      <c r="D3" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="E3" s="8" t="n">
-        <v>8</v>
-      </c>
-      <c r="F3" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G3" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="H3" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="I3" s="9" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="n">
         <v>8</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>2</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
+        <v>156</v>
+      </c>
+      <c r="B5" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="C5" s="6" t="n">
+        <v>56</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="H5" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="n">
+      <c r="I5" s="6" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8" t="n">
+        <v>9</v>
+      </c>
+      <c r="I6" s="9" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D5" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F5" s="6" t="n">
+      <c r="E7" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="G7" s="1" t="n">
         <v>7</v>
-      </c>
-      <c r="G5" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="I5" s="6" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
-        <v>9</v>
-      </c>
-      <c r="B6" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="C6" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="E6" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="F6" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="G6" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="H6" s="8" t="n">
-        <v>8</v>
-      </c>
-      <c r="I6" s="9" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="C7" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F7" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>2</v>
       </c>
       <c r="H7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>4</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C8" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="F8" s="6" t="n">
         <v>8</v>
-      </c>
-      <c r="D8" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F8" s="6" t="n">
-        <v>2</v>
       </c>
       <c r="G8" s="4" t="n">
         <v>6</v>
       </c>
       <c r="H8" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="I8" s="6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="F9" s="9" t="n">
+        <v>36</v>
+      </c>
+      <c r="G9" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="I8" s="6" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="D9" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="E9" s="8" t="n">
-        <v>9</v>
-      </c>
-      <c r="F9" s="9" t="n">
+      <c r="H9" s="8" t="n">
+        <v>28</v>
+      </c>
+      <c r="I9" s="9" t="n">
         <v>4</v>
-      </c>
-      <c r="G9" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="H9" s="8" t="n">
-        <v>5</v>
-      </c>
-      <c r="I9" s="9" t="n">
-        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5887,7 +5867,7 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -6771,7 +6751,7 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -7526,7 +7506,7 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -8409,7 +8389,7 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K27" activeCellId="0" sqref="K27"/>
     </sheetView>
   </sheetViews>
@@ -9292,7 +9272,7 @@
   </sheetPr>
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -10035,7 +10015,7 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -10284,7 +10264,7 @@
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="168" zoomScaleNormal="168" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G44" activeCellId="0" sqref="G44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ensure df is only the 9x9 and ignores other cells in excel sheet
</commit_message>
<xml_diff>
--- a/data/SDK.xlsx
+++ b/data/SDK.xlsx
@@ -90,11 +90,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -119,6 +120,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -151,7 +160,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="44">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -181,6 +190,13 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right/>
       <top/>
@@ -190,6 +206,13 @@
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="medium"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -213,6 +236,13 @@
       <right style="medium"/>
       <top/>
       <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -465,7 +495,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -482,7 +512,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -490,27 +524,35 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -526,7 +568,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -534,19 +576,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -666,6 +696,18 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5516,273 +5558,309 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1048576"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="C1" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3" t="n">
-        <v>5</v>
-      </c>
       <c r="D1" s="1" t="n">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="E1" s="2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F1" s="3" t="n">
         <v>9</v>
       </c>
       <c r="G1" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H1" s="2" t="n">
+        <v>258</v>
+      </c>
+      <c r="I1" s="3" t="n">
+        <v>258</v>
+      </c>
+      <c r="K1" s="4" t="n">
+        <f aca="false">IF(COUNTIF($A$1:$I$9,1)=9,1,"")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="B2" s="6" t="n">
+        <v>35</v>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>358</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="H2" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="B2" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="C2" s="6" t="n">
+      <c r="I2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="8" t="str">
+        <f aca="false">IF(COUNTIF($A$1:$I$9,2)=9,2,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="n">
+        <v>268</v>
+      </c>
+      <c r="B3" s="10" t="n">
+        <v>236</v>
+      </c>
+      <c r="C3" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" s="5" t="n">
+      <c r="D3" s="9" t="n">
+        <v>38</v>
+      </c>
+      <c r="E3" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="G2" s="4" t="n">
+      <c r="F3" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="H2" s="5" t="n">
+      <c r="G3" s="9" t="n">
+        <v>238</v>
+      </c>
+      <c r="H3" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="I2" s="6" t="n">
+      <c r="I3" s="11" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="B3" s="8" t="n">
-        <v>9</v>
-      </c>
-      <c r="C3" s="9" t="n">
-        <v>3</v>
-      </c>
-      <c r="D3" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="E3" s="8" t="n">
-        <v>8</v>
-      </c>
-      <c r="F3" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G3" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="H3" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="I3" s="9" t="n">
-        <v>1</v>
+      <c r="K3" s="8" t="str">
+        <f aca="false">IF(COUNTIF($A$1:$I$9,3)=9,3,"")</f>
+        <v/>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="n">
         <v>8</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>2</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="K4" s="8" t="n">
+        <f aca="false">IF(COUNTIF($A$1:$I$9,4)=9,4,"")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>56</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>56</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="H4" s="2" t="n">
+      <c r="F5" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I5" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="K5" s="8" t="str">
+        <f aca="false">IF(COUNTIF($A$1:$I$9,5)=9,5,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="G6" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="H6" s="10" t="n">
+        <v>9</v>
+      </c>
+      <c r="I6" s="11" t="n">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F5" s="6" t="n">
-        <v>7</v>
-      </c>
-      <c r="G5" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="I5" s="6" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
-        <v>9</v>
-      </c>
-      <c r="B6" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="C6" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="E6" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="F6" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="G6" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="H6" s="8" t="n">
-        <v>8</v>
-      </c>
-      <c r="I6" s="9" t="n">
-        <v>2</v>
+      <c r="K6" s="8" t="str">
+        <f aca="false">IF(COUNTIF($A$1:$I$9,6)=9,6,"")</f>
+        <v/>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>3</v>
+        <v>568</v>
       </c>
       <c r="B7" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>3568</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="G7" s="1" t="n">
         <v>7</v>
-      </c>
-      <c r="C7" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F7" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>2</v>
       </c>
       <c r="H7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="I7" s="3" t="n">
+        <v>58</v>
+      </c>
+      <c r="K7" s="8" t="n">
+        <f aca="false">IF(COUNTIF($A$1:$I$9,7)=9,7,"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="n">
+      <c r="B8" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>25</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="F8" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="H8" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="I8" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K8" s="8" t="str">
+        <f aca="false">IF(COUNTIF($A$1:$I$9,8)=9,8,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="n">
+        <v>268</v>
+      </c>
+      <c r="B9" s="10" t="n">
+        <v>2368</v>
+      </c>
+      <c r="C9" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="5" t="n">
+      <c r="F9" s="11" t="n">
+        <v>36</v>
+      </c>
+      <c r="G9" s="9" t="n">
+        <v>9</v>
+      </c>
+      <c r="H9" s="10" t="n">
+        <v>28</v>
+      </c>
+      <c r="I9" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="C8" s="6" t="n">
-        <v>8</v>
-      </c>
-      <c r="D8" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="F8" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="H8" s="5" t="n">
+      <c r="K9" s="12" t="n">
+        <f aca="false">IF(COUNTIF($A$1:$I$9,9)=9,9,"")</f>
         <v>9</v>
-      </c>
-      <c r="I8" s="6" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="D9" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="E9" s="8" t="n">
-        <v>9</v>
-      </c>
-      <c r="F9" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="G9" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="H9" s="8" t="n">
-        <v>5</v>
-      </c>
-      <c r="I9" s="9" t="n">
-        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5888,47 +5966,39 @@
   <dimension ref="B1:U27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="1.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="10" width="7.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="6.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="12" style="10" width="8.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="10" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="10" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="1.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="13" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="13" width="6.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="12" style="13" width="8.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="13" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="13" width="3.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="n">
-        <v>4789</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C1" s="2"/>
       <c r="D1" s="3" t="n">
-        <v>289</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>3</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E1" s="1"/>
       <c r="F1" s="2" t="n">
-        <v>479</v>
+        <v>6</v>
       </c>
       <c r="G1" s="3" t="n">
-        <v>289</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1" t="n">
-        <v>78</v>
-      </c>
-      <c r="I1" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J1" s="3" t="n">
-        <v>6</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="3"/>
       <c r="L1" s="1"/>
       <c r="M1" s="2"/>
       <c r="N1" s="3"/>
@@ -5938,114 +6008,96 @@
       <c r="R1" s="1"/>
       <c r="S1" s="2"/>
       <c r="T1" s="3"/>
-      <c r="U1" s="5"/>
+      <c r="U1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="4" t="n">
-        <v>29</v>
-      </c>
-      <c r="C2" s="5" t="n">
-        <v>3789</v>
-      </c>
-      <c r="D2" s="6" t="n">
+      <c r="B2" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="F2" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="n">
-        <v>279</v>
-      </c>
-      <c r="F2" s="5" t="n">
+      <c r="J2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="6" t="n">
+      <c r="L2" s="5"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="6"/>
+    </row>
+    <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="n">
-        <v>378</v>
-      </c>
-      <c r="I2" s="5" t="n">
-        <v>389</v>
-      </c>
-      <c r="J2" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="5"/>
-    </row>
-    <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="8" t="n">
-        <v>34789</v>
-      </c>
-      <c r="D3" s="9" t="n">
-        <v>389</v>
-      </c>
-      <c r="E3" s="7" t="n">
-        <v>679</v>
-      </c>
-      <c r="F3" s="8" t="n">
-        <v>34679</v>
-      </c>
-      <c r="G3" s="9" t="n">
-        <v>689</v>
-      </c>
-      <c r="H3" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="I3" s="8" t="n">
-        <v>389</v>
-      </c>
-      <c r="J3" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="5"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="J3" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="L3" s="9"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="F4" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3" t="n">
+      <c r="G4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="E4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="H4" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="I4" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="J4" s="3" t="n">
-        <v>3</v>
-      </c>
+      <c r="J4" s="3"/>
       <c r="L4" s="1"/>
       <c r="M4" s="2"/>
       <c r="N4" s="3"/>
@@ -6055,115 +6107,95 @@
       <c r="R4" s="1"/>
       <c r="S4" s="2"/>
       <c r="T4" s="3"/>
-      <c r="U4" s="5"/>
+      <c r="U4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4" t="n">
-        <v>29</v>
-      </c>
-      <c r="C5" s="5" t="n">
+      <c r="B5" s="5"/>
+      <c r="C5" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="G5" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="J5" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="K5" s="6"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="6"/>
+    </row>
+    <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="9"/>
+      <c r="C6" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="10" t="n">
+        <v>9</v>
+      </c>
+      <c r="J6" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="D5" s="6" t="n">
-        <v>29</v>
-      </c>
-      <c r="E5" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="F5" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="G5" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="H5" s="4" t="n">
+      <c r="L6" s="9"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="6"/>
+    </row>
+    <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="1"/>
+      <c r="C7" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="I5" s="5" t="n">
+      <c r="G7" s="3"/>
+      <c r="H7" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="J5" s="6" t="n">
+      <c r="I7" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="C6" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="E6" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="F6" s="8" t="n">
-        <v>69</v>
-      </c>
-      <c r="G6" s="9" t="n">
-        <v>69</v>
-      </c>
-      <c r="H6" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="I6" s="8" t="n">
-        <v>5</v>
-      </c>
-      <c r="J6" s="9" t="n">
-        <v>8</v>
-      </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>38</v>
-      </c>
-      <c r="D7" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>37</v>
-      </c>
-      <c r="G7" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="H7" s="1" t="n">
-        <v>138</v>
-      </c>
-      <c r="I7" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="J7" s="3" t="n">
-        <v>9</v>
-      </c>
+      <c r="J7" s="3"/>
       <c r="L7" s="1"/>
       <c r="M7" s="2"/>
       <c r="N7" s="3"/>
@@ -6173,96 +6205,84 @@
       <c r="R7" s="1"/>
       <c r="S7" s="2"/>
       <c r="T7" s="3"/>
-      <c r="U7" s="5"/>
+      <c r="U7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="4" t="n">
+      <c r="B8" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="C8" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="D8" s="6" t="n">
-        <v>139</v>
-      </c>
-      <c r="E8" s="4" t="n">
+      <c r="C8" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="G8" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="L8" s="5"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="E9" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="F8" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="G8" s="6" t="n">
-        <v>19</v>
-      </c>
-      <c r="H8" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="I8" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="J8" s="6" t="n">
-        <v>7</v>
-      </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="5"/>
-    </row>
-    <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="C9" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" s="9" t="n">
-        <v>1389</v>
-      </c>
-      <c r="E9" s="7" t="n">
-        <v>69</v>
-      </c>
-      <c r="F9" s="8" t="n">
-        <v>369</v>
-      </c>
-      <c r="G9" s="9" t="n">
+      <c r="G9" s="11"/>
+      <c r="H9" s="9" t="n">
+        <v>9</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="H9" s="7" t="n">
-        <v>138</v>
-      </c>
-      <c r="I9" s="8" t="n">
-        <v>38</v>
-      </c>
-      <c r="J9" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="5"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6277,26 +6297,26 @@
       <c r="J12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="6"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1"/>
@@ -6310,26 +6330,26 @@
       <c r="J15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="6"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="1"/>
@@ -6343,130 +6363,130 @@
       <c r="J18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="6"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="13" t="n">
+      <c r="C22" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="13" t="n">
+      <c r="D22" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="13" t="n">
+      <c r="E22" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="13" t="n">
+      <c r="F22" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="13" t="n">
+      <c r="G22" s="16" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="13" t="n">
+      <c r="B23" s="16" t="n">
         <v>15</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14" t="n">
+      <c r="C23" s="17"/>
+      <c r="D23" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14" t="n">
+      <c r="E23" s="17"/>
+      <c r="F23" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="G23" s="14" t="n">
+      <c r="G23" s="17" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="13" t="n">
+      <c r="B24" s="16" t="n">
         <v>35</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14" t="n">
+      <c r="C24" s="17"/>
+      <c r="D24" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14" t="n">
+      <c r="E24" s="17"/>
+      <c r="F24" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="G24" s="14" t="n">
+      <c r="G24" s="17" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="13" t="n">
+      <c r="B25" s="16" t="n">
         <v>45</v>
       </c>
-      <c r="C25" s="15" t="n">
+      <c r="C25" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="14" t="n">
+      <c r="D25" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14" t="n">
+      <c r="E25" s="17"/>
+      <c r="F25" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="G25" s="14" t="n">
+      <c r="G25" s="17" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="13" t="n">
+      <c r="B26" s="16" t="n">
         <v>75</v>
       </c>
-      <c r="C26" s="14" t="n">
+      <c r="C26" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14" t="n">
+      <c r="D26" s="17"/>
+      <c r="E26" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="15" t="n">
+      <c r="F26" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G26" s="15" t="n">
+      <c r="G26" s="18" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="13" t="n">
+      <c r="B27" s="16" t="n">
         <v>95</v>
       </c>
-      <c r="C27" s="14" t="n">
+      <c r="C27" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14" t="n">
+      <c r="D27" s="17"/>
+      <c r="E27" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="F27" s="15" t="n">
+      <c r="F27" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="14"/>
+      <c r="G27" s="17"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B10">
@@ -6777,11 +6797,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="1.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="10" width="7.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="6.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="10" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="10" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="1.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="13" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="13" width="6.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="13" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="13" width="3.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6809,67 +6829,67 @@
       <c r="R1" s="1"/>
       <c r="S1" s="2"/>
       <c r="T1" s="3"/>
-      <c r="U1" s="5"/>
+      <c r="U1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="4" t="n">
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F2" s="5" t="n">
+      <c r="F2" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="4" t="n">
+      <c r="G2" s="7"/>
+      <c r="H2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I2" s="5" t="n">
+      <c r="I2" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="5"/>
+      <c r="J2" s="7"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="7" t="n">
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="8" t="n">
+      <c r="F3" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="7" t="n">
+      <c r="G3" s="11"/>
+      <c r="H3" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="I3" s="8" t="n">
+      <c r="I3" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="J3" s="9" t="n">
+      <c r="J3" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="5"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
@@ -6896,66 +6916,66 @@
       <c r="R4" s="1"/>
       <c r="S4" s="2"/>
       <c r="T4" s="3"/>
-      <c r="U4" s="5"/>
+      <c r="U4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4" t="n">
+      <c r="B5" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5" t="n">
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="4" t="n">
+      <c r="G5" s="7"/>
+      <c r="H5" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="6" t="n">
+      <c r="I5" s="6"/>
+      <c r="J5" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="5"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9" t="n">
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="F6" s="8" t="n">
+      <c r="F6" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="7" t="n">
+      <c r="G6" s="11"/>
+      <c r="H6" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="9"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="5"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="11"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="n">
@@ -6986,80 +7006,80 @@
       <c r="R7" s="1"/>
       <c r="S7" s="2"/>
       <c r="T7" s="3"/>
-      <c r="U7" s="5"/>
+      <c r="U7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="4"/>
-      <c r="C8" s="5" t="n">
+      <c r="B8" s="5"/>
+      <c r="C8" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="D8" s="6" t="n">
+      <c r="D8" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="5" t="n">
+      <c r="E8" s="5"/>
+      <c r="F8" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="G8" s="6" t="n">
+      <c r="G8" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="5" t="n">
+      <c r="H8" s="5"/>
+      <c r="I8" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="J8" s="6" t="n">
+      <c r="J8" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="7" t="n">
+      <c r="B9" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9" t="n">
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="H9" s="7" t="n">
+      <c r="H9" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="I9" s="8" t="n">
+      <c r="I9" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="J9" s="9"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="5"/>
+      <c r="J9" s="11"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7074,26 +7094,26 @@
       <c r="J12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="6"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1"/>
@@ -7107,26 +7127,26 @@
       <c r="J15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="6"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="1"/>
@@ -7140,130 +7160,130 @@
       <c r="J18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="6"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="13" t="n">
+      <c r="C22" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="13" t="n">
+      <c r="D22" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="13" t="n">
+      <c r="E22" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="13" t="n">
+      <c r="F22" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="13" t="n">
+      <c r="G22" s="16" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="13" t="n">
+      <c r="B23" s="16" t="n">
         <v>15</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14" t="n">
+      <c r="C23" s="17"/>
+      <c r="D23" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14" t="n">
+      <c r="E23" s="17"/>
+      <c r="F23" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="G23" s="14" t="n">
+      <c r="G23" s="17" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="13" t="n">
+      <c r="B24" s="16" t="n">
         <v>35</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14" t="n">
+      <c r="C24" s="17"/>
+      <c r="D24" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14" t="n">
+      <c r="E24" s="17"/>
+      <c r="F24" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="G24" s="14" t="n">
+      <c r="G24" s="17" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="13" t="n">
+      <c r="B25" s="16" t="n">
         <v>45</v>
       </c>
-      <c r="C25" s="15" t="n">
+      <c r="C25" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="14" t="n">
+      <c r="D25" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14" t="n">
+      <c r="E25" s="17"/>
+      <c r="F25" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="G25" s="14" t="n">
+      <c r="G25" s="17" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="13" t="n">
+      <c r="B26" s="16" t="n">
         <v>75</v>
       </c>
-      <c r="C26" s="14" t="n">
+      <c r="C26" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14" t="n">
+      <c r="D26" s="17"/>
+      <c r="E26" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="15" t="n">
+      <c r="F26" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G26" s="15" t="n">
+      <c r="G26" s="18" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="13" t="n">
+      <c r="B27" s="16" t="n">
         <v>95</v>
       </c>
-      <c r="C27" s="14" t="n">
+      <c r="C27" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14" t="n">
+      <c r="D27" s="17"/>
+      <c r="E27" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="F27" s="15" t="n">
+      <c r="F27" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="14"/>
+      <c r="G27" s="17"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B10">
@@ -7532,11 +7552,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="1.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="10" width="7.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="6.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="10" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="10" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="1.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="13" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="13" width="6.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="13" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="13" width="3.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7576,85 +7596,85 @@
       <c r="R1" s="1"/>
       <c r="S1" s="2"/>
       <c r="T1" s="3"/>
-      <c r="U1" s="5"/>
+      <c r="U1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="C2" s="5" t="n">
+      <c r="C2" s="6" t="n">
         <v>1467</v>
       </c>
-      <c r="D2" s="6" t="n">
+      <c r="D2" s="7" t="n">
         <v>1467</v>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="E2" s="5" t="n">
         <v>25</v>
       </c>
-      <c r="F2" s="5" t="n">
+      <c r="F2" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="G2" s="6" t="n">
+      <c r="G2" s="7" t="n">
         <v>25</v>
       </c>
-      <c r="H2" s="4" t="n">
+      <c r="H2" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="I2" s="5" t="n">
+      <c r="I2" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="J2" s="6" t="n">
+      <c r="J2" s="7" t="n">
         <v>178</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="7" t="n">
+      <c r="B3" s="9" t="n">
         <v>18</v>
       </c>
-      <c r="C3" s="8" t="n">
+      <c r="C3" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="D3" s="9" t="n">
+      <c r="D3" s="11" t="n">
         <v>178</v>
       </c>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="F3" s="8" t="n">
+      <c r="F3" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="G3" s="9" t="n">
+      <c r="G3" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="H3" s="7" t="n">
+      <c r="H3" s="9" t="n">
         <v>17</v>
       </c>
-      <c r="I3" s="8" t="n">
+      <c r="I3" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="J3" s="9" t="n">
+      <c r="J3" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="5"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="n">
@@ -7693,86 +7713,86 @@
       <c r="R4" s="1"/>
       <c r="S4" s="2"/>
       <c r="T4" s="3"/>
-      <c r="U4" s="5"/>
+      <c r="U4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4" t="n">
+      <c r="B5" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="D5" s="6" t="n">
+      <c r="D5" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="F5" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="G5" s="6" t="n">
+      <c r="G5" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="H5" s="4" t="n">
+      <c r="H5" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="I5" s="5" t="n">
+      <c r="I5" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="J5" s="6" t="n">
+      <c r="J5" s="7" t="n">
         <v>13</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="5"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="7" t="n">
+      <c r="B6" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="C6" s="8" t="n">
+      <c r="C6" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="D6" s="9" t="n">
+      <c r="D6" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="F6" s="8" t="n">
+      <c r="F6" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="G6" s="9" t="n">
+      <c r="G6" s="11" t="n">
         <v>13</v>
       </c>
-      <c r="H6" s="7" t="n">
+      <c r="H6" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="I6" s="8" t="n">
+      <c r="I6" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="J6" s="9" t="n">
+      <c r="J6" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="5"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="n">
@@ -7811,96 +7831,96 @@
       <c r="R7" s="1"/>
       <c r="S7" s="2"/>
       <c r="T7" s="3"/>
-      <c r="U7" s="5"/>
+      <c r="U7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="4" t="n">
+      <c r="B8" s="5" t="n">
         <v>148</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="6" t="n">
         <v>1467</v>
       </c>
-      <c r="D8" s="6" t="n">
+      <c r="D8" s="7" t="n">
         <v>14678</v>
       </c>
-      <c r="E8" s="4" t="n">
+      <c r="E8" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="F8" s="5" t="n">
+      <c r="F8" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="G8" s="6" t="n">
+      <c r="G8" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="H8" s="4" t="n">
+      <c r="H8" s="5" t="n">
         <v>1357</v>
       </c>
-      <c r="I8" s="5" t="n">
+      <c r="I8" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="J8" s="6" t="n">
+      <c r="J8" s="7" t="n">
         <v>13678</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="7" t="n">
+      <c r="B9" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="8" t="n">
+      <c r="C9" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="D9" s="9" t="n">
+      <c r="D9" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="E9" s="7" t="n">
+      <c r="E9" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="F9" s="8" t="n">
+      <c r="F9" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="G9" s="9" t="n">
+      <c r="G9" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="H9" s="7" t="n">
+      <c r="H9" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="I9" s="8" t="n">
+      <c r="I9" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="J9" s="9" t="n">
+      <c r="J9" s="11" t="n">
         <v>17</v>
       </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="5"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7915,26 +7935,26 @@
       <c r="J12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="6"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1"/>
@@ -7948,26 +7968,26 @@
       <c r="J15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="6"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="1"/>
@@ -7981,130 +8001,130 @@
       <c r="J18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="6"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="13" t="n">
+      <c r="C22" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="13" t="n">
+      <c r="D22" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="13" t="n">
+      <c r="E22" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="13" t="n">
+      <c r="F22" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="13" t="n">
+      <c r="G22" s="16" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="13" t="n">
+      <c r="B23" s="16" t="n">
         <v>15</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14" t="n">
+      <c r="C23" s="17"/>
+      <c r="D23" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14" t="n">
+      <c r="E23" s="17"/>
+      <c r="F23" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="G23" s="14" t="n">
+      <c r="G23" s="17" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="13" t="n">
+      <c r="B24" s="16" t="n">
         <v>35</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14" t="n">
+      <c r="C24" s="17"/>
+      <c r="D24" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14" t="n">
+      <c r="E24" s="17"/>
+      <c r="F24" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="G24" s="14" t="n">
+      <c r="G24" s="17" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="13" t="n">
+      <c r="B25" s="16" t="n">
         <v>45</v>
       </c>
-      <c r="C25" s="15" t="n">
+      <c r="C25" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="14" t="n">
+      <c r="D25" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14" t="n">
+      <c r="E25" s="17"/>
+      <c r="F25" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="G25" s="14" t="n">
+      <c r="G25" s="17" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="13" t="n">
+      <c r="B26" s="16" t="n">
         <v>75</v>
       </c>
-      <c r="C26" s="14" t="n">
+      <c r="C26" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14" t="n">
+      <c r="D26" s="17"/>
+      <c r="E26" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="15" t="n">
+      <c r="F26" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G26" s="15" t="n">
+      <c r="G26" s="18" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="13" t="n">
+      <c r="B27" s="16" t="n">
         <v>95</v>
       </c>
-      <c r="C27" s="14" t="n">
+      <c r="C27" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14" t="n">
+      <c r="D27" s="17"/>
+      <c r="E27" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="F27" s="15" t="n">
+      <c r="F27" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="14"/>
+      <c r="G27" s="17"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B10">
@@ -8415,11 +8435,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="1.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="10" width="7.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="6.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="10" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="10" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="1.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="13" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="13" width="6.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="13" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="13" width="3.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8459,85 +8479,85 @@
       <c r="R1" s="1"/>
       <c r="S1" s="2"/>
       <c r="T1" s="3"/>
-      <c r="U1" s="5"/>
+      <c r="U1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="5" t="n">
         <v>458</v>
       </c>
-      <c r="C2" s="5" t="n">
+      <c r="C2" s="6" t="n">
         <v>45</v>
       </c>
-      <c r="D2" s="6" t="n">
+      <c r="D2" s="7" t="n">
         <v>458</v>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="E2" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="F2" s="5" t="n">
+      <c r="F2" s="6" t="n">
         <v>67</v>
       </c>
-      <c r="G2" s="6" t="n">
+      <c r="G2" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="H2" s="4" t="n">
+      <c r="H2" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="I2" s="5" t="n">
+      <c r="I2" s="6" t="n">
         <v>67</v>
       </c>
-      <c r="J2" s="6" t="n">
+      <c r="J2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="7" t="n">
+      <c r="B3" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="C3" s="8" t="n">
+      <c r="C3" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="D3" s="9" t="n">
+      <c r="D3" s="11" t="n">
         <v>19</v>
       </c>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="9" t="n">
         <v>14</v>
       </c>
-      <c r="F3" s="8" t="n">
+      <c r="F3" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="9" t="n">
+      <c r="G3" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="H3" s="7" t="n">
+      <c r="H3" s="9" t="n">
         <v>49</v>
       </c>
-      <c r="I3" s="8" t="n">
+      <c r="I3" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="J3" s="9" t="n">
+      <c r="J3" s="11" t="n">
         <v>8</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="5"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="n">
@@ -8576,86 +8596,86 @@
       <c r="R4" s="1"/>
       <c r="S4" s="2"/>
       <c r="T4" s="3"/>
-      <c r="U4" s="5"/>
+      <c r="U4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4" t="n">
+      <c r="B5" s="5" t="n">
         <v>348</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="6" t="n">
         <v>146</v>
       </c>
-      <c r="D5" s="6" t="n">
+      <c r="D5" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="F5" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="G5" s="6" t="n">
+      <c r="G5" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="H5" s="4" t="n">
+      <c r="H5" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I5" s="5" t="n">
+      <c r="I5" s="6" t="n">
         <v>468</v>
       </c>
-      <c r="J5" s="6" t="n">
+      <c r="J5" s="7" t="n">
         <v>34</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="5"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="7" t="n">
+      <c r="B6" s="9" t="n">
         <v>458</v>
       </c>
-      <c r="C6" s="8" t="n">
+      <c r="C6" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="D6" s="9" t="n">
+      <c r="D6" s="11" t="n">
         <v>458</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="F6" s="8" t="n">
+      <c r="F6" s="10" t="n">
         <v>145</v>
       </c>
-      <c r="G6" s="9" t="n">
+      <c r="G6" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="H6" s="7" t="n">
+      <c r="H6" s="9" t="n">
         <v>149</v>
       </c>
-      <c r="I6" s="8" t="n">
+      <c r="I6" s="10" t="n">
         <v>489</v>
       </c>
-      <c r="J6" s="9" t="n">
+      <c r="J6" s="11" t="n">
         <v>7</v>
       </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="5"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="n">
@@ -8694,96 +8714,96 @@
       <c r="R7" s="1"/>
       <c r="S7" s="2"/>
       <c r="T7" s="3"/>
-      <c r="U7" s="5"/>
+      <c r="U7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="4" t="n">
+      <c r="B8" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="6" t="n">
         <v>46</v>
       </c>
-      <c r="D8" s="6" t="n">
+      <c r="D8" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="E8" s="4" t="n">
+      <c r="E8" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="F8" s="5" t="n">
+      <c r="F8" s="6" t="n">
         <v>367</v>
       </c>
-      <c r="G8" s="6" t="n">
+      <c r="G8" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="H8" s="4" t="n">
+      <c r="H8" s="5" t="n">
         <v>3479</v>
       </c>
-      <c r="I8" s="5" t="n">
+      <c r="I8" s="6" t="n">
         <v>479</v>
       </c>
-      <c r="J8" s="6" t="n">
+      <c r="J8" s="7" t="n">
         <v>349</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="7" t="n">
+      <c r="B9" s="9" t="n">
         <v>347</v>
       </c>
-      <c r="C9" s="8" t="n">
+      <c r="C9" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="D9" s="9" t="n">
+      <c r="D9" s="11" t="n">
         <v>346</v>
       </c>
-      <c r="E9" s="7" t="n">
+      <c r="E9" s="9" t="n">
         <v>1467</v>
       </c>
-      <c r="F9" s="8" t="n">
+      <c r="F9" s="10" t="n">
         <v>367</v>
       </c>
-      <c r="G9" s="9" t="n">
+      <c r="G9" s="11" t="n">
         <v>14</v>
       </c>
-      <c r="H9" s="7" t="n">
+      <c r="H9" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="I9" s="8" t="n">
+      <c r="I9" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="J9" s="9" t="n">
+      <c r="J9" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="5"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8798,26 +8818,26 @@
       <c r="J12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="6"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1"/>
@@ -8831,26 +8851,26 @@
       <c r="J15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="6"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="1"/>
@@ -8864,130 +8884,130 @@
       <c r="J18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="6"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="13" t="n">
+      <c r="C22" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="13" t="n">
+      <c r="D22" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="13" t="n">
+      <c r="E22" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="13" t="n">
+      <c r="F22" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="13" t="n">
+      <c r="G22" s="16" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="13" t="n">
+      <c r="B23" s="16" t="n">
         <v>15</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14" t="n">
+      <c r="C23" s="17"/>
+      <c r="D23" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14" t="n">
+      <c r="E23" s="17"/>
+      <c r="F23" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="G23" s="14" t="n">
+      <c r="G23" s="17" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="13" t="n">
+      <c r="B24" s="16" t="n">
         <v>35</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14" t="n">
+      <c r="C24" s="17"/>
+      <c r="D24" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14" t="n">
+      <c r="E24" s="17"/>
+      <c r="F24" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="G24" s="14" t="n">
+      <c r="G24" s="17" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="13" t="n">
+      <c r="B25" s="16" t="n">
         <v>45</v>
       </c>
-      <c r="C25" s="15" t="n">
+      <c r="C25" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="14" t="n">
+      <c r="D25" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14" t="n">
+      <c r="E25" s="17"/>
+      <c r="F25" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="G25" s="14" t="n">
+      <c r="G25" s="17" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="13" t="n">
+      <c r="B26" s="16" t="n">
         <v>75</v>
       </c>
-      <c r="C26" s="14" t="n">
+      <c r="C26" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14" t="n">
+      <c r="D26" s="17"/>
+      <c r="E26" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="15" t="n">
+      <c r="F26" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G26" s="15" t="n">
+      <c r="G26" s="18" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="13" t="n">
+      <c r="B27" s="16" t="n">
         <v>95</v>
       </c>
-      <c r="C27" s="14" t="n">
+      <c r="C27" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14" t="n">
+      <c r="D27" s="17"/>
+      <c r="E27" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="F27" s="15" t="n">
+      <c r="F27" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="14"/>
+      <c r="G27" s="17"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B10">
@@ -9298,9 +9318,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="8.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="10" width="7.64"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="20" min="12" style="10" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="8.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="13" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="20" min="12" style="13" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9330,91 +9350,91 @@
       <c r="R1" s="1"/>
       <c r="S1" s="2"/>
       <c r="T1" s="3"/>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6" t="n">
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="5" t="n">
+      <c r="E2" s="5"/>
+      <c r="F2" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="6" t="n">
+      <c r="G2" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="6"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="13" t="s">
+      <c r="H2" s="5"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="7"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="V2" s="13" t="n">
+      <c r="V2" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="W2" s="13" t="n">
+      <c r="W2" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="X2" s="13" t="n">
+      <c r="X2" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="Y2" s="13" t="n">
+      <c r="Y2" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="Z2" s="13" t="n">
+      <c r="Z2" s="16" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="7" t="n">
+      <c r="B3" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="7" t="n">
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="9" t="n">
+      <c r="I3" s="10"/>
+      <c r="J3" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="13" t="n">
+      <c r="L3" s="9"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="16" t="n">
         <v>15</v>
       </c>
-      <c r="V3" s="14"/>
-      <c r="W3" s="16" t="n">
+      <c r="V3" s="17"/>
+      <c r="W3" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="16" t="n">
+      <c r="X3" s="17"/>
+      <c r="Y3" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="Z3" s="16" t="n">
+      <c r="Z3" s="19" t="n">
         <v>9</v>
       </c>
     </row>
@@ -9447,124 +9467,124 @@
       <c r="R4" s="1"/>
       <c r="S4" s="2"/>
       <c r="T4" s="3"/>
-      <c r="U4" s="13" t="n">
+      <c r="U4" s="16" t="n">
         <v>35</v>
       </c>
-      <c r="V4" s="14"/>
-      <c r="W4" s="16" t="n">
+      <c r="V4" s="17"/>
+      <c r="W4" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="16" t="n">
+      <c r="X4" s="17"/>
+      <c r="Y4" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="Z4" s="16" t="n">
+      <c r="Z4" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="n">
+      <c r="A5" s="13" t="n">
         <v>12489</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="F5" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="G5" s="6" t="n">
+      <c r="G5" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="5" t="n">
+      <c r="I5" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="13" t="n">
+      <c r="K5" s="6"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="16" t="n">
         <v>45</v>
       </c>
-      <c r="V5" s="15" t="n">
+      <c r="V5" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="W5" s="16" t="n">
+      <c r="W5" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="16" t="n">
+      <c r="X5" s="17"/>
+      <c r="Y5" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="Z5" s="16" t="n">
+      <c r="Z5" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="7" t="n">
+      <c r="B6" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="8" t="n">
+      <c r="C6" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="9" t="n">
+      <c r="D6" s="11" t="n">
         <v>7</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="7" t="n">
+      <c r="F6" s="10"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="I6" s="8" t="n">
+      <c r="I6" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="J6" s="9"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="13" t="n">
+      <c r="J6" s="11"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="16" t="n">
         <v>75</v>
       </c>
-      <c r="V6" s="14" t="n">
+      <c r="V6" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="W6" s="14"/>
-      <c r="X6" s="14" t="n">
+      <c r="W6" s="17"/>
+      <c r="X6" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="Y6" s="15" t="n">
+      <c r="Y6" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="Z6" s="15" t="n">
+      <c r="Z6" s="18" t="n">
         <v>9</v>
       </c>
     </row>
@@ -9593,86 +9613,86 @@
       <c r="R7" s="1"/>
       <c r="S7" s="2"/>
       <c r="T7" s="3"/>
-      <c r="U7" s="13" t="n">
+      <c r="U7" s="16" t="n">
         <v>95</v>
       </c>
-      <c r="V7" s="14" t="n">
+      <c r="V7" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="W7" s="14"/>
-      <c r="X7" s="14" t="n">
+      <c r="W7" s="17"/>
+      <c r="X7" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="Y7" s="15" t="n">
+      <c r="Y7" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="Z7" s="14"/>
+      <c r="Z7" s="17"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="4" t="n">
+      <c r="C8" s="6"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="F8" s="5" t="n">
+      <c r="F8" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="4" t="n">
+      <c r="G8" s="7"/>
+      <c r="H8" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="6"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="7"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="7" t="n">
+      <c r="B9" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="C9" s="8" t="n">
+      <c r="C9" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9" t="n">
+      <c r="D9" s="11"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="9" t="n">
+      <c r="H9" s="9"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="5"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="6"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="6"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9687,26 +9707,26 @@
       <c r="J12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="6"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1"/>
@@ -9720,26 +9740,26 @@
       <c r="J15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="6"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="1"/>
@@ -9753,26 +9773,26 @@
       <c r="J18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="6"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="11"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B10">
@@ -10041,7 +10061,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="10" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="13" width="7.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10056,122 +10076,122 @@
       <c r="I1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="21" t="n">
+      <c r="A2" s="5"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="24" t="n">
         <v>8</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="23" t="n">
+      <c r="G2" s="25"/>
+      <c r="H2" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="I2" s="6"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="25" t="n">
+      <c r="A3" s="9"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="9" t="n">
+      <c r="E3" s="10"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="11" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="31" t="n">
+      <c r="F4" s="34" t="n">
         <v>4</v>
       </c>
-      <c r="G4" s="32"/>
-      <c r="H4" s="33" t="n">
+      <c r="G4" s="35"/>
+      <c r="H4" s="36" t="n">
         <v>1</v>
       </c>
       <c r="I4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="6"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="36" t="n">
+      <c r="A6" s="9"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="39" t="n">
         <v>7</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
-      <c r="B7" s="40" t="n">
+      <c r="B7" s="43" t="n">
         <v>8</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="41"/>
+      <c r="D7" s="44"/>
       <c r="E7" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="F7" s="42"/>
+      <c r="F7" s="45"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="43"/>
+      <c r="H7" s="46"/>
       <c r="I7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="45" t="n">
+      <c r="A8" s="5"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="48" t="n">
         <v>9</v>
       </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="5" t="n">
+      <c r="D8" s="49"/>
+      <c r="E8" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="47"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="49" t="n">
+      <c r="F8" s="50"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="52" t="n">
         <v>7</v>
       </c>
-      <c r="I8" s="6"/>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9" t="n">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8" t="n">
+      <c r="G9" s="9"/>
+      <c r="H9" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="I9" s="9"/>
+      <c r="I9" s="11"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A9">
@@ -10290,102 +10310,102 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="4.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="4.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14"/>
-      <c r="D2" s="10" t="s">
+      <c r="A2" s="17"/>
+      <c r="D2" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14"/>
-      <c r="D3" s="10" t="s">
+      <c r="A3" s="17"/>
+      <c r="D3" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="n">
+      <c r="A5" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14"/>
+      <c r="A6" s="17"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="n">
+      <c r="A7" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14"/>
+      <c r="A8" s="17"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="n">
+      <c r="A9" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14"/>
+      <c r="A10" s="17"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="n">
+      <c r="A11" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14"/>
+      <c r="A12" s="17"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14"/>
+      <c r="A13" s="17"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14"/>
+      <c r="A14" s="17"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14"/>
+      <c r="A15" s="17"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14"/>
-    </row>
-    <row r="17" s="14" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A16" s="17"/>
+    </row>
+    <row r="17" s="17" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14"/>
+      <c r="A18" s="17"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
x_wing_ index rows 1 to 9
</commit_message>
<xml_diff>
--- a/data/SDK.xlsx
+++ b/data/SDK.xlsx
@@ -512,7 +512,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5560,72 +5560,75 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.92"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="n">
+        <v>246</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="n">
+        <v>158</v>
+      </c>
+      <c r="F1" s="3" t="n">
+        <v>156</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="H1" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="I1" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="n">
-        <v>25</v>
-      </c>
-      <c r="C1" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="E1" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="F1" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="n">
-        <v>258</v>
-      </c>
-      <c r="I1" s="3" t="n">
-        <v>258</v>
-      </c>
-      <c r="K1" s="4" t="n">
+      <c r="K1" s="4" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,1)=9,1,"")</f>
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>467</v>
+      </c>
+      <c r="D2" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="B2" s="6" t="n">
-        <v>35</v>
-      </c>
-      <c r="C2" s="7" t="n">
-        <v>358</v>
-      </c>
-      <c r="D2" s="5" t="n">
-        <v>7</v>
-      </c>
       <c r="E2" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="F2" s="7" t="n">
+        <v>167</v>
+      </c>
+      <c r="G2" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="F2" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="G2" s="5" t="n">
-        <v>35</v>
-      </c>
       <c r="H2" s="6" t="n">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="I2" s="7" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="K2" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,2)=9,2,"")</f>
@@ -5634,35 +5637,35 @@
     </row>
     <row r="3" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="n">
-        <v>268</v>
+        <v>8</v>
       </c>
       <c r="B3" s="10" t="n">
-        <v>236</v>
+        <v>17</v>
       </c>
       <c r="C3" s="11" t="n">
+        <v>67</v>
+      </c>
+      <c r="D3" s="9" t="n">
+        <v>167</v>
+      </c>
+      <c r="E3" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="D3" s="9" t="n">
-        <v>38</v>
-      </c>
-      <c r="E3" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="11" t="n">
+      <c r="G3" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3" s="10" t="n">
         <v>5</v>
-      </c>
-      <c r="G3" s="9" t="n">
-        <v>238</v>
-      </c>
-      <c r="H3" s="10" t="n">
-        <v>7</v>
       </c>
       <c r="I3" s="11" t="n">
         <v>9</v>
       </c>
-      <c r="K3" s="8" t="str">
+      <c r="K3" s="8" t="n">
         <f aca="false">IF(COUNTIF($A$1:$I$9,3)=9,3,"")</f>
-        <v/>
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5670,61 +5673,61 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C4" s="3" t="n">
+        <v>257</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="H4" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="E4" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="H4" s="2" t="n">
+      <c r="I4" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="I4" s="3" t="n">
-        <v>25</v>
-      </c>
-      <c r="K4" s="8" t="n">
+      <c r="K4" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,4)=9,4,"")</f>
-        <v>4</v>
+        <v/>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="B5" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="C5" s="7" t="n">
-        <v>56</v>
-      </c>
       <c r="D5" s="5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E5" s="6" t="n">
         <v>9</v>
       </c>
       <c r="F5" s="7" t="n">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="G5" s="5" t="n">
+        <v>57</v>
+      </c>
+      <c r="H5" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H5" s="6" t="n">
+      <c r="I5" s="7" t="n">
         <v>3</v>
-      </c>
-      <c r="I5" s="7" t="n">
-        <v>7</v>
       </c>
       <c r="K5" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,5)=9,5,"")</f>
@@ -5736,28 +5739,28 @@
         <v>1</v>
       </c>
       <c r="B6" s="10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C6" s="11" t="n">
+        <v>57</v>
+      </c>
+      <c r="D6" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="C6" s="11" t="n">
+      <c r="E6" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="F6" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" s="9" t="n">
+        <v>57</v>
+      </c>
+      <c r="H6" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="D6" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="E6" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="F6" s="11" t="n">
-        <v>7</v>
-      </c>
-      <c r="G6" s="9" t="n">
+      <c r="I6" s="11" t="n">
         <v>8</v>
-      </c>
-      <c r="H6" s="10" t="n">
-        <v>9</v>
-      </c>
-      <c r="I6" s="11" t="n">
-        <v>6</v>
       </c>
       <c r="K6" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,6)=9,6,"")</f>
@@ -5766,64 +5769,64 @@
     </row>
     <row r="7" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>568</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="H7" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="C7" s="3" t="n">
-        <v>3568</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="F7" s="3" t="n">
-        <v>36</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>1</v>
-      </c>
       <c r="I7" s="3" t="n">
-        <v>58</v>
-      </c>
-      <c r="K7" s="8" t="n">
+        <v>16</v>
+      </c>
+      <c r="K7" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,7)=9,7,"")</f>
-        <v>7</v>
+        <v/>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F8" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="G8" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7" t="n">
-        <v>25</v>
-      </c>
-      <c r="D8" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="E8" s="6" t="n">
+      <c r="H8" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="F8" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="G8" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="H8" s="6" t="n">
-        <v>25</v>
-      </c>
       <c r="I8" s="7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K8" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,8)=9,8,"")</f>
@@ -5832,31 +5835,31 @@
     </row>
     <row r="9" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="n">
-        <v>268</v>
+        <v>7</v>
       </c>
       <c r="B9" s="10" t="n">
-        <v>2368</v>
+        <v>8</v>
       </c>
       <c r="C9" s="11" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D9" s="9" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E9" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="F9" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="9" t="n">
+        <v>16</v>
+      </c>
+      <c r="H9" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="I9" s="11" t="n">
         <v>5</v>
-      </c>
-      <c r="F9" s="11" t="n">
-        <v>36</v>
-      </c>
-      <c r="G9" s="9" t="n">
-        <v>9</v>
-      </c>
-      <c r="H9" s="10" t="n">
-        <v>28</v>
-      </c>
-      <c r="I9" s="11" t="n">
-        <v>4</v>
       </c>
       <c r="K9" s="12" t="n">
         <f aca="false">IF(COUNTIF($A$1:$I$9,9)=9,9,"")</f>
@@ -5965,8 +5968,8 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5980,23 +5983,19 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="1"/>
+      <c r="C1" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="G1" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>4</v>
-      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="3"/>
       <c r="L1" s="1"/>
@@ -6012,26 +6011,20 @@
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="C2" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="C2" s="6" t="n">
+        <v>2</v>
+      </c>
       <c r="D2" s="7"/>
-      <c r="E2" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="F2" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" s="7" t="n">
-        <v>4</v>
-      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="7"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="J2" s="7" t="n">
-        <v>1</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="J2" s="7"/>
       <c r="L2" s="5"/>
       <c r="M2" s="6"/>
       <c r="N2" s="7"/>
@@ -6047,21 +6040,21 @@
       <c r="B3" s="9"/>
       <c r="C3" s="10"/>
       <c r="D3" s="11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" s="9"/>
-      <c r="F3" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="F3" s="10"/>
       <c r="G3" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="H3" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I3" s="10" t="n">
+        <v>9</v>
+      </c>
+      <c r="J3" s="11" t="n">
         <v>5</v>
-      </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10" t="n">
-        <v>7</v>
-      </c>
-      <c r="J3" s="11" t="n">
-        <v>9</v>
       </c>
       <c r="L3" s="9"/>
       <c r="M3" s="10"/>
@@ -6075,28 +6068,18 @@
       <c r="U3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="n">
+      <c r="B4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="G4" s="3" t="n">
-        <v>1</v>
-      </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="2" t="n">
-        <v>4</v>
-      </c>
+      <c r="I4" s="2"/>
       <c r="J4" s="3"/>
       <c r="L4" s="1"/>
       <c r="M4" s="2"/>
@@ -6112,25 +6095,21 @@
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="5"/>
       <c r="C5" s="6" t="n">
-        <v>8</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="I5" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="F5" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="G5" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="J5" s="7" t="n">
-        <v>7</v>
-      </c>
+      <c r="J5" s="7"/>
       <c r="K5" s="6"/>
       <c r="L5" s="5"/>
       <c r="M5" s="6"/>
@@ -6145,26 +6124,18 @@
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="9"/>
-      <c r="C6" s="10" t="n">
-        <v>4</v>
-      </c>
+      <c r="C6" s="10"/>
       <c r="D6" s="11"/>
       <c r="E6" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="F6" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="G6" s="11" t="n">
-        <v>7</v>
-      </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="10" t="n">
-        <v>9</v>
-      </c>
-      <c r="J6" s="11" t="n">
-        <v>6</v>
-      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="11"/>
       <c r="L6" s="9"/>
       <c r="M6" s="10"/>
       <c r="N6" s="11"/>
@@ -6177,24 +6148,24 @@
       <c r="U6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="C7" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>6</v>
+      </c>
       <c r="E7" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>4</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F7" s="2"/>
       <c r="G7" s="3"/>
       <c r="H7" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="I7" s="2" t="n">
-        <v>1</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="I7" s="2"/>
       <c r="J7" s="3"/>
       <c r="L7" s="1"/>
       <c r="M7" s="2"/>
@@ -6208,28 +6179,20 @@
       <c r="U7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5" t="n">
-        <v>4</v>
-      </c>
+      <c r="B8" s="5"/>
       <c r="C8" s="6" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="5"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="J8" s="7" t="n">
         <v>9</v>
-      </c>
-      <c r="F8" s="6" t="n">
-        <v>7</v>
-      </c>
-      <c r="G8" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="H8" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="7" t="n">
-        <v>3</v>
       </c>
       <c r="L8" s="5"/>
       <c r="M8" s="6"/>
@@ -6245,23 +6208,19 @@
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
-      <c r="D9" s="11" t="n">
-        <v>7</v>
-      </c>
-      <c r="E9" s="9" t="n">
+      <c r="D9" s="11"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="G9" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F9" s="10" t="n">
-        <v>5</v>
-      </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="9" t="n">
-        <v>9</v>
-      </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="11" t="n">
-        <v>4</v>
-      </c>
+      <c r="J9" s="11"/>
       <c r="L9" s="9"/>
       <c r="M9" s="10"/>
       <c r="N9" s="11"/>
@@ -6791,7 +6750,7 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -7546,7 +7505,7 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -8429,7 +8388,7 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K27" activeCellId="0" sqref="K27"/>
     </sheetView>
   </sheetViews>
@@ -9312,7 +9271,7 @@
   </sheetPr>
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -10055,7 +10014,7 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -10304,7 +10263,7 @@
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G44" activeCellId="0" sqref="G44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
all files show dataframe with row 1 to 9
</commit_message>
<xml_diff>
--- a/data/SDK.xlsx
+++ b/data/SDK.xlsx
@@ -9,13 +9,14 @@
   </bookViews>
   <sheets>
     <sheet name="python" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="SDK_1" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="SDK_2" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="SDK_3" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="SDK_4" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Trip square" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="NRC" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Trucs" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="elimination" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="SDK_1" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="x-wing" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="swordfish" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="jellyfish" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Trip square" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="NRC" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Trucs" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -528,7 +529,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -717,677 +718,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="478">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="411">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5561,7 +4892,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5571,31 +4902,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
+        <v>357</v>
+      </c>
+      <c r="B1" s="2" t="n">
+        <v>3567</v>
+      </c>
+      <c r="C1" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="C1" s="3" t="n">
-        <v>246</v>
-      </c>
       <c r="D1" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E1" s="2" t="n">
-        <v>158</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="n">
-        <v>156</v>
+        <v>567</v>
       </c>
       <c r="G1" s="1" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="H1" s="2" t="n">
-        <v>48</v>
+        <v>3678</v>
       </c>
       <c r="I1" s="3" t="n">
-        <v>7</v>
+        <v>378</v>
       </c>
       <c r="K1" s="4" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,1)=9,1,"")</f>
@@ -5604,31 +4935,31 @@
     </row>
     <row r="2" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
-        <v>5</v>
+        <v>357</v>
       </c>
       <c r="B2" s="6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="7" t="n">
-        <v>467</v>
+        <v>8</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>9</v>
+        <v>567</v>
       </c>
       <c r="E2" s="6" t="n">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="F2" s="7" t="n">
-        <v>167</v>
+        <v>2</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>2</v>
+        <v>369</v>
       </c>
       <c r="H2" s="6" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="I2" s="7" t="n">
-        <v>16</v>
+        <v>378</v>
       </c>
       <c r="K2" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,2)=9,2,"")</f>
@@ -5637,64 +4968,64 @@
     </row>
     <row r="3" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="n">
+        <v>27</v>
+      </c>
+      <c r="B3" s="10" t="n">
+        <v>267</v>
+      </c>
+      <c r="C3" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="B3" s="10" t="n">
-        <v>17</v>
-      </c>
-      <c r="C3" s="11" t="n">
-        <v>67</v>
-      </c>
-      <c r="D3" s="9" t="n">
-        <v>167</v>
-      </c>
       <c r="E3" s="10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" s="11" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G3" s="9" t="n">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="H3" s="10" t="n">
+        <v>467</v>
+      </c>
+      <c r="I3" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="I3" s="11" t="n">
-        <v>9</v>
-      </c>
-      <c r="K3" s="8" t="n">
+      <c r="K3" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,3)=9,3,"")</f>
-        <v>3</v>
+        <v/>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>27</v>
+        <v>123</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>257</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="n">
+        <v>2457</v>
+      </c>
+      <c r="E4" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="E4" s="2" t="n">
-        <v>15</v>
-      </c>
       <c r="F4" s="3" t="n">
+        <v>357</v>
+      </c>
+      <c r="G4" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="G4" s="1" t="n">
-        <v>9</v>
-      </c>
       <c r="H4" s="2" t="n">
-        <v>6</v>
+        <v>2347</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>4</v>
+        <v>2347</v>
       </c>
       <c r="K4" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,4)=9,4,"")</f>
@@ -5706,28 +5037,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="n">
+        <v>1238</v>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>1789</v>
+      </c>
+      <c r="F5" s="7" t="n">
+        <v>378</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="H5" s="6" t="n">
+        <v>2379</v>
+      </c>
+      <c r="I5" s="7" t="n">
         <v>6</v>
-      </c>
-      <c r="C5" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="F5" s="7" t="n">
-        <v>57</v>
-      </c>
-      <c r="G5" s="5" t="n">
-        <v>57</v>
-      </c>
-      <c r="H5" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="7" t="n">
-        <v>3</v>
       </c>
       <c r="K5" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,5)=9,5,"")</f>
@@ -5736,31 +5067,31 @@
     </row>
     <row r="6" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="n">
+        <v>238</v>
+      </c>
+      <c r="B6" s="10" t="n">
+        <v>238</v>
+      </c>
+      <c r="C6" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>246</v>
+      </c>
+      <c r="E6" s="10" t="n">
+        <v>689</v>
+      </c>
+      <c r="F6" s="11" t="n">
+        <v>368</v>
+      </c>
+      <c r="G6" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="H6" s="10" t="n">
+        <v>2349</v>
+      </c>
+      <c r="I6" s="11" t="n">
         <v>1</v>
-      </c>
-      <c r="B6" s="10" t="n">
-        <v>9</v>
-      </c>
-      <c r="C6" s="11" t="n">
-        <v>57</v>
-      </c>
-      <c r="D6" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="E6" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="F6" s="11" t="n">
-        <v>3</v>
-      </c>
-      <c r="G6" s="9" t="n">
-        <v>57</v>
-      </c>
-      <c r="H6" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="I6" s="11" t="n">
-        <v>8</v>
       </c>
       <c r="K6" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,6)=9,6,"")</f>
@@ -5769,31 +5100,31 @@
     </row>
     <row r="7" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="E7" s="2" t="n">
-        <v>7</v>
-      </c>
       <c r="F7" s="3" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="K7" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,7)=9,7,"")</f>
@@ -5802,31 +5133,31 @@
     </row>
     <row r="8" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B8" s="6" t="n">
+        <v>189</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" s="7" t="n">
+        <v>68</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="H8" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="C8" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="E8" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="F8" s="7" t="n">
-        <v>9</v>
-      </c>
-      <c r="G8" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="H8" s="6" t="n">
-        <v>7</v>
-      </c>
       <c r="I8" s="7" t="n">
-        <v>2</v>
+        <v>89</v>
       </c>
       <c r="K8" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,8)=9,8,"")</f>
@@ -5835,35 +5166,35 @@
     </row>
     <row r="9" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="n">
-        <v>7</v>
+        <v>578</v>
       </c>
       <c r="B9" s="10" t="n">
-        <v>8</v>
+        <v>5789</v>
       </c>
       <c r="C9" s="11" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D9" s="9" t="n">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="E9" s="10" t="n">
-        <v>4</v>
+        <v>678</v>
       </c>
       <c r="F9" s="11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="9" t="n">
-        <v>16</v>
+        <v>3469</v>
       </c>
       <c r="H9" s="10" t="n">
-        <v>3</v>
+        <v>34689</v>
       </c>
       <c r="I9" s="11" t="n">
-        <v>5</v>
-      </c>
-      <c r="K9" s="12" t="n">
+        <v>3489</v>
+      </c>
+      <c r="K9" s="12" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,9)=9,9,"")</f>
-        <v>9</v>
+        <v/>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5962,6 +5293,372 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="n">
+        <v>357</v>
+      </c>
+      <c r="B1" s="2" t="n">
+        <v>3567</v>
+      </c>
+      <c r="C1" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="n">
+        <v>567</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2" t="n">
+        <v>3678</v>
+      </c>
+      <c r="I1" s="3" t="n">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>357</v>
+      </c>
+      <c r="B2" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>567</v>
+      </c>
+      <c r="E2" s="6" t="n">
+        <v>67</v>
+      </c>
+      <c r="F2" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" s="5" t="n">
+        <v>369</v>
+      </c>
+      <c r="H2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="7" t="n">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="n">
+        <v>27</v>
+      </c>
+      <c r="B3" s="10" t="n">
+        <v>267</v>
+      </c>
+      <c r="C3" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="G3" s="9" t="n">
+        <v>46</v>
+      </c>
+      <c r="H3" s="10" t="n">
+        <v>467</v>
+      </c>
+      <c r="I3" s="11" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>123</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>2457</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>357</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>2347</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>2347</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>1238</v>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>1789</v>
+      </c>
+      <c r="F5" s="7" t="n">
+        <v>378</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="H5" s="6" t="n">
+        <v>2379</v>
+      </c>
+      <c r="I5" s="7" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="n">
+        <v>238</v>
+      </c>
+      <c r="B6" s="10" t="n">
+        <v>238</v>
+      </c>
+      <c r="C6" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>246</v>
+      </c>
+      <c r="E6" s="10" t="n">
+        <v>689</v>
+      </c>
+      <c r="F6" s="11" t="n">
+        <v>368</v>
+      </c>
+      <c r="G6" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="H6" s="10" t="n">
+        <v>2349</v>
+      </c>
+      <c r="I6" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>189</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" s="7" t="n">
+        <v>68</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="H8" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="I8" s="7" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="n">
+        <v>578</v>
+      </c>
+      <c r="B9" s="10" t="n">
+        <v>5789</v>
+      </c>
+      <c r="C9" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>67</v>
+      </c>
+      <c r="E9" s="10" t="n">
+        <v>678</v>
+      </c>
+      <c r="F9" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9" t="n">
+        <v>3469</v>
+      </c>
+      <c r="H9" s="10" t="n">
+        <v>34689</v>
+      </c>
+      <c r="I9" s="11" t="n">
+        <v>3489</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:A9">
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:I1">
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C9">
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:I2">
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:I3">
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:I4">
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:C6">
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:I5">
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B9">
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C3">
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:I6">
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7:C9">
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7:I7">
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:I8">
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:I9">
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:F3">
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D9">
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:F6">
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7:F9">
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E9">
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F9">
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:I3">
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G9">
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:I6">
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7:I9">
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H9">
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I9">
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -6736,761 +6433,6 @@
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="B1:U27"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="1.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="13" width="7.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="13" width="6.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="13" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="13" width="3.46"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="J1" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="6"/>
-    </row>
-    <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F2" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="J2" s="7"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="6"/>
-    </row>
-    <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="10" t="n">
-        <v>5</v>
-      </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="I3" s="10" t="n">
-        <v>4</v>
-      </c>
-      <c r="J3" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="L3" s="9"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="6"/>
-    </row>
-    <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="3"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="6"/>
-    </row>
-    <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="6"/>
-    </row>
-    <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="F6" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="11"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="6"/>
-    </row>
-    <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="D7" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="G7" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="3"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="6"/>
-    </row>
-    <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5"/>
-      <c r="C8" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="D8" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="G8" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="J8" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="6"/>
-    </row>
-    <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="11" t="n">
-        <v>5</v>
-      </c>
-      <c r="H9" s="9" t="n">
-        <v>9</v>
-      </c>
-      <c r="I9" s="10" t="n">
-        <v>6</v>
-      </c>
-      <c r="J9" s="11"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="6"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="7"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="11"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="7"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="11"/>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="1"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="7"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="11"/>
-    </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" s="16" t="n">
-        <v>2</v>
-      </c>
-      <c r="E22" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="F22" s="16" t="n">
-        <v>8</v>
-      </c>
-      <c r="G22" s="16" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="16" t="n">
-        <v>15</v>
-      </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17" t="n">
-        <v>2</v>
-      </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17" t="n">
-        <v>8</v>
-      </c>
-      <c r="G23" s="17" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="16" t="n">
-        <v>35</v>
-      </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17" t="n">
-        <v>2</v>
-      </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17" t="n">
-        <v>8</v>
-      </c>
-      <c r="G24" s="17" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="16" t="n">
-        <v>45</v>
-      </c>
-      <c r="C25" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="D25" s="17" t="n">
-        <v>2</v>
-      </c>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17" t="n">
-        <v>8</v>
-      </c>
-      <c r="G25" s="17" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="16" t="n">
-        <v>75</v>
-      </c>
-      <c r="C26" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17" t="n">
-        <v>4</v>
-      </c>
-      <c r="F26" s="18" t="n">
-        <v>8</v>
-      </c>
-      <c r="G26" s="18" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="16" t="n">
-        <v>95</v>
-      </c>
-      <c r="C27" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17" t="n">
-        <v>4</v>
-      </c>
-      <c r="F27" s="18" t="n">
-        <v>8</v>
-      </c>
-      <c r="G27" s="17"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B1:B10">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="95"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:J1">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D10">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="97"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:J2">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="98"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:J3">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:J4">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="100"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:D6">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="101"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5:K5">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C10">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="103"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D3">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="104"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6:J6">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="105"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7:D10">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="106"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7:J7">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:J8">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="108"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9:J9 H10:J10 B10:F10">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="109"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1:G3">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="110"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E10">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="111"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4:G6">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="112"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7:G9 E10:F10">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="113"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F10">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="114"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="115"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1:J3">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="116"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H10">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="117"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4:J6 K5">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="118"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H7:J10">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="119"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I10">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="120"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J10 K5">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="121"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B12:B20">
-    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="122"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B12:J12">
-    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="123"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12:D20">
-    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="124"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13:J13">
-    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="125"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:J14">
-    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="126"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15:J15">
-    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="127"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15:D17">
-    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="128"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16:J16">
-    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="129"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12:C20">
-    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="130"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B12:D14">
-    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="131"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17:J17">
-    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="132"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18:D20">
-    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="133"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18:J18">
-    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="134"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19:J19">
-    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="135"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20:J20">
-    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="136"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12:G14">
-    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="137"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12:E20">
-    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="138"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E15:G17">
-    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="139"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18:G20">
-    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="140"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12:F20">
-    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="141"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G12:G20">
-    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="142"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H12:J14">
-    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="143"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H12:H20">
-    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="144"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15:J17">
-    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="145"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H18:J20">
-    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="146"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12:I20">
-    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="147"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J12:J20">
-    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="148"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L9">
-    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="149"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L1:U1">
-    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="150"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N9">
-    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="151"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L2:U2">
-    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="152"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L3:U3">
-    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="153"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L4:U4">
-    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="154"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L4:N6">
-    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="155"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L5:U5">
-    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="156"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M9">
-    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="157"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L1:N3">
-    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="158"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L6:U6">
-    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="159"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L7:N9">
-    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="160"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L7:U7">
-    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="161"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L8:U8">
-    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="162"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L9:U9">
-    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="163"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O1:Q3">
-    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="164"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O9">
-    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="165"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O4:Q6">
-    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="166"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O7:Q9">
-    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="167"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P9">
-    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="168"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q1:Q9">
-    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="169"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R1:U3">
-    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="170"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R1:R9">
-    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="171"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R4:U6">
-    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="172"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R7:U9">
-    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="173"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S1:S9">
-    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="174"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T1:U9">
-    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="175"/>
-  </conditionalFormatting>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -7523,28 +6465,28 @@
         <v>9</v>
       </c>
       <c r="C1" s="2" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D1" s="3" t="n">
+        <v>246</v>
+      </c>
+      <c r="E1" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="F1" s="2" t="n">
+        <v>158</v>
+      </c>
+      <c r="G1" s="3" t="n">
+        <v>156</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="J1" s="3" t="n">
         <v>7</v>
-      </c>
-      <c r="F1" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G1" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="J1" s="3" t="n">
-        <v>4</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="2"/>
@@ -7559,31 +6501,31 @@
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="5" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C2" s="6" t="n">
-        <v>1467</v>
+        <v>3</v>
       </c>
       <c r="D2" s="7" t="n">
-        <v>1467</v>
+        <v>467</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="F2" s="6" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="G2" s="7" t="n">
-        <v>25</v>
+        <v>167</v>
       </c>
       <c r="H2" s="5" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I2" s="6" t="n">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="J2" s="7" t="n">
-        <v>178</v>
+        <v>16</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="6"/>
@@ -7598,31 +6540,31 @@
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="9" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C3" s="10" t="n">
+        <v>17</v>
+      </c>
+      <c r="D3" s="11" t="n">
+        <v>67</v>
+      </c>
+      <c r="E3" s="9" t="n">
+        <v>167</v>
+      </c>
+      <c r="F3" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="D3" s="11" t="n">
-        <v>178</v>
-      </c>
-      <c r="E3" s="9" t="n">
+      <c r="J3" s="11" t="n">
         <v>9</v>
-      </c>
-      <c r="F3" s="10" t="n">
-        <v>4</v>
-      </c>
-      <c r="G3" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="H3" s="9" t="n">
-        <v>17</v>
-      </c>
-      <c r="I3" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="J3" s="11" t="n">
-        <v>2</v>
       </c>
       <c r="L3" s="9"/>
       <c r="M3" s="10"/>
@@ -7637,31 +6579,31 @@
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>134</v>
+        <v>27</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>14</v>
+        <v>257</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>123</v>
+        <v>8</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I4" s="2" t="n">
         <v>6</v>
       </c>
       <c r="J4" s="3" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="2"/>
@@ -7676,31 +6618,31 @@
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="D5" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="E5" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="E5" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F5" s="6" t="n">
-        <v>6</v>
-      </c>
       <c r="G5" s="7" t="n">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="H5" s="5" t="n">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="I5" s="6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J5" s="7" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="5"/>
@@ -7716,31 +6658,31 @@
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="10" t="n">
+        <v>9</v>
+      </c>
+      <c r="D6" s="11" t="n">
+        <v>57</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="C6" s="10" t="n">
-        <v>13</v>
-      </c>
-      <c r="D6" s="11" t="n">
+      <c r="G6" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="H6" s="9" t="n">
+        <v>57</v>
+      </c>
+      <c r="I6" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="E6" s="9" t="n">
+      <c r="J6" s="11" t="n">
         <v>8</v>
-      </c>
-      <c r="F6" s="10" t="n">
-        <v>9</v>
-      </c>
-      <c r="G6" s="11" t="n">
-        <v>13</v>
-      </c>
-      <c r="H6" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="I6" s="10" t="n">
-        <v>7</v>
-      </c>
-      <c r="J6" s="11" t="n">
-        <v>5</v>
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="10"/>
@@ -7758,28 +6700,28 @@
         <v>2</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>7</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="J7" s="3" t="n">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="2"/>
@@ -7794,31 +6736,31 @@
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="5" t="n">
-        <v>148</v>
+        <v>6</v>
       </c>
       <c r="C8" s="6" t="n">
-        <v>1467</v>
+        <v>5</v>
       </c>
       <c r="D8" s="7" t="n">
-        <v>14678</v>
+        <v>1</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F8" s="6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G8" s="7" t="n">
         <v>9</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>1357</v>
+        <v>4</v>
       </c>
       <c r="I8" s="6" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="J8" s="7" t="n">
-        <v>13678</v>
+        <v>2</v>
       </c>
       <c r="L8" s="5"/>
       <c r="M8" s="6"/>
@@ -7833,31 +6775,31 @@
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="E9" s="9" t="n">
+        <v>16</v>
+      </c>
+      <c r="F9" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="G9" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" s="9" t="n">
+        <v>16</v>
+      </c>
+      <c r="I9" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="10" t="n">
-        <v>17</v>
-      </c>
-      <c r="D9" s="11" t="n">
+      <c r="J9" s="11" t="n">
         <v>5</v>
-      </c>
-      <c r="E9" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F9" s="10" t="n">
-        <v>8</v>
-      </c>
-      <c r="G9" s="11" t="n">
-        <v>4</v>
-      </c>
-      <c r="H9" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="I9" s="10" t="n">
-        <v>9</v>
-      </c>
-      <c r="J9" s="11" t="n">
-        <v>17</v>
       </c>
       <c r="L9" s="9"/>
       <c r="M9" s="10"/>
@@ -8086,290 +7028,290 @@
       <c r="G27" s="17"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="176"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="177"/>
+  <conditionalFormatting sqref="B2:B10">
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="95"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D10">
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="178"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="179"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="97"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C10">
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="98"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:D10">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="180"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10 B10:F10">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="181"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E10">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="182"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="100"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E10">
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="101"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:F10">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="183"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="184"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="185"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F10">
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="103"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H10">
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="104"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="186"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="105"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="187"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="188"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10 K5">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="189"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="106"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I10">
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J10 K5">
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="108"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B20">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="190"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="109"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:J12">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="191"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="110"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D20">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="192"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="111"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:J13">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="193"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="112"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:J14">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="194"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="113"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:J15">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="195"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="114"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:D17">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="196"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="115"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:J16">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="197"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="116"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C20">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="198"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="117"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:D14">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="199"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="118"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:J17">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="200"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="119"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:D20">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="201"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="120"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:J18">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="202"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="121"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:J19">
-    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="203"/>
+    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="122"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:J20">
-    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="204"/>
+    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="123"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:G14">
-    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="205"/>
+    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="124"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:E20">
-    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="206"/>
+    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="125"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:G17">
-    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="207"/>
+    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="126"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:G20">
-    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="208"/>
+    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="127"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F20">
-    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="209"/>
+    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="128"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G20">
-    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="210"/>
+    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="129"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:J14">
-    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="211"/>
+    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="130"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H20">
-    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="212"/>
+    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="131"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:J17">
-    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="213"/>
+    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="132"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:J20">
-    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="214"/>
+    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="133"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I20">
-    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="215"/>
+    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="134"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:J20">
-    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="216"/>
+    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="135"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L9">
-    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="217"/>
+    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="136"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:U1">
-    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="218"/>
+    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="137"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N9">
-    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="219"/>
+    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="138"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:U2">
-    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="220"/>
+    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="139"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:U3">
-    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="221"/>
+    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="140"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:U4">
-    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="222"/>
+    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="141"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:N6">
-    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="223"/>
+    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="142"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:U5">
-    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="224"/>
+    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="143"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M9">
-    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="225"/>
+    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="144"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:N3">
-    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="226"/>
+    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="145"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:U6">
-    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="227"/>
+    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="146"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:N9">
-    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="228"/>
+    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="147"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:U7">
-    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="229"/>
+    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="148"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:U8">
-    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="230"/>
+    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="149"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:U9">
-    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="231"/>
+    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="150"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:Q3">
-    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="232"/>
+    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="151"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O9">
-    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="233"/>
+    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="152"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:Q6">
-    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="234"/>
+    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="153"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7:Q9">
-    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="235"/>
+    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="154"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P9">
-    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="236"/>
+    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="155"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q9">
-    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="237"/>
+    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="156"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:U3">
-    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="238"/>
+    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="157"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R9">
-    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="239"/>
+    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="158"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4:U6">
-    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="240"/>
+    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="159"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7:U9">
-    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="241"/>
+    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="160"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S9">
-    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="242"/>
+    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="161"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:U9">
-    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="243"/>
+    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="162"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="244"/>
+    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:J1">
-    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="245"/>
+    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="246"/>
+    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J2">
-    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="247"/>
+    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J3">
-    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="248"/>
+    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:J4">
-    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="249"/>
+    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:D6">
-    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="250"/>
+    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:J5">
-    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="251"/>
+    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="252"/>
+    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D3">
-    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="253"/>
+    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:J6">
-    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="254"/>
+    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D9">
-    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="255"/>
+    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:J7">
-    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="256"/>
+    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:J8">
-    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="257"/>
+    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:J9">
-    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="258"/>
+    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G3">
-    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="259"/>
+    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="260"/>
+    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:G6">
-    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="261"/>
+    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:G9">
-    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="262"/>
+    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="263"/>
+    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="264"/>
+    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J3">
-    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="265"/>
+    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="266"/>
+    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J6">
-    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="267"/>
+    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:J9">
-    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="268"/>
+    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="269"/>
+    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J9">
-    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="270"/>
+    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8389,7 +7331,7 @@
   <dimension ref="B1:U27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K27" activeCellId="0" sqref="K27"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8970,289 +7912,289 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="271"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="163"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="272"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="164"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="273"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="165"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="274"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="166"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:D10">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="275"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="167"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10 B10:F10">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="276"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="168"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="277"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="169"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:F10">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="278"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="170"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="279"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="171"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="280"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="172"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="281"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="173"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="282"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="174"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="283"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="175"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10 K5">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="284"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="176"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B20">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="285"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="177"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:J12">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="286"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="178"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D20">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="287"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="179"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:J13">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="288"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="180"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:J14">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="289"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="181"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:J15">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="290"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="182"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:D17">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="291"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="183"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:J16">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="292"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="184"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C20">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="293"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="185"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:D14">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="294"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="186"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:J17">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="295"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="187"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:D20">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="296"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="188"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:J18">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="297"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="189"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:J19">
-    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="298"/>
+    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="190"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:J20">
-    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="299"/>
+    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="191"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:G14">
-    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="300"/>
+    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="192"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:E20">
-    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="301"/>
+    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="193"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:G17">
-    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="302"/>
+    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="194"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:G20">
-    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="303"/>
+    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="195"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F20">
-    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="304"/>
+    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="196"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G20">
-    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="305"/>
+    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="197"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:J14">
-    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="306"/>
+    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="198"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H20">
-    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="307"/>
+    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="199"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:J17">
-    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="308"/>
+    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="200"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:J20">
-    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="309"/>
+    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="201"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I20">
-    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="310"/>
+    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="202"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:J20">
-    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="311"/>
+    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="203"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L9">
-    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="312"/>
+    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="204"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:U1">
-    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="313"/>
+    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="205"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N9">
-    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="314"/>
+    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="206"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:U2">
-    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="315"/>
+    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="207"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:U3">
-    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="316"/>
+    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="208"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:U4">
-    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="317"/>
+    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="209"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:N6">
-    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="318"/>
+    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="210"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:U5">
-    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="319"/>
+    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="211"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M9">
-    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="320"/>
+    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="212"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:N3">
-    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="321"/>
+    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="213"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:U6">
-    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="322"/>
+    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="214"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:N9">
-    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="323"/>
+    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="215"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:U7">
-    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="324"/>
+    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="216"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:U8">
-    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="325"/>
+    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="217"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:U9">
-    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="326"/>
+    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="218"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:Q3">
-    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="327"/>
+    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="219"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O9">
-    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="328"/>
+    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="220"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:Q6">
-    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="329"/>
+    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="221"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7:Q9">
-    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="330"/>
+    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="222"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P9">
-    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="331"/>
+    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="223"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q9">
-    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="332"/>
+    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="224"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:U3">
-    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="333"/>
+    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="225"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R9">
-    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="334"/>
+    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="226"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4:U6">
-    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="335"/>
+    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="227"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7:U9">
-    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="336"/>
+    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="228"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S9">
-    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="337"/>
+    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="229"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:U9">
-    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="338"/>
+    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="230"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="339"/>
+    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:J1">
-    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="340"/>
+    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="341"/>
+    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J2">
-    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="342"/>
+    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J3">
-    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="343"/>
+    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:J4">
-    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="344"/>
+    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:D6">
-    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="345"/>
+    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:J5">
-    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="346"/>
+    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="347"/>
+    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D3">
-    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="348"/>
+    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:J6">
-    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="349"/>
+    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D9">
-    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="350"/>
+    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:J7">
-    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="351"/>
+    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:J8">
-    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="352"/>
+    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:J9">
-    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="353"/>
+    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G3">
-    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="354"/>
+    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="355"/>
+    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:G6">
-    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="356"/>
+    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:G9">
-    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="357"/>
+    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="358"/>
+    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="359"/>
+    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J3">
-    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="360"/>
+    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="361"/>
+    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J6">
-    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="362"/>
+    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:J9">
-    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="363"/>
+    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="364"/>
+    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J9">
-    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="365"/>
+    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -9269,10 +8211,893 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="B1:U27"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="1.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="13" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="13" width="6.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="13" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="13" width="3.46"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G1" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J1" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="6"/>
+    </row>
+    <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="C2" s="6" t="n">
+        <v>1467</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <v>1467</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="F2" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" s="7" t="n">
+        <v>25</v>
+      </c>
+      <c r="H2" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="I2" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="J2" s="7" t="n">
+        <v>178</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="6"/>
+    </row>
+    <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="9" t="n">
+        <v>18</v>
+      </c>
+      <c r="C3" s="10" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" s="11" t="n">
+        <v>178</v>
+      </c>
+      <c r="E3" s="9" t="n">
+        <v>9</v>
+      </c>
+      <c r="F3" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="I3" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="J3" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="L3" s="9"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="6"/>
+    </row>
+    <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>134</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B5" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="G5" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="I5" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="J5" s="7" t="n">
+        <v>13</v>
+      </c>
+      <c r="K5" s="6"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="6"/>
+    </row>
+    <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" s="10" t="n">
+        <v>13</v>
+      </c>
+      <c r="D6" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="F6" s="10" t="n">
+        <v>9</v>
+      </c>
+      <c r="G6" s="11" t="n">
+        <v>13</v>
+      </c>
+      <c r="H6" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="I6" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="J6" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="L6" s="9"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="6"/>
+    </row>
+    <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>68</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="J7" s="3" t="n">
+        <v>68</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="6"/>
+    </row>
+    <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="5" t="n">
+        <v>148</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>1467</v>
+      </c>
+      <c r="D8" s="7" t="n">
+        <v>14678</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <v>1357</v>
+      </c>
+      <c r="I8" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="J8" s="7" t="n">
+        <v>13678</v>
+      </c>
+      <c r="L8" s="5"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" s="10" t="n">
+        <v>17</v>
+      </c>
+      <c r="D9" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="E9" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F9" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="G9" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="H9" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" s="10" t="n">
+        <v>9</v>
+      </c>
+      <c r="J9" s="11" t="n">
+        <v>17</v>
+      </c>
+      <c r="L9" s="9"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="11"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="11"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="11"/>
+    </row>
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E22" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="F22" s="16" t="n">
+        <v>8</v>
+      </c>
+      <c r="G22" s="16" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="16" t="n">
+        <v>15</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17" t="n">
+        <v>8</v>
+      </c>
+      <c r="G23" s="17" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="16" t="n">
+        <v>35</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17" t="n">
+        <v>8</v>
+      </c>
+      <c r="G24" s="17" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="16" t="n">
+        <v>45</v>
+      </c>
+      <c r="C25" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17" t="n">
+        <v>8</v>
+      </c>
+      <c r="G25" s="17" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="16" t="n">
+        <v>75</v>
+      </c>
+      <c r="C26" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="F26" s="18" t="n">
+        <v>8</v>
+      </c>
+      <c r="G26" s="18" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="16" t="n">
+        <v>95</v>
+      </c>
+      <c r="C27" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="F27" s="18" t="n">
+        <v>8</v>
+      </c>
+      <c r="G27" s="17"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B10">
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="231"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="232"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5">
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="233"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="234"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:D10">
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="235"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10:J10 B10:F10">
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="236"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="237"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10:F10">
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="238"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10">
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="239"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="240"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5">
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="241"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10:J10">
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="242"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10">
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="243"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10 K5">
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="244"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:B20">
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="245"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:J12">
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="246"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:D20">
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="247"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:J13">
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="248"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:J14">
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="249"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:J15">
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="250"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:D17">
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="251"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16:J16">
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="252"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:C20">
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="253"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:D14">
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="254"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:J17">
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="255"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:D20">
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="256"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:J18">
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="257"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19:J19">
+    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="258"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20:J20">
+    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="259"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12:G14">
+    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="260"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12:E20">
+    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="261"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15:G17">
+    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="262"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18:G20">
+    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="263"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12:F20">
+    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="264"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12:G20">
+    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="265"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12:J14">
+    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="266"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12:H20">
+    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="267"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15:J17">
+    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="268"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18:J20">
+    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="269"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12:I20">
+    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="270"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J12:J20">
+    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="271"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:L9">
+    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="272"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:U1">
+    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="273"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N1:N9">
+    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="274"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:U2">
+    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="275"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:U3">
+    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="276"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4:U4">
+    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="277"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4:N6">
+    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="278"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L5:U5">
+    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="279"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M1:M9">
+    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="280"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:N3">
+    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="281"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L6:U6">
+    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="282"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L7:N9">
+    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="283"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L7:U7">
+    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="284"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L8:U8">
+    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="285"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L9:U9">
+    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="286"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O1:Q3">
+    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="287"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O1:O9">
+    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="288"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O4:Q6">
+    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="289"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O7:Q9">
+    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="290"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P1:P9">
+    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="291"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q1:Q9">
+    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="292"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R1:U3">
+    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="293"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R1:R9">
+    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="294"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R4:U6">
+    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="295"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R7:U9">
+    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="296"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S1:S9">
+    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="297"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T1:U9">
+    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="298"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B9">
+    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:J1">
+    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D9">
+    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:J2">
+    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:J3">
+    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:J4">
+    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:D6">
+    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:J5">
+    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C9">
+    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:D3">
+    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:J6">
+    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:D9">
+    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:J7">
+    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:J8">
+    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:J9">
+    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:G3">
+    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E9">
+    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:G6">
+    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7:G9">
+    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F9">
+    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G9">
+    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:J3">
+    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H9">
+    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:J6">
+    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7:J9">
+    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I9">
+    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:J9">
+    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9755,247 +9580,247 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B10">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="366"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="299"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:J1">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="367"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="300"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D10">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="368"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="301"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J2">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="369"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="302"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J3">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="370"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="303"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:J4">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="371"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="304"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:D6">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="372"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="305"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:K5">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="373"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="306"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C10">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="374"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="307"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D3">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="375"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="308"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:J6">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="376"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="309"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D10">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="377"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="310"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:J7">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="378"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="311"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:J8">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="379"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="312"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:J9 H10:J10 B10:F10">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="380"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="313"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G3">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="381"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="314"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E10">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="382"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="315"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:G6">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="383"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="316"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:G9 E10:F10">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="384"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="317"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F10">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="385"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="318"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="386"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="319"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J3">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="387"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="320"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H10">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="388"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="321"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J6 K5">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="389"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="322"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:J10">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="390"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="323"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I10">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="391"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="324"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J10 K5">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="392"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="325"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B20">
-    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="393"/>
+    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="326"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:J12">
-    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="394"/>
+    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="327"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D20">
-    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="395"/>
+    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="328"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:J13">
-    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="396"/>
+    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="329"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:J14">
-    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="397"/>
+    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="330"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:J15">
-    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="398"/>
+    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="331"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:D17">
-    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="399"/>
+    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="332"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:J16">
-    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="400"/>
+    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="333"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C20">
-    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="401"/>
+    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="334"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:D14">
-    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="402"/>
+    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="335"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:J17">
-    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="403"/>
+    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="336"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:D20">
-    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="404"/>
+    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="337"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:J18">
-    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="405"/>
+    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="338"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:J19">
-    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="406"/>
+    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="339"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:J20">
-    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="407"/>
+    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="340"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:G14">
-    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="408"/>
+    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="341"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:E20">
-    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="409"/>
+    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="342"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:G17">
-    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="410"/>
+    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="343"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:G20">
-    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="411"/>
+    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="344"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F20">
-    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="412"/>
+    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="345"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G20">
-    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="413"/>
+    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="346"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:J14">
-    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="414"/>
+    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="347"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H20">
-    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="415"/>
+    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="348"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:J17">
-    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="416"/>
+    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="349"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:J20">
-    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="417"/>
+    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="350"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I20">
-    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="418"/>
+    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="351"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:J20">
-    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="419"/>
+    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="352"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L9">
-    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="420"/>
+    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="353"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:T1">
-    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="421"/>
+    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="354"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N9">
-    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="422"/>
+    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="355"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:T2">
-    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="423"/>
+    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="356"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:T3">
-    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="424"/>
+    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="357"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:T4">
-    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="425"/>
+    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="358"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:N6">
-    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="426"/>
+    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="359"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:T5">
-    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="427"/>
+    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="360"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M9">
-    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="428"/>
+    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="361"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:N3">
-    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="429"/>
+    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="362"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:T6">
-    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="430"/>
+    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="363"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:N9">
-    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="431"/>
+    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="364"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:T7">
-    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="432"/>
+    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="365"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:T8">
-    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="433"/>
+    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="366"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:T9">
-    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="434"/>
+    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="367"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:Q3">
-    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="435"/>
+    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="368"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O9">
-    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="436"/>
+    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="369"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:Q6">
-    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="437"/>
+    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="370"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7:Q9">
-    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="438"/>
+    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="371"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P9">
-    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="439"/>
+    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="372"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q9">
-    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="440"/>
+    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="373"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:T3">
-    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="441"/>
+    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="374"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R9">
-    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="442"/>
+    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="375"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4:T6">
-    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="443"/>
+    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="376"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7:T9">
-    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="444"/>
+    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="377"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S9">
-    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="445"/>
+    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="378"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T9">
-    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="446"/>
+    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="379"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -10007,7 +9832,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -10154,97 +9979,97 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A9">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="447"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="380"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:I1">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="448"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="381"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="449"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="382"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:I2">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="450"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="383"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:I3">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="451"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="384"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:I4">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="452"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="385"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C6">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="453"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="386"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:I5">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="454"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="387"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="455"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="388"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C3">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="456"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="389"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:I6">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="457"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="390"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:C9">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="458"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="391"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:I7">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="459"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="392"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:I8">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="460"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="393"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:I9">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="461"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="394"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F3">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="462"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="395"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="463"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="396"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:F6">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="464"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="397"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F9">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="465"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="398"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="466"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="399"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="467"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="400"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:I3">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="468"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="401"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="469"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="402"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:I6">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="470"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="403"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:I9">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="471"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="404"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="472"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="405"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="473"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="406"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:D4">
-    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="474"/>
+    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="407"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:H4">
-    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="475"/>
+    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="408"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:D8">
-    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="476"/>
+    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="409"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:H8">
-    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="477"/>
+    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="410"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -10256,7 +10081,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>

</xml_diff>

<commit_message>
avoid forced check out
</commit_message>
<xml_diff>
--- a/data/SDK.xlsx
+++ b/data/SDK.xlsx
@@ -496,7 +496,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -529,7 +529,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -545,7 +545,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4892,7 +4896,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4902,31 +4906,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
-        <v>357</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="n">
-        <v>3567</v>
+        <v>6</v>
       </c>
       <c r="C1" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="n">
-        <v>567</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H1" s="2" t="n">
-        <v>3678</v>
-      </c>
       <c r="I1" s="3" t="n">
-        <v>378</v>
+        <v>7</v>
       </c>
       <c r="K1" s="4" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,1)=9,1,"")</f>
@@ -4935,32 +4939,26 @@
     </row>
     <row r="2" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
-        <v>357</v>
+        <v>9</v>
       </c>
       <c r="B2" s="6" t="n">
+        <v>35</v>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="F2" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="D2" s="5" t="n">
-        <v>567</v>
-      </c>
-      <c r="E2" s="6" t="n">
-        <v>67</v>
-      </c>
-      <c r="F2" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" s="5" t="n">
-        <v>369</v>
-      </c>
-      <c r="H2" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" s="7" t="n">
-        <v>378</v>
-      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="7"/>
       <c r="K2" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,2)=9,2,"")</f>
         <v/>
@@ -4968,31 +4966,27 @@
     </row>
     <row r="3" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="n">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B3" s="10" t="n">
-        <v>267</v>
+        <v>7</v>
       </c>
       <c r="C3" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9" t="n">
+        <v>9</v>
+      </c>
+      <c r="E3" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="11" t="n">
         <v>1</v>
-      </c>
-      <c r="D3" s="9" t="n">
-        <v>8</v>
-      </c>
-      <c r="E3" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="F3" s="11" t="n">
-        <v>9</v>
-      </c>
-      <c r="G3" s="9" t="n">
-        <v>46</v>
-      </c>
-      <c r="H3" s="10" t="n">
-        <v>467</v>
-      </c>
-      <c r="I3" s="11" t="n">
-        <v>5</v>
       </c>
       <c r="K3" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,3)=9,3,"")</f>
@@ -5001,35 +4995,27 @@
     </row>
     <row r="4" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>123</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="3" t="n">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>2457</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>17</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E4" s="2"/>
       <c r="F4" s="3" t="n">
-        <v>357</v>
+        <v>3</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>2347</v>
-      </c>
-      <c r="I4" s="3" t="n">
-        <v>2347</v>
-      </c>
-      <c r="K4" s="8" t="str">
+        <v>7</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="3"/>
+      <c r="K4" s="12" t="n">
         <f aca="false">IF(COUNTIF($A$1:$I$9,4)=9,4,"")</f>
-        <v/>
+        <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5037,26 +5023,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="n">
-        <v>1238</v>
+        <v>1</v>
       </c>
       <c r="C5" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="F5" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="D5" s="5" t="n">
-        <v>27</v>
-      </c>
-      <c r="E5" s="6" t="n">
-        <v>1789</v>
-      </c>
-      <c r="F5" s="7" t="n">
-        <v>378</v>
-      </c>
-      <c r="G5" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="H5" s="6" t="n">
-        <v>2379</v>
-      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
       <c r="I5" s="7" t="n">
         <v>6</v>
       </c>
@@ -5067,31 +5049,23 @@
     </row>
     <row r="6" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="n">
-        <v>238</v>
-      </c>
-      <c r="B6" s="10" t="n">
-        <v>238</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="B6" s="10"/>
       <c r="C6" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11" t="n">
         <v>7</v>
       </c>
-      <c r="D6" s="9" t="n">
-        <v>246</v>
-      </c>
-      <c r="E6" s="10" t="n">
-        <v>689</v>
-      </c>
-      <c r="F6" s="11" t="n">
-        <v>368</v>
-      </c>
-      <c r="G6" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="H6" s="10" t="n">
-        <v>2349</v>
-      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10"/>
       <c r="I6" s="11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K6" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,6)=9,6,"")</f>
@@ -5100,64 +5074,62 @@
     </row>
     <row r="7" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>1</v>
+        <v>369</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>28</v>
-      </c>
-      <c r="K7" s="8" t="str">
+        <v>39</v>
+      </c>
+      <c r="K7" s="12" t="n">
         <f aca="false">IF(COUNTIF($A$1:$I$9,7)=9,7,"")</f>
-        <v/>
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
-        <v>18</v>
-      </c>
-      <c r="B8" s="6" t="n">
-        <v>189</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B8" s="6"/>
       <c r="C8" s="7" t="n">
+        <v>69</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="D8" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E8" s="6" t="n">
+      <c r="F8" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="I8" s="7" t="n">
         <v>2</v>
-      </c>
-      <c r="F8" s="7" t="n">
-        <v>68</v>
-      </c>
-      <c r="G8" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="H8" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="I8" s="7" t="n">
-        <v>89</v>
       </c>
       <c r="K8" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,8)=9,8,"")</f>
@@ -5166,39 +5138,43 @@
     </row>
     <row r="9" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="n">
-        <v>578</v>
+        <v>7</v>
       </c>
       <c r="B9" s="10" t="n">
-        <v>5789</v>
+        <v>2</v>
       </c>
       <c r="C9" s="11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="9" t="n">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="E9" s="10" t="n">
-        <v>678</v>
+        <v>3</v>
       </c>
       <c r="F9" s="11" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G9" s="9" t="n">
-        <v>3469</v>
+        <v>5</v>
       </c>
       <c r="H9" s="10" t="n">
-        <v>34689</v>
+        <v>4</v>
       </c>
       <c r="I9" s="11" t="n">
-        <v>3489</v>
-      </c>
-      <c r="K9" s="12" t="str">
+        <v>8</v>
+      </c>
+      <c r="K9" s="13" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,9)=9,9,"")</f>
         <v/>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <conditionalFormatting sqref="A1:A9">
@@ -5303,7 +5279,7 @@
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
@@ -5671,12 +5647,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="1.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="13" width="7.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="13" width="6.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="12" style="13" width="8.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="13" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="13" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="1.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="14" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="14" width="6.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="12" style="14" width="8.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="14" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="14" width="3.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5933,9 +5909,9 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="14"/>
+      <c r="E10" s="15"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="15"/>
+      <c r="G10" s="16"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
@@ -6041,108 +6017,108 @@
       <c r="J20" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="16" t="n">
+      <c r="C22" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="16" t="n">
+      <c r="D22" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="16" t="n">
+      <c r="E22" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="16" t="n">
+      <c r="F22" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="16" t="n">
+      <c r="G22" s="17" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="16" t="n">
+      <c r="B23" s="17" t="n">
         <v>15</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17" t="n">
+      <c r="C23" s="18"/>
+      <c r="D23" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17" t="n">
+      <c r="E23" s="18"/>
+      <c r="F23" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G23" s="17" t="n">
+      <c r="G23" s="18" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="16" t="n">
+      <c r="B24" s="17" t="n">
         <v>35</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17" t="n">
+      <c r="C24" s="18"/>
+      <c r="D24" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17" t="n">
+      <c r="E24" s="18"/>
+      <c r="F24" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G24" s="17" t="n">
+      <c r="G24" s="18" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="16" t="n">
+      <c r="B25" s="17" t="n">
         <v>45</v>
       </c>
-      <c r="C25" s="18" t="n">
+      <c r="C25" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="17" t="n">
+      <c r="D25" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17" t="n">
+      <c r="E25" s="18"/>
+      <c r="F25" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G25" s="17" t="n">
+      <c r="G25" s="18" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="16" t="n">
+      <c r="B26" s="17" t="n">
         <v>75</v>
       </c>
-      <c r="C26" s="17" t="n">
+      <c r="C26" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17" t="n">
+      <c r="D26" s="18"/>
+      <c r="E26" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="18" t="n">
+      <c r="F26" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G26" s="18" t="n">
+      <c r="G26" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="16" t="n">
+      <c r="B27" s="17" t="n">
         <v>95</v>
       </c>
-      <c r="C27" s="17" t="n">
+      <c r="C27" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17" t="n">
+      <c r="D27" s="18"/>
+      <c r="E27" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="F27" s="18" t="n">
+      <c r="F27" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="17"/>
+      <c r="G27" s="18"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B10">
@@ -6453,11 +6429,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="1.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="13" width="7.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="13" width="6.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="13" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="13" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="1.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="14" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="14" width="6.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="14" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="14" width="3.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6816,9 +6792,9 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="14"/>
+      <c r="E10" s="15"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="15"/>
+      <c r="G10" s="16"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
@@ -6924,108 +6900,108 @@
       <c r="J20" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="16" t="n">
+      <c r="C22" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="16" t="n">
+      <c r="D22" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="16" t="n">
+      <c r="E22" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="16" t="n">
+      <c r="F22" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="16" t="n">
+      <c r="G22" s="17" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="16" t="n">
+      <c r="B23" s="17" t="n">
         <v>15</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17" t="n">
+      <c r="C23" s="18"/>
+      <c r="D23" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17" t="n">
+      <c r="E23" s="18"/>
+      <c r="F23" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G23" s="17" t="n">
+      <c r="G23" s="18" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="16" t="n">
+      <c r="B24" s="17" t="n">
         <v>35</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17" t="n">
+      <c r="C24" s="18"/>
+      <c r="D24" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17" t="n">
+      <c r="E24" s="18"/>
+      <c r="F24" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G24" s="17" t="n">
+      <c r="G24" s="18" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="16" t="n">
+      <c r="B25" s="17" t="n">
         <v>45</v>
       </c>
-      <c r="C25" s="18" t="n">
+      <c r="C25" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="17" t="n">
+      <c r="D25" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17" t="n">
+      <c r="E25" s="18"/>
+      <c r="F25" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G25" s="17" t="n">
+      <c r="G25" s="18" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="16" t="n">
+      <c r="B26" s="17" t="n">
         <v>75</v>
       </c>
-      <c r="C26" s="17" t="n">
+      <c r="C26" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17" t="n">
+      <c r="D26" s="18"/>
+      <c r="E26" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="18" t="n">
+      <c r="F26" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G26" s="18" t="n">
+      <c r="G26" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="16" t="n">
+      <c r="B27" s="17" t="n">
         <v>95</v>
       </c>
-      <c r="C27" s="17" t="n">
+      <c r="C27" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17" t="n">
+      <c r="D27" s="18"/>
+      <c r="E27" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="F27" s="18" t="n">
+      <c r="F27" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="17"/>
+      <c r="G27" s="18"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B10">
@@ -7336,11 +7312,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="1.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="13" width="7.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="13" width="6.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="13" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="13" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="1.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="14" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="14" width="6.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="14" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="14" width="3.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7699,9 +7675,9 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="14"/>
+      <c r="E10" s="15"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="15"/>
+      <c r="G10" s="16"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
@@ -7807,108 +7783,108 @@
       <c r="J20" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="16" t="n">
+      <c r="C22" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="16" t="n">
+      <c r="D22" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="16" t="n">
+      <c r="E22" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="16" t="n">
+      <c r="F22" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="16" t="n">
+      <c r="G22" s="17" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="16" t="n">
+      <c r="B23" s="17" t="n">
         <v>15</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17" t="n">
+      <c r="C23" s="18"/>
+      <c r="D23" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17" t="n">
+      <c r="E23" s="18"/>
+      <c r="F23" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G23" s="17" t="n">
+      <c r="G23" s="18" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="16" t="n">
+      <c r="B24" s="17" t="n">
         <v>35</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17" t="n">
+      <c r="C24" s="18"/>
+      <c r="D24" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17" t="n">
+      <c r="E24" s="18"/>
+      <c r="F24" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G24" s="17" t="n">
+      <c r="G24" s="18" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="16" t="n">
+      <c r="B25" s="17" t="n">
         <v>45</v>
       </c>
-      <c r="C25" s="18" t="n">
+      <c r="C25" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="17" t="n">
+      <c r="D25" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17" t="n">
+      <c r="E25" s="18"/>
+      <c r="F25" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G25" s="17" t="n">
+      <c r="G25" s="18" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="16" t="n">
+      <c r="B26" s="17" t="n">
         <v>75</v>
       </c>
-      <c r="C26" s="17" t="n">
+      <c r="C26" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17" t="n">
+      <c r="D26" s="18"/>
+      <c r="E26" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="18" t="n">
+      <c r="F26" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G26" s="18" t="n">
+      <c r="G26" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="16" t="n">
+      <c r="B27" s="17" t="n">
         <v>95</v>
       </c>
-      <c r="C27" s="17" t="n">
+      <c r="C27" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17" t="n">
+      <c r="D27" s="18"/>
+      <c r="E27" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="F27" s="18" t="n">
+      <c r="F27" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="17"/>
+      <c r="G27" s="18"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B10">
@@ -8219,11 +8195,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="1.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="13" width="7.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="13" width="6.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="13" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="13" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="1.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="14" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="14" width="6.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="14" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="14" width="3.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8582,9 +8558,9 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="14"/>
+      <c r="E10" s="15"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="15"/>
+      <c r="G10" s="16"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
@@ -8690,108 +8666,108 @@
       <c r="J20" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="16" t="n">
+      <c r="C22" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="16" t="n">
+      <c r="D22" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="16" t="n">
+      <c r="E22" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="16" t="n">
+      <c r="F22" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="16" t="n">
+      <c r="G22" s="17" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="16" t="n">
+      <c r="B23" s="17" t="n">
         <v>15</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17" t="n">
+      <c r="C23" s="18"/>
+      <c r="D23" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17" t="n">
+      <c r="E23" s="18"/>
+      <c r="F23" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G23" s="17" t="n">
+      <c r="G23" s="18" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="16" t="n">
+      <c r="B24" s="17" t="n">
         <v>35</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17" t="n">
+      <c r="C24" s="18"/>
+      <c r="D24" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17" t="n">
+      <c r="E24" s="18"/>
+      <c r="F24" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G24" s="17" t="n">
+      <c r="G24" s="18" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="16" t="n">
+      <c r="B25" s="17" t="n">
         <v>45</v>
       </c>
-      <c r="C25" s="18" t="n">
+      <c r="C25" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="17" t="n">
+      <c r="D25" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17" t="n">
+      <c r="E25" s="18"/>
+      <c r="F25" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G25" s="17" t="n">
+      <c r="G25" s="18" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="16" t="n">
+      <c r="B26" s="17" t="n">
         <v>75</v>
       </c>
-      <c r="C26" s="17" t="n">
+      <c r="C26" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17" t="n">
+      <c r="D26" s="18"/>
+      <c r="E26" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="18" t="n">
+      <c r="F26" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G26" s="18" t="n">
+      <c r="G26" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="16" t="n">
+      <c r="B27" s="17" t="n">
         <v>95</v>
       </c>
-      <c r="C27" s="17" t="n">
+      <c r="C27" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17" t="n">
+      <c r="D27" s="18"/>
+      <c r="E27" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="F27" s="18" t="n">
+      <c r="F27" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="17"/>
+      <c r="G27" s="18"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B10">
@@ -9102,9 +9078,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="8.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="13" width="7.64"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="20" min="12" style="13" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="8.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="14" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="20" min="12" style="14" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9134,7 +9110,7 @@
       <c r="R1" s="1"/>
       <c r="S1" s="2"/>
       <c r="T1" s="3"/>
-      <c r="U1" s="13" t="s">
+      <c r="U1" s="14" t="s">
         <v>1</v>
       </c>
     </row>
@@ -9163,22 +9139,22 @@
       <c r="R2" s="5"/>
       <c r="S2" s="6"/>
       <c r="T2" s="7"/>
-      <c r="U2" s="16" t="s">
+      <c r="U2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="V2" s="16" t="n">
+      <c r="V2" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="W2" s="16" t="n">
+      <c r="W2" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="X2" s="16" t="n">
+      <c r="X2" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="Y2" s="16" t="n">
+      <c r="Y2" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="Z2" s="16" t="n">
+      <c r="Z2" s="17" t="n">
         <v>9</v>
       </c>
     </row>
@@ -9207,18 +9183,18 @@
       <c r="R3" s="9"/>
       <c r="S3" s="10"/>
       <c r="T3" s="11"/>
-      <c r="U3" s="16" t="n">
+      <c r="U3" s="17" t="n">
         <v>15</v>
       </c>
-      <c r="V3" s="17"/>
-      <c r="W3" s="19" t="n">
+      <c r="V3" s="18"/>
+      <c r="W3" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="X3" s="17"/>
-      <c r="Y3" s="19" t="n">
+      <c r="X3" s="18"/>
+      <c r="Y3" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="Z3" s="19" t="n">
+      <c r="Z3" s="20" t="n">
         <v>9</v>
       </c>
     </row>
@@ -9251,23 +9227,23 @@
       <c r="R4" s="1"/>
       <c r="S4" s="2"/>
       <c r="T4" s="3"/>
-      <c r="U4" s="16" t="n">
+      <c r="U4" s="17" t="n">
         <v>35</v>
       </c>
-      <c r="V4" s="17"/>
-      <c r="W4" s="19" t="n">
+      <c r="V4" s="18"/>
+      <c r="W4" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="X4" s="17"/>
-      <c r="Y4" s="19" t="n">
+      <c r="X4" s="18"/>
+      <c r="Y4" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="Z4" s="19" t="n">
+      <c r="Z4" s="20" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="n">
+      <c r="A5" s="14" t="n">
         <v>12489</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -9307,20 +9283,20 @@
       <c r="R5" s="5"/>
       <c r="S5" s="6"/>
       <c r="T5" s="7"/>
-      <c r="U5" s="16" t="n">
+      <c r="U5" s="17" t="n">
         <v>45</v>
       </c>
-      <c r="V5" s="18" t="n">
+      <c r="V5" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="W5" s="19" t="n">
+      <c r="W5" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="X5" s="17"/>
-      <c r="Y5" s="19" t="n">
+      <c r="X5" s="18"/>
+      <c r="Y5" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="Z5" s="19" t="n">
+      <c r="Z5" s="20" t="n">
         <v>9</v>
       </c>
     </row>
@@ -9355,20 +9331,20 @@
       <c r="R6" s="9"/>
       <c r="S6" s="10"/>
       <c r="T6" s="11"/>
-      <c r="U6" s="16" t="n">
+      <c r="U6" s="17" t="n">
         <v>75</v>
       </c>
-      <c r="V6" s="17" t="n">
+      <c r="V6" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="W6" s="17"/>
-      <c r="X6" s="17" t="n">
+      <c r="W6" s="18"/>
+      <c r="X6" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="Y6" s="18" t="n">
+      <c r="Y6" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="Z6" s="18" t="n">
+      <c r="Z6" s="19" t="n">
         <v>9</v>
       </c>
     </row>
@@ -9397,20 +9373,20 @@
       <c r="R7" s="1"/>
       <c r="S7" s="2"/>
       <c r="T7" s="3"/>
-      <c r="U7" s="16" t="n">
+      <c r="U7" s="17" t="n">
         <v>95</v>
       </c>
-      <c r="V7" s="17" t="n">
+      <c r="V7" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="W7" s="17"/>
-      <c r="X7" s="17" t="n">
+      <c r="W7" s="18"/>
+      <c r="X7" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="Y7" s="18" t="n">
+      <c r="Y7" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="Z7" s="17"/>
+      <c r="Z7" s="18"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="5" t="s">
@@ -9472,7 +9448,7 @@
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="20"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="6"/>
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
@@ -9845,7 +9821,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="13" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="14" width="7.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9861,45 +9837,45 @@
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
       <c r="E2" s="6"/>
-      <c r="F2" s="24" t="n">
+      <c r="F2" s="25" t="n">
         <v>8</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26" t="n">
+      <c r="G2" s="26"/>
+      <c r="H2" s="27" t="n">
         <v>3</v>
       </c>
       <c r="I2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9"/>
-      <c r="B3" s="27"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="11"/>
-      <c r="D3" s="28" t="n">
+      <c r="D3" s="29" t="n">
         <v>5</v>
       </c>
       <c r="E3" s="10"/>
-      <c r="F3" s="29"/>
+      <c r="F3" s="30"/>
       <c r="G3" s="9"/>
-      <c r="H3" s="30"/>
+      <c r="H3" s="31"/>
       <c r="I3" s="11" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="33"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="34" t="n">
+      <c r="F4" s="35" t="n">
         <v>4</v>
       </c>
-      <c r="G4" s="35"/>
-      <c r="H4" s="36" t="n">
+      <c r="G4" s="36"/>
+      <c r="H4" s="37" t="n">
         <v>1</v>
       </c>
       <c r="I4" s="3"/>
@@ -9917,47 +9893,47 @@
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="9"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="39" t="n">
+      <c r="B6" s="38"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="40" t="n">
         <v>7</v>
       </c>
       <c r="E6" s="10"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="42"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="43"/>
       <c r="I6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
-      <c r="B7" s="43" t="n">
+      <c r="B7" s="44" t="n">
         <v>8</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="44"/>
+      <c r="D7" s="45"/>
       <c r="E7" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="F7" s="45"/>
+      <c r="F7" s="46"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="46"/>
+      <c r="H7" s="47"/>
       <c r="I7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="48" t="n">
+      <c r="B8" s="48"/>
+      <c r="C8" s="49" t="n">
         <v>9</v>
       </c>
-      <c r="D8" s="49"/>
+      <c r="D8" s="50"/>
       <c r="E8" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="50"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="52" t="n">
+      <c r="F8" s="51"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="53" t="n">
         <v>7</v>
       </c>
       <c r="I8" s="7"/>
@@ -10094,102 +10070,102 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="4.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="4.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17"/>
-      <c r="D2" s="13" t="s">
+      <c r="A2" s="18"/>
+      <c r="D2" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17"/>
-      <c r="D3" s="13" t="s">
+      <c r="A3" s="18"/>
+      <c r="D3" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="n">
+      <c r="A5" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17"/>
+      <c r="A6" s="18"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="n">
+      <c r="A7" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17"/>
+      <c r="A8" s="18"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="n">
+      <c r="A9" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17"/>
+      <c r="A10" s="18"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="n">
+      <c r="A11" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17"/>
+      <c r="A12" s="18"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17"/>
+      <c r="A13" s="18"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="17"/>
+      <c r="A14" s="18"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="17"/>
+      <c r="A15" s="18"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="17"/>
-    </row>
-    <row r="17" s="17" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A16" s="18"/>
+    </row>
+    <row r="17" s="18" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="17"/>
+      <c r="A18" s="18"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
ensured df is defined correctly
</commit_message>
<xml_diff>
--- a/data/SDK.xlsx
+++ b/data/SDK.xlsx
@@ -17,6 +17,7 @@
     <sheet name="Trip square" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="NRC" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="Trucs" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="book_8" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -549,7 +550,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4896,7 +4897,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4906,28 +4907,28 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C1" s="3" t="n">
-        <v>8</v>
+        <v>246</v>
       </c>
       <c r="D1" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="n">
-        <v>5</v>
+        <v>158</v>
       </c>
       <c r="F1" s="3" t="n">
-        <v>2</v>
+        <v>156</v>
       </c>
       <c r="G1" s="1" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="H1" s="2" t="n">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="I1" s="3" t="n">
         <v>7</v>
@@ -4939,26 +4940,32 @@
     </row>
     <row r="2" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>467</v>
+      </c>
+      <c r="D2" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="B2" s="6" t="n">
-        <v>35</v>
-      </c>
-      <c r="C2" s="7" t="n">
+      <c r="E2" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="F2" s="7" t="n">
+        <v>167</v>
+      </c>
+      <c r="G2" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="6" t="n">
-        <v>7</v>
-      </c>
-      <c r="F2" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="7"/>
+      <c r="H2" s="6" t="n">
+        <v>48</v>
+      </c>
+      <c r="I2" s="7" t="n">
+        <v>16</v>
+      </c>
       <c r="K2" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,2)=9,2,"")</f>
         <v/>
@@ -4966,56 +4973,68 @@
     </row>
     <row r="3" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="n">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="B3" s="10" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C3" s="11" t="n">
+        <v>67</v>
+      </c>
+      <c r="D3" s="9" t="n">
+        <v>167</v>
+      </c>
+      <c r="E3" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="D3" s="9" t="n">
+      <c r="G3" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3" s="10" t="n">
+        <v>5</v>
+      </c>
+      <c r="I3" s="11" t="n">
         <v>9</v>
       </c>
-      <c r="E3" s="10" t="n">
-        <v>8</v>
-      </c>
-      <c r="F3" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" s="8" t="str">
+      <c r="K3" s="12" t="n">
         <f aca="false">IF(COUNTIF($A$1:$I$9,3)=9,3,"")</f>
-        <v/>
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>27</v>
+      </c>
       <c r="C4" s="3" t="n">
-        <v>69</v>
+        <v>257</v>
       </c>
       <c r="D4" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="I4" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="3"/>
-      <c r="K4" s="12" t="n">
+      <c r="K4" s="12" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,4)=9,4,"")</f>
-        <v>4</v>
+        <v/>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5023,24 +5042,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C5" s="7" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E5" s="6" t="n">
         <v>9</v>
       </c>
       <c r="F5" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
+        <v>57</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>57</v>
+      </c>
+      <c r="H5" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="I5" s="7" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K5" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,5)=9,5,"")</f>
@@ -5049,23 +5072,31 @@
     </row>
     <row r="6" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="n">
-        <v>56</v>
-      </c>
-      <c r="B6" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="B6" s="10" t="n">
+        <v>9</v>
+      </c>
       <c r="C6" s="11" t="n">
+        <v>57</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="F6" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="D6" s="9" t="n">
+      <c r="G6" s="9" t="n">
+        <v>57</v>
+      </c>
+      <c r="H6" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11" t="n">
-        <v>7</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="10"/>
       <c r="I6" s="11" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K6" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,6)=9,6,"")</f>
@@ -5074,56 +5105,58 @@
     </row>
     <row r="7" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C7" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="E7" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="E7" s="2" t="n">
-        <v>2</v>
-      </c>
       <c r="F7" s="3" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>369</v>
+        <v>8</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>39</v>
-      </c>
-      <c r="K7" s="12" t="n">
+        <v>16</v>
+      </c>
+      <c r="K7" s="12" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,7)=9,7,"")</f>
-        <v>7</v>
+        <v/>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="B8" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>5</v>
+      </c>
       <c r="C8" s="7" t="n">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E8" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F8" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="G8" s="5" t="n">
         <v>4</v>
-      </c>
-      <c r="F8" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="G8" s="5" t="n">
-        <v>1</v>
       </c>
       <c r="H8" s="6" t="n">
         <v>7</v>
@@ -5141,122 +5174,142 @@
         <v>7</v>
       </c>
       <c r="B9" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>16</v>
+      </c>
+      <c r="E9" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="F9" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="E9" s="10" t="n">
+      <c r="G9" s="9" t="n">
+        <v>16</v>
+      </c>
+      <c r="H9" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="F9" s="11" t="n">
+      <c r="I9" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="K9" s="13" t="n">
+        <f aca="false">IF(COUNTIF($A$1:$I$9,9)=9,9,"")</f>
         <v>9</v>
       </c>
-      <c r="G9" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="H9" s="10" t="n">
-        <v>4</v>
-      </c>
-      <c r="I9" s="11" t="n">
-        <v>8</v>
-      </c>
-      <c r="K9" s="13" t="str">
-        <f aca="false">IF(COUNTIF($A$1:$I$9,9)=9,9,"")</f>
-        <v/>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E11" s="0" t="n">
-        <v>16</v>
-      </c>
-    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <conditionalFormatting sqref="A2:A9">
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C9">
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B9">
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D9">
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E9">
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G9">
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H9">
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I9">
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A1:A9">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:I1">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:I2">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:I3">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:I4">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C6">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:I5">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C3">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:I6">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:C9">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:I7">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:I8">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:I9">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F3">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:F6">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F9">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
+    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
+    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:I3">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
+    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
+    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:I6">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
+    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:I9">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
+    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
+    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
+    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -5264,6 +5317,340 @@
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="I1" s="3" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="B2" s="6" t="n">
+        <v>35</v>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="F2" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="n">
+        <v>35</v>
+      </c>
+      <c r="B3" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="C3" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9" t="n">
+        <v>9</v>
+      </c>
+      <c r="E3" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3" t="n">
+        <v>69</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="F5" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="7" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="n">
+        <v>56</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="11" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>369</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7" t="n">
+        <v>69</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="I8" s="7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="E9" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="G9" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="H9" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="I9" s="11" t="n">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:A9">
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:I1">
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C9">
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:I2">
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:I3">
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:I4">
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:C6">
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:I5">
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B9">
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C3">
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:I6">
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7:C9">
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7:I7">
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:I8">
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:I9">
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:F3">
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D9">
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:F6">
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7:F9">
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E9">
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F9">
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:I3">
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G9">
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:I6">
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7:I9">
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H9">
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I9">
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -5279,7 +5666,7 @@
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
@@ -5544,85 +5931,85 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A9">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:I1">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:I2">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:I3">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:I4">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C6">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:I5">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C3">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:I6">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:C9">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:I7">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:I8">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:I9">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F3">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:F6">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F9">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:I3">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:I6">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:I9">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -6122,289 +6509,289 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B10">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D10">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C10">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:D10">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10 B10:F10">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E10">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:F10">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F10">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H10">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I10">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J10 K5">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B20">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:J12">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D20">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:J13">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:J14">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:J15">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:D17">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:J16">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C20">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:D14">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="58"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:J17">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="59"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:D20">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="60"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:J18">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="61"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:J19">
-    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54"/>
+    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="62"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:J20">
-    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55"/>
+    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:G14">
-    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56"/>
+    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:E20">
-    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="57"/>
+    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:G17">
-    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="58"/>
+    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:G20">
-    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="59"/>
+    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F20">
-    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="60"/>
+    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G20">
-    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="61"/>
+    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:J14">
-    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="62"/>
+    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H20">
-    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63"/>
+    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="71"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:J17">
-    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64"/>
+    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="72"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:J20">
-    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65"/>
+    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="73"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I20">
-    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66"/>
+    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:J20">
-    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67"/>
+    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="75"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L9">
-    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68"/>
+    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:U1">
-    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69"/>
+    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N9">
-    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70"/>
+    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:U2">
-    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="71"/>
+    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="79"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:U3">
-    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="72"/>
+    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:U4">
-    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="73"/>
+    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="81"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:N6">
-    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74"/>
+    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="82"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:U5">
-    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="75"/>
+    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="83"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M9">
-    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76"/>
+    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="84"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:N3">
-    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77"/>
+    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:U6">
-    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78"/>
+    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="86"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:N9">
-    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="79"/>
+    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="87"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:U7">
-    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80"/>
+    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="88"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:U8">
-    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="81"/>
+    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="89"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:U9">
-    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="82"/>
+    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="90"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:Q3">
-    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="83"/>
+    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="91"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O9">
-    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="84"/>
+    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="92"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:Q6">
-    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85"/>
+    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="93"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7:Q9">
-    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="86"/>
+    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="94"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P9">
-    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="87"/>
+    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="95"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q9">
-    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="88"/>
+    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:U3">
-    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="89"/>
+    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R9">
-    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="90"/>
+    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="98"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4:U6">
-    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="91"/>
+    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7:U9">
-    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="92"/>
+    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="100"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S9">
-    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="93"/>
+    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="101"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:U9">
-    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="94"/>
+    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:J1">
-    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
+    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
+    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J2">
-    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
+    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J3">
-    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
+    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:J4">
-    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
+    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:D6">
-    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
+    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:J5">
-    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
+    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
+    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D3">
-    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
+    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:J6">
-    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
+    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D9">
-    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
+    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:J7">
-    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
+    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:J8">
-    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
+    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:J9">
-    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
+    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G3">
-    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
+    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
+    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:G6">
-    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
+    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:G9">
-    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
+    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
+    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
+    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J3">
-    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
+    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
+    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J6">
-    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
+    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:J9">
-    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
+    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
+    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J9">
-    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
+    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -7005,46 +7392,46 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B10">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="95"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D10">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="97"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="103"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C10">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="98"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:D10">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="104"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10 B10:F10">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="100"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="105"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E10">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="101"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:F10">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="106"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F10">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="103"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H10">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="104"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="105"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="106"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="108"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I10">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J10 K5">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="108"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B20">
     <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="109"/>
@@ -7209,85 +7596,85 @@
     <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="162"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:J1">
-    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
+    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
+    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J2">
-    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
+    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J3">
-    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
+    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:J4">
-    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
+    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:D6">
-    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
+    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:J5">
-    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
+    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
+    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D3">
-    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
+    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:J6">
-    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
+    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D9">
-    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
+    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:J7">
-    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
+    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:J8">
-    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
+    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:J9">
-    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
+    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G3">
-    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
+    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
+    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:G6">
-    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
+    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:G9">
-    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
+    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
+    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
+    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J3">
-    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
+    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
+    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J6">
-    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
+    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:J9">
-    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
+    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
+    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J9">
-    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
+    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8092,85 +8479,85 @@
     <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="230"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:J1">
-    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
+    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
+    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J2">
-    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
+    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J3">
-    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
+    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:J4">
-    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
+    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:D6">
-    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
+    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:J5">
-    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
+    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
+    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D3">
-    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
+    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:J6">
-    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
+    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D9">
-    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
+    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:J7">
-    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
+    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:J8">
-    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
+    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:J9">
-    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
+    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G3">
-    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
+    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
+    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:G6">
-    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
+    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:G9">
-    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
+    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
+    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
+    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J3">
-    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
+    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
+    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J6">
-    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
+    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:J9">
-    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
+    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
+    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J9">
-    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
+    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8975,85 +9362,85 @@
     <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="298"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:J1">
-    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
+    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
+    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J2">
-    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
+    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J3">
-    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
+    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:J4">
-    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
+    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:D6">
-    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
+    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:J5">
-    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
+    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
+    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D3">
-    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
+    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:J6">
-    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
+    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D9">
-    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
+    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:J7">
-    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
+    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:J8">
-    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
+    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:J9">
-    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
+    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G3">
-    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
+    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
+    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:G6">
-    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
+    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:G9">
-    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
+    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
+    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
+    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J3">
-    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
+    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
+    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J6">
-    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
+    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:J9">
-    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
+    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
+    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J9">
-    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
+    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Swordfish has code for user input if to use multiple choice function
</commit_message>
<xml_diff>
--- a/data/SDK.xlsx
+++ b/data/SDK.xlsx
@@ -530,7 +530,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -546,11 +546,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -723,7 +723,385 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="411">
+  <dxfs count="438">
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4897,7 +5275,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4907,31 +5285,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C1" s="3" t="n">
-        <v>246</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="n">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="E1" s="2" t="n">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="F1" s="3" t="n">
-        <v>156</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="n">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="H1" s="2" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="I1" s="3" t="n">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="K1" s="4" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,1)=9,1,"")</f>
@@ -4940,376 +5318,350 @@
     </row>
     <row r="2" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
-        <v>5</v>
+        <v>458</v>
       </c>
       <c r="B2" s="6" t="n">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C2" s="7" t="n">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>9</v>
       </c>
       <c r="E2" s="6" t="n">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="F2" s="7" t="n">
-        <v>167</v>
+        <v>3</v>
       </c>
       <c r="G2" s="5" t="n">
         <v>2</v>
       </c>
       <c r="H2" s="6" t="n">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="I2" s="7" t="n">
-        <v>16</v>
-      </c>
-      <c r="K2" s="8" t="str">
+        <v>1</v>
+      </c>
+      <c r="K2" s="8" t="n">
         <f aca="false">IF(COUNTIF($A$1:$I$9,2)=9,2,"")</f>
-        <v/>
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="10" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C3" s="11" t="n">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="D3" s="9" t="n">
-        <v>167</v>
+        <v>14</v>
       </c>
       <c r="E3" s="10" t="n">
         <v>2</v>
       </c>
       <c r="F3" s="11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G3" s="9" t="n">
+        <v>49</v>
+      </c>
+      <c r="H3" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="H3" s="10" t="n">
-        <v>5</v>
-      </c>
       <c r="I3" s="11" t="n">
-        <v>9</v>
-      </c>
-      <c r="K3" s="12" t="n">
+        <v>8</v>
+      </c>
+      <c r="K3" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,3)=9,3,"")</f>
-        <v>3</v>
+        <v/>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>27</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="3" t="n">
-        <v>257</v>
+        <v>3456</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>15</v>
+        <v>145</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>9</v>
+        <v>1346</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="K4" s="12" t="str">
+        <v>2</v>
+      </c>
+      <c r="K4" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,4)=9,4,"")</f>
         <v/>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
-        <v>4</v>
+        <v>348</v>
       </c>
       <c r="B5" s="6" t="n">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="C5" s="7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>2</v>
       </c>
       <c r="E5" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="F5" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="F5" s="7" t="n">
-        <v>57</v>
-      </c>
       <c r="G5" s="5" t="n">
-        <v>57</v>
+        <v>5</v>
       </c>
       <c r="H5" s="6" t="n">
-        <v>1</v>
+        <v>468</v>
       </c>
       <c r="I5" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="K5" s="8" t="str">
+        <v>34</v>
+      </c>
+      <c r="K5" s="12" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,5)=9,5,"")</f>
         <v/>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="n">
-        <v>1</v>
+        <v>458</v>
       </c>
       <c r="B6" s="10" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C6" s="11" t="n">
-        <v>57</v>
+        <v>458</v>
       </c>
       <c r="D6" s="9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6" s="10" t="n">
+        <v>145</v>
+      </c>
+      <c r="F6" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="F6" s="11" t="n">
-        <v>3</v>
-      </c>
       <c r="G6" s="9" t="n">
-        <v>57</v>
+        <v>149</v>
       </c>
       <c r="H6" s="10" t="n">
-        <v>2</v>
+        <v>489</v>
       </c>
       <c r="I6" s="11" t="n">
-        <v>8</v>
-      </c>
-      <c r="K6" s="8" t="str">
+        <v>7</v>
+      </c>
+      <c r="K6" s="12" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,6)=9,6,"")</f>
         <v/>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
+        <v>3457</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>345</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="F7" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B7" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="F7" s="3" t="n">
-        <v>16</v>
-      </c>
       <c r="G7" s="1" t="n">
-        <v>8</v>
+        <v>347</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>16</v>
-      </c>
-      <c r="K7" s="12" t="str">
+        <v>6</v>
+      </c>
+      <c r="K7" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,7)=9,7,"")</f>
         <v/>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B8" s="6" t="n">
+        <v>46</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="C8" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5" t="n">
+      <c r="E8" s="6" t="n">
+        <v>367</v>
+      </c>
+      <c r="F8" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="E8" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="F8" s="7" t="n">
-        <v>9</v>
-      </c>
       <c r="G8" s="5" t="n">
-        <v>4</v>
+        <v>3479</v>
       </c>
       <c r="H8" s="6" t="n">
-        <v>7</v>
+        <v>479</v>
       </c>
       <c r="I8" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="K8" s="8" t="str">
+        <v>349</v>
+      </c>
+      <c r="K8" s="12" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,8)=9,8,"")</f>
         <v/>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="n">
-        <v>7</v>
+        <v>347</v>
       </c>
       <c r="B9" s="10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C9" s="11" t="n">
+        <v>346</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>1467</v>
+      </c>
+      <c r="E9" s="10" t="n">
+        <v>367</v>
+      </c>
+      <c r="F9" s="11" t="n">
+        <v>14</v>
+      </c>
+      <c r="G9" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="C9" s="11" t="n">
-        <v>9</v>
-      </c>
-      <c r="D9" s="9" t="n">
-        <v>16</v>
-      </c>
-      <c r="E9" s="10" t="n">
-        <v>4</v>
-      </c>
-      <c r="F9" s="11" t="n">
+      <c r="H9" s="10" t="n">
         <v>2</v>
-      </c>
-      <c r="G9" s="9" t="n">
-        <v>16</v>
-      </c>
-      <c r="H9" s="10" t="n">
-        <v>3</v>
       </c>
       <c r="I9" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="K9" s="13" t="n">
+      <c r="K9" s="13" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,9)=9,9,"")</f>
-        <v>9</v>
+        <v/>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="A2:A9">
+  <conditionalFormatting sqref="A1:A9">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C9">
+  <conditionalFormatting sqref="A1:I1">
     <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B9">
+  <conditionalFormatting sqref="C1:C9">
     <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="A2:I2">
     <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E9">
+  <conditionalFormatting sqref="A3:I3">
     <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="A4:I4">
     <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H9">
+  <conditionalFormatting sqref="A4:C6">
     <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I9">
+  <conditionalFormatting sqref="A5:I5">
     <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A9">
+  <conditionalFormatting sqref="B1:B9">
     <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:I1">
+  <conditionalFormatting sqref="A1:C3">
     <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C9">
+  <conditionalFormatting sqref="A6:I6">
     <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:I2">
+  <conditionalFormatting sqref="A7:C9">
     <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:I3">
+  <conditionalFormatting sqref="A7:I7">
     <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:I4">
+  <conditionalFormatting sqref="A8:I8">
     <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:C6">
+  <conditionalFormatting sqref="A9:I9">
     <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:I5">
+  <conditionalFormatting sqref="D1:F3">
     <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B9">
+  <conditionalFormatting sqref="D1:D9">
     <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:C3">
+  <conditionalFormatting sqref="D4:F6">
     <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6:I6">
+  <conditionalFormatting sqref="D7:F9">
     <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7:C9">
+  <conditionalFormatting sqref="E1:E9">
     <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7:I7">
+  <conditionalFormatting sqref="F1:F9">
     <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8:I8">
+  <conditionalFormatting sqref="G1:I3">
     <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:I9">
+  <conditionalFormatting sqref="G1:G9">
     <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:F3">
+  <conditionalFormatting sqref="G4:I6">
     <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D9">
+  <conditionalFormatting sqref="G7:I9">
     <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:F6">
+  <conditionalFormatting sqref="H1:H9">
     <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7:F9">
+  <conditionalFormatting sqref="I1:I9">
     <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:I3">
-    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G4:I6">
-    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7:I9">
-    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -5329,10 +5681,10 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
@@ -5565,85 +5917,85 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A9">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:I1">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:I2">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:I3">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:I4">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C6">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:I5">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C3">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:I6">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:C9">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:I7">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:I8">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:I9">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F3">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:F6">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F9">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:I3">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:I6">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:I9">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -5931,85 +6283,85 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A9">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:I1">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:I2">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:I3">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:I4">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C6">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:I5">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C3">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:I6">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:C9">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:I7">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:I8">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:I9">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F3">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:F6">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F9">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:I3">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:I6">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:I9">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -6509,289 +6861,289 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B10">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D10">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C10">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:D10">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="58"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10 B10:F10">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="59"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E10">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="60"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:F10">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="61"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F10">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="62"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H10">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I10">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J10 K5">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B20">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:J12">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D20">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:J13">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="71"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:J14">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="72"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:J15">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="73"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:D17">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:J16">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="75"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C20">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="57"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:D14">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="58"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:J17">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="59"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:D20">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="60"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="79"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:J18">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="61"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:J19">
-    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="62"/>
+    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="81"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:J20">
-    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63"/>
+    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="82"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:G14">
-    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64"/>
+    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="83"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:E20">
-    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65"/>
+    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="84"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:G17">
-    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66"/>
+    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:G20">
-    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67"/>
+    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="86"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F20">
-    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68"/>
+    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="87"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G20">
-    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69"/>
+    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="88"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:J14">
-    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70"/>
+    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="89"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H20">
-    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="71"/>
+    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="90"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:J17">
-    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="72"/>
+    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="91"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:J20">
-    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="73"/>
+    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="92"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I20">
-    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74"/>
+    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="93"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:J20">
-    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="75"/>
+    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="94"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L9">
-    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76"/>
+    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="95"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:U1">
-    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77"/>
+    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N9">
-    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78"/>
+    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:U2">
-    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="79"/>
+    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="98"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:U3">
-    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80"/>
+    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:U4">
-    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="81"/>
+    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="100"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:N6">
-    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="82"/>
+    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="101"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:U5">
-    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="83"/>
+    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M9">
-    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="84"/>
+    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="103"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:N3">
-    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85"/>
+    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="104"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:U6">
-    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="86"/>
+    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="105"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:N9">
-    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="87"/>
+    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="106"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:U7">
-    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="88"/>
+    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:U8">
-    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="89"/>
+    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="108"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:U9">
-    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="90"/>
+    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="109"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:Q3">
-    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="91"/>
+    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="110"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O9">
-    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="92"/>
+    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="111"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:Q6">
-    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="93"/>
+    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="112"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7:Q9">
-    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="94"/>
+    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="113"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P9">
-    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="95"/>
+    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="114"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q9">
-    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96"/>
+    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="115"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:U3">
-    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="97"/>
+    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="116"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R9">
-    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="98"/>
+    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="117"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4:U6">
-    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99"/>
+    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="118"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7:U9">
-    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="100"/>
+    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="119"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S9">
-    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="101"/>
+    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="120"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:U9">
-    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102"/>
+    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="121"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
+    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:J1">
-    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
+    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
+    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J2">
-    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
+    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J3">
-    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
+    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:J4">
-    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
+    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:D6">
-    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
+    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:J5">
-    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
+    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
+    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D3">
-    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
+    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:J6">
-    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
+    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D9">
-    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
+    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:J7">
-    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
+    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:J8">
-    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
+    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:J9">
-    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
+    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G3">
-    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
+    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
+    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:G6">
-    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
+    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:G9">
-    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
+    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
+    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
+    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J3">
-    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
+    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
+    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J6">
-    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
+    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:J9">
-    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
+    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
+    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J9">
-    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
+    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -7392,289 +7744,289 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B10">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="122"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D10">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="123"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="103"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="124"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C10">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="125"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:D10">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="104"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="126"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10 B10:F10">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="105"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="127"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E10">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="128"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:F10">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="106"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="129"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F10">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="130"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H10">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="131"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="132"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="108"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="133"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I10">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="134"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J10 K5">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="135"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B20">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="109"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="136"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:J12">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="110"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="137"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D20">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="111"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="138"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:J13">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="112"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="139"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:J14">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="113"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="140"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:J15">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="114"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="141"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:D17">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="115"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="142"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:J16">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="116"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="143"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C20">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="117"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="144"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:D14">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="118"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="145"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:J17">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="119"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="146"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:D20">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="120"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="147"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:J18">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="121"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="148"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:J19">
-    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="122"/>
+    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="149"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:J20">
-    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="123"/>
+    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="150"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:G14">
-    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="124"/>
+    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="151"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:E20">
-    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="125"/>
+    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="152"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:G17">
-    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="126"/>
+    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="153"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:G20">
-    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="127"/>
+    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="154"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F20">
-    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="128"/>
+    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="155"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G20">
-    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="129"/>
+    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="156"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:J14">
-    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="130"/>
+    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="157"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H20">
-    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="131"/>
+    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="158"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:J17">
-    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="132"/>
+    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="159"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:J20">
-    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="133"/>
+    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="160"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I20">
-    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="134"/>
+    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="161"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:J20">
-    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="135"/>
+    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="162"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L9">
-    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="136"/>
+    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="163"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:U1">
-    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="137"/>
+    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="164"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N9">
-    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="138"/>
+    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="165"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:U2">
-    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="139"/>
+    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="166"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:U3">
-    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="140"/>
+    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="167"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:U4">
-    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="141"/>
+    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="168"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:N6">
-    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="142"/>
+    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="169"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:U5">
-    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="143"/>
+    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="170"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M9">
-    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="144"/>
+    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="171"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:N3">
-    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="145"/>
+    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="172"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:U6">
-    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="146"/>
+    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="173"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:N9">
-    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="147"/>
+    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="174"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:U7">
-    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="148"/>
+    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="175"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:U8">
-    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="149"/>
+    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="176"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:U9">
-    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="150"/>
+    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="177"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:Q3">
-    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="151"/>
+    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="178"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O9">
-    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="152"/>
+    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="179"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:Q6">
-    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="153"/>
+    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="180"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7:Q9">
-    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="154"/>
+    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="181"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P9">
-    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="155"/>
+    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="182"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q9">
-    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="156"/>
+    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="183"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:U3">
-    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="157"/>
+    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="184"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R9">
-    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="158"/>
+    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="185"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4:U6">
-    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="159"/>
+    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="186"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7:U9">
-    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="160"/>
+    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="187"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S9">
-    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="161"/>
+    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="188"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:U9">
-    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="162"/>
+    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="189"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
+    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:J1">
-    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
+    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
+    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J2">
-    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
+    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J3">
-    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
+    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:J4">
-    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
+    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:D6">
-    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
+    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:J5">
-    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
+    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
+    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D3">
-    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
+    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:J6">
-    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
+    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D9">
-    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
+    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:J7">
-    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
+    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:J8">
-    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
+    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:J9">
-    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
+    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G3">
-    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
+    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
+    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:G6">
-    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
+    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:G9">
-    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
+    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
+    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
+    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J3">
-    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
+    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
+    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J6">
-    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
+    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:J9">
-    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
+    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
+    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J9">
-    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
+    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8275,289 +8627,289 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="163"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="190"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="164"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="191"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="165"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="192"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="166"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="193"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:D10">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="167"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="194"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10 B10:F10">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="168"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="195"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="169"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="196"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:F10">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="170"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="197"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="171"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="198"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="172"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="199"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="173"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="200"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="174"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="201"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="175"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="202"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10 K5">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="176"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="203"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B20">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="177"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="204"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:J12">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="178"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="205"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D20">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="179"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="206"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:J13">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="180"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="207"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:J14">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="181"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="208"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:J15">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="182"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="209"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:D17">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="183"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="210"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:J16">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="184"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="211"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C20">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="185"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="212"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:D14">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="186"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="213"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:J17">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="187"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="214"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:D20">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="188"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="215"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:J18">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="189"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="216"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:J19">
-    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="190"/>
+    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="217"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:J20">
-    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="191"/>
+    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="218"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:G14">
-    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="192"/>
+    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="219"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:E20">
-    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="193"/>
+    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="220"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:G17">
-    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="194"/>
+    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="221"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:G20">
-    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="195"/>
+    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="222"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F20">
-    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="196"/>
+    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="223"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G20">
-    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="197"/>
+    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="224"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:J14">
-    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="198"/>
+    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="225"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H20">
-    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="199"/>
+    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="226"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:J17">
-    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="200"/>
+    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="227"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:J20">
-    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="201"/>
+    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="228"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I20">
-    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="202"/>
+    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="229"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:J20">
-    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="203"/>
+    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="230"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L9">
-    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="204"/>
+    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="231"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:U1">
-    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="205"/>
+    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="232"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N9">
-    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="206"/>
+    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="233"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:U2">
-    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="207"/>
+    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="234"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:U3">
-    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="208"/>
+    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="235"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:U4">
-    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="209"/>
+    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="236"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:N6">
-    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="210"/>
+    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="237"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:U5">
-    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="211"/>
+    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="238"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M9">
-    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="212"/>
+    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="239"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:N3">
-    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="213"/>
+    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="240"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:U6">
-    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="214"/>
+    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="241"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:N9">
-    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="215"/>
+    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="242"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:U7">
-    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="216"/>
+    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="243"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:U8">
-    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="217"/>
+    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="244"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:U9">
-    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="218"/>
+    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="245"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:Q3">
-    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="219"/>
+    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="246"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O9">
-    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="220"/>
+    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="247"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:Q6">
-    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="221"/>
+    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="248"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7:Q9">
-    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="222"/>
+    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="249"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P9">
-    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="223"/>
+    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="250"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q9">
-    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="224"/>
+    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="251"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:U3">
-    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="225"/>
+    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="252"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R9">
-    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="226"/>
+    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="253"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4:U6">
-    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="227"/>
+    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="254"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7:U9">
-    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="228"/>
+    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="255"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S9">
-    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="229"/>
+    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="256"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:U9">
-    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="230"/>
+    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="257"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
+    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:J1">
-    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
+    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
+    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J2">
-    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
+    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J3">
-    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
+    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:J4">
-    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
+    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:D6">
-    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
+    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:J5">
-    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
+    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
+    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D3">
-    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
+    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:J6">
-    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
+    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D9">
-    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
+    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:J7">
-    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
+    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:J8">
-    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
+    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:J9">
-    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
+    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G3">
-    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
+    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
+    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:G6">
-    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
+    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:G9">
-    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
+    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
+    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
+    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J3">
-    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
+    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
+    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J6">
-    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
+    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:J9">
-    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
+    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
+    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J9">
-    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
+    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -9158,289 +9510,289 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="231"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="258"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="232"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="259"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="233"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="260"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="234"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="261"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:D10">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="235"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="262"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10 B10:F10">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="236"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="263"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="237"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="264"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:F10">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="238"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="265"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="239"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="266"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="240"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="267"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="241"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="268"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="242"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="269"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="243"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="270"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10 K5">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="244"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="271"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B20">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="245"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="272"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:J12">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="246"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="273"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D20">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="247"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="274"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:J13">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="248"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="275"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:J14">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="249"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="276"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:J15">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="250"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="277"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:D17">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="251"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="278"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:J16">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="252"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="279"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C20">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="253"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="280"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:D14">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="254"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="281"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:J17">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="255"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="282"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:D20">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="256"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="283"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:J18">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="257"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="284"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:J19">
-    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="258"/>
+    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="285"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:J20">
-    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="259"/>
+    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="286"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:G14">
-    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="260"/>
+    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="287"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:E20">
-    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="261"/>
+    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="288"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:G17">
-    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="262"/>
+    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="289"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:G20">
-    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="263"/>
+    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="290"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F20">
-    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="264"/>
+    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="291"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G20">
-    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="265"/>
+    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="292"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:J14">
-    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="266"/>
+    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="293"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H20">
-    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="267"/>
+    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="294"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:J17">
-    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="268"/>
+    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="295"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:J20">
-    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="269"/>
+    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="296"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I20">
-    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="270"/>
+    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="297"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:J20">
-    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="271"/>
+    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="298"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L9">
-    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="272"/>
+    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="299"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:U1">
-    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="273"/>
+    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="300"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N9">
-    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="274"/>
+    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="301"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:U2">
-    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="275"/>
+    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="302"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:U3">
-    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="276"/>
+    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="303"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:U4">
-    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="277"/>
+    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="304"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:N6">
-    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="278"/>
+    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="305"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:U5">
-    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="279"/>
+    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="306"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M9">
-    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="280"/>
+    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="307"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:N3">
-    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="281"/>
+    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="308"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:U6">
-    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="282"/>
+    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="309"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:N9">
-    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="283"/>
+    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="310"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:U7">
-    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="284"/>
+    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="311"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:U8">
-    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="285"/>
+    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="312"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:U9">
-    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="286"/>
+    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="313"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:Q3">
-    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="287"/>
+    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="314"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O9">
-    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="288"/>
+    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="315"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:Q6">
-    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="289"/>
+    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="316"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7:Q9">
-    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="290"/>
+    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="317"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P9">
-    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="291"/>
+    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="318"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q9">
-    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="292"/>
+    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="319"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:U3">
-    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="293"/>
+    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="320"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R9">
-    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="294"/>
+    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="321"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4:U6">
-    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="295"/>
+    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="322"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7:U9">
-    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="296"/>
+    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="323"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S9">
-    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="297"/>
+    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="324"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:U9">
-    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="298"/>
+    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="325"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
+    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:J1">
-    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
+    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
+    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J2">
-    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
+    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J3">
-    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
+    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:J4">
-    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
+    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:D6">
-    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
+    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:J5">
-    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
+    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
+    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D3">
-    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
+    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:J6">
-    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
+    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D9">
-    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
+    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:J7">
-    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
+    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:J8">
-    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
+    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:J9">
-    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
+    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G3">
-    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
+    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
+    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:G6">
-    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
+    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:G9">
-    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
+    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
+    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
+    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J3">
-    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
+    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
+    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J6">
-    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
+    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:J9">
-    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
+    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
+    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J9">
-    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
+    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -9943,247 +10295,247 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B10">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="299"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="326"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:J1">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="300"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="327"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D10">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="301"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="328"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J2">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="302"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="329"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J3">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="303"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="330"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:J4">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="304"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="331"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:D6">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="305"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="332"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:K5">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="306"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="333"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C10">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="307"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="334"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D3">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="308"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="335"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:J6">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="309"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="336"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D10">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="310"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="337"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:J7">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="311"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="338"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:J8">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="312"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="339"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:J9 H10:J10 B10:F10">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="313"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="340"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G3">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="314"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="341"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E10">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="315"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="342"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:G6">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="316"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="343"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:G9 E10:F10">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="317"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="344"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F10">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="318"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="345"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="319"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="346"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J3">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="320"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="347"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H10">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="321"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="348"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J6 K5">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="322"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="349"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:J10">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="323"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="350"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I10">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="324"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="351"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J10 K5">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="325"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="352"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B20">
-    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="326"/>
+    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="353"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:J12">
-    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="327"/>
+    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="354"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D20">
-    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="328"/>
+    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="355"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:J13">
-    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="329"/>
+    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="356"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:J14">
-    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="330"/>
+    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="357"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:J15">
-    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="331"/>
+    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="358"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:D17">
-    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="332"/>
+    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="359"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:J16">
-    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="333"/>
+    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="360"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C20">
-    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="334"/>
+    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="361"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:D14">
-    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="335"/>
+    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="362"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:J17">
-    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="336"/>
+    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="363"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:D20">
-    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="337"/>
+    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="364"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:J18">
-    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="338"/>
+    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="365"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:J19">
-    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="339"/>
+    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="366"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:J20">
-    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="340"/>
+    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="367"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:G14">
-    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="341"/>
+    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="368"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:E20">
-    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="342"/>
+    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="369"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:G17">
-    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="343"/>
+    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="370"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:G20">
-    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="344"/>
+    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="371"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F20">
-    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="345"/>
+    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="372"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G20">
-    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="346"/>
+    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="373"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:J14">
-    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="347"/>
+    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="374"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H20">
-    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="348"/>
+    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="375"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:J17">
-    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="349"/>
+    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="376"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:J20">
-    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="350"/>
+    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="377"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I20">
-    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="351"/>
+    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="378"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:J20">
-    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="352"/>
+    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="379"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L9">
-    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="353"/>
+    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="380"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:T1">
-    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="354"/>
+    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="381"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N9">
-    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="355"/>
+    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="382"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:T2">
-    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="356"/>
+    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="383"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:T3">
-    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="357"/>
+    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="384"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:T4">
-    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="358"/>
+    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="385"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:N6">
-    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="359"/>
+    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="386"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:T5">
-    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="360"/>
+    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="387"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M9">
-    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="361"/>
+    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="388"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:N3">
-    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="362"/>
+    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="389"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:T6">
-    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="363"/>
+    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="390"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:N9">
-    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="364"/>
+    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="391"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:T7">
-    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="365"/>
+    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="392"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:T8">
-    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="366"/>
+    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="393"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:T9">
-    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="367"/>
+    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="394"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:Q3">
-    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="368"/>
+    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="395"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O9">
-    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="369"/>
+    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="396"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:Q6">
-    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="370"/>
+    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="397"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7:Q9">
-    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="371"/>
+    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="398"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P9">
-    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="372"/>
+    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="399"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q9">
-    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="373"/>
+    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="400"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:T3">
-    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="374"/>
+    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="401"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R9">
-    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="375"/>
+    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="402"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4:T6">
-    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="376"/>
+    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="403"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7:T9">
-    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="377"/>
+    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="404"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S9">
-    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="378"/>
+    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="405"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T9">
-    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="379"/>
+    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="406"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -10342,97 +10694,97 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A9">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="380"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="407"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:I1">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="381"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="408"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="382"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="409"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:I2">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="383"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="410"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:I3">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="384"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="411"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:I4">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="385"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="412"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C6">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="386"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="413"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:I5">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="387"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="414"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="388"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="415"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C3">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="389"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="416"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:I6">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="390"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="417"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:C9">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="391"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="418"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:I7">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="392"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="419"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:I8">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="393"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="420"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:I9">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="394"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="421"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F3">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="395"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="422"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="396"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="423"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:F6">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="397"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="424"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F9">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="398"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="425"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="399"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="426"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="400"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="427"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:I3">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="401"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="428"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="402"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="429"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:I6">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="403"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="430"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:I9">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="404"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="431"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="405"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="432"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="406"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="433"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:D4">
-    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="407"/>
+    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="434"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:H4">
-    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="408"/>
+    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="435"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:D8">
-    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="409"/>
+    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="436"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:H8">
-    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="410"/>
+    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="437"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
In X-wing family reduced number of oprint lines and always ask user input to fill empty cells
</commit_message>
<xml_diff>
--- a/data/SDK.xlsx
+++ b/data/SDK.xlsx
@@ -550,7 +550,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -723,385 +723,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="438">
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="411">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5274,8 +4896,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5285,31 +4907,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="n">
+      <c r="C1" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="n">
-        <v>19</v>
-      </c>
       <c r="D1" s="1" t="n">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="E1" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="n">
-        <v>14</v>
-      </c>
       <c r="G1" s="1" t="n">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="n">
         <v>5</v>
       </c>
       <c r="I1" s="3" t="n">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="K1" s="4" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,1)=9,1,"")</f>
@@ -5318,64 +4940,64 @@
     </row>
     <row r="2" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
-        <v>458</v>
+        <v>14</v>
       </c>
       <c r="B2" s="6" t="n">
-        <v>45</v>
+        <v>1467</v>
       </c>
       <c r="C2" s="7" t="n">
-        <v>458</v>
+        <v>1467</v>
       </c>
       <c r="D2" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="E2" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" s="7" t="n">
+        <v>25</v>
+      </c>
+      <c r="G2" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="n">
-        <v>67</v>
-      </c>
-      <c r="F2" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="G2" s="5" t="n">
-        <v>2</v>
-      </c>
       <c r="H2" s="6" t="n">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="I2" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" s="8" t="n">
+        <v>178</v>
+      </c>
+      <c r="K2" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,2)=9,2,"")</f>
-        <v>2</v>
+        <v/>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="n">
+        <v>18</v>
+      </c>
+      <c r="B3" s="10" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" s="11" t="n">
+        <v>178</v>
+      </c>
+      <c r="D3" s="9" t="n">
+        <v>9</v>
+      </c>
+      <c r="E3" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="B3" s="10" t="n">
-        <v>7</v>
-      </c>
-      <c r="C3" s="11" t="n">
-        <v>19</v>
-      </c>
-      <c r="D3" s="9" t="n">
-        <v>14</v>
-      </c>
-      <c r="E3" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="F3" s="11" t="n">
-        <v>5</v>
-      </c>
       <c r="G3" s="9" t="n">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="H3" s="10" t="n">
         <v>3</v>
       </c>
       <c r="I3" s="11" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="K3" s="8" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,3)=9,3,"")</f>
@@ -5384,62 +5006,64 @@
     </row>
     <row r="4" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>134</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>123</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="I4" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3" t="n">
-        <v>3456</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>145</v>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>1346</v>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>46</v>
-      </c>
-      <c r="I4" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="K4" s="8" t="str">
+      <c r="K4" s="12" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,4)=9,4,"")</f>
         <v/>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
-        <v>348</v>
+        <v>5</v>
       </c>
       <c r="B5" s="6" t="n">
-        <v>146</v>
+        <v>8</v>
       </c>
       <c r="C5" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="F5" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="G5" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="H5" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="E5" s="6" t="n">
-        <v>14</v>
-      </c>
-      <c r="F5" s="7" t="n">
-        <v>9</v>
-      </c>
-      <c r="G5" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="H5" s="6" t="n">
-        <v>468</v>
-      </c>
       <c r="I5" s="7" t="n">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="K5" s="12" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,5)=9,5,"")</f>
@@ -5448,31 +5072,31 @@
     </row>
     <row r="6" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="n">
-        <v>458</v>
+        <v>6</v>
       </c>
       <c r="B6" s="10" t="n">
+        <v>13</v>
+      </c>
+      <c r="C6" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="11" t="n">
-        <v>458</v>
-      </c>
       <c r="D6" s="9" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E6" s="10" t="n">
-        <v>145</v>
+        <v>9</v>
       </c>
       <c r="F6" s="11" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="G6" s="9" t="n">
-        <v>149</v>
+        <v>4</v>
       </c>
       <c r="H6" s="10" t="n">
-        <v>489</v>
+        <v>7</v>
       </c>
       <c r="I6" s="11" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K6" s="12" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,6)=9,6,"")</f>
@@ -5481,64 +5105,64 @@
     </row>
     <row r="7" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>3457</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>345</v>
+        <v>68</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>347</v>
+        <v>15</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="K7" s="8" t="str">
+        <v>68</v>
+      </c>
+      <c r="K7" s="12" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,7)=9,7,"")</f>
         <v/>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
-        <v>1</v>
+        <v>148</v>
       </c>
       <c r="B8" s="6" t="n">
-        <v>46</v>
+        <v>1467</v>
       </c>
       <c r="C8" s="7" t="n">
+        <v>14678</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="E8" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="D8" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E8" s="6" t="n">
-        <v>367</v>
-      </c>
       <c r="F8" s="7" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>3479</v>
+        <v>1357</v>
       </c>
       <c r="H8" s="6" t="n">
-        <v>479</v>
+        <v>18</v>
       </c>
       <c r="I8" s="7" t="n">
-        <v>349</v>
+        <v>13678</v>
       </c>
       <c r="K8" s="12" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9,8)=9,8,"")</f>
@@ -5547,35 +5171,35 @@
     </row>
     <row r="9" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="n">
-        <v>347</v>
+        <v>3</v>
       </c>
       <c r="B9" s="10" t="n">
+        <v>17</v>
+      </c>
+      <c r="C9" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="E9" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="F9" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G9" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="C9" s="11" t="n">
-        <v>346</v>
-      </c>
-      <c r="D9" s="9" t="n">
-        <v>1467</v>
-      </c>
-      <c r="E9" s="10" t="n">
-        <v>367</v>
-      </c>
-      <c r="F9" s="11" t="n">
-        <v>14</v>
-      </c>
-      <c r="G9" s="9" t="n">
-        <v>8</v>
-      </c>
-      <c r="H9" s="10" t="n">
-        <v>2</v>
-      </c>
       <c r="I9" s="11" t="n">
-        <v>5</v>
-      </c>
-      <c r="K9" s="13" t="str">
+        <v>17</v>
+      </c>
+      <c r="K9" s="13" t="n">
         <f aca="false">IF(COUNTIF($A$1:$I$9,9)=9,9,"")</f>
-        <v/>
+        <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5680,11 +5304,11 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
@@ -5917,85 +5541,85 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A9">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:I1">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:I2">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:I3">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:I4">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C6">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:I5">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C3">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:I6">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:C9">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:I7">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:I8">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:I9">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F3">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:F6">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F9">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:I3">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:I6">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:I9">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -6014,7 +5638,7 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -6283,85 +5907,85 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A9">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:I1">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:I2">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:I3">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:I4">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C6">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:I5">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C3">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:I6">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:C9">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:I7">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:I8">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:I9">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F3">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:F6">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F9">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:I3">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:I6">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:I9">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -6380,7 +6004,7 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -6861,289 +6485,289 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B10">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D10">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C10">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="57"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:D10">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="58"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10 B10:F10">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="59"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E10">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="60"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:F10">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="61"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F10">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="62"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H10">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I10">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J10 K5">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B20">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:J12">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D20">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:J13">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="71"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:J14">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="72"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:J15">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="73"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:D17">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:J16">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="75"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C20">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:D14">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:J17">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:D20">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="79"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:J18">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:J19">
-    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="81"/>
+    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:J20">
-    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="82"/>
+    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:G14">
-    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="83"/>
+    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:E20">
-    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="84"/>
+    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:G17">
-    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85"/>
+    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="58"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:G20">
-    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="86"/>
+    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="59"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F20">
-    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="87"/>
+    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="60"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G20">
-    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="88"/>
+    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="61"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:J14">
-    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="89"/>
+    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="62"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H20">
-    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="90"/>
+    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:J17">
-    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="91"/>
+    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:J20">
-    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="92"/>
+    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I20">
-    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="93"/>
+    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:J20">
-    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="94"/>
+    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L9">
-    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="95"/>
+    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:U1">
-    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96"/>
+    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N9">
-    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="97"/>
+    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:U2">
-    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="98"/>
+    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="71"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:U3">
-    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99"/>
+    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="72"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:U4">
-    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="100"/>
+    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="73"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:N6">
-    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="101"/>
+    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:U5">
-    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102"/>
+    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="75"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M9">
-    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="103"/>
+    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:N3">
-    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="104"/>
+    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:U6">
-    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="105"/>
+    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:N9">
-    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="106"/>
+    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="79"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:U7">
-    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107"/>
+    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:U8">
-    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="108"/>
+    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="81"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:U9">
-    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="109"/>
+    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="82"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:Q3">
-    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="110"/>
+    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="83"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O9">
-    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="111"/>
+    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="84"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:Q6">
-    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="112"/>
+    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7:Q9">
-    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="113"/>
+    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="86"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P9">
-    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="114"/>
+    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="87"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q9">
-    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="115"/>
+    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="88"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:U3">
-    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="116"/>
+    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="89"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R9">
-    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="117"/>
+    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="90"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4:U6">
-    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="118"/>
+    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="91"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7:U9">
-    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="119"/>
+    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="92"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S9">
-    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="120"/>
+    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="93"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:U9">
-    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="121"/>
+    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="94"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
+    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:J1">
-    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
+    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
+    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J2">
-    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
+    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J3">
-    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
+    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:J4">
-    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
+    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:D6">
-    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
+    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:J5">
-    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
+    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35"/>
+    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D3">
-    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36"/>
+    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:J6">
-    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37"/>
+    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D9">
-    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38"/>
+    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:J7">
-    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39"/>
+    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:J8">
-    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40"/>
+    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:J9">
-    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41"/>
+    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G3">
-    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42"/>
+    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43"/>
+    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:G6">
-    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44"/>
+    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:G9">
-    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45"/>
+    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46"/>
+    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47"/>
+    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J3">
-    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48"/>
+    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49"/>
+    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J6">
-    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50"/>
+    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:J9">
-    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51"/>
+    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52"/>
+    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J9">
-    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53"/>
+    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -7162,7 +6786,7 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -7744,289 +7368,289 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B10">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="122"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="95"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D10">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="123"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="124"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C10">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="125"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="98"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:D10">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="126"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10 B10:F10">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="127"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="100"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E10">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="128"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="101"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:F10">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="129"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F10">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="130"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="103"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H10">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="131"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="104"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="132"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="105"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="133"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="106"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I10">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="134"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J10 K5">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="135"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="108"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B20">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="136"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="109"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:J12">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="137"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="110"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D20">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="138"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="111"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:J13">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="139"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="112"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:J14">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="140"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="113"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:J15">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="141"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="114"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:D17">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="142"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="115"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:J16">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="143"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="116"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C20">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="144"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="117"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:D14">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="145"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="118"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:J17">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="146"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="119"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:D20">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="147"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="120"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:J18">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="148"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="121"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:J19">
-    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="149"/>
+    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="122"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:J20">
-    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="150"/>
+    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="123"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:G14">
-    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="151"/>
+    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="124"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:E20">
-    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="152"/>
+    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="125"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:G17">
-    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="153"/>
+    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="126"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:G20">
-    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="154"/>
+    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="127"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F20">
-    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="155"/>
+    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="128"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G20">
-    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="156"/>
+    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="129"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:J14">
-    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="157"/>
+    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="130"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H20">
-    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="158"/>
+    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="131"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:J17">
-    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="159"/>
+    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="132"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:J20">
-    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="160"/>
+    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="133"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I20">
-    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="161"/>
+    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="134"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:J20">
-    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="162"/>
+    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="135"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L9">
-    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="163"/>
+    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="136"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:U1">
-    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="164"/>
+    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="137"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N9">
-    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="165"/>
+    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="138"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:U2">
-    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="166"/>
+    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="139"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:U3">
-    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="167"/>
+    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="140"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:U4">
-    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="168"/>
+    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="141"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:N6">
-    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="169"/>
+    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="142"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:U5">
-    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="170"/>
+    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="143"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M9">
-    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="171"/>
+    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="144"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:N3">
-    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="172"/>
+    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="145"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:U6">
-    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="173"/>
+    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="146"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:N9">
-    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="174"/>
+    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="147"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:U7">
-    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="175"/>
+    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="148"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:U8">
-    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="176"/>
+    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="149"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:U9">
-    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="177"/>
+    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="150"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:Q3">
-    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="178"/>
+    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="151"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O9">
-    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="179"/>
+    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="152"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:Q6">
-    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="180"/>
+    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="153"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7:Q9">
-    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="181"/>
+    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="154"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P9">
-    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="182"/>
+    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="155"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q9">
-    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="183"/>
+    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="156"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:U3">
-    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="184"/>
+    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="157"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R9">
-    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="185"/>
+    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="158"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4:U6">
-    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="186"/>
+    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="159"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7:U9">
-    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="187"/>
+    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="160"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S9">
-    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="188"/>
+    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="161"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:U9">
-    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="189"/>
+    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="162"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
+    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:J1">
-    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
+    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
+    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J2">
-    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
+    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J3">
-    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
+    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:J4">
-    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
+    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:D6">
-    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
+    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:J5">
-    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
+    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35"/>
+    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D3">
-    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36"/>
+    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:J6">
-    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37"/>
+    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D9">
-    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38"/>
+    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:J7">
-    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39"/>
+    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:J8">
-    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40"/>
+    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:J9">
-    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41"/>
+    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G3">
-    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42"/>
+    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43"/>
+    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:G6">
-    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44"/>
+    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:G9">
-    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45"/>
+    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46"/>
+    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47"/>
+    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J3">
-    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48"/>
+    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49"/>
+    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J6">
-    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50"/>
+    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:J9">
-    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51"/>
+    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52"/>
+    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J9">
-    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53"/>
+    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8045,7 +7669,7 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -8627,289 +8251,289 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="190"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="163"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="191"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="164"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="192"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="165"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="193"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="166"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:D10">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="194"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="167"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10 B10:F10">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="195"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="168"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="196"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="169"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:F10">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="197"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="170"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="198"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="171"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="199"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="172"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="200"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="173"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="201"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="174"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="202"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="175"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10 K5">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="203"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="176"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B20">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="204"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="177"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:J12">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="205"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="178"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D20">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="206"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="179"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:J13">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="207"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="180"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:J14">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="208"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="181"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:J15">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="209"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="182"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:D17">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="210"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="183"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:J16">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="211"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="184"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C20">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="212"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="185"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:D14">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="213"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="186"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:J17">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="214"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="187"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:D20">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="215"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="188"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:J18">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="216"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="189"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:J19">
-    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="217"/>
+    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="190"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:J20">
-    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="218"/>
+    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="191"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:G14">
-    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="219"/>
+    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="192"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:E20">
-    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="220"/>
+    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="193"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:G17">
-    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="221"/>
+    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="194"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:G20">
-    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="222"/>
+    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="195"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F20">
-    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="223"/>
+    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="196"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G20">
-    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="224"/>
+    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="197"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:J14">
-    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="225"/>
+    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="198"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H20">
-    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="226"/>
+    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="199"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:J17">
-    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="227"/>
+    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="200"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:J20">
-    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="228"/>
+    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="201"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I20">
-    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="229"/>
+    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="202"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:J20">
-    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="230"/>
+    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="203"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L9">
-    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="231"/>
+    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="204"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:U1">
-    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="232"/>
+    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="205"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N9">
-    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="233"/>
+    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="206"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:U2">
-    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="234"/>
+    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="207"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:U3">
-    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="235"/>
+    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="208"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:U4">
-    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="236"/>
+    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="209"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:N6">
-    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="237"/>
+    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="210"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:U5">
-    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="238"/>
+    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="211"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M9">
-    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="239"/>
+    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="212"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:N3">
-    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="240"/>
+    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="213"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:U6">
-    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="241"/>
+    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="214"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:N9">
-    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="242"/>
+    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="215"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:U7">
-    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="243"/>
+    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="216"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:U8">
-    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="244"/>
+    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="217"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:U9">
-    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="245"/>
+    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="218"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:Q3">
-    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="246"/>
+    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="219"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O9">
-    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="247"/>
+    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="220"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:Q6">
-    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="248"/>
+    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="221"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7:Q9">
-    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="249"/>
+    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="222"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P9">
-    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="250"/>
+    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="223"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q9">
-    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="251"/>
+    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="224"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:U3">
-    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="252"/>
+    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="225"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R9">
-    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="253"/>
+    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="226"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4:U6">
-    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="254"/>
+    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="227"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7:U9">
-    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="255"/>
+    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="228"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S9">
-    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="256"/>
+    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="229"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:U9">
-    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="257"/>
+    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="230"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
+    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:J1">
-    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
+    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
+    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J2">
-    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
+    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J3">
-    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
+    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:J4">
-    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
+    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:D6">
-    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
+    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:J5">
-    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
+    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35"/>
+    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D3">
-    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36"/>
+    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:J6">
-    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37"/>
+    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D9">
-    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38"/>
+    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:J7">
-    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39"/>
+    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:J8">
-    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40"/>
+    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:J9">
-    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41"/>
+    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G3">
-    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42"/>
+    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43"/>
+    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:G6">
-    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44"/>
+    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:G9">
-    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45"/>
+    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46"/>
+    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47"/>
+    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J3">
-    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48"/>
+    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49"/>
+    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J6">
-    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50"/>
+    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:J9">
-    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51"/>
+    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52"/>
+    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J9">
-    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53"/>
+    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8928,7 +8552,7 @@
   </sheetPr>
   <dimension ref="B1:U27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -9510,289 +9134,289 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="258"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="231"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="259"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="232"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="260"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="233"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="261"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="234"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:D10">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="262"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="235"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10 B10:F10">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="263"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="236"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="264"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="237"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:F10">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="265"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="238"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="266"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="239"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="267"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="240"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="268"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="241"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:J10">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="269"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="242"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="270"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="243"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10 K5">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="271"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="244"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B20">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="272"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="245"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:J12">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="273"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="246"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D20">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="274"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="247"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:J13">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="275"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="248"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:J14">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="276"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="249"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:J15">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="277"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="250"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:D17">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="278"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="251"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:J16">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="279"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="252"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C20">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="280"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="253"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:D14">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="281"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="254"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:J17">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="282"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="255"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:D20">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="283"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="256"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:J18">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="284"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="257"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:J19">
-    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="285"/>
+    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="258"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:J20">
-    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="286"/>
+    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="259"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:G14">
-    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="287"/>
+    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="260"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:E20">
-    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="288"/>
+    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="261"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:G17">
-    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="289"/>
+    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="262"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:G20">
-    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="290"/>
+    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="263"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F20">
-    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="291"/>
+    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="264"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G20">
-    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="292"/>
+    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="265"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:J14">
-    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="293"/>
+    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="266"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H20">
-    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="294"/>
+    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="267"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:J17">
-    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="295"/>
+    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="268"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:J20">
-    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="296"/>
+    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="269"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I20">
-    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="297"/>
+    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="270"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:J20">
-    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="298"/>
+    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="271"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L9">
-    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="299"/>
+    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="272"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:U1">
-    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="300"/>
+    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="273"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N9">
-    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="301"/>
+    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="274"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:U2">
-    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="302"/>
+    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="275"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:U3">
-    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="303"/>
+    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="276"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:U4">
-    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="304"/>
+    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="277"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:N6">
-    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="305"/>
+    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="278"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:U5">
-    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="306"/>
+    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="279"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M9">
-    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="307"/>
+    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="280"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:N3">
-    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="308"/>
+    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="281"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:U6">
-    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="309"/>
+    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="282"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:N9">
-    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="310"/>
+    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="283"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:U7">
-    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="311"/>
+    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="284"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:U8">
-    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="312"/>
+    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="285"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:U9">
-    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="313"/>
+    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="286"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:Q3">
-    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="314"/>
+    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="287"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O9">
-    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="315"/>
+    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="288"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:Q6">
-    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="316"/>
+    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="289"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7:Q9">
-    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="317"/>
+    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="290"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P9">
-    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="318"/>
+    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="291"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q9">
-    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="319"/>
+    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="292"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:U3">
-    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="320"/>
+    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="293"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R9">
-    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="321"/>
+    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="294"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4:U6">
-    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="322"/>
+    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="295"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7:U9">
-    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="323"/>
+    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="296"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S9">
-    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="324"/>
+    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="297"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:U9">
-    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="325"/>
+    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="298"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
+    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:J1">
-    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28"/>
+    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29"/>
+    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J2">
-    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30"/>
+    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J3">
-    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
+    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:J4">
-    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32"/>
+    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:D6">
-    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33"/>
+    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:J5">
-    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
+    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35"/>
+    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D3">
-    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36"/>
+    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:J6">
-    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37"/>
+    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D9">
-    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38"/>
+    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:J7">
-    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39"/>
+    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:J8">
-    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40"/>
+    <cfRule type="duplicateValues" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:J9">
-    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41"/>
+    <cfRule type="duplicateValues" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G3">
-    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42"/>
+    <cfRule type="duplicateValues" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43"/>
+    <cfRule type="duplicateValues" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:G6">
-    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44"/>
+    <cfRule type="duplicateValues" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:G9">
-    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45"/>
+    <cfRule type="duplicateValues" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46"/>
+    <cfRule type="duplicateValues" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47"/>
+    <cfRule type="duplicateValues" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J3">
-    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48"/>
+    <cfRule type="duplicateValues" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49"/>
+    <cfRule type="duplicateValues" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J6">
-    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50"/>
+    <cfRule type="duplicateValues" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:J9">
-    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51"/>
+    <cfRule type="duplicateValues" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52"/>
+    <cfRule type="duplicateValues" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J9">
-    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53"/>
+    <cfRule type="duplicateValues" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -9811,7 +9435,7 @@
   </sheetPr>
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
@@ -10295,247 +9919,247 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B10">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="326"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="299"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:J1">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="327"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="300"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D10">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="328"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="301"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J2">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="329"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="302"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J3">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="330"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="303"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:J4">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="331"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="304"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:D6">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="332"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="305"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:K5">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="333"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="306"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C10">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="334"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="307"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D3">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="335"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="308"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:J6">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="336"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="309"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D10">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="337"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="310"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:J7">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="338"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="311"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:J8">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="339"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="312"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:J9 H10:J10 B10:F10">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="340"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="313"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G3">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="341"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="314"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E10">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="342"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="315"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:G6">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="343"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="316"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:G9 E10:F10">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="344"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="317"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F10">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="345"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="318"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="346"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="319"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J3">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="347"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="320"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H10">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="348"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="321"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:J6 K5">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="349"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="322"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:J10">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="350"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="323"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I10">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="351"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="324"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J10 K5">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="352"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="325"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B20">
-    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="353"/>
+    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="326"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:J12">
-    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="354"/>
+    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="327"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D20">
-    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="355"/>
+    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="328"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:J13">
-    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="356"/>
+    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="329"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:J14">
-    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="357"/>
+    <cfRule type="duplicateValues" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="330"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:J15">
-    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="358"/>
+    <cfRule type="duplicateValues" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="331"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:D17">
-    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="359"/>
+    <cfRule type="duplicateValues" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="332"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:J16">
-    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="360"/>
+    <cfRule type="duplicateValues" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="333"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C20">
-    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="361"/>
+    <cfRule type="duplicateValues" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="334"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:D14">
-    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="362"/>
+    <cfRule type="duplicateValues" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="335"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:J17">
-    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="363"/>
+    <cfRule type="duplicateValues" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="336"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:D20">
-    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="364"/>
+    <cfRule type="duplicateValues" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="337"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:J18">
-    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="365"/>
+    <cfRule type="duplicateValues" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="338"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:J19">
-    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="366"/>
+    <cfRule type="duplicateValues" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="339"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:J20">
-    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="367"/>
+    <cfRule type="duplicateValues" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="340"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:G14">
-    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="368"/>
+    <cfRule type="duplicateValues" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="341"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:E20">
-    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="369"/>
+    <cfRule type="duplicateValues" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="342"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:G17">
-    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="370"/>
+    <cfRule type="duplicateValues" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="343"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:G20">
-    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="371"/>
+    <cfRule type="duplicateValues" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="344"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F20">
-    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="372"/>
+    <cfRule type="duplicateValues" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="345"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G20">
-    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="373"/>
+    <cfRule type="duplicateValues" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="346"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:J14">
-    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="374"/>
+    <cfRule type="duplicateValues" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="347"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H20">
-    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="375"/>
+    <cfRule type="duplicateValues" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="348"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15:J17">
-    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="376"/>
+    <cfRule type="duplicateValues" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="349"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:J20">
-    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="377"/>
+    <cfRule type="duplicateValues" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="350"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I20">
-    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="378"/>
+    <cfRule type="duplicateValues" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="351"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:J20">
-    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="379"/>
+    <cfRule type="duplicateValues" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="352"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L9">
-    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="380"/>
+    <cfRule type="duplicateValues" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="353"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:T1">
-    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="381"/>
+    <cfRule type="duplicateValues" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="354"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N9">
-    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="382"/>
+    <cfRule type="duplicateValues" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="355"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:T2">
-    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="383"/>
+    <cfRule type="duplicateValues" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="356"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:T3">
-    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="384"/>
+    <cfRule type="duplicateValues" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="357"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:T4">
-    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="385"/>
+    <cfRule type="duplicateValues" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="358"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:N6">
-    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="386"/>
+    <cfRule type="duplicateValues" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="359"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:T5">
-    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="387"/>
+    <cfRule type="duplicateValues" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="360"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M9">
-    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="388"/>
+    <cfRule type="duplicateValues" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="361"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:N3">
-    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="389"/>
+    <cfRule type="duplicateValues" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="362"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:T6">
-    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="390"/>
+    <cfRule type="duplicateValues" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="363"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:N9">
-    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="391"/>
+    <cfRule type="duplicateValues" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="364"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:T7">
-    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="392"/>
+    <cfRule type="duplicateValues" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="365"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:T8">
-    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="393"/>
+    <cfRule type="duplicateValues" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="366"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:T9">
-    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="394"/>
+    <cfRule type="duplicateValues" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="367"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:Q3">
-    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="395"/>
+    <cfRule type="duplicateValues" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="368"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O9">
-    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="396"/>
+    <cfRule type="duplicateValues" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="369"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:Q6">
-    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="397"/>
+    <cfRule type="duplicateValues" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="370"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7:Q9">
-    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="398"/>
+    <cfRule type="duplicateValues" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="371"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P9">
-    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="399"/>
+    <cfRule type="duplicateValues" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="372"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q9">
-    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="400"/>
+    <cfRule type="duplicateValues" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="373"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:T3">
-    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="401"/>
+    <cfRule type="duplicateValues" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="374"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R9">
-    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="402"/>
+    <cfRule type="duplicateValues" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="375"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4:T6">
-    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="403"/>
+    <cfRule type="duplicateValues" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="376"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7:T9">
-    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="404"/>
+    <cfRule type="duplicateValues" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="377"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1:S9">
-    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="405"/>
+    <cfRule type="duplicateValues" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="378"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1:T9">
-    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="406"/>
+    <cfRule type="duplicateValues" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="379"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -10554,7 +10178,7 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -10694,97 +10318,97 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A9">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="407"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="380"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:I1">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="408"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="381"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="409"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="382"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:I2">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="410"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="383"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:I3">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="411"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="384"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:I4">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="412"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="385"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C6">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="413"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="386"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:I5">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="414"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="387"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="415"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="388"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C3">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="416"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="389"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:I6">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="417"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="390"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:C9">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="418"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="391"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:I7">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="419"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="392"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:I8">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="420"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="393"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:I9">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="421"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="394"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F3">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="422"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="395"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D9">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="423"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="396"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:F6">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="424"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="397"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F9">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="425"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="398"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="426"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="399"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="427"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="400"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:I3">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="428"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="401"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G9">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="429"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="402"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:I6">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="430"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="403"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:I9">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="431"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="404"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H9">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="432"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="405"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I9">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="433"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="406"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:D4">
-    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="434"/>
+    <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="407"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:H4">
-    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="435"/>
+    <cfRule type="duplicateValues" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="408"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:D8">
-    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="436"/>
+    <cfRule type="duplicateValues" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="409"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:H8">
-    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="437"/>
+    <cfRule type="duplicateValues" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="410"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -10803,7 +10427,7 @@
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G44" activeCellId="0" sqref="G44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
XY wing on broken Tensorbook
</commit_message>
<xml_diff>
--- a/data/SDK.xlsx
+++ b/data/SDK.xlsx
@@ -96,9 +96,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="#,##0"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -507,7 +508,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -564,11 +565,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -596,7 +601,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7498,7 +7503,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7509,7 +7514,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="n">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B1" s="3" t="n">
         <v>1469</v>
@@ -7530,7 +7535,7 @@
         <v>8</v>
       </c>
       <c r="H1" s="3" t="n">
-        <v>89</v>
+        <v>5</v>
       </c>
       <c r="I1" s="4" t="n">
         <v>3</v>
@@ -7670,14 +7675,14 @@
       <c r="I5" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="K5" s="10" t="str">
+      <c r="K5" s="14" t="n">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "5")=9, 5, "")</f>
-        <v/>
+        <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="B6" s="12" t="n">
         <v>5</v>
@@ -7802,7 +7807,7 @@
       <c r="I9" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="K9" s="14" t="str">
+      <c r="K9" s="15" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "9")=9, 9, "")</f>
         <v/>
       </c>
@@ -8144,7 +8149,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="110" id="{505B6B78-2FB9-4AF6-93FD-7E33DBCC87E9}">
+          <x14:cfRule type="expression" priority="110" id="{6351BE87-CE99-4FB4-B2BA-302DE1B7A6F5}">
             <xm:f>AND((A2&lt;10),(A2&lt;&gt;solved!A2))</xm:f>
             <x14:dxf>
               <font>
@@ -8160,7 +8165,7 @@
           <xm:sqref>A2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="111" id="{D3D91ABA-1560-41D0-8EDD-8AD92DF18F67}">
+          <x14:cfRule type="expression" priority="111" id="{D818F26E-E4AF-49E5-9B4C-A4DC60882353}">
             <xm:f>AND((A3&lt;10),(A3&lt;&gt;solved!A3))</xm:f>
             <x14:dxf>
               <font>
@@ -8171,7 +8176,7 @@
           <xm:sqref>A3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="112" id="{90D13275-90F1-4C70-AB95-9274AF397575}">
+          <x14:cfRule type="expression" priority="112" id="{49EBE05F-7A44-4240-BDF2-FE551EFCC411}">
             <xm:f>AND((A5&lt;10),(A5&lt;&gt;solved!A5))</xm:f>
             <x14:dxf>
               <font>
@@ -8182,7 +8187,7 @@
           <xm:sqref>A5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="113" id="{BFAD24CD-A74D-434D-A6C4-65DAB7167A2E}">
+          <x14:cfRule type="expression" priority="113" id="{FE72E9BC-C38C-49C0-90D0-6D7A10153D5C}">
             <xm:f>AND((A6&lt;10),(A6&lt;&gt;solved!A6))</xm:f>
             <x14:dxf>
               <font>
@@ -8193,7 +8198,7 @@
           <xm:sqref>A6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="114" id="{D4C13C20-F0A8-4985-A272-60D841CFDD46}">
+          <x14:cfRule type="expression" priority="114" id="{87B1441E-C4DE-46B8-B2F6-1BE0512E6125}">
             <xm:f>AND((A7&lt;10),(A7&lt;&gt;solved!A7))</xm:f>
             <x14:dxf>
               <font>
@@ -8204,7 +8209,7 @@
           <xm:sqref>A7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="115" id="{8BE6883B-E035-4642-83AB-6152BCA99A40}">
+          <x14:cfRule type="expression" priority="115" id="{441495E0-C33E-4DD9-85E3-EC43457EA524}">
             <xm:f>AND((A8&lt;10),(A8&lt;&gt;solved!A8))</xm:f>
             <x14:dxf>
               <font>
@@ -8215,7 +8220,7 @@
           <xm:sqref>A8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="116" id="{9351F82B-608C-4EDB-8B14-779390246EB1}">
+          <x14:cfRule type="expression" priority="116" id="{0077F593-20D6-4034-AC57-5038B3C5E070}">
             <xm:f>AND((A9&lt;10),(A9&lt;&gt;solved!A9))</xm:f>
             <x14:dxf>
               <font>
@@ -8226,7 +8231,7 @@
           <xm:sqref>A9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="117" id="{7725B8AB-D3F6-4538-AECF-C720B6E58867}">
+          <x14:cfRule type="expression" priority="117" id="{171DD56F-3163-4472-B565-58C47E8DEB18}">
             <xm:f>AND((B1&lt;10),(B1&lt;&gt;solved!B1))</xm:f>
             <x14:dxf>
               <font>
@@ -8237,7 +8242,7 @@
           <xm:sqref>B1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="118" id="{1813D060-EF39-4F16-AB99-BA2849BD3428}">
+          <x14:cfRule type="expression" priority="118" id="{73527E9A-18AA-48F6-A027-B48840DE3B4F}">
             <xm:f>AND((B2&lt;10),(B2&lt;&gt;solved!B2))</xm:f>
             <x14:dxf>
               <font>
@@ -8248,7 +8253,7 @@
           <xm:sqref>B2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="119" id="{CF79F554-4ED3-4294-AF6F-40B563BCD1DB}">
+          <x14:cfRule type="expression" priority="119" id="{7D469051-B766-4425-BBF1-24D0583FA711}">
             <xm:f>AND((B3&lt;10),(B3&lt;&gt;solved!B3))</xm:f>
             <x14:dxf>
               <font>
@@ -8259,7 +8264,7 @@
           <xm:sqref>B3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="120" id="{547E0042-4C4C-44BE-BA14-32CB32F47247}">
+          <x14:cfRule type="expression" priority="120" id="{7EDC896D-F3CC-4F8B-AD69-388A2FF72C9F}">
             <xm:f>AND((B4&lt;10),(B4&lt;&gt;solved!B4))</xm:f>
             <x14:dxf>
               <font>
@@ -8270,7 +8275,7 @@
           <xm:sqref>B4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="121" id="{CBD39284-A51C-45D2-A1B1-5DA0D41A56BA}">
+          <x14:cfRule type="expression" priority="121" id="{9DA4DAEA-6BA0-46EE-9F4F-903B8AA3811C}">
             <xm:f>AND((B5&lt;10),(B5&lt;&gt;solved!B5))</xm:f>
             <x14:dxf>
               <font>
@@ -8281,7 +8286,7 @@
           <xm:sqref>B5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="122" id="{76D52FE3-1653-4B5B-9A8D-7B88379AF6F9}">
+          <x14:cfRule type="expression" priority="122" id="{43B4A639-2983-4691-ADB0-CA142B4161D3}">
             <xm:f>AND((B6&lt;10),(B6&lt;&gt;solved!B6))</xm:f>
             <x14:dxf>
               <font>
@@ -8292,7 +8297,7 @@
           <xm:sqref>B6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="123" id="{FCDD41B7-215F-4093-92E6-5AB3D34C363E}">
+          <x14:cfRule type="expression" priority="123" id="{93207440-A9DE-49F4-B245-3D4FCE70AAB3}">
             <xm:f>AND((B7&lt;10),(B7&lt;&gt;solved!B7))</xm:f>
             <x14:dxf>
               <font>
@@ -8303,7 +8308,7 @@
           <xm:sqref>B7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="124" id="{B6D334BB-2259-48D3-92AD-2FE850A78FA9}">
+          <x14:cfRule type="expression" priority="124" id="{C01A3FEF-BC57-4B20-9E9F-5F5AE04D735E}">
             <xm:f>AND((B8&lt;10),(B8&lt;&gt;solved!B8))</xm:f>
             <x14:dxf>
               <font>
@@ -8314,7 +8319,7 @@
           <xm:sqref>B8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="125" id="{80638FCB-D890-46D4-9BA9-B53838655190}">
+          <x14:cfRule type="expression" priority="125" id="{F3AFE260-58E9-4CA3-BC7D-9A73EFE9AEA1}">
             <xm:f>AND((B9&lt;10),(B9&lt;&gt;solved!B9))</xm:f>
             <x14:dxf>
               <font>
@@ -8325,7 +8330,7 @@
           <xm:sqref>B9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="126" id="{F06CE87A-B475-45A9-8857-FC90532BCD69}">
+          <x14:cfRule type="expression" priority="126" id="{7BA31384-8592-4F4A-A071-4FAF92B76085}">
             <xm:f>AND((C1&lt;10),(C1&lt;&gt;solved!C1))</xm:f>
             <x14:dxf>
               <font>
@@ -8336,7 +8341,7 @@
           <xm:sqref>C1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="127" id="{D2C11724-77FC-40E9-BABE-35EA2BE919DB}">
+          <x14:cfRule type="expression" priority="127" id="{233E973C-6032-419C-8112-22C083A8A16A}">
             <xm:f>AND((C2&lt;10),(C2&lt;&gt;solved!C2))</xm:f>
             <x14:dxf>
               <font>
@@ -8347,7 +8352,7 @@
           <xm:sqref>C2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="128" id="{BBC8967B-27E5-448E-BFFC-DADDA7BB2056}">
+          <x14:cfRule type="expression" priority="128" id="{60C785D3-4086-4341-B32D-FB5CBBAD457E}">
             <xm:f>AND((C3&lt;10),(C3&lt;&gt;solved!C3))</xm:f>
             <x14:dxf>
               <font>
@@ -8358,7 +8363,7 @@
           <xm:sqref>C3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="129" id="{A78010B1-956A-427E-BABE-1A9C7F92478E}">
+          <x14:cfRule type="expression" priority="129" id="{9615D044-72CB-43A9-9FB2-8092CDA09E70}">
             <xm:f>AND((C4&lt;10),(C4&lt;&gt;solved!C4))</xm:f>
             <x14:dxf>
               <font>
@@ -8369,7 +8374,7 @@
           <xm:sqref>C4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="130" id="{80CAE336-A122-40C9-80C6-C2E870A05794}">
+          <x14:cfRule type="expression" priority="130" id="{1083A068-47BE-4683-8712-E0B066E6A77C}">
             <xm:f>AND((C5&lt;10),(C5&lt;&gt;solved!C5))</xm:f>
             <x14:dxf>
               <font>
@@ -8380,7 +8385,7 @@
           <xm:sqref>C5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="131" id="{997A347A-5165-4754-884A-E3EA70338DA2}">
+          <x14:cfRule type="expression" priority="131" id="{9A78E628-D592-40DC-8D40-2099E4898FAC}">
             <xm:f>AND((C6&lt;10),(C6&lt;&gt;solved!C6))</xm:f>
             <x14:dxf>
               <font>
@@ -8391,7 +8396,7 @@
           <xm:sqref>C6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="132" id="{67F5F64E-6CBB-4AE2-AAFA-C9E95A3356BF}">
+          <x14:cfRule type="expression" priority="132" id="{30219D80-1ACF-47E6-8F15-30414448735D}">
             <xm:f>AND((C7&lt;10),(C7&lt;&gt;solved!C7))</xm:f>
             <x14:dxf>
               <font>
@@ -8402,7 +8407,7 @@
           <xm:sqref>C7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="133" id="{B1CF3A72-AFC9-4132-BD79-B0CD207840BF}">
+          <x14:cfRule type="expression" priority="133" id="{DDE7D810-D84E-46C0-895D-CFE340FC7B55}">
             <xm:f>AND((C8&lt;10),(C8&lt;&gt;solved!C8))</xm:f>
             <x14:dxf>
               <font>
@@ -8413,7 +8418,7 @@
           <xm:sqref>C8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="134" id="{7011FE5A-D986-4132-87E2-F075FCA8BC98}">
+          <x14:cfRule type="expression" priority="134" id="{88B01EA8-204A-43B9-BEF8-90835389CD70}">
             <xm:f>AND((C9&lt;10),(C9&lt;&gt;solved!C9))</xm:f>
             <x14:dxf>
               <font>
@@ -8424,7 +8429,7 @@
           <xm:sqref>C9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="135" id="{1039907E-7275-4066-B4E6-738FF6C115D5}">
+          <x14:cfRule type="expression" priority="135" id="{CFA81DA7-9CA0-468E-AFB9-A17CC4F016FD}">
             <xm:f>AND((D1&lt;10),(D1&lt;&gt;solved!D1))</xm:f>
             <x14:dxf>
               <font>
@@ -8435,7 +8440,7 @@
           <xm:sqref>D1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="136" id="{96C06AA9-39B5-4999-BAF8-E4188F576622}">
+          <x14:cfRule type="expression" priority="136" id="{8B8CE535-5635-4CB4-BA9A-FDD813F41FE9}">
             <xm:f>AND((D2&lt;10),(D2&lt;&gt;solved!D2))</xm:f>
             <x14:dxf>
               <font>
@@ -8446,7 +8451,7 @@
           <xm:sqref>D2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="137" id="{E487D17D-E065-40D4-A0B0-19CCBD4D90A7}">
+          <x14:cfRule type="expression" priority="137" id="{AD443EB9-1CAC-4E94-874E-2B9F7AF7A3B1}">
             <xm:f>AND((D3&lt;10),(D3&lt;&gt;solved!D3))</xm:f>
             <x14:dxf>
               <font>
@@ -8457,7 +8462,7 @@
           <xm:sqref>D3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="138" id="{F0432F23-B0EE-4A1F-8FF6-C8C26F3BA01E}">
+          <x14:cfRule type="expression" priority="138" id="{2F17D41C-F71E-4A5F-9432-6C32EEA257F6}">
             <xm:f>AND((D4&lt;10),(D4&lt;&gt;solved!D4))</xm:f>
             <x14:dxf>
               <font>
@@ -8468,7 +8473,7 @@
           <xm:sqref>D4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="139" id="{91D83A75-ABF2-4C5A-8B77-DD94A088942A}">
+          <x14:cfRule type="expression" priority="139" id="{7961F05B-3A50-4428-874D-A26DF45F1A70}">
             <xm:f>AND((D5&lt;10),(D5&lt;&gt;solved!D5))</xm:f>
             <x14:dxf>
               <font>
@@ -8479,7 +8484,7 @@
           <xm:sqref>D5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="140" id="{AB771369-2C57-4162-8FD4-AA9117CBBD80}">
+          <x14:cfRule type="expression" priority="140" id="{93F4EBA0-746A-432D-AE5D-A690F7E2BA59}">
             <xm:f>AND((D6&lt;10),(D6&lt;&gt;solved!D6))</xm:f>
             <x14:dxf>
               <font>
@@ -8490,7 +8495,7 @@
           <xm:sqref>D6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="141" id="{8E9A3FF9-4C2B-47C4-AC5F-42644E8656EC}">
+          <x14:cfRule type="expression" priority="141" id="{509E2E24-11AD-40F4-8F1E-4F5411C7F814}">
             <xm:f>AND((D7&lt;10),(D7&lt;&gt;solved!D7))</xm:f>
             <x14:dxf>
               <font>
@@ -8501,7 +8506,7 @@
           <xm:sqref>D7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="142" id="{E04CF672-72F2-49D7-9776-51EBBD21EB83}">
+          <x14:cfRule type="expression" priority="142" id="{6B55AA60-ABDE-4790-A5E7-242D84704F74}">
             <xm:f>AND((D8&lt;10),(D8&lt;&gt;solved!D8))</xm:f>
             <x14:dxf>
               <font>
@@ -8512,7 +8517,7 @@
           <xm:sqref>D8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="143" id="{9ACA7871-63D5-4233-8B85-72B499F84F54}">
+          <x14:cfRule type="expression" priority="143" id="{6CAA50CC-AE84-4C84-AD8F-C1E71055C911}">
             <xm:f>AND((D9&lt;10),(D9&lt;&gt;solved!D9))</xm:f>
             <x14:dxf>
               <font>
@@ -8523,7 +8528,7 @@
           <xm:sqref>D9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="144" id="{4F67C42D-DD73-423C-B865-577916AE5EF3}">
+          <x14:cfRule type="expression" priority="144" id="{208030C2-8772-4835-9390-48595F5CC04A}">
             <xm:f>AND((E1&lt;10),(E1&lt;&gt;solved!E1))</xm:f>
             <x14:dxf>
               <font>
@@ -8534,7 +8539,7 @@
           <xm:sqref>E1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="145" id="{5024A82C-6427-4475-B63F-37D8C76EFB8D}">
+          <x14:cfRule type="expression" priority="145" id="{80D37D4D-B27B-4FF0-B529-135FFB8DE52F}">
             <xm:f>AND((E2&lt;10),(E2&lt;&gt;solved!E2))</xm:f>
             <x14:dxf>
               <font>
@@ -8545,7 +8550,7 @@
           <xm:sqref>E2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="146" id="{65F3E42C-AB65-4D5A-8133-195DD837EFF3}">
+          <x14:cfRule type="expression" priority="146" id="{1DA95BE0-526F-4AC6-92D0-B600CB705FC3}">
             <xm:f>AND((E3&lt;10),(E3&lt;&gt;solved!E3))</xm:f>
             <x14:dxf>
               <font>
@@ -8556,7 +8561,7 @@
           <xm:sqref>E3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="147" id="{9CD59D1F-88D5-4FB6-9238-D57AC8C4D92A}">
+          <x14:cfRule type="expression" priority="147" id="{CF77B0E4-9FFA-4CBD-80BD-BD699EA6C4A5}">
             <xm:f>AND((E4&lt;10),(E4&lt;&gt;solved!E4))</xm:f>
             <x14:dxf>
               <font>
@@ -8567,7 +8572,7 @@
           <xm:sqref>E4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="148" id="{939F8073-C0AA-41E5-BE8B-FD93AF9E25D7}">
+          <x14:cfRule type="expression" priority="148" id="{DAEC3566-7150-4253-B843-3E68E390E619}">
             <xm:f>AND((E5&lt;10),(E5&lt;&gt;solved!E5))</xm:f>
             <x14:dxf>
               <font>
@@ -8578,7 +8583,7 @@
           <xm:sqref>E5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="149" id="{60F75266-2F8A-4129-AD46-E0DAFBF0B217}">
+          <x14:cfRule type="expression" priority="149" id="{626218C9-FEC6-4220-AB6F-F8EDB4323D6B}">
             <xm:f>AND((E6&lt;10),(E6&lt;&gt;solved!E6))</xm:f>
             <x14:dxf>
               <font>
@@ -8589,7 +8594,7 @@
           <xm:sqref>E6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="150" id="{6AF0F28A-E9DF-4668-B86A-23718B96D2EA}">
+          <x14:cfRule type="expression" priority="150" id="{F47E2037-5AE9-4280-A257-81F6945BD8C0}">
             <xm:f>AND((E7&lt;10),(E7&lt;&gt;solved!E7))</xm:f>
             <x14:dxf>
               <font>
@@ -8600,7 +8605,7 @@
           <xm:sqref>E7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="151" id="{41D22027-EE96-4219-9E82-A1612A3FE43E}">
+          <x14:cfRule type="expression" priority="151" id="{2D345FC2-62E7-4DCD-B932-A3F17AEBAC52}">
             <xm:f>AND((E8&lt;10),(E8&lt;&gt;solved!E8))</xm:f>
             <x14:dxf>
               <font>
@@ -8611,7 +8616,7 @@
           <xm:sqref>E8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="152" id="{391B3CB2-ADD4-463E-B846-8DBBF29EB12E}">
+          <x14:cfRule type="expression" priority="152" id="{70FD4C54-70F1-4E2F-80E4-A989B6405AEA}">
             <xm:f>AND((E9&lt;10),(E9&lt;&gt;solved!E9))</xm:f>
             <x14:dxf>
               <font>
@@ -8622,7 +8627,7 @@
           <xm:sqref>E9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="153" id="{2A5A89B4-C935-44FF-A3E4-5B8DB91C9DF7}">
+          <x14:cfRule type="expression" priority="153" id="{3B56C6E2-51D9-4899-B7E6-646315BBC48A}">
             <xm:f>AND((F1&lt;10),(F1&lt;&gt;solved!F1))</xm:f>
             <x14:dxf>
               <font>
@@ -8633,7 +8638,7 @@
           <xm:sqref>F1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="154" id="{20389034-9C91-4D60-9315-9770E0F64D8F}">
+          <x14:cfRule type="expression" priority="154" id="{47F43AFC-BF33-4031-8B40-934E6F933038}">
             <xm:f>AND((F2&lt;10),(F2&lt;&gt;solved!F2))</xm:f>
             <x14:dxf>
               <font>
@@ -8644,7 +8649,7 @@
           <xm:sqref>F2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="155" id="{E664E5FC-7290-462D-96E5-4EE3F4558838}">
+          <x14:cfRule type="expression" priority="155" id="{F17DB0FB-BB6D-455D-8580-8EF13D4DB3BE}">
             <xm:f>AND((F3&lt;10),(F3&lt;&gt;solved!F3))</xm:f>
             <x14:dxf>
               <font>
@@ -8655,7 +8660,7 @@
           <xm:sqref>F3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="156" id="{8F5361F0-8CF2-4E50-9766-2FBB6E711C40}">
+          <x14:cfRule type="expression" priority="156" id="{B2873B96-1C00-48F0-8736-ED4759C04C85}">
             <xm:f>AND((F4&lt;10),(F4&lt;&gt;solved!F4))</xm:f>
             <x14:dxf>
               <font>
@@ -8666,7 +8671,7 @@
           <xm:sqref>F4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="157" id="{DEE985CC-81DF-4A00-A19D-5141377F338C}">
+          <x14:cfRule type="expression" priority="157" id="{46FDA267-84BF-4E66-8349-E1B4D7B0A0F9}">
             <xm:f>AND((F5&lt;10),(F5&lt;&gt;solved!F5))</xm:f>
             <x14:dxf>
               <font>
@@ -8677,7 +8682,7 @@
           <xm:sqref>F5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="158" id="{EA741FF0-60C9-44B0-B8A7-4027C477C04F}">
+          <x14:cfRule type="expression" priority="158" id="{34A16078-7DA0-493E-957B-EAC86BEE6DCF}">
             <xm:f>AND((F6&lt;10),(F6&lt;&gt;solved!F6))</xm:f>
             <x14:dxf>
               <font>
@@ -8688,7 +8693,7 @@
           <xm:sqref>F6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="159" id="{293AB7A0-175C-4FA9-A35C-D6EDEC5599F3}">
+          <x14:cfRule type="expression" priority="159" id="{425FF41F-C32C-40AA-B5A2-705EA94BEF98}">
             <xm:f>AND((F7&lt;10),(F7&lt;&gt;solved!F7))</xm:f>
             <x14:dxf>
               <font>
@@ -8699,7 +8704,7 @@
           <xm:sqref>F7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="160" id="{B54055BA-D3D1-46A3-ADD2-9E1BB6ABE055}">
+          <x14:cfRule type="expression" priority="160" id="{468F7C76-30D9-46F2-9E8E-F69436BA2C70}">
             <xm:f>AND((F8&lt;10),(F8&lt;&gt;solved!F8))</xm:f>
             <x14:dxf>
               <font>
@@ -8710,7 +8715,7 @@
           <xm:sqref>F8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="161" id="{318F3A84-40B8-489A-9F35-6E7351DCFEC7}">
+          <x14:cfRule type="expression" priority="161" id="{9220E981-D852-40C4-BFF8-3C94D0288D16}">
             <xm:f>AND((F9&lt;10),(F9&lt;&gt;solved!F9))</xm:f>
             <x14:dxf>
               <font>
@@ -8721,7 +8726,7 @@
           <xm:sqref>F9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="162" id="{3E59643E-B5E2-4E9A-AAAE-A2836DF44638}">
+          <x14:cfRule type="expression" priority="162" id="{63186030-B1D0-44D9-8C79-D7EBF014675E}">
             <xm:f>AND((G1&lt;10),(G1&lt;&gt;solved!G1))</xm:f>
             <x14:dxf>
               <font>
@@ -8732,7 +8737,7 @@
           <xm:sqref>G1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="163" id="{F25AD1C3-29C2-43A4-9BAB-D19F70A9652E}">
+          <x14:cfRule type="expression" priority="163" id="{21BC1CD7-7D18-4014-AD5F-75DDA9B0FE75}">
             <xm:f>AND((G2&lt;10),(G2&lt;&gt;solved!G2))</xm:f>
             <x14:dxf>
               <font>
@@ -8743,7 +8748,7 @@
           <xm:sqref>G2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="164" id="{7C80FA9B-F972-4159-9241-B0D0B071FC59}">
+          <x14:cfRule type="expression" priority="164" id="{90D19B8F-FBF4-4A4C-8875-1A54BACCF4D6}">
             <xm:f>AND((G3&lt;10),(G3&lt;&gt;solved!G3))</xm:f>
             <x14:dxf>
               <font>
@@ -8754,7 +8759,7 @@
           <xm:sqref>G3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="165" id="{F0A7D083-D0CD-451C-BFD8-F1B49830B4F8}">
+          <x14:cfRule type="expression" priority="165" id="{18C0A8CB-16E4-45D8-9F20-39E8E1A99895}">
             <xm:f>AND((G4&lt;10),(G4&lt;&gt;solved!G4))</xm:f>
             <x14:dxf>
               <font>
@@ -8765,7 +8770,7 @@
           <xm:sqref>G4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="166" id="{E155975A-1730-4FA5-A8D1-196045459663}">
+          <x14:cfRule type="expression" priority="166" id="{212C1642-3227-43FA-88D7-E16F91199E3E}">
             <xm:f>AND((G5&lt;10),(G5&lt;&gt;solved!G5))</xm:f>
             <x14:dxf>
               <font>
@@ -8776,7 +8781,7 @@
           <xm:sqref>G5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="167" id="{D5ADE4B3-6916-4A97-B1C3-9F20B1573BC0}">
+          <x14:cfRule type="expression" priority="167" id="{AEB19DCA-2CA9-4A20-9B15-DA3DE56573D0}">
             <xm:f>AND((G6&lt;10),(G6&lt;&gt;solved!G6))</xm:f>
             <x14:dxf>
               <font>
@@ -8787,7 +8792,7 @@
           <xm:sqref>G6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="168" id="{D2CBDB12-1E60-40B6-845B-511A8CAABD31}">
+          <x14:cfRule type="expression" priority="168" id="{E7597ECC-9D54-4379-80B1-2B3FC628A2ED}">
             <xm:f>AND((G7&lt;10),(G7&lt;&gt;solved!G7))</xm:f>
             <x14:dxf>
               <font>
@@ -8798,7 +8803,7 @@
           <xm:sqref>G7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="169" id="{404081E0-9DC9-48BE-9134-4E681CDB5D2B}">
+          <x14:cfRule type="expression" priority="169" id="{B9E64F3D-89A8-478A-A996-2038D6E360A7}">
             <xm:f>AND((G8&lt;10),(G8&lt;&gt;solved!G8))</xm:f>
             <x14:dxf>
               <font>
@@ -8809,7 +8814,7 @@
           <xm:sqref>G8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="170" id="{97E6AC5C-9F90-43FC-BAC0-78A1436729E3}">
+          <x14:cfRule type="expression" priority="170" id="{EE89A5FE-DAFB-4A5D-A22B-5471D4308A53}">
             <xm:f>AND((G9&lt;10),(G9&lt;&gt;solved!G9))</xm:f>
             <x14:dxf>
               <font>
@@ -8820,7 +8825,7 @@
           <xm:sqref>G9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="171" id="{204318B0-11DD-445C-B644-21ABC5A22BDC}">
+          <x14:cfRule type="expression" priority="171" id="{27DDCB26-2195-4AC9-BB7F-3F7F3BB2F791}">
             <xm:f>AND((H1&lt;10),(H1&lt;&gt;solved!H1))</xm:f>
             <x14:dxf>
               <font>
@@ -8831,7 +8836,7 @@
           <xm:sqref>H1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="172" id="{ED867226-0086-4846-B44C-19A96216C844}">
+          <x14:cfRule type="expression" priority="172" id="{68BBACEC-2744-4AC0-BCEC-BDE0E1E0EB20}">
             <xm:f>AND((H2&lt;10),(H2&lt;&gt;solved!H2))</xm:f>
             <x14:dxf>
               <font>
@@ -8842,7 +8847,7 @@
           <xm:sqref>H2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="173" id="{33C5C671-B1BA-4338-B245-12D1C6AAC636}">
+          <x14:cfRule type="expression" priority="173" id="{3FA8AEFD-C45A-40BF-BD50-114A6AF121E5}">
             <xm:f>AND((H3&lt;10),(H3&lt;&gt;solved!H3))</xm:f>
             <x14:dxf>
               <font>
@@ -8853,7 +8858,7 @@
           <xm:sqref>H3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="174" id="{688BB97A-88F1-43D3-874A-40BE2EE689B6}">
+          <x14:cfRule type="expression" priority="174" id="{685EF828-F31A-46A5-94C5-1D34A84355D7}">
             <xm:f>AND((H4&lt;10),(H4&lt;&gt;solved!H4))</xm:f>
             <x14:dxf>
               <font>
@@ -8864,7 +8869,7 @@
           <xm:sqref>H4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="175" id="{C0AFC0C6-E559-4333-8C4D-ADFB22DD4BD5}">
+          <x14:cfRule type="expression" priority="175" id="{DD606118-2F9B-438C-9D94-403C77122364}">
             <xm:f>AND((H5&lt;10),(H5&lt;&gt;solved!H5))</xm:f>
             <x14:dxf>
               <font>
@@ -8875,7 +8880,7 @@
           <xm:sqref>H5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="176" id="{FFB1F5C5-28D0-42ED-80BC-684EEB533FE9}">
+          <x14:cfRule type="expression" priority="176" id="{CD2A1552-F0D5-4758-961B-A47BF160B340}">
             <xm:f>AND((H6&lt;10),(H6&lt;&gt;solved!H6))</xm:f>
             <x14:dxf>
               <font>
@@ -8886,7 +8891,7 @@
           <xm:sqref>H6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="177" id="{9A21A6CF-EF30-4EE6-93EE-265663F0624B}">
+          <x14:cfRule type="expression" priority="177" id="{8998A06D-F9FD-4E8C-8F73-94D879E8E192}">
             <xm:f>AND((H7&lt;10),(H7&lt;&gt;solved!H7))</xm:f>
             <x14:dxf>
               <font>
@@ -8897,7 +8902,7 @@
           <xm:sqref>H7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="178" id="{C040FD51-13D7-4BF8-A6CE-7B911985CDD5}">
+          <x14:cfRule type="expression" priority="178" id="{811575BD-E86D-461E-B840-404FB04CEBA4}">
             <xm:f>AND((H8&lt;10),(H8&lt;&gt;solved!H8))</xm:f>
             <x14:dxf>
               <font>
@@ -8908,7 +8913,7 @@
           <xm:sqref>H8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="179" id="{B6D5177C-8DE6-4E9C-A26A-77411E7BFAE0}">
+          <x14:cfRule type="expression" priority="179" id="{21487049-2F6B-4C70-8385-27CCA6DAC249}">
             <xm:f>AND((H9&lt;10),(H9&lt;&gt;solved!H9))</xm:f>
             <x14:dxf>
               <font>
@@ -8919,7 +8924,7 @@
           <xm:sqref>H9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="180" id="{B230696F-C354-4F10-BCC9-E4E1DA751FCE}">
+          <x14:cfRule type="expression" priority="180" id="{34981E72-2ADD-4B77-A845-E5B091F9BA9D}">
             <xm:f>AND((I2&lt;10),(I2&lt;&gt;solved!I2))</xm:f>
             <x14:dxf>
               <font>
@@ -8930,7 +8935,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="181" id="{587021BB-23B0-4959-8A1B-F773C5E25450}">
+          <x14:cfRule type="expression" priority="181" id="{ADC88FD7-DD1A-4482-AF00-ED73268E39F9}">
             <xm:f>AND((I3&lt;10),(I3&lt;&gt;solved!I3))</xm:f>
             <x14:dxf>
               <font>
@@ -8941,7 +8946,7 @@
           <xm:sqref>I3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="182" id="{7270EF10-3416-4089-9766-E88332A48232}">
+          <x14:cfRule type="expression" priority="182" id="{C9756028-82B2-4A48-A710-8DB0C0F5B975}">
             <xm:f>AND((I4&lt;10),(I4&lt;&gt;solved!I4))</xm:f>
             <x14:dxf>
               <font>
@@ -8952,7 +8957,7 @@
           <xm:sqref>I4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="183" id="{565D6BE8-5224-4EA1-AF2A-4530D07631BA}">
+          <x14:cfRule type="expression" priority="183" id="{9976A5AB-E9A7-40D5-83AD-A0C2ED1BE9A0}">
             <xm:f>AND((I5&lt;10),(I5&lt;&gt;solved!I5))</xm:f>
             <x14:dxf>
               <font>
@@ -8963,7 +8968,7 @@
           <xm:sqref>I5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="184" id="{C5CD54B3-BF59-47F6-AECB-38A6D5E0D7BE}">
+          <x14:cfRule type="expression" priority="184" id="{FEE4598D-D8CC-44C0-8CAC-BBC1E9BF1DA5}">
             <xm:f>AND((I6&lt;10),(I6&lt;&gt;solved!I6))</xm:f>
             <x14:dxf>
               <font>
@@ -8974,7 +8979,7 @@
           <xm:sqref>I6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="185" id="{8BFBCD10-D6C2-4056-BE5D-B81A87EF64A4}">
+          <x14:cfRule type="expression" priority="185" id="{202C607F-6952-4276-8C67-6867367F27C0}">
             <xm:f>AND((I7&lt;10),(I7&lt;&gt;solved!I7))</xm:f>
             <x14:dxf>
               <font>
@@ -8985,7 +8990,7 @@
           <xm:sqref>I7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="186" id="{D9F69024-357F-443A-98FB-3F9FAAEAF742}">
+          <x14:cfRule type="expression" priority="186" id="{226921BE-5956-4817-BCA9-AE3065DAC490}">
             <xm:f>AND((I8&lt;10),(I8&lt;&gt;solved!I8))</xm:f>
             <x14:dxf>
               <font>
@@ -8996,7 +9001,7 @@
           <xm:sqref>I8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="187" id="{5A91C7B8-4398-461A-AC97-2291AE84112E}">
+          <x14:cfRule type="expression" priority="187" id="{715BDA19-C616-432E-A3FD-AA83B85FFAAF}">
             <xm:f>AND((I9&lt;10),(I9&lt;&gt;solved!I9))</xm:f>
             <x14:dxf>
               <font>
@@ -9007,7 +9012,7 @@
           <xm:sqref>I9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="188" id="{6EEE4B1A-8DD7-4330-BB38-64843B604534}">
+          <x14:cfRule type="expression" priority="188" id="{ADDAB711-1EC4-4EF1-B8F3-ABF5D2A9BFA7}">
             <xm:f>AND(($A$1&lt;10),($A$1&lt;&gt;solved!$A$1))</xm:f>
             <x14:dxf>
               <font>
@@ -9018,7 +9023,7 @@
           <xm:sqref>A1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="189" id="{931F9447-A4D3-4F3F-B3AD-D760D81A1F2E}">
+          <x14:cfRule type="expression" priority="189" id="{80B6D72E-13DA-4390-9E56-BFF022BE9984}">
             <xm:f>AND(($A$4&lt;10),($A$4&lt;&gt;solved!$A$4))</xm:f>
             <x14:dxf>
               <font>
@@ -9053,7 +9058,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -9061,22 +9066,22 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18"/>
+      <c r="A2" s="19"/>
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18"/>
+      <c r="A3" s="19"/>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="n">
+      <c r="A5" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="56" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -9084,10 +9089,10 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18"/>
+      <c r="A6" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18" t="n">
+      <c r="A7" s="19" t="n">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -9098,10 +9103,10 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18"/>
+      <c r="A8" s="19"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18" t="n">
+      <c r="A9" s="19" t="n">
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -9112,10 +9117,10 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18"/>
+      <c r="A10" s="19"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="18" t="n">
+      <c r="A11" s="19" t="n">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -9126,23 +9131,23 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="18"/>
+      <c r="A12" s="19"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18"/>
+      <c r="A13" s="19"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="18"/>
+      <c r="A14" s="19"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="18"/>
+      <c r="A15" s="19"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="18"/>
-    </row>
-    <row r="17" s="18" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A16" s="19"/>
+    </row>
+    <row r="17" s="19" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="18"/>
+      <c r="A18" s="19"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -9868,7 +9873,7 @@
       <c r="G9" s="11"/>
       <c r="H9" s="12"/>
       <c r="I9" s="13"/>
-      <c r="K9" s="14" t="str">
+      <c r="K9" s="15" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "9")=9, 9, "")</f>
         <v/>
       </c>
@@ -9966,7 +9971,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="29" id="{E730413E-10C9-4D2D-9F5E-781B3873ECF8}">
+          <x14:cfRule type="expression" priority="29" id="{7539C153-2B20-49DE-A938-2327E2384D1C}">
             <xm:f>AND(($A$1&lt;10),($A$1&lt;&gt;solved!$A$1))</xm:f>
             <x14:dxf>
               <font>
@@ -9982,7 +9987,7 @@
           <xm:sqref>A1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="30" id="{20C965FE-B658-4058-8F70-9D41EB3DD9E4}">
+          <x14:cfRule type="expression" priority="30" id="{46C81B7B-9031-4AD0-A8C5-3615804E80E0}">
             <xm:f>AND((A2&lt;10),(A2&lt;&gt;solved!A2))</xm:f>
             <x14:dxf>
               <font>
@@ -9993,7 +9998,7 @@
           <xm:sqref>A2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="31" id="{47B5154A-C650-4CBE-8370-B6B0167ED640}">
+          <x14:cfRule type="expression" priority="31" id="{B7449C79-9D88-4776-BEF9-C0BEE07455A1}">
             <xm:f>AND((A3&lt;10),(A3&lt;&gt;solved!A3))</xm:f>
             <x14:dxf>
               <font>
@@ -10004,7 +10009,7 @@
           <xm:sqref>A3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="32" id="{ED286551-706C-4D50-AD80-8179331436E6}">
+          <x14:cfRule type="expression" priority="32" id="{9F3A75D0-A4A0-4177-B538-BD6CB25FD485}">
             <xm:f>AND((A4&lt;10),(A4&lt;&gt;solved!A4))</xm:f>
             <x14:dxf>
               <font>
@@ -10015,7 +10020,7 @@
           <xm:sqref>A4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="33" id="{CB771815-F04E-472B-AED6-90B890D0A3BE}">
+          <x14:cfRule type="expression" priority="33" id="{E5BE80C4-DEF1-494B-89EB-F34636E34B4C}">
             <xm:f>AND((A5&lt;10),(A5&lt;&gt;solved!A5))</xm:f>
             <x14:dxf>
               <font>
@@ -10026,7 +10031,7 @@
           <xm:sqref>A5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="34" id="{F21C614A-7A41-4394-8414-74F06C4D65B6}">
+          <x14:cfRule type="expression" priority="34" id="{6D3EB4B1-C018-4772-AF8B-11DA4D33F1F9}">
             <xm:f>AND((A6&lt;10),(A6&lt;&gt;solved!A6))</xm:f>
             <x14:dxf>
               <font>
@@ -10037,7 +10042,7 @@
           <xm:sqref>A6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="35" id="{D030A120-E3CF-4442-B090-80761B26FA84}">
+          <x14:cfRule type="expression" priority="35" id="{79619EB2-E574-4437-AFE7-F9C367C23B2B}">
             <xm:f>AND((A7&lt;10),(A7&lt;&gt;solved!A7))</xm:f>
             <x14:dxf>
               <font>
@@ -10048,7 +10053,7 @@
           <xm:sqref>A7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="36" id="{44C295B9-7A2E-46E5-9B20-2157CDC8B4F5}">
+          <x14:cfRule type="expression" priority="36" id="{F064B4D2-545A-4291-8FC6-3AEA66FE69ED}">
             <xm:f>AND((A8&lt;10),(A8&lt;&gt;solved!A8))</xm:f>
             <x14:dxf>
               <font>
@@ -10059,7 +10064,7 @@
           <xm:sqref>A8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="37" id="{7FC04D6B-3C46-41E7-8382-C78C60653E33}">
+          <x14:cfRule type="expression" priority="37" id="{60EB2AE8-C420-4F25-A574-DAABC14579F9}">
             <xm:f>AND((A9&lt;10),(A9&lt;&gt;solved!A9))</xm:f>
             <x14:dxf>
               <font>
@@ -10070,7 +10075,7 @@
           <xm:sqref>A9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="38" id="{DF10218F-AF25-4DB9-91E6-20BA19151FCB}">
+          <x14:cfRule type="expression" priority="38" id="{14A0D927-DA93-4541-AD84-1E53C556B080}">
             <xm:f>AND((B1&lt;10),(B1&lt;&gt;solved!B1))</xm:f>
             <x14:dxf>
               <font>
@@ -10081,7 +10086,7 @@
           <xm:sqref>B1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="39" id="{4FECCC75-30FF-46DA-B0D6-86CAC8A0F9A1}">
+          <x14:cfRule type="expression" priority="39" id="{316C5A5A-DC39-44A0-BF7D-41BD7A82E075}">
             <xm:f>AND((B2&lt;10),(B2&lt;&gt;solved!B2))</xm:f>
             <x14:dxf>
               <font>
@@ -10092,7 +10097,7 @@
           <xm:sqref>B2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="40" id="{72E9C3E0-E9DC-47F7-97B7-1ACA49833559}">
+          <x14:cfRule type="expression" priority="40" id="{EACECEA2-6DA1-4439-86CF-77A040F01A79}">
             <xm:f>AND((B3&lt;10),(B3&lt;&gt;solved!B3))</xm:f>
             <x14:dxf>
               <font>
@@ -10103,7 +10108,7 @@
           <xm:sqref>B3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="41" id="{2022F2C6-1C70-4BD5-99B0-4ECB7A1351A5}">
+          <x14:cfRule type="expression" priority="41" id="{EA5015D0-1B4F-416A-9CA0-E47581CEB2A4}">
             <xm:f>AND((B4&lt;10),(B4&lt;&gt;solved!B4))</xm:f>
             <x14:dxf>
               <font>
@@ -10114,7 +10119,7 @@
           <xm:sqref>B4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="42" id="{BBD58ACE-B67C-44D9-9754-204C3A97C126}">
+          <x14:cfRule type="expression" priority="42" id="{3D67F619-5228-44A3-B87C-DA41FBCC6AFA}">
             <xm:f>AND((B5&lt;10),(B5&lt;&gt;solved!B5))</xm:f>
             <x14:dxf>
               <font>
@@ -10125,7 +10130,7 @@
           <xm:sqref>B5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="43" id="{1EC22D9F-869A-4F3D-B4C2-4096413F7C45}">
+          <x14:cfRule type="expression" priority="43" id="{274DA53D-8184-4C8C-A6FC-F724BB3AAB48}">
             <xm:f>AND((B6&lt;10),(B6&lt;&gt;solved!B6))</xm:f>
             <x14:dxf>
               <font>
@@ -10136,7 +10141,7 @@
           <xm:sqref>B6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="44" id="{A0C04A9C-D9D3-429D-97EE-3D6024A44014}">
+          <x14:cfRule type="expression" priority="44" id="{7182A52A-5FCB-4CDD-9441-623D854EE2CD}">
             <xm:f>AND((B7&lt;10),(B7&lt;&gt;solved!B7))</xm:f>
             <x14:dxf>
               <font>
@@ -10147,7 +10152,7 @@
           <xm:sqref>B7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="45" id="{CEFE7A42-708D-494C-AB51-E944785F5480}">
+          <x14:cfRule type="expression" priority="45" id="{C5843042-49DA-4826-AFDA-47EAB6CD19FF}">
             <xm:f>AND((B8&lt;10),(B8&lt;&gt;solved!B8))</xm:f>
             <x14:dxf>
               <font>
@@ -10158,7 +10163,7 @@
           <xm:sqref>B8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="46" id="{3D7B74F9-1F6F-4EC1-8393-D022406F84F8}">
+          <x14:cfRule type="expression" priority="46" id="{E7605124-AD37-4D9A-A2E7-3B6177719474}">
             <xm:f>AND((B9&lt;10),(B9&lt;&gt;solved!B9))</xm:f>
             <x14:dxf>
               <font>
@@ -10169,7 +10174,7 @@
           <xm:sqref>B9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="47" id="{7D209345-33ED-4CC1-B8E9-109B84B6E3EE}">
+          <x14:cfRule type="expression" priority="47" id="{E2F3132C-81D5-4560-A580-C35B4E5E8184}">
             <xm:f>AND((C1&lt;10),(C1&lt;&gt;solved!C1))</xm:f>
             <x14:dxf>
               <font>
@@ -10180,7 +10185,7 @@
           <xm:sqref>C1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="48" id="{E2FEBE8F-9667-402D-AFC8-EF74F2417FCC}">
+          <x14:cfRule type="expression" priority="48" id="{BF7389FB-2B75-4079-9C1D-4060FCD58629}">
             <xm:f>AND((C2&lt;10),(C2&lt;&gt;solved!C2))</xm:f>
             <x14:dxf>
               <font>
@@ -10191,7 +10196,7 @@
           <xm:sqref>C2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="49" id="{EA30E0E2-DAEB-415B-A673-13E2CEA09CC6}">
+          <x14:cfRule type="expression" priority="49" id="{2D3873E0-5675-46B0-9D73-80791B4FA4DE}">
             <xm:f>AND((C3&lt;10),(C3&lt;&gt;solved!C3))</xm:f>
             <x14:dxf>
               <font>
@@ -10202,7 +10207,7 @@
           <xm:sqref>C3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="50" id="{1089BFB7-CEDC-4776-811F-F33E3C128068}">
+          <x14:cfRule type="expression" priority="50" id="{244CE7E0-7D4D-474A-A3ED-1491D7371DCA}">
             <xm:f>AND((C4&lt;10),(C4&lt;&gt;solved!C4))</xm:f>
             <x14:dxf>
               <font>
@@ -10213,7 +10218,7 @@
           <xm:sqref>C4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="51" id="{B3E863C4-FA30-4C4E-8D88-6BF683F071B7}">
+          <x14:cfRule type="expression" priority="51" id="{287CCF51-18A2-4111-A27C-ED7CCCB88112}">
             <xm:f>AND((C5&lt;10),(C5&lt;&gt;solved!C5))</xm:f>
             <x14:dxf>
               <font>
@@ -10224,7 +10229,7 @@
           <xm:sqref>C5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="52" id="{5F7612A0-70FD-43AA-A02F-539C33CE3260}">
+          <x14:cfRule type="expression" priority="52" id="{D57F4B52-539E-4DCA-B290-AE487CF69B6B}">
             <xm:f>AND((C6&lt;10),(C6&lt;&gt;solved!C6))</xm:f>
             <x14:dxf>
               <font>
@@ -10235,7 +10240,7 @@
           <xm:sqref>C6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="53" id="{715E303F-C1FE-49C8-A029-65FA93806F7F}">
+          <x14:cfRule type="expression" priority="53" id="{69E0ED97-4D7E-4F75-B1DC-701D13B3602F}">
             <xm:f>AND((C7&lt;10),(C7&lt;&gt;solved!C7))</xm:f>
             <x14:dxf>
               <font>
@@ -10246,7 +10251,7 @@
           <xm:sqref>C7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="54" id="{62FD66D9-1B53-4D57-A9C7-E62F2F7CF2C5}">
+          <x14:cfRule type="expression" priority="54" id="{10A3C415-64C3-4889-A222-CDBC7F373897}">
             <xm:f>AND((C8&lt;10),(C8&lt;&gt;solved!C8))</xm:f>
             <x14:dxf>
               <font>
@@ -10257,7 +10262,7 @@
           <xm:sqref>C8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="55" id="{E41EEB31-722E-4768-A9F0-2A50B1C06D2E}">
+          <x14:cfRule type="expression" priority="55" id="{E9ABA69C-90F0-4CEC-A07C-152A5A40F1A7}">
             <xm:f>AND((C9&lt;10),(C9&lt;&gt;solved!C9))</xm:f>
             <x14:dxf>
               <font>
@@ -10268,7 +10273,7 @@
           <xm:sqref>C9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="56" id="{EB7310B5-427A-413B-92A1-AF56BD2BB73E}">
+          <x14:cfRule type="expression" priority="56" id="{3D8F99B6-A622-4255-89E7-19D1E755DE36}">
             <xm:f>AND((D1&lt;10),(D1&lt;&gt;solved!D1))</xm:f>
             <x14:dxf>
               <font>
@@ -10279,7 +10284,7 @@
           <xm:sqref>D1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="57" id="{BCE3B042-60DB-4C2E-8136-A7244E83B19E}">
+          <x14:cfRule type="expression" priority="57" id="{F22FC078-9BF1-4ED1-A7F1-A0155A2FC49C}">
             <xm:f>AND((D2&lt;10),(D2&lt;&gt;solved!D2))</xm:f>
             <x14:dxf>
               <font>
@@ -10290,7 +10295,7 @@
           <xm:sqref>D2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="58" id="{8DBC3692-60AE-46E0-936B-4330D0BBE371}">
+          <x14:cfRule type="expression" priority="58" id="{DB927BDC-4452-4C89-A13A-CA1DB22CAA1A}">
             <xm:f>AND((D3&lt;10),(D3&lt;&gt;solved!D3))</xm:f>
             <x14:dxf>
               <font>
@@ -10301,7 +10306,7 @@
           <xm:sqref>D3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="59" id="{79B0CD48-B0BA-40B8-98BF-4E89C57D7187}">
+          <x14:cfRule type="expression" priority="59" id="{90F07B63-90C0-4DD4-BA24-EDA4AFB64330}">
             <xm:f>AND((D4&lt;10),(D4&lt;&gt;solved!D4))</xm:f>
             <x14:dxf>
               <font>
@@ -10312,7 +10317,7 @@
           <xm:sqref>D4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="60" id="{2C35D6D8-9A27-41D9-A4BB-5AF07061B3BD}">
+          <x14:cfRule type="expression" priority="60" id="{A7A16DA0-4052-49DB-85A1-5FD8FEAE268B}">
             <xm:f>AND((D5&lt;10),(D5&lt;&gt;solved!D5))</xm:f>
             <x14:dxf>
               <font>
@@ -10323,7 +10328,7 @@
           <xm:sqref>D5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="61" id="{8CB727EB-BAA0-4A70-837C-E34B8B41D2F5}">
+          <x14:cfRule type="expression" priority="61" id="{ADD18667-5353-461F-ACEA-7F184056176B}">
             <xm:f>AND((D6&lt;10),(D6&lt;&gt;solved!D6))</xm:f>
             <x14:dxf>
               <font>
@@ -10334,7 +10339,7 @@
           <xm:sqref>D6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="62" id="{E8B210FF-171E-451F-9FA9-70B61EBBDAFE}">
+          <x14:cfRule type="expression" priority="62" id="{5BCFBEF0-1D32-47D0-B991-DB851B8088CD}">
             <xm:f>AND((D7&lt;10),(D7&lt;&gt;solved!D7))</xm:f>
             <x14:dxf>
               <font>
@@ -10345,7 +10350,7 @@
           <xm:sqref>D7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="63" id="{909A9116-3C43-46BF-915C-AF1B249B10E0}">
+          <x14:cfRule type="expression" priority="63" id="{D700D7EF-2827-4274-8115-CAE74CF9F67D}">
             <xm:f>AND((D8&lt;10),(D8&lt;&gt;solved!D8))</xm:f>
             <x14:dxf>
               <font>
@@ -10356,7 +10361,7 @@
           <xm:sqref>D8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="64" id="{90EFD8E5-9717-4D67-88C5-BFA9598C8436}">
+          <x14:cfRule type="expression" priority="64" id="{50D89F8B-EA92-4EBE-B245-E7906F458BD0}">
             <xm:f>AND((D9&lt;10),(D9&lt;&gt;solved!D9))</xm:f>
             <x14:dxf>
               <font>
@@ -10367,7 +10372,7 @@
           <xm:sqref>D9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="65" id="{D3A7E53C-BE64-4D3F-83CB-E1CC71A3C470}">
+          <x14:cfRule type="expression" priority="65" id="{5E14944E-9472-48D5-9BF0-13FE4B1288F1}">
             <xm:f>AND((E1&lt;10),(E1&lt;&gt;solved!E1))</xm:f>
             <x14:dxf>
               <font>
@@ -10378,7 +10383,7 @@
           <xm:sqref>E1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="66" id="{21721FCD-8423-4E73-AA64-1250A0F740B1}">
+          <x14:cfRule type="expression" priority="66" id="{A0F7F199-949A-407E-9B97-75244A4DC266}">
             <xm:f>AND((E2&lt;10),(E2&lt;&gt;solved!E2))</xm:f>
             <x14:dxf>
               <font>
@@ -10389,7 +10394,7 @@
           <xm:sqref>E2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="67" id="{34523B90-24A9-4EEA-9FBD-643E60E057A5}">
+          <x14:cfRule type="expression" priority="67" id="{F7C494AD-C562-4668-9C7E-305E94959619}">
             <xm:f>AND((E3&lt;10),(E3&lt;&gt;solved!E3))</xm:f>
             <x14:dxf>
               <font>
@@ -10400,7 +10405,7 @@
           <xm:sqref>E3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="68" id="{20307FA0-744D-4A80-9FED-BBB4CE2F9618}">
+          <x14:cfRule type="expression" priority="68" id="{8E179444-16AB-4DE0-A1B6-8013BDC0FCE6}">
             <xm:f>AND((E4&lt;10),(E4&lt;&gt;solved!E4))</xm:f>
             <x14:dxf>
               <font>
@@ -10411,7 +10416,7 @@
           <xm:sqref>E4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="69" id="{D2D32FEB-EFB9-4AE6-BDF5-1550865A7B84}">
+          <x14:cfRule type="expression" priority="69" id="{6D0025CE-95BB-4FE5-807C-D6B37DB4ABE3}">
             <xm:f>AND((E5&lt;10),(E5&lt;&gt;solved!E5))</xm:f>
             <x14:dxf>
               <font>
@@ -10422,7 +10427,7 @@
           <xm:sqref>E5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="70" id="{35D18714-9FAB-4DE5-B6B3-12A884B66647}">
+          <x14:cfRule type="expression" priority="70" id="{84761D51-7060-4548-BA33-CF35B774FAC8}">
             <xm:f>AND((E6&lt;10),(E6&lt;&gt;solved!E6))</xm:f>
             <x14:dxf>
               <font>
@@ -10433,7 +10438,7 @@
           <xm:sqref>E6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="71" id="{B6A8F7DB-B5BC-469F-9ED2-9A8D6393A06F}">
+          <x14:cfRule type="expression" priority="71" id="{DD46A0CB-71A6-4B5F-B439-DF91D82F3451}">
             <xm:f>AND((E7&lt;10),(E7&lt;&gt;solved!E7))</xm:f>
             <x14:dxf>
               <font>
@@ -10444,7 +10449,7 @@
           <xm:sqref>E7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="72" id="{CED14811-D21E-4826-B638-D3F457E0FAEF}">
+          <x14:cfRule type="expression" priority="72" id="{205CB6C0-9350-4766-A0C8-E0F024AA8739}">
             <xm:f>AND((E8&lt;10),(E8&lt;&gt;solved!E8))</xm:f>
             <x14:dxf>
               <font>
@@ -10455,7 +10460,7 @@
           <xm:sqref>E8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="73" id="{9ABC308D-28EE-4776-B671-63D5AEC2CC63}">
+          <x14:cfRule type="expression" priority="73" id="{3050BD79-8CDD-4E38-BF7D-A9692315FFA0}">
             <xm:f>AND((E9&lt;10),(E9&lt;&gt;solved!E9))</xm:f>
             <x14:dxf>
               <font>
@@ -10466,7 +10471,7 @@
           <xm:sqref>E9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="74" id="{32CD13BB-FC3D-4A00-86E6-D52DBD9E6BC0}">
+          <x14:cfRule type="expression" priority="74" id="{B51DB8CB-D91E-46A7-9A43-CD39902FA8BA}">
             <xm:f>AND((F1&lt;10),(F1&lt;&gt;solved!F1))</xm:f>
             <x14:dxf>
               <font>
@@ -10477,7 +10482,7 @@
           <xm:sqref>F1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="75" id="{9453C437-1291-4D5A-BBEB-D7DD89F379BE}">
+          <x14:cfRule type="expression" priority="75" id="{5670E0B6-9049-4550-818B-E940CCB067A9}">
             <xm:f>AND((F2&lt;10),(F2&lt;&gt;solved!F2))</xm:f>
             <x14:dxf>
               <font>
@@ -10488,7 +10493,7 @@
           <xm:sqref>F2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="76" id="{4DCA50BC-C63B-4652-A3EF-6C8C22B9F398}">
+          <x14:cfRule type="expression" priority="76" id="{363C9EED-5952-4429-AE2A-3563723988D1}">
             <xm:f>AND((F3&lt;10),(F3&lt;&gt;solved!F3))</xm:f>
             <x14:dxf>
               <font>
@@ -10499,7 +10504,7 @@
           <xm:sqref>F3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="77" id="{FCC68859-63EB-4186-AE8D-66B11C5A195D}">
+          <x14:cfRule type="expression" priority="77" id="{D5B59E65-E076-4A32-A87B-1FF5557E699C}">
             <xm:f>AND((F4&lt;10),(F4&lt;&gt;solved!F4))</xm:f>
             <x14:dxf>
               <font>
@@ -10510,7 +10515,7 @@
           <xm:sqref>F4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="78" id="{65BAB832-2532-46F4-8C14-B423F1D0195E}">
+          <x14:cfRule type="expression" priority="78" id="{E3FA793C-22B6-44D0-9B11-8B34F190B720}">
             <xm:f>AND((F5&lt;10),(F5&lt;&gt;solved!F5))</xm:f>
             <x14:dxf>
               <font>
@@ -10521,7 +10526,7 @@
           <xm:sqref>F5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="79" id="{6590DA56-8882-42FF-A2F2-951470304CA7}">
+          <x14:cfRule type="expression" priority="79" id="{98FDAEBC-3844-4029-AFE5-DE8D452FE957}">
             <xm:f>AND((F6&lt;10),(F6&lt;&gt;solved!F6))</xm:f>
             <x14:dxf>
               <font>
@@ -10532,7 +10537,7 @@
           <xm:sqref>F6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="80" id="{3067A733-691B-405C-A726-BB95A09D2FFE}">
+          <x14:cfRule type="expression" priority="80" id="{2C19D19D-E9F8-4810-8928-A2C0F940B267}">
             <xm:f>AND((F7&lt;10),(F7&lt;&gt;solved!F7))</xm:f>
             <x14:dxf>
               <font>
@@ -10543,7 +10548,7 @@
           <xm:sqref>F7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="81" id="{AE859C78-DAD0-4C6B-9070-A5AA7272D97A}">
+          <x14:cfRule type="expression" priority="81" id="{EB4D845F-2F4D-42A3-BB52-EB483E30ADF6}">
             <xm:f>AND((F8&lt;10),(F8&lt;&gt;solved!F8))</xm:f>
             <x14:dxf>
               <font>
@@ -10554,7 +10559,7 @@
           <xm:sqref>F8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="82" id="{46804FDC-8970-41BE-A3A6-19E3416477A2}">
+          <x14:cfRule type="expression" priority="82" id="{795AF5F5-4374-4BA0-BE9D-17211AA4C0BE}">
             <xm:f>AND((F9&lt;10),(F9&lt;&gt;solved!F9))</xm:f>
             <x14:dxf>
               <font>
@@ -10565,7 +10570,7 @@
           <xm:sqref>F9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="83" id="{C098DF84-54FC-4343-BFAA-792ADF40406E}">
+          <x14:cfRule type="expression" priority="83" id="{C08AF1F2-5B99-4D40-8CF2-63E222103057}">
             <xm:f>AND((G1&lt;10),(G1&lt;&gt;solved!G1))</xm:f>
             <x14:dxf>
               <font>
@@ -10576,7 +10581,7 @@
           <xm:sqref>G1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="84" id="{11C53496-9736-4AAF-A8B7-246C148EB085}">
+          <x14:cfRule type="expression" priority="84" id="{C0235744-AE27-4B1B-83EB-704F1B3767FD}">
             <xm:f>AND((G2&lt;10),(G2&lt;&gt;solved!G2))</xm:f>
             <x14:dxf>
               <font>
@@ -10587,7 +10592,7 @@
           <xm:sqref>G2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="85" id="{DF55C4D1-288F-403A-A82E-76DC1D5540F0}">
+          <x14:cfRule type="expression" priority="85" id="{194E2B54-BE58-453B-8FFB-D667F54CEA7D}">
             <xm:f>AND((G3&lt;10),(G3&lt;&gt;solved!G3))</xm:f>
             <x14:dxf>
               <font>
@@ -10598,7 +10603,7 @@
           <xm:sqref>G3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="86" id="{B07CD127-B0FF-47AA-816E-521D9DC45916}">
+          <x14:cfRule type="expression" priority="86" id="{2B472846-2ECB-4EB7-8321-DCCB1D7F8CFE}">
             <xm:f>AND((G4&lt;10),(G4&lt;&gt;solved!G4))</xm:f>
             <x14:dxf>
               <font>
@@ -10609,7 +10614,7 @@
           <xm:sqref>G4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="87" id="{93B63A1F-12F0-4F83-86DE-4780EF95E586}">
+          <x14:cfRule type="expression" priority="87" id="{B2AF7015-AE58-4A47-87D0-B860FDB8D952}">
             <xm:f>AND((G5&lt;10),(G5&lt;&gt;solved!G5))</xm:f>
             <x14:dxf>
               <font>
@@ -10620,7 +10625,7 @@
           <xm:sqref>G5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="88" id="{11BD81B4-CEA2-4980-9D52-F030C98E8457}">
+          <x14:cfRule type="expression" priority="88" id="{D0EDFDD7-68C2-4EC1-B49D-E89BA9FFC619}">
             <xm:f>AND((G6&lt;10),(G6&lt;&gt;solved!G6))</xm:f>
             <x14:dxf>
               <font>
@@ -10631,7 +10636,7 @@
           <xm:sqref>G6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="89" id="{6416466D-B378-4D37-9344-6FE01B77BC44}">
+          <x14:cfRule type="expression" priority="89" id="{5E1374C4-F06D-4177-89A6-5B107A63D8F9}">
             <xm:f>AND((G7&lt;10),(G7&lt;&gt;solved!G7))</xm:f>
             <x14:dxf>
               <font>
@@ -10642,7 +10647,7 @@
           <xm:sqref>G7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="90" id="{47A414C8-AB68-449C-88AB-E4559F8610F7}">
+          <x14:cfRule type="expression" priority="90" id="{F3F9BCF4-7878-481C-9D4A-179D208F32EA}">
             <xm:f>AND((G8&lt;10),(G8&lt;&gt;solved!G8))</xm:f>
             <x14:dxf>
               <font>
@@ -10653,7 +10658,7 @@
           <xm:sqref>G8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="91" id="{92EBA9B3-541D-4646-BE78-32A6CE475A64}">
+          <x14:cfRule type="expression" priority="91" id="{CC9790C0-C14C-4C79-ABD8-A3C97050A7FC}">
             <xm:f>AND((G9&lt;10),(G9&lt;&gt;solved!G9))</xm:f>
             <x14:dxf>
               <font>
@@ -10664,7 +10669,7 @@
           <xm:sqref>G9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="92" id="{D16C749E-C1BD-4274-BCE3-73C272D82FDB}">
+          <x14:cfRule type="expression" priority="92" id="{2C3071D0-6F35-4220-BADB-F190DDADC876}">
             <xm:f>AND((H1&lt;10),(H1&lt;&gt;solved!H1))</xm:f>
             <x14:dxf>
               <font>
@@ -10675,7 +10680,7 @@
           <xm:sqref>H1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="93" id="{AA6A2349-59F5-4880-9B6E-E06B61FE9387}">
+          <x14:cfRule type="expression" priority="93" id="{75FEA520-B8BF-44B6-8969-3EB2D056D517}">
             <xm:f>AND((H2&lt;10),(H2&lt;&gt;solved!H2))</xm:f>
             <x14:dxf>
               <font>
@@ -10686,7 +10691,7 @@
           <xm:sqref>H2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="94" id="{4E53EC6B-6322-425F-8CD0-15D955786D60}">
+          <x14:cfRule type="expression" priority="94" id="{56152ABE-4F7D-4BAB-B58F-F9AA103CE37D}">
             <xm:f>AND((H3&lt;10),(H3&lt;&gt;solved!H3))</xm:f>
             <x14:dxf>
               <font>
@@ -10697,7 +10702,7 @@
           <xm:sqref>H3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="95" id="{A561EB81-CD4C-4B17-847C-4BEF3781611C}">
+          <x14:cfRule type="expression" priority="95" id="{AF33FDBA-9400-4AAD-BC31-C860185EC31A}">
             <xm:f>AND((H4&lt;10),(H4&lt;&gt;solved!H4))</xm:f>
             <x14:dxf>
               <font>
@@ -10708,7 +10713,7 @@
           <xm:sqref>H4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="96" id="{5670AF86-5A10-4FCD-92CF-4C1DD9F6C861}">
+          <x14:cfRule type="expression" priority="96" id="{CDC0A3AD-E060-4C36-B28C-5B1111C37FAC}">
             <xm:f>AND((H5&lt;10),(H5&lt;&gt;solved!H5))</xm:f>
             <x14:dxf>
               <font>
@@ -10719,7 +10724,7 @@
           <xm:sqref>H5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="97" id="{39DC4E60-4531-47E8-A137-E14FCC51F05D}">
+          <x14:cfRule type="expression" priority="97" id="{732018E5-F4F3-4866-8F2B-304415D7438F}">
             <xm:f>AND((H6&lt;10),(H6&lt;&gt;solved!H6))</xm:f>
             <x14:dxf>
               <font>
@@ -10730,7 +10735,7 @@
           <xm:sqref>H6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="98" id="{EED072D1-FE10-4392-9C63-B6C786F849F3}">
+          <x14:cfRule type="expression" priority="98" id="{5F616B5E-A91B-44D4-907B-5DDD5BA5C91E}">
             <xm:f>AND((H7&lt;10),(H7&lt;&gt;solved!H7))</xm:f>
             <x14:dxf>
               <font>
@@ -10741,7 +10746,7 @@
           <xm:sqref>H7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="99" id="{E071D356-4F10-43AC-A810-C66C54A7C626}">
+          <x14:cfRule type="expression" priority="99" id="{73BC3FF3-80F4-4BAA-A7C1-F0ABE88F56E7}">
             <xm:f>AND((H8&lt;10),(H8&lt;&gt;solved!H8))</xm:f>
             <x14:dxf>
               <font>
@@ -10752,7 +10757,7 @@
           <xm:sqref>H8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="100" id="{8C867F42-C8F4-4561-84E5-146AA39CDF10}">
+          <x14:cfRule type="expression" priority="100" id="{60BF6A20-A2FA-4B84-BD35-2D5960DE37D1}">
             <xm:f>AND((H9&lt;10),(H9&lt;&gt;solved!H9))</xm:f>
             <x14:dxf>
               <font>
@@ -10763,7 +10768,7 @@
           <xm:sqref>H9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="101" id="{B41022C1-4F38-4140-B7C9-006514238AA0}">
+          <x14:cfRule type="expression" priority="101" id="{98E4C9A0-7BEB-4C68-86A3-84CC2D44E424}">
             <xm:f>AND((I2&lt;10),(I2&lt;&gt;solved!I2))</xm:f>
             <x14:dxf>
               <font>
@@ -10774,7 +10779,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="102" id="{9F2D475F-8911-4785-84A8-DB1D8634965E}">
+          <x14:cfRule type="expression" priority="102" id="{F5E02BEB-9564-475B-84C4-6E2040D1EF34}">
             <xm:f>AND((I1&lt;10),(I1&lt;&gt;solved!I1))</xm:f>
             <x14:dxf>
               <font>
@@ -10785,7 +10790,7 @@
           <xm:sqref>I1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="103" id="{FEFC34CA-E0F2-4AF0-B58C-FC8F745E8FCE}">
+          <x14:cfRule type="expression" priority="103" id="{B717C49A-7A5D-47F7-8D18-5263C2C9692E}">
             <xm:f>AND((I3&lt;10),(I3&lt;&gt;solved!I3))</xm:f>
             <x14:dxf>
               <font>
@@ -10796,7 +10801,7 @@
           <xm:sqref>I3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="104" id="{995E725C-86D9-4044-8CE7-B64E2DEA88F5}">
+          <x14:cfRule type="expression" priority="104" id="{D19ECBC3-1600-4FB6-8A20-2548473822AE}">
             <xm:f>AND((I4&lt;10),(I4&lt;&gt;solved!I4))</xm:f>
             <x14:dxf>
               <font>
@@ -10807,7 +10812,7 @@
           <xm:sqref>I4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="105" id="{BFB6EC3F-B023-4083-9884-875875BD6572}">
+          <x14:cfRule type="expression" priority="105" id="{7285EC32-8274-44D7-A01A-75B015EFD3D8}">
             <xm:f>AND((I5&lt;10),(I5&lt;&gt;solved!I5))</xm:f>
             <x14:dxf>
               <font>
@@ -10818,7 +10823,7 @@
           <xm:sqref>I5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="106" id="{7E589961-FB94-4FD0-B95D-20BFDBD74162}">
+          <x14:cfRule type="expression" priority="106" id="{3C7BE698-3628-43F7-A6D0-837E8A4531E2}">
             <xm:f>AND((I6&lt;10),(I6&lt;&gt;solved!I6))</xm:f>
             <x14:dxf>
               <font>
@@ -10829,7 +10834,7 @@
           <xm:sqref>I6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="107" id="{CF257F25-C498-4B8E-9C26-183A2970F224}">
+          <x14:cfRule type="expression" priority="107" id="{B6DBC365-F06B-40ED-B31F-502F13B62B76}">
             <xm:f>AND((I7&lt;10),(I7&lt;&gt;solved!I7))</xm:f>
             <x14:dxf>
               <font>
@@ -10840,7 +10845,7 @@
           <xm:sqref>I7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="108" id="{5BA425E4-814D-4628-86F9-FFD34C586125}">
+          <x14:cfRule type="expression" priority="108" id="{64877415-8335-4143-A748-AD9296D05696}">
             <xm:f>AND((I8&lt;10),(I8&lt;&gt;solved!I8))</xm:f>
             <x14:dxf>
               <font>
@@ -10851,7 +10856,7 @@
           <xm:sqref>I8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="109" id="{7D10EC4E-B7B3-42C6-A080-6A4EEADCBC00}">
+          <x14:cfRule type="expression" priority="109" id="{1842BE19-BDC2-47C0-8EE7-984388B94C99}">
             <xm:f>AND((I9&lt;10),(I9&lt;&gt;solved!I9))</xm:f>
             <x14:dxf>
               <font>
@@ -11249,9 +11254,9 @@
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="15"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="16"/>
+      <c r="G10" s="17"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -11357,108 +11362,108 @@
       <c r="J20" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="17" t="n">
+      <c r="C22" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="17" t="n">
+      <c r="D22" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="17" t="n">
+      <c r="E22" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="17" t="n">
+      <c r="F22" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="17" t="n">
+      <c r="G22" s="18" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="17" t="n">
+      <c r="B23" s="18" t="n">
         <v>15</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18" t="n">
+      <c r="C23" s="19"/>
+      <c r="D23" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18" t="n">
+      <c r="E23" s="19"/>
+      <c r="F23" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G23" s="18" t="n">
+      <c r="G23" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="17" t="n">
+      <c r="B24" s="18" t="n">
         <v>35</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18" t="n">
+      <c r="C24" s="19"/>
+      <c r="D24" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18" t="n">
+      <c r="E24" s="19"/>
+      <c r="F24" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G24" s="18" t="n">
+      <c r="G24" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="17" t="n">
+      <c r="B25" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="C25" s="19" t="n">
+      <c r="C25" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="18" t="n">
+      <c r="D25" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18" t="n">
+      <c r="E25" s="19"/>
+      <c r="F25" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G25" s="18" t="n">
+      <c r="G25" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="17" t="n">
+      <c r="B26" s="18" t="n">
         <v>75</v>
       </c>
-      <c r="C26" s="18" t="n">
+      <c r="C26" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18" t="n">
+      <c r="D26" s="19"/>
+      <c r="E26" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="19" t="n">
+      <c r="F26" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G26" s="19" t="n">
+      <c r="G26" s="20" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="17" t="n">
+      <c r="B27" s="18" t="n">
         <v>95</v>
       </c>
-      <c r="C27" s="18" t="n">
+      <c r="C27" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18" t="n">
+      <c r="D27" s="19"/>
+      <c r="E27" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="F27" s="19" t="n">
+      <c r="F27" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="18"/>
+      <c r="G27" s="19"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B10">
@@ -12000,7 +12005,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="96" id="{5D16FEB1-B089-42DA-98DE-60E8E7994A20}">
+          <x14:cfRule type="expression" priority="96" id="{A5F33DC4-18AC-458A-8643-DDAC8C3956CD}">
             <xm:f>AND(($A$1&lt;10),($A$1&lt;&gt;solved!$A$1))</xm:f>
             <x14:dxf>
               <font>
@@ -12016,7 +12021,7 @@
           <xm:sqref>B1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="98" id="{F0665839-E390-43E5-9484-CD32B85FFB71}">
+          <x14:cfRule type="expression" priority="98" id="{DE3FEE18-855C-4857-81D6-10C6622F24D7}">
             <xm:f>AND((B2&lt;10),(B2&lt;&gt;solved!B2))</xm:f>
             <x14:dxf>
               <font>
@@ -12027,7 +12032,7 @@
           <xm:sqref>B2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="100" id="{ED591441-20E2-4F95-83D2-E0DC804432A7}">
+          <x14:cfRule type="expression" priority="100" id="{72C3BC1F-AC98-49EB-A5F6-985749FCD444}">
             <xm:f>AND((B3&lt;10),(B3&lt;&gt;solved!B3))</xm:f>
             <x14:dxf>
               <font>
@@ -12038,7 +12043,7 @@
           <xm:sqref>B3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="102" id="{F3746E13-BA1A-4049-A763-66BC4A72D018}">
+          <x14:cfRule type="expression" priority="102" id="{6D2F4A23-9A3F-454D-92B2-BFD018991D7A}">
             <xm:f>AND(($A$4&lt;10),($A$4&lt;&gt;solved!$A$4))</xm:f>
             <x14:dxf>
               <font>
@@ -12049,7 +12054,7 @@
           <xm:sqref>B4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="104" id="{66C04C33-2DC7-4A72-87AD-F127C382533E}">
+          <x14:cfRule type="expression" priority="104" id="{E0442AAF-EBB6-4184-8B16-7D33F449A069}">
             <xm:f>AND((B5&lt;10),(B5&lt;&gt;solved!B5))</xm:f>
             <x14:dxf>
               <font>
@@ -12060,7 +12065,7 @@
           <xm:sqref>B5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="106" id="{ED1CFAA6-924E-4289-B9F3-B96A48CC1D30}">
+          <x14:cfRule type="expression" priority="106" id="{3F6B69B0-3DAE-46AD-8C71-EC685EB0EBF4}">
             <xm:f>AND((B6&lt;10),(B6&lt;&gt;solved!B6))</xm:f>
             <x14:dxf>
               <font>
@@ -12071,7 +12076,7 @@
           <xm:sqref>B6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="108" id="{ECD3C682-F9DF-41CF-8221-BD53EFCBC550}">
+          <x14:cfRule type="expression" priority="108" id="{BA83C387-1E7A-487B-83F7-EFDCC0813D26}">
             <xm:f>AND((B7&lt;10),(B7&lt;&gt;solved!B7))</xm:f>
             <x14:dxf>
               <font>
@@ -12082,7 +12087,7 @@
           <xm:sqref>B7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="110" id="{41585362-F394-41EB-843E-47E6AB3A8414}">
+          <x14:cfRule type="expression" priority="110" id="{C97C3439-5072-42D0-97DC-6FD5606A58C0}">
             <xm:f>AND((B8&lt;10),(B8&lt;&gt;solved!B8))</xm:f>
             <x14:dxf>
               <font>
@@ -12093,7 +12098,7 @@
           <xm:sqref>B8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="112" id="{601D1783-8DDB-4E11-AE45-90D89940D6DF}">
+          <x14:cfRule type="expression" priority="112" id="{A1F07FF6-E030-4A60-96E2-DB82D626AA00}">
             <xm:f>AND((B9&lt;10),(B9&lt;&gt;solved!B9))</xm:f>
             <x14:dxf>
               <font>
@@ -12104,7 +12109,7 @@
           <xm:sqref>B9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="114" id="{618E10BB-FF87-47A1-BB91-67F9B458372A}">
+          <x14:cfRule type="expression" priority="114" id="{F2D64F72-EF25-4D74-99B2-372D8A1729B0}">
             <xm:f>AND((C1&lt;10),(C1&lt;&gt;solved!C1))</xm:f>
             <x14:dxf>
               <font>
@@ -12115,7 +12120,7 @@
           <xm:sqref>C1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="116" id="{9549513C-FDD7-4320-B058-22B173685A4A}">
+          <x14:cfRule type="expression" priority="116" id="{B36DA600-2A60-48E7-9B50-37DDDB54485F}">
             <xm:f>AND((C2&lt;10),(C2&lt;&gt;solved!C2))</xm:f>
             <x14:dxf>
               <font>
@@ -12126,7 +12131,7 @@
           <xm:sqref>C2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="118" id="{8914A8D1-90A5-4EB6-B913-D2AB153037AF}">
+          <x14:cfRule type="expression" priority="118" id="{E768D9AD-8F1F-4EBD-B080-7FFF872D743C}">
             <xm:f>AND((C3&lt;10),(C3&lt;&gt;solved!C3))</xm:f>
             <x14:dxf>
               <font>
@@ -12137,7 +12142,7 @@
           <xm:sqref>C3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="120" id="{A0989249-D0E1-48BA-BD7D-34B8DA80A7F0}">
+          <x14:cfRule type="expression" priority="120" id="{15D9F02D-6A81-4D68-B320-C2F6E654D522}">
             <xm:f>AND((C4&lt;10),(C4&lt;&gt;solved!C4))</xm:f>
             <x14:dxf>
               <font>
@@ -12148,7 +12153,7 @@
           <xm:sqref>C4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="122" id="{C184F182-708F-4558-8CA3-EB72A38EDA7B}">
+          <x14:cfRule type="expression" priority="122" id="{1A644C35-21C9-496F-AF6E-D24BDF40B03A}">
             <xm:f>AND((C5&lt;10),(C5&lt;&gt;solved!C5))</xm:f>
             <x14:dxf>
               <font>
@@ -12159,7 +12164,7 @@
           <xm:sqref>C5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="124" id="{48C0EE32-2FD0-44F2-A7F7-49CDD0A22B67}">
+          <x14:cfRule type="expression" priority="124" id="{EF1E1EAD-47E9-44F0-8049-7842236ACB44}">
             <xm:f>AND((C6&lt;10),(C6&lt;&gt;solved!C6))</xm:f>
             <x14:dxf>
               <font>
@@ -12170,7 +12175,7 @@
           <xm:sqref>C6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="126" id="{70B0F74A-10AA-4379-9848-BB33B3A97616}">
+          <x14:cfRule type="expression" priority="126" id="{4080516F-C26B-4C7C-81B3-204D7049D25B}">
             <xm:f>AND((C7&lt;10),(C7&lt;&gt;solved!C7))</xm:f>
             <x14:dxf>
               <font>
@@ -12181,7 +12186,7 @@
           <xm:sqref>C7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="128" id="{D0CC556D-BE74-40E3-BA28-892751E77838}">
+          <x14:cfRule type="expression" priority="128" id="{948AA4C9-6B2B-4AAB-B6D5-C1B977690067}">
             <xm:f>AND((C8&lt;10),(C8&lt;&gt;solved!C8))</xm:f>
             <x14:dxf>
               <font>
@@ -12192,7 +12197,7 @@
           <xm:sqref>C8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="130" id="{809D38E9-CE26-4DBF-8BF7-15767C95A3A4}">
+          <x14:cfRule type="expression" priority="130" id="{65CB6F13-AB86-4BFC-8A57-D9AC4AED50F9}">
             <xm:f>AND((C9&lt;10),(C9&lt;&gt;solved!C9))</xm:f>
             <x14:dxf>
               <font>
@@ -12203,7 +12208,7 @@
           <xm:sqref>C9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="132" id="{46741ECC-6632-426E-B631-471553163956}">
+          <x14:cfRule type="expression" priority="132" id="{7C4F41CE-70E0-4111-AEE9-926D2560F023}">
             <xm:f>AND((D1&lt;10),(D1&lt;&gt;solved!D1))</xm:f>
             <x14:dxf>
               <font>
@@ -12214,7 +12219,7 @@
           <xm:sqref>D1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="134" id="{EE976B38-DDE6-4010-A9C7-FC9F8F1B439C}">
+          <x14:cfRule type="expression" priority="134" id="{DED4F0D2-8C70-4631-9B8D-6E3453C02350}">
             <xm:f>AND((D2&lt;10),(D2&lt;&gt;solved!D2))</xm:f>
             <x14:dxf>
               <font>
@@ -12225,7 +12230,7 @@
           <xm:sqref>D2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="136" id="{535EAC6F-BA74-4A4F-9E50-6437E056ACDD}">
+          <x14:cfRule type="expression" priority="136" id="{73F287A5-5C3F-417B-9C16-F9CEDF85AAF3}">
             <xm:f>AND((D3&lt;10),(D3&lt;&gt;solved!D3))</xm:f>
             <x14:dxf>
               <font>
@@ -12236,7 +12241,7 @@
           <xm:sqref>D3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="138" id="{3FA62970-CAC0-404F-833C-598A932CDB7C}">
+          <x14:cfRule type="expression" priority="138" id="{A9ACD475-4BA6-4228-A8F7-BB9B36C0B68D}">
             <xm:f>AND((D4&lt;10),(D4&lt;&gt;solved!D4))</xm:f>
             <x14:dxf>
               <font>
@@ -12247,7 +12252,7 @@
           <xm:sqref>D4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="140" id="{FA2266B4-5167-4F26-882C-29B0FBD27166}">
+          <x14:cfRule type="expression" priority="140" id="{B683DC1D-4DB4-41E0-BC4D-41A67DB8C8A5}">
             <xm:f>AND((D5&lt;10),(D5&lt;&gt;solved!D5))</xm:f>
             <x14:dxf>
               <font>
@@ -12258,7 +12263,7 @@
           <xm:sqref>D5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="142" id="{6DC8D020-2176-44E9-8CBC-A1A12C20907F}">
+          <x14:cfRule type="expression" priority="142" id="{B5537281-E0AE-4B4D-87F8-5A58A3A7724F}">
             <xm:f>AND((D6&lt;10),(D6&lt;&gt;solved!D6))</xm:f>
             <x14:dxf>
               <font>
@@ -12269,7 +12274,7 @@
           <xm:sqref>D6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="144" id="{31869CE7-4CAC-4C1B-8CF8-B0FF616DE1CE}">
+          <x14:cfRule type="expression" priority="144" id="{44AB8440-A375-43BB-8B80-123B7955BDBA}">
             <xm:f>AND((D7&lt;10),(D7&lt;&gt;solved!D7))</xm:f>
             <x14:dxf>
               <font>
@@ -12280,7 +12285,7 @@
           <xm:sqref>D7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="146" id="{BED380E4-2C9A-4940-B1AB-A156C6C0A7B0}">
+          <x14:cfRule type="expression" priority="146" id="{2CCF92F0-5FE6-431F-B3A0-2F7AC0B6F521}">
             <xm:f>AND((D8&lt;10),(D8&lt;&gt;solved!D8))</xm:f>
             <x14:dxf>
               <font>
@@ -12291,7 +12296,7 @@
           <xm:sqref>D8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="148" id="{B54A66C0-D18F-4F3E-98DC-1ACDADCAB16B}">
+          <x14:cfRule type="expression" priority="148" id="{2F51354B-A3B8-43A0-A1E6-9827C9294DCF}">
             <xm:f>AND((D9&lt;10),(D9&lt;&gt;solved!D9))</xm:f>
             <x14:dxf>
               <font>
@@ -12302,7 +12307,7 @@
           <xm:sqref>D9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="150" id="{63A3DE10-9B71-49EB-B979-33E0F59C29A6}">
+          <x14:cfRule type="expression" priority="150" id="{9C26CED9-B9AA-4060-9C2A-D420C121F08E}">
             <xm:f>AND((E1&lt;10),(E1&lt;&gt;solved!E1))</xm:f>
             <x14:dxf>
               <font>
@@ -12313,7 +12318,7 @@
           <xm:sqref>E1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="152" id="{FE47CF6D-B58D-4180-8C4E-43CABA19CE81}">
+          <x14:cfRule type="expression" priority="152" id="{10B85836-2943-454C-A2E2-89413AACB746}">
             <xm:f>AND((E2&lt;10),(E2&lt;&gt;solved!E2))</xm:f>
             <x14:dxf>
               <font>
@@ -12324,7 +12329,7 @@
           <xm:sqref>E2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="154" id="{B39050D5-4353-44B3-8A70-C7734AA2D1E1}">
+          <x14:cfRule type="expression" priority="154" id="{26131E92-ED5D-49E0-A9A0-10B2C0954ADA}">
             <xm:f>AND((E3&lt;10),(E3&lt;&gt;solved!E3))</xm:f>
             <x14:dxf>
               <font>
@@ -12335,7 +12340,7 @@
           <xm:sqref>E3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="156" id="{66A7464B-44F2-4EFF-88DA-37F9A6AD3EAB}">
+          <x14:cfRule type="expression" priority="156" id="{2627F490-D1FF-48FC-A12F-E5C3856174A8}">
             <xm:f>AND((E4&lt;10),(E4&lt;&gt;solved!E4))</xm:f>
             <x14:dxf>
               <font>
@@ -12346,7 +12351,7 @@
           <xm:sqref>E4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="158" id="{301B32C9-64E4-4283-B9B8-6EC500FD2465}">
+          <x14:cfRule type="expression" priority="158" id="{E943E350-DDEE-42A8-9750-60BF88686530}">
             <xm:f>AND((E5&lt;10),(E5&lt;&gt;solved!E5))</xm:f>
             <x14:dxf>
               <font>
@@ -12357,7 +12362,7 @@
           <xm:sqref>E5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="160" id="{C0FD88C4-F2D5-4DB2-9991-82DAB045EFFE}">
+          <x14:cfRule type="expression" priority="160" id="{C9812FF0-FB78-40EF-945D-B955DCDFEF12}">
             <xm:f>AND((E6&lt;10),(E6&lt;&gt;solved!E6))</xm:f>
             <x14:dxf>
               <font>
@@ -12368,7 +12373,7 @@
           <xm:sqref>E6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="162" id="{7BEA8E79-2887-41BC-8C2C-5E339A9CB3B3}">
+          <x14:cfRule type="expression" priority="162" id="{5A1BEA4B-BDC3-41DA-9A6E-504F9BA0D1F6}">
             <xm:f>AND((E7&lt;10),(E7&lt;&gt;solved!E7))</xm:f>
             <x14:dxf>
               <font>
@@ -12379,7 +12384,7 @@
           <xm:sqref>E7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="164" id="{D75DDB2C-54D1-4459-81C1-89A6A0E0808A}">
+          <x14:cfRule type="expression" priority="164" id="{60DECE9A-E593-47F0-A93E-CFEF3EF3D1F4}">
             <xm:f>AND((E8&lt;10),(E8&lt;&gt;solved!E8))</xm:f>
             <x14:dxf>
               <font>
@@ -12390,7 +12395,7 @@
           <xm:sqref>E8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="166" id="{8DCD1EE5-2BBC-4033-B86E-C4EFB73CBD78}">
+          <x14:cfRule type="expression" priority="166" id="{DEEF8E83-DA5B-4B69-BA9D-5E77EAED2987}">
             <xm:f>AND((E9&lt;10),(E9&lt;&gt;solved!E9))</xm:f>
             <x14:dxf>
               <font>
@@ -12401,7 +12406,7 @@
           <xm:sqref>E9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="168" id="{272E2BB2-39A3-4266-9DB7-F5AE3F76CFEC}">
+          <x14:cfRule type="expression" priority="168" id="{DC4E9AB5-C482-4A93-92CB-3A1AAE9AFEAC}">
             <xm:f>AND((F1&lt;10),(F1&lt;&gt;solved!F1))</xm:f>
             <x14:dxf>
               <font>
@@ -12412,7 +12417,7 @@
           <xm:sqref>F1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="170" id="{C2D6224F-F8EC-4C58-B5BE-8CA2721C9DC4}">
+          <x14:cfRule type="expression" priority="170" id="{E02D22D7-1F49-4BB2-86FB-DD352897B990}">
             <xm:f>AND((F2&lt;10),(F2&lt;&gt;solved!F2))</xm:f>
             <x14:dxf>
               <font>
@@ -12423,7 +12428,7 @@
           <xm:sqref>F2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="172" id="{3D6A9D74-89B7-4054-B6C9-F083626A8DBA}">
+          <x14:cfRule type="expression" priority="172" id="{402A3742-50A6-4055-9A13-865FCCE6486C}">
             <xm:f>AND((F3&lt;10),(F3&lt;&gt;solved!F3))</xm:f>
             <x14:dxf>
               <font>
@@ -12434,7 +12439,7 @@
           <xm:sqref>F3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="174" id="{C96B307E-742C-46DB-8471-66FBE75DAE35}">
+          <x14:cfRule type="expression" priority="174" id="{40C85853-3353-4BB4-82C4-E09025BA8EB9}">
             <xm:f>AND((F4&lt;10),(F4&lt;&gt;solved!F4))</xm:f>
             <x14:dxf>
               <font>
@@ -12445,7 +12450,7 @@
           <xm:sqref>F4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="176" id="{E457F6AB-7EC8-4BE8-998F-3295FC3F3953}">
+          <x14:cfRule type="expression" priority="176" id="{A094D0DB-E93B-4416-B740-521750CFF0D4}">
             <xm:f>AND((F5&lt;10),(F5&lt;&gt;solved!F5))</xm:f>
             <x14:dxf>
               <font>
@@ -12456,7 +12461,7 @@
           <xm:sqref>F5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="178" id="{4FEF504B-9BF3-4D1E-A267-FCF82F5A4664}">
+          <x14:cfRule type="expression" priority="178" id="{842B2540-F054-4B6A-A1A9-1CE3679E4195}">
             <xm:f>AND((F6&lt;10),(F6&lt;&gt;solved!F6))</xm:f>
             <x14:dxf>
               <font>
@@ -12467,7 +12472,7 @@
           <xm:sqref>F6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="180" id="{A8793041-F460-4EDF-8EE3-B4DDC6EBED10}">
+          <x14:cfRule type="expression" priority="180" id="{27E07BB6-35E3-4F40-BA89-29E1F73843FB}">
             <xm:f>AND((F7&lt;10),(F7&lt;&gt;solved!F7))</xm:f>
             <x14:dxf>
               <font>
@@ -12478,7 +12483,7 @@
           <xm:sqref>F7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="182" id="{A43D6BC6-C7C4-4D46-97BE-E2ADEDF9305E}">
+          <x14:cfRule type="expression" priority="182" id="{3D815949-C5F0-4056-AA76-CF9BF51D84CA}">
             <xm:f>AND((F8&lt;10),(F8&lt;&gt;solved!F8))</xm:f>
             <x14:dxf>
               <font>
@@ -12489,7 +12494,7 @@
           <xm:sqref>F8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="184" id="{F9E0C6A3-DF7E-4B7A-BAB3-EFCAC9D3B9C0}">
+          <x14:cfRule type="expression" priority="184" id="{59655A37-2349-4237-ABDF-8179C16C63F9}">
             <xm:f>AND((F9&lt;10),(F9&lt;&gt;solved!F9))</xm:f>
             <x14:dxf>
               <font>
@@ -12500,7 +12505,7 @@
           <xm:sqref>F9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="186" id="{E416133D-4F68-4E89-A344-6863437E00F2}">
+          <x14:cfRule type="expression" priority="186" id="{C03DA796-9D55-4E1F-9BF9-2ADE3F57F24D}">
             <xm:f>AND((G1&lt;10),(G1&lt;&gt;solved!G1))</xm:f>
             <x14:dxf>
               <font>
@@ -12511,7 +12516,7 @@
           <xm:sqref>G1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="188" id="{90ADCE10-95B4-4783-A5C4-4AAF2A8FC270}">
+          <x14:cfRule type="expression" priority="188" id="{42442B2D-3D80-456B-BF74-A91AE6313462}">
             <xm:f>AND((G2&lt;10),(G2&lt;&gt;solved!G2))</xm:f>
             <x14:dxf>
               <font>
@@ -12522,7 +12527,7 @@
           <xm:sqref>G2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="190" id="{E442FFFB-2DCE-44C0-8F40-B7FB6F9F238F}">
+          <x14:cfRule type="expression" priority="190" id="{B0A420F0-E140-436F-BA54-BD8B57E04052}">
             <xm:f>AND((G3&lt;10),(G3&lt;&gt;solved!G3))</xm:f>
             <x14:dxf>
               <font>
@@ -12533,7 +12538,7 @@
           <xm:sqref>G3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="192" id="{2193AE29-5639-4911-BDD0-2B489C4845D5}">
+          <x14:cfRule type="expression" priority="192" id="{C4143533-F5DB-4894-8870-8C20104A40B5}">
             <xm:f>AND((G4&lt;10),(G4&lt;&gt;solved!G4))</xm:f>
             <x14:dxf>
               <font>
@@ -12544,7 +12549,7 @@
           <xm:sqref>G4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="194" id="{73342276-5AA6-4031-A3A7-6B718B41858E}">
+          <x14:cfRule type="expression" priority="194" id="{E3FFC3E8-547F-4258-96B6-D19C48801950}">
             <xm:f>AND((G5&lt;10),(G5&lt;&gt;solved!G5))</xm:f>
             <x14:dxf>
               <font>
@@ -12555,7 +12560,7 @@
           <xm:sqref>G5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="196" id="{3BCAD598-B4AA-44AF-B4B3-F3AB41FF99DE}">
+          <x14:cfRule type="expression" priority="196" id="{F26C5C44-9175-4912-8A8D-CB692C723131}">
             <xm:f>AND((G6&lt;10),(G6&lt;&gt;solved!G6))</xm:f>
             <x14:dxf>
               <font>
@@ -12566,7 +12571,7 @@
           <xm:sqref>G6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="198" id="{94FAC6B9-7027-4FE8-A99F-61A8CEA9B085}">
+          <x14:cfRule type="expression" priority="198" id="{C4FDC051-A7E3-4695-A29A-AECC22D5F97F}">
             <xm:f>AND((G7&lt;10),(G7&lt;&gt;solved!G7))</xm:f>
             <x14:dxf>
               <font>
@@ -12577,7 +12582,7 @@
           <xm:sqref>G7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="200" id="{4E3F713B-5DBC-4B5D-AEAF-26B95EBE7FC2}">
+          <x14:cfRule type="expression" priority="200" id="{40B63368-794F-4130-9077-6588CC71DF42}">
             <xm:f>AND((G8&lt;10),(G8&lt;&gt;solved!G8))</xm:f>
             <x14:dxf>
               <font>
@@ -12588,7 +12593,7 @@
           <xm:sqref>G8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="202" id="{53BB9C43-434A-46C4-B752-9AD0CB22FEF8}">
+          <x14:cfRule type="expression" priority="202" id="{4ED47FFC-DAA5-4F00-B3F1-C364A514B0EC}">
             <xm:f>AND((G9&lt;10),(G9&lt;&gt;solved!G9))</xm:f>
             <x14:dxf>
               <font>
@@ -12599,7 +12604,7 @@
           <xm:sqref>G9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="204" id="{845CCBBF-86F6-4D80-B3FD-E5A8107FB680}">
+          <x14:cfRule type="expression" priority="204" id="{C7AA4172-5035-4BDC-A179-2980B1D8899D}">
             <xm:f>AND((H1&lt;10),(H1&lt;&gt;solved!H1))</xm:f>
             <x14:dxf>
               <font>
@@ -12610,7 +12615,7 @@
           <xm:sqref>H1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="207" id="{EF3CAD50-68D4-4053-A5E4-5D19FC4010DC}">
+          <x14:cfRule type="expression" priority="207" id="{6A92751A-B820-49E4-AA97-D0E988B4D0AA}">
             <xm:f>AND((H2&lt;10),(H2&lt;&gt;solved!H2))</xm:f>
             <x14:dxf>
               <font>
@@ -12621,7 +12626,7 @@
           <xm:sqref>H2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="209" id="{625847D5-134E-44F6-A3EE-FF2E4A7E9BDC}">
+          <x14:cfRule type="expression" priority="209" id="{FCAF241A-197E-4D45-B63A-4F5BC050EF35}">
             <xm:f>AND((H3&lt;10),(H3&lt;&gt;solved!H3))</xm:f>
             <x14:dxf>
               <font>
@@ -12632,7 +12637,7 @@
           <xm:sqref>H3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="211" id="{9C78FA52-A893-4353-966C-7CCCE4953BCE}">
+          <x14:cfRule type="expression" priority="211" id="{DAC5409A-A55A-4DCC-BF38-E8707D97732F}">
             <xm:f>AND((H4&lt;10),(H4&lt;&gt;solved!H4))</xm:f>
             <x14:dxf>
               <font>
@@ -12643,7 +12648,7 @@
           <xm:sqref>H4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="213" id="{7BC06048-D5A5-4468-80CB-2F4ADBC3BAA0}">
+          <x14:cfRule type="expression" priority="213" id="{407933B1-7D55-4EBD-8B15-CB5CF078304C}">
             <xm:f>AND((H5&lt;10),(H5&lt;&gt;solved!H5))</xm:f>
             <x14:dxf>
               <font>
@@ -12654,7 +12659,7 @@
           <xm:sqref>H5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="215" id="{E54981B2-6FD6-405E-B2C0-50ABADFF9A71}">
+          <x14:cfRule type="expression" priority="215" id="{86FC9482-2BB1-4619-8F60-E0A2C69464D2}">
             <xm:f>AND((H6&lt;10),(H6&lt;&gt;solved!H6))</xm:f>
             <x14:dxf>
               <font>
@@ -12665,7 +12670,7 @@
           <xm:sqref>H6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="217" id="{ECB0C894-2010-4A30-80DB-77D800DCC065}">
+          <x14:cfRule type="expression" priority="217" id="{403CDB2E-D3A0-4041-B05B-4A5CDCB17A62}">
             <xm:f>AND((H7&lt;10),(H7&lt;&gt;solved!H7))</xm:f>
             <x14:dxf>
               <font>
@@ -12676,7 +12681,7 @@
           <xm:sqref>H7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="219" id="{77A86400-2B37-4C72-9C88-44A7351E2C55}">
+          <x14:cfRule type="expression" priority="219" id="{EFB8A170-40ED-41AE-B53A-A0AD338C8781}">
             <xm:f>AND((H8&lt;10),(H8&lt;&gt;solved!H8))</xm:f>
             <x14:dxf>
               <font>
@@ -12687,7 +12692,7 @@
           <xm:sqref>H8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="221" id="{503DE42D-421A-4BE0-B645-AE5B4EBBE8F7}">
+          <x14:cfRule type="expression" priority="221" id="{EC3095E0-6633-4055-8871-E0FAB956EBEF}">
             <xm:f>AND((H9&lt;10),(H9&lt;&gt;solved!H9))</xm:f>
             <x14:dxf>
               <font>
@@ -12698,7 +12703,7 @@
           <xm:sqref>H9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="223" id="{4A708150-6F9A-4F53-B950-F589738BD3CB}">
+          <x14:cfRule type="expression" priority="223" id="{8FC7EBAD-B428-4933-A520-D17627861E14}">
             <xm:f>AND((I1&lt;10),(I1&lt;&gt;solved!I1))</xm:f>
             <x14:dxf>
               <font>
@@ -12709,7 +12714,7 @@
           <xm:sqref>I1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="225" id="{BB2DCBCD-49EB-4370-A2F3-C0112BCC26AE}">
+          <x14:cfRule type="expression" priority="225" id="{BECCE285-568F-4927-8C1B-90B697D4C4E7}">
             <xm:f>AND((I2&lt;10),(I2&lt;&gt;solved!I2))</xm:f>
             <x14:dxf>
               <font>
@@ -12720,7 +12725,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="227" id="{9013D9E9-2823-4EE6-A3E8-27FB4D3FCB5D}">
+          <x14:cfRule type="expression" priority="227" id="{C162B62C-30CC-46AB-A33A-28D5C95D36B7}">
             <xm:f>AND((I3&lt;10),(I3&lt;&gt;solved!I3))</xm:f>
             <x14:dxf>
               <font>
@@ -12731,7 +12736,7 @@
           <xm:sqref>I3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="229" id="{2F2F1538-D7EC-40F5-A17C-22C02699F129}">
+          <x14:cfRule type="expression" priority="229" id="{621A24C8-17F5-45D3-B32D-57293020CFC8}">
             <xm:f>AND((I4&lt;10),(I4&lt;&gt;solved!I4))</xm:f>
             <x14:dxf>
               <font>
@@ -12742,7 +12747,7 @@
           <xm:sqref>I4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="231" id="{D7C1902D-F935-42E4-8166-48C5EDD7E9F4}">
+          <x14:cfRule type="expression" priority="231" id="{6C14E1BA-3073-4C70-99D9-5A8B9B1358C3}">
             <xm:f>AND((I5&lt;10),(I5&lt;&gt;solved!I5))</xm:f>
             <x14:dxf>
               <font>
@@ -12753,7 +12758,7 @@
           <xm:sqref>I5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="233" id="{3E30C52C-F530-471E-87AB-1276202570AF}">
+          <x14:cfRule type="expression" priority="233" id="{F8DA2D40-8A31-4BD8-8A70-275EB5158B60}">
             <xm:f>AND((I6&lt;10),(I6&lt;&gt;solved!I6))</xm:f>
             <x14:dxf>
               <font>
@@ -12764,7 +12769,7 @@
           <xm:sqref>I6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="235" id="{601E5A4F-B0A4-41E9-9A4E-60903097DCED}">
+          <x14:cfRule type="expression" priority="235" id="{61ACC6B7-97CB-4519-8A8B-FCBCD61BF6F2}">
             <xm:f>AND((I7&lt;10),(I7&lt;&gt;solved!I7))</xm:f>
             <x14:dxf>
               <font>
@@ -12775,7 +12780,7 @@
           <xm:sqref>I7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="237" id="{8A12BFD2-5480-4DE7-9523-5F74953EC0DD}">
+          <x14:cfRule type="expression" priority="237" id="{C9E1E2E7-8A9B-4AE5-8AD0-955E90AC1662}">
             <xm:f>AND((I8&lt;10),(I8&lt;&gt;solved!I8))</xm:f>
             <x14:dxf>
               <font>
@@ -12786,7 +12791,7 @@
           <xm:sqref>I8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="239" id="{B25FE0C5-F3B2-46AA-A076-7ACB55E08EF4}">
+          <x14:cfRule type="expression" priority="239" id="{C8A6A08F-5D9D-4340-AF90-8FB4D31DAE53}">
             <xm:f>AND((I9&lt;10),(I9&lt;&gt;solved!I9))</xm:f>
             <x14:dxf>
               <font>
@@ -12797,7 +12802,7 @@
           <xm:sqref>I9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="242" id="{EE148AEF-B731-4522-8347-685027203FE7}">
+          <x14:cfRule type="expression" priority="242" id="{A0CE263D-3B3F-40E0-BC40-6B5FD225AC51}">
             <xm:f>AND((J2&lt;10),(J2&lt;&gt;solved!J2))</xm:f>
             <x14:dxf>
               <font>
@@ -12808,7 +12813,7 @@
           <xm:sqref>J2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="244" id="{2682B2AF-70A5-41F7-ADD6-7678C1E42435}">
+          <x14:cfRule type="expression" priority="244" id="{C75656C6-6D33-48A6-8167-D090DBFF56C9}">
             <xm:f>AND((J3&lt;10),(J3&lt;&gt;solved!J3))</xm:f>
             <x14:dxf>
               <font>
@@ -12819,7 +12824,7 @@
           <xm:sqref>J3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="246" id="{46268E1E-5C46-44BB-B9AD-EF652BC6A467}">
+          <x14:cfRule type="expression" priority="246" id="{A1C23B17-1713-4946-8E92-7937F24A9DBD}">
             <xm:f>AND((J4&lt;10),(J4&lt;&gt;solved!J4))</xm:f>
             <x14:dxf>
               <font>
@@ -12830,7 +12835,7 @@
           <xm:sqref>J4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="249" id="{8D7031BB-B7F5-4B8E-95AF-DE30E8D18871}">
+          <x14:cfRule type="expression" priority="249" id="{E43F70CD-C6C2-4DDB-9CE3-F629474D4A34}">
             <xm:f>AND((J5&lt;10),(J5&lt;&gt;solved!J5))</xm:f>
             <x14:dxf>
               <font>
@@ -12841,7 +12846,7 @@
           <xm:sqref>J5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="251" id="{554A3BBB-321E-45A0-8674-C229D0C75BF3}">
+          <x14:cfRule type="expression" priority="251" id="{4A16B8C8-D161-4F13-8A24-679D3AD23F00}">
             <xm:f>AND((J6&lt;10),(J6&lt;&gt;solved!J6))</xm:f>
             <x14:dxf>
               <font>
@@ -12852,7 +12857,7 @@
           <xm:sqref>J6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="253" id="{807084FF-8B68-4F55-981E-2BA6ACA76CA8}">
+          <x14:cfRule type="expression" priority="253" id="{AA6C1B8F-4448-427F-85DD-5133E8551BC0}">
             <xm:f>AND((J7&lt;10),(J7&lt;&gt;solved!J7))</xm:f>
             <x14:dxf>
               <font>
@@ -12863,7 +12868,7 @@
           <xm:sqref>J7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="255" id="{3415A43B-E39E-4994-A099-81693F4AA663}">
+          <x14:cfRule type="expression" priority="255" id="{F588F359-3C69-4375-8D94-264BBDE23540}">
             <xm:f>AND((J8&lt;10),(J8&lt;&gt;solved!J8))</xm:f>
             <x14:dxf>
               <font>
@@ -12874,7 +12879,7 @@
           <xm:sqref>J8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="257" id="{339E74AF-1C88-4214-9D65-438F291736F3}">
+          <x14:cfRule type="expression" priority="257" id="{BDBDB1B5-FBC5-4097-A48F-343E901B901D}">
             <xm:f>AND((J9&lt;10),(J9&lt;&gt;solved!J9))</xm:f>
             <x14:dxf>
               <font>
@@ -13180,9 +13185,9 @@
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="15"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="16"/>
+      <c r="G10" s="17"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -13288,108 +13293,108 @@
       <c r="J20" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="17" t="n">
+      <c r="C22" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="17" t="n">
+      <c r="D22" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="17" t="n">
+      <c r="E22" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="17" t="n">
+      <c r="F22" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="17" t="n">
+      <c r="G22" s="18" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="17" t="n">
+      <c r="B23" s="18" t="n">
         <v>15</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18" t="n">
+      <c r="C23" s="19"/>
+      <c r="D23" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18" t="n">
+      <c r="E23" s="19"/>
+      <c r="F23" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G23" s="18" t="n">
+      <c r="G23" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="17" t="n">
+      <c r="B24" s="18" t="n">
         <v>35</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18" t="n">
+      <c r="C24" s="19"/>
+      <c r="D24" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18" t="n">
+      <c r="E24" s="19"/>
+      <c r="F24" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G24" s="18" t="n">
+      <c r="G24" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="17" t="n">
+      <c r="B25" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="C25" s="19" t="n">
+      <c r="C25" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="18" t="n">
+      <c r="D25" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18" t="n">
+      <c r="E25" s="19"/>
+      <c r="F25" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G25" s="18" t="n">
+      <c r="G25" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="17" t="n">
+      <c r="B26" s="18" t="n">
         <v>75</v>
       </c>
-      <c r="C26" s="18" t="n">
+      <c r="C26" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18" t="n">
+      <c r="D26" s="19"/>
+      <c r="E26" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="19" t="n">
+      <c r="F26" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G26" s="19" t="n">
+      <c r="G26" s="20" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="17" t="n">
+      <c r="B27" s="18" t="n">
         <v>95</v>
       </c>
-      <c r="C27" s="18" t="n">
+      <c r="C27" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18" t="n">
+      <c r="D27" s="19"/>
+      <c r="E27" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="F27" s="19" t="n">
+      <c r="F27" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="18"/>
+      <c r="G27" s="19"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B10">
@@ -13889,9 +13894,9 @@
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="15"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="16"/>
+      <c r="G10" s="17"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -13997,108 +14002,108 @@
       <c r="J20" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="17" t="n">
+      <c r="C22" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="17" t="n">
+      <c r="D22" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="17" t="n">
+      <c r="E22" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="17" t="n">
+      <c r="F22" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="17" t="n">
+      <c r="G22" s="18" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="17" t="n">
+      <c r="B23" s="18" t="n">
         <v>15</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18" t="n">
+      <c r="C23" s="19"/>
+      <c r="D23" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18" t="n">
+      <c r="E23" s="19"/>
+      <c r="F23" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G23" s="18" t="n">
+      <c r="G23" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="17" t="n">
+      <c r="B24" s="18" t="n">
         <v>35</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18" t="n">
+      <c r="C24" s="19"/>
+      <c r="D24" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18" t="n">
+      <c r="E24" s="19"/>
+      <c r="F24" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G24" s="18" t="n">
+      <c r="G24" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="17" t="n">
+      <c r="B25" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="C25" s="19" t="n">
+      <c r="C25" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="18" t="n">
+      <c r="D25" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18" t="n">
+      <c r="E25" s="19"/>
+      <c r="F25" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G25" s="18" t="n">
+      <c r="G25" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="17" t="n">
+      <c r="B26" s="18" t="n">
         <v>75</v>
       </c>
-      <c r="C26" s="18" t="n">
+      <c r="C26" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18" t="n">
+      <c r="D26" s="19"/>
+      <c r="E26" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="19" t="n">
+      <c r="F26" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G26" s="19" t="n">
+      <c r="G26" s="20" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="17" t="n">
+      <c r="B27" s="18" t="n">
         <v>95</v>
       </c>
-      <c r="C27" s="18" t="n">
+      <c r="C27" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18" t="n">
+      <c r="D27" s="19"/>
+      <c r="E27" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="F27" s="19" t="n">
+      <c r="F27" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="18"/>
+      <c r="G27" s="19"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B10">
@@ -14442,7 +14447,7 @@
       <c r="U1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20"/>
+      <c r="A2" s="21"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
       <c r="D2" s="9"/>
@@ -14468,7 +14473,7 @@
       <c r="U2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="11"/>
       <c r="C3" s="12"/>
       <c r="D3" s="13"/>
@@ -14490,7 +14495,7 @@
       <c r="U3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="n">
         <v>6</v>
@@ -14520,7 +14525,7 @@
       <c r="U4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="7"/>
@@ -14549,7 +14554,7 @@
       <c r="U5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="20"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
@@ -14571,7 +14576,7 @@
       <c r="U6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="20"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
@@ -14593,7 +14598,7 @@
       <c r="U7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8" t="n">
         <v>6</v>
@@ -14619,7 +14624,7 @@
       <c r="U8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="11"/>
       <c r="C9" s="12"/>
       <c r="D9" s="13" t="n">
@@ -14647,13 +14652,13 @@
       <c r="U9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="15"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="16"/>
+      <c r="G10" s="17"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -14759,113 +14764,113 @@
       <c r="J20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="21" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="17" t="n">
+      <c r="C22" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="17" t="n">
+      <c r="D22" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="17" t="n">
+      <c r="E22" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="17" t="n">
+      <c r="F22" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="17" t="n">
+      <c r="G22" s="18" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="17" t="n">
+      <c r="B23" s="18" t="n">
         <v>15</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18" t="n">
+      <c r="C23" s="19"/>
+      <c r="D23" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18" t="n">
+      <c r="E23" s="19"/>
+      <c r="F23" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G23" s="18" t="n">
+      <c r="G23" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="17" t="n">
+      <c r="B24" s="18" t="n">
         <v>35</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18" t="n">
+      <c r="C24" s="19"/>
+      <c r="D24" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18" t="n">
+      <c r="E24" s="19"/>
+      <c r="F24" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G24" s="18" t="n">
+      <c r="G24" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="17" t="n">
+      <c r="B25" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="C25" s="19" t="n">
+      <c r="C25" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="18" t="n">
+      <c r="D25" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18" t="n">
+      <c r="E25" s="19"/>
+      <c r="F25" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G25" s="18" t="n">
+      <c r="G25" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="17" t="n">
+      <c r="B26" s="18" t="n">
         <v>75</v>
       </c>
-      <c r="C26" s="18" t="n">
+      <c r="C26" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18" t="n">
+      <c r="D26" s="19"/>
+      <c r="E26" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="19" t="n">
+      <c r="F26" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G26" s="19" t="n">
+      <c r="G26" s="20" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="17" t="n">
+      <c r="B27" s="18" t="n">
         <v>95</v>
       </c>
-      <c r="C27" s="18" t="n">
+      <c r="C27" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18" t="n">
+      <c r="D27" s="19"/>
+      <c r="E27" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="F27" s="19" t="n">
+      <c r="F27" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="18"/>
+      <c r="G27" s="19"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B10">
@@ -15195,22 +15200,22 @@
       <c r="R2" s="7"/>
       <c r="S2" s="8"/>
       <c r="T2" s="9"/>
-      <c r="U2" s="17" t="s">
+      <c r="U2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="V2" s="17" t="n">
+      <c r="V2" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="W2" s="17" t="n">
+      <c r="W2" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="X2" s="17" t="n">
+      <c r="X2" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="Y2" s="17" t="n">
+      <c r="Y2" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="Z2" s="17" t="n">
+      <c r="Z2" s="18" t="n">
         <v>9</v>
       </c>
     </row>
@@ -15239,18 +15244,18 @@
       <c r="R3" s="11"/>
       <c r="S3" s="12"/>
       <c r="T3" s="13"/>
-      <c r="U3" s="17" t="n">
+      <c r="U3" s="18" t="n">
         <v>15</v>
       </c>
-      <c r="V3" s="18"/>
-      <c r="W3" s="21" t="n">
+      <c r="V3" s="19"/>
+      <c r="W3" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="X3" s="18"/>
-      <c r="Y3" s="21" t="n">
+      <c r="X3" s="19"/>
+      <c r="Y3" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="Z3" s="21" t="n">
+      <c r="Z3" s="22" t="n">
         <v>9</v>
       </c>
     </row>
@@ -15283,18 +15288,18 @@
       <c r="R4" s="2"/>
       <c r="S4" s="3"/>
       <c r="T4" s="4"/>
-      <c r="U4" s="17" t="n">
+      <c r="U4" s="18" t="n">
         <v>35</v>
       </c>
-      <c r="V4" s="18"/>
-      <c r="W4" s="21" t="n">
+      <c r="V4" s="19"/>
+      <c r="W4" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="21" t="n">
+      <c r="X4" s="19"/>
+      <c r="Y4" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="Z4" s="21" t="n">
+      <c r="Z4" s="22" t="n">
         <v>9</v>
       </c>
     </row>
@@ -15339,20 +15344,20 @@
       <c r="R5" s="7"/>
       <c r="S5" s="8"/>
       <c r="T5" s="9"/>
-      <c r="U5" s="17" t="n">
+      <c r="U5" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="V5" s="19" t="n">
+      <c r="V5" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="W5" s="21" t="n">
+      <c r="W5" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="X5" s="18"/>
-      <c r="Y5" s="21" t="n">
+      <c r="X5" s="19"/>
+      <c r="Y5" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="Z5" s="21" t="n">
+      <c r="Z5" s="22" t="n">
         <v>9</v>
       </c>
     </row>
@@ -15387,20 +15392,20 @@
       <c r="R6" s="11"/>
       <c r="S6" s="12"/>
       <c r="T6" s="13"/>
-      <c r="U6" s="17" t="n">
+      <c r="U6" s="18" t="n">
         <v>75</v>
       </c>
-      <c r="V6" s="18" t="n">
+      <c r="V6" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="W6" s="18"/>
-      <c r="X6" s="18" t="n">
+      <c r="W6" s="19"/>
+      <c r="X6" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="Y6" s="19" t="n">
+      <c r="Y6" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="Z6" s="19" t="n">
+      <c r="Z6" s="20" t="n">
         <v>9</v>
       </c>
     </row>
@@ -15429,20 +15434,20 @@
       <c r="R7" s="2"/>
       <c r="S7" s="3"/>
       <c r="T7" s="4"/>
-      <c r="U7" s="17" t="n">
+      <c r="U7" s="18" t="n">
         <v>95</v>
       </c>
-      <c r="V7" s="18" t="n">
+      <c r="V7" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18" t="n">
+      <c r="W7" s="19"/>
+      <c r="X7" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="Y7" s="19" t="n">
+      <c r="Y7" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="Z7" s="18"/>
+      <c r="Z7" s="19"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="7" t="s">
@@ -15504,7 +15509,7 @@
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="9"/>
-      <c r="E10" s="22"/>
+      <c r="E10" s="23"/>
       <c r="F10" s="8"/>
       <c r="H10" s="7"/>
       <c r="I10" s="8"/>
@@ -15893,45 +15898,45 @@
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="8"/>
-      <c r="F2" s="26" t="n">
+      <c r="F2" s="27" t="n">
         <v>8</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="28" t="n">
+      <c r="G2" s="28"/>
+      <c r="H2" s="29" t="n">
         <v>3</v>
       </c>
       <c r="I2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="11"/>
-      <c r="B3" s="29"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="30" t="n">
+      <c r="D3" s="31" t="n">
         <v>5</v>
       </c>
       <c r="E3" s="12"/>
-      <c r="F3" s="31"/>
+      <c r="F3" s="32"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="32"/>
+      <c r="H3" s="33"/>
       <c r="I3" s="13" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="35"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="36"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="36" t="n">
+      <c r="F4" s="37" t="n">
         <v>4</v>
       </c>
-      <c r="G4" s="37"/>
-      <c r="H4" s="38" t="n">
+      <c r="G4" s="38"/>
+      <c r="H4" s="39" t="n">
         <v>1</v>
       </c>
       <c r="I4" s="4"/>
@@ -15949,47 +15954,47 @@
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="11"/>
-      <c r="B6" s="39"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="41" t="n">
+      <c r="B6" s="40"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="42" t="n">
         <v>7</v>
       </c>
       <c r="E6" s="12"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="44"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="45"/>
       <c r="I6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
-      <c r="B7" s="45" t="n">
+      <c r="B7" s="46" t="n">
         <v>8</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="46"/>
+      <c r="D7" s="47"/>
       <c r="E7" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="F7" s="47"/>
+      <c r="F7" s="48"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="48"/>
+      <c r="H7" s="49"/>
       <c r="I7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="50" t="n">
+      <c r="B8" s="50"/>
+      <c r="C8" s="51" t="n">
         <v>9</v>
       </c>
-      <c r="D8" s="51"/>
+      <c r="D8" s="52"/>
       <c r="E8" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="52"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="54" t="n">
+      <c r="F8" s="53"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="55" t="n">
         <v>7</v>
       </c>
       <c r="I8" s="9"/>

</xml_diff>

<commit_message>
all working, except creation buddy list not flexible for correct box and too many prints
</commit_message>
<xml_diff>
--- a/data/SDK.xlsx
+++ b/data/SDK.xlsx
@@ -96,10 +96,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
-    <numFmt numFmtId="166" formatCode="#,##0"/>
+    <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -508,7 +507,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -565,7 +564,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -573,7 +580,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -601,7 +608,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7503,7 +7510,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7675,7 +7682,7 @@
       <c r="I5" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="K5" s="14" t="n">
+      <c r="K5" s="10" t="n">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "5")=9, 5, "")</f>
         <v>5</v>
       </c>
@@ -7807,7 +7814,7 @@
       <c r="I9" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="K9" s="15" t="str">
+      <c r="K9" s="14" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "9")=9, 9, "")</f>
         <v/>
       </c>
@@ -8149,7 +8156,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="110" id="{6351BE87-CE99-4FB4-B2BA-302DE1B7A6F5}">
+          <x14:cfRule type="expression" priority="110" id="{753D30A5-1ADC-4085-927E-889966503F50}">
             <xm:f>AND((A2&lt;10),(A2&lt;&gt;solved!A2))</xm:f>
             <x14:dxf>
               <font>
@@ -8165,7 +8172,7 @@
           <xm:sqref>A2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="111" id="{D818F26E-E4AF-49E5-9B4C-A4DC60882353}">
+          <x14:cfRule type="expression" priority="111" id="{AD75D7E4-744B-4BAC-B629-7BF04DC4E158}">
             <xm:f>AND((A3&lt;10),(A3&lt;&gt;solved!A3))</xm:f>
             <x14:dxf>
               <font>
@@ -8176,7 +8183,7 @@
           <xm:sqref>A3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="112" id="{49EBE05F-7A44-4240-BDF2-FE551EFCC411}">
+          <x14:cfRule type="expression" priority="112" id="{11243AC7-B089-4F6A-9917-5B1CD624F42E}">
             <xm:f>AND((A5&lt;10),(A5&lt;&gt;solved!A5))</xm:f>
             <x14:dxf>
               <font>
@@ -8187,7 +8194,7 @@
           <xm:sqref>A5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="113" id="{FE72E9BC-C38C-49C0-90D0-6D7A10153D5C}">
+          <x14:cfRule type="expression" priority="113" id="{00482B8A-AD36-46CD-A3AE-A32851E03AE6}">
             <xm:f>AND((A6&lt;10),(A6&lt;&gt;solved!A6))</xm:f>
             <x14:dxf>
               <font>
@@ -8198,7 +8205,7 @@
           <xm:sqref>A6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="114" id="{87B1441E-C4DE-46B8-B2F6-1BE0512E6125}">
+          <x14:cfRule type="expression" priority="114" id="{374C92A7-F600-4F50-B214-E5FBBD2FCA16}">
             <xm:f>AND((A7&lt;10),(A7&lt;&gt;solved!A7))</xm:f>
             <x14:dxf>
               <font>
@@ -8209,7 +8216,7 @@
           <xm:sqref>A7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="115" id="{441495E0-C33E-4DD9-85E3-EC43457EA524}">
+          <x14:cfRule type="expression" priority="115" id="{2E4E88AD-D9EE-4689-B854-649C70548010}">
             <xm:f>AND((A8&lt;10),(A8&lt;&gt;solved!A8))</xm:f>
             <x14:dxf>
               <font>
@@ -8220,7 +8227,7 @@
           <xm:sqref>A8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="116" id="{0077F593-20D6-4034-AC57-5038B3C5E070}">
+          <x14:cfRule type="expression" priority="116" id="{9E50F0E4-207A-4339-8291-9F911956DC20}">
             <xm:f>AND((A9&lt;10),(A9&lt;&gt;solved!A9))</xm:f>
             <x14:dxf>
               <font>
@@ -8231,7 +8238,7 @@
           <xm:sqref>A9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="117" id="{171DD56F-3163-4472-B565-58C47E8DEB18}">
+          <x14:cfRule type="expression" priority="117" id="{7B4FA8ED-C714-47B4-9DB7-F8B780964C5D}">
             <xm:f>AND((B1&lt;10),(B1&lt;&gt;solved!B1))</xm:f>
             <x14:dxf>
               <font>
@@ -8242,7 +8249,7 @@
           <xm:sqref>B1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="118" id="{73527E9A-18AA-48F6-A027-B48840DE3B4F}">
+          <x14:cfRule type="expression" priority="118" id="{3850683C-71E3-444E-9F9B-A2FDB87E7FC0}">
             <xm:f>AND((B2&lt;10),(B2&lt;&gt;solved!B2))</xm:f>
             <x14:dxf>
               <font>
@@ -8253,7 +8260,7 @@
           <xm:sqref>B2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="119" id="{7D469051-B766-4425-BBF1-24D0583FA711}">
+          <x14:cfRule type="expression" priority="119" id="{12AB4CFE-83BA-4730-982E-DFA84993233B}">
             <xm:f>AND((B3&lt;10),(B3&lt;&gt;solved!B3))</xm:f>
             <x14:dxf>
               <font>
@@ -8264,7 +8271,7 @@
           <xm:sqref>B3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="120" id="{7EDC896D-F3CC-4F8B-AD69-388A2FF72C9F}">
+          <x14:cfRule type="expression" priority="120" id="{A6C4AB22-843C-4584-AFEA-86293555C4BE}">
             <xm:f>AND((B4&lt;10),(B4&lt;&gt;solved!B4))</xm:f>
             <x14:dxf>
               <font>
@@ -8275,7 +8282,7 @@
           <xm:sqref>B4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="121" id="{9DA4DAEA-6BA0-46EE-9F4F-903B8AA3811C}">
+          <x14:cfRule type="expression" priority="121" id="{42A8AF99-6FB3-4067-957D-4498B3A04E54}">
             <xm:f>AND((B5&lt;10),(B5&lt;&gt;solved!B5))</xm:f>
             <x14:dxf>
               <font>
@@ -8286,7 +8293,7 @@
           <xm:sqref>B5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="122" id="{43B4A639-2983-4691-ADB0-CA142B4161D3}">
+          <x14:cfRule type="expression" priority="122" id="{64DCB9C6-4A2B-431A-9690-903A5A8E9178}">
             <xm:f>AND((B6&lt;10),(B6&lt;&gt;solved!B6))</xm:f>
             <x14:dxf>
               <font>
@@ -8297,7 +8304,7 @@
           <xm:sqref>B6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="123" id="{93207440-A9DE-49F4-B245-3D4FCE70AAB3}">
+          <x14:cfRule type="expression" priority="123" id="{4F8BA03E-B256-45A9-ACBD-C2F7B73D3068}">
             <xm:f>AND((B7&lt;10),(B7&lt;&gt;solved!B7))</xm:f>
             <x14:dxf>
               <font>
@@ -8308,7 +8315,7 @@
           <xm:sqref>B7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="124" id="{C01A3FEF-BC57-4B20-9E9F-5F5AE04D735E}">
+          <x14:cfRule type="expression" priority="124" id="{267055DA-D830-47A4-836A-A9DE736E85FC}">
             <xm:f>AND((B8&lt;10),(B8&lt;&gt;solved!B8))</xm:f>
             <x14:dxf>
               <font>
@@ -8319,7 +8326,7 @@
           <xm:sqref>B8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="125" id="{F3AFE260-58E9-4CA3-BC7D-9A73EFE9AEA1}">
+          <x14:cfRule type="expression" priority="125" id="{AED6A576-C4FA-4647-B1F1-C64C69276E6E}">
             <xm:f>AND((B9&lt;10),(B9&lt;&gt;solved!B9))</xm:f>
             <x14:dxf>
               <font>
@@ -8330,7 +8337,7 @@
           <xm:sqref>B9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="126" id="{7BA31384-8592-4F4A-A071-4FAF92B76085}">
+          <x14:cfRule type="expression" priority="126" id="{E2606020-A93D-4AA8-9455-ADE1288E746C}">
             <xm:f>AND((C1&lt;10),(C1&lt;&gt;solved!C1))</xm:f>
             <x14:dxf>
               <font>
@@ -8341,7 +8348,7 @@
           <xm:sqref>C1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="127" id="{233E973C-6032-419C-8112-22C083A8A16A}">
+          <x14:cfRule type="expression" priority="127" id="{3C6C242B-70FF-41A1-81F9-1110EE649867}">
             <xm:f>AND((C2&lt;10),(C2&lt;&gt;solved!C2))</xm:f>
             <x14:dxf>
               <font>
@@ -8352,7 +8359,7 @@
           <xm:sqref>C2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="128" id="{60C785D3-4086-4341-B32D-FB5CBBAD457E}">
+          <x14:cfRule type="expression" priority="128" id="{45A0BC51-A247-4C7E-B6E9-203AA9182B1A}">
             <xm:f>AND((C3&lt;10),(C3&lt;&gt;solved!C3))</xm:f>
             <x14:dxf>
               <font>
@@ -8363,7 +8370,7 @@
           <xm:sqref>C3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="129" id="{9615D044-72CB-43A9-9FB2-8092CDA09E70}">
+          <x14:cfRule type="expression" priority="129" id="{10D3F471-5035-4CC6-BF10-E58D8F77D616}">
             <xm:f>AND((C4&lt;10),(C4&lt;&gt;solved!C4))</xm:f>
             <x14:dxf>
               <font>
@@ -8374,7 +8381,7 @@
           <xm:sqref>C4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="130" id="{1083A068-47BE-4683-8712-E0B066E6A77C}">
+          <x14:cfRule type="expression" priority="130" id="{83D08CF8-FC13-4B70-83AF-98EFBB27A251}">
             <xm:f>AND((C5&lt;10),(C5&lt;&gt;solved!C5))</xm:f>
             <x14:dxf>
               <font>
@@ -8385,7 +8392,7 @@
           <xm:sqref>C5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="131" id="{9A78E628-D592-40DC-8D40-2099E4898FAC}">
+          <x14:cfRule type="expression" priority="131" id="{84111A30-A55F-4F3C-B57B-48C3AF7C56F9}">
             <xm:f>AND((C6&lt;10),(C6&lt;&gt;solved!C6))</xm:f>
             <x14:dxf>
               <font>
@@ -8396,7 +8403,7 @@
           <xm:sqref>C6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="132" id="{30219D80-1ACF-47E6-8F15-30414448735D}">
+          <x14:cfRule type="expression" priority="132" id="{3194DE60-FE68-4B38-AF99-5CFE6021BEFC}">
             <xm:f>AND((C7&lt;10),(C7&lt;&gt;solved!C7))</xm:f>
             <x14:dxf>
               <font>
@@ -8407,7 +8414,7 @@
           <xm:sqref>C7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="133" id="{DDE7D810-D84E-46C0-895D-CFE340FC7B55}">
+          <x14:cfRule type="expression" priority="133" id="{30101C70-BB3D-4EA4-B432-80944A2F62E3}">
             <xm:f>AND((C8&lt;10),(C8&lt;&gt;solved!C8))</xm:f>
             <x14:dxf>
               <font>
@@ -8418,7 +8425,7 @@
           <xm:sqref>C8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="134" id="{88B01EA8-204A-43B9-BEF8-90835389CD70}">
+          <x14:cfRule type="expression" priority="134" id="{9B2C9B35-5D39-40C8-8818-54DECBF66CC4}">
             <xm:f>AND((C9&lt;10),(C9&lt;&gt;solved!C9))</xm:f>
             <x14:dxf>
               <font>
@@ -8429,7 +8436,7 @@
           <xm:sqref>C9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="135" id="{CFA81DA7-9CA0-468E-AFB9-A17CC4F016FD}">
+          <x14:cfRule type="expression" priority="135" id="{64195FD3-B268-4377-9419-C8854CD8C8CB}">
             <xm:f>AND((D1&lt;10),(D1&lt;&gt;solved!D1))</xm:f>
             <x14:dxf>
               <font>
@@ -8440,7 +8447,7 @@
           <xm:sqref>D1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="136" id="{8B8CE535-5635-4CB4-BA9A-FDD813F41FE9}">
+          <x14:cfRule type="expression" priority="136" id="{F74FD2ED-2CAB-4B40-8B8F-1694C4D9181C}">
             <xm:f>AND((D2&lt;10),(D2&lt;&gt;solved!D2))</xm:f>
             <x14:dxf>
               <font>
@@ -8451,7 +8458,7 @@
           <xm:sqref>D2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="137" id="{AD443EB9-1CAC-4E94-874E-2B9F7AF7A3B1}">
+          <x14:cfRule type="expression" priority="137" id="{8F1A4AFF-7030-4C93-B6D0-6F193DBB1DE6}">
             <xm:f>AND((D3&lt;10),(D3&lt;&gt;solved!D3))</xm:f>
             <x14:dxf>
               <font>
@@ -8462,7 +8469,7 @@
           <xm:sqref>D3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="138" id="{2F17D41C-F71E-4A5F-9432-6C32EEA257F6}">
+          <x14:cfRule type="expression" priority="138" id="{EA646CEB-E1E4-4548-BB9D-994C74D755E1}">
             <xm:f>AND((D4&lt;10),(D4&lt;&gt;solved!D4))</xm:f>
             <x14:dxf>
               <font>
@@ -8473,7 +8480,7 @@
           <xm:sqref>D4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="139" id="{7961F05B-3A50-4428-874D-A26DF45F1A70}">
+          <x14:cfRule type="expression" priority="139" id="{7EA480EF-399D-47D7-B5ED-96F79F29B822}">
             <xm:f>AND((D5&lt;10),(D5&lt;&gt;solved!D5))</xm:f>
             <x14:dxf>
               <font>
@@ -8484,7 +8491,7 @@
           <xm:sqref>D5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="140" id="{93F4EBA0-746A-432D-AE5D-A690F7E2BA59}">
+          <x14:cfRule type="expression" priority="140" id="{DF80499C-7550-4F18-9517-B48E4545F8E8}">
             <xm:f>AND((D6&lt;10),(D6&lt;&gt;solved!D6))</xm:f>
             <x14:dxf>
               <font>
@@ -8495,7 +8502,7 @@
           <xm:sqref>D6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="141" id="{509E2E24-11AD-40F4-8F1E-4F5411C7F814}">
+          <x14:cfRule type="expression" priority="141" id="{8FCCE53A-5070-446B-A2AE-F62B415A51EE}">
             <xm:f>AND((D7&lt;10),(D7&lt;&gt;solved!D7))</xm:f>
             <x14:dxf>
               <font>
@@ -8506,7 +8513,7 @@
           <xm:sqref>D7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="142" id="{6B55AA60-ABDE-4790-A5E7-242D84704F74}">
+          <x14:cfRule type="expression" priority="142" id="{104CB490-2B18-4B34-8C93-17C8133F6C62}">
             <xm:f>AND((D8&lt;10),(D8&lt;&gt;solved!D8))</xm:f>
             <x14:dxf>
               <font>
@@ -8517,7 +8524,7 @@
           <xm:sqref>D8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="143" id="{6CAA50CC-AE84-4C84-AD8F-C1E71055C911}">
+          <x14:cfRule type="expression" priority="143" id="{C7168083-6B70-41E0-A7EF-24F835807470}">
             <xm:f>AND((D9&lt;10),(D9&lt;&gt;solved!D9))</xm:f>
             <x14:dxf>
               <font>
@@ -8528,7 +8535,7 @@
           <xm:sqref>D9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="144" id="{208030C2-8772-4835-9390-48595F5CC04A}">
+          <x14:cfRule type="expression" priority="144" id="{D289298E-F0D5-46F0-B82F-AFE42160259F}">
             <xm:f>AND((E1&lt;10),(E1&lt;&gt;solved!E1))</xm:f>
             <x14:dxf>
               <font>
@@ -8539,7 +8546,7 @@
           <xm:sqref>E1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="145" id="{80D37D4D-B27B-4FF0-B529-135FFB8DE52F}">
+          <x14:cfRule type="expression" priority="145" id="{15722564-9914-42B3-AB7D-729B182CB098}">
             <xm:f>AND((E2&lt;10),(E2&lt;&gt;solved!E2))</xm:f>
             <x14:dxf>
               <font>
@@ -8550,7 +8557,7 @@
           <xm:sqref>E2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="146" id="{1DA95BE0-526F-4AC6-92D0-B600CB705FC3}">
+          <x14:cfRule type="expression" priority="146" id="{1B224356-4E5E-4094-98B5-C9A443BC2E11}">
             <xm:f>AND((E3&lt;10),(E3&lt;&gt;solved!E3))</xm:f>
             <x14:dxf>
               <font>
@@ -8561,7 +8568,7 @@
           <xm:sqref>E3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="147" id="{CF77B0E4-9FFA-4CBD-80BD-BD699EA6C4A5}">
+          <x14:cfRule type="expression" priority="147" id="{12B36D39-B99C-4D69-9F6D-F84D7AA982DA}">
             <xm:f>AND((E4&lt;10),(E4&lt;&gt;solved!E4))</xm:f>
             <x14:dxf>
               <font>
@@ -8572,7 +8579,7 @@
           <xm:sqref>E4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="148" id="{DAEC3566-7150-4253-B843-3E68E390E619}">
+          <x14:cfRule type="expression" priority="148" id="{CF117986-35CB-4741-AC64-E5C04A53CDC8}">
             <xm:f>AND((E5&lt;10),(E5&lt;&gt;solved!E5))</xm:f>
             <x14:dxf>
               <font>
@@ -8583,7 +8590,7 @@
           <xm:sqref>E5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="149" id="{626218C9-FEC6-4220-AB6F-F8EDB4323D6B}">
+          <x14:cfRule type="expression" priority="149" id="{F3B977B7-DD74-4D40-8085-F293D1544A73}">
             <xm:f>AND((E6&lt;10),(E6&lt;&gt;solved!E6))</xm:f>
             <x14:dxf>
               <font>
@@ -8594,7 +8601,7 @@
           <xm:sqref>E6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="150" id="{F47E2037-5AE9-4280-A257-81F6945BD8C0}">
+          <x14:cfRule type="expression" priority="150" id="{F0A98032-CC16-4619-AEDE-1C30DF4778D9}">
             <xm:f>AND((E7&lt;10),(E7&lt;&gt;solved!E7))</xm:f>
             <x14:dxf>
               <font>
@@ -8605,7 +8612,7 @@
           <xm:sqref>E7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="151" id="{2D345FC2-62E7-4DCD-B932-A3F17AEBAC52}">
+          <x14:cfRule type="expression" priority="151" id="{B9F4B34E-CDC3-4440-804E-FC5FD95CCC2E}">
             <xm:f>AND((E8&lt;10),(E8&lt;&gt;solved!E8))</xm:f>
             <x14:dxf>
               <font>
@@ -8616,7 +8623,7 @@
           <xm:sqref>E8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="152" id="{70FD4C54-70F1-4E2F-80E4-A989B6405AEA}">
+          <x14:cfRule type="expression" priority="152" id="{22CFBDA6-39DC-44D7-938B-13275DBA6380}">
             <xm:f>AND((E9&lt;10),(E9&lt;&gt;solved!E9))</xm:f>
             <x14:dxf>
               <font>
@@ -8627,7 +8634,7 @@
           <xm:sqref>E9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="153" id="{3B56C6E2-51D9-4899-B7E6-646315BBC48A}">
+          <x14:cfRule type="expression" priority="153" id="{17E9F411-6031-465E-B75C-9EC388F9CC6F}">
             <xm:f>AND((F1&lt;10),(F1&lt;&gt;solved!F1))</xm:f>
             <x14:dxf>
               <font>
@@ -8638,7 +8645,7 @@
           <xm:sqref>F1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="154" id="{47F43AFC-BF33-4031-8B40-934E6F933038}">
+          <x14:cfRule type="expression" priority="154" id="{FBA481F0-CE50-4FF0-85AE-BE89AB13EF2B}">
             <xm:f>AND((F2&lt;10),(F2&lt;&gt;solved!F2))</xm:f>
             <x14:dxf>
               <font>
@@ -8649,7 +8656,7 @@
           <xm:sqref>F2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="155" id="{F17DB0FB-BB6D-455D-8580-8EF13D4DB3BE}">
+          <x14:cfRule type="expression" priority="155" id="{F5E03465-DFFE-4B1D-B24C-A71A819628D9}">
             <xm:f>AND((F3&lt;10),(F3&lt;&gt;solved!F3))</xm:f>
             <x14:dxf>
               <font>
@@ -8660,7 +8667,7 @@
           <xm:sqref>F3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="156" id="{B2873B96-1C00-48F0-8736-ED4759C04C85}">
+          <x14:cfRule type="expression" priority="156" id="{A62BD337-D3EF-4542-B3E5-88993BAB3B56}">
             <xm:f>AND((F4&lt;10),(F4&lt;&gt;solved!F4))</xm:f>
             <x14:dxf>
               <font>
@@ -8671,7 +8678,7 @@
           <xm:sqref>F4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="157" id="{46FDA267-84BF-4E66-8349-E1B4D7B0A0F9}">
+          <x14:cfRule type="expression" priority="157" id="{B5AE38AF-3841-4D32-A550-9B40BB6C605E}">
             <xm:f>AND((F5&lt;10),(F5&lt;&gt;solved!F5))</xm:f>
             <x14:dxf>
               <font>
@@ -8682,7 +8689,7 @@
           <xm:sqref>F5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="158" id="{34A16078-7DA0-493E-957B-EAC86BEE6DCF}">
+          <x14:cfRule type="expression" priority="158" id="{9110EB1B-42D3-48B5-84CA-4ACA5B6B93D5}">
             <xm:f>AND((F6&lt;10),(F6&lt;&gt;solved!F6))</xm:f>
             <x14:dxf>
               <font>
@@ -8693,7 +8700,7 @@
           <xm:sqref>F6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="159" id="{425FF41F-C32C-40AA-B5A2-705EA94BEF98}">
+          <x14:cfRule type="expression" priority="159" id="{12B770DD-40E5-4A5B-90D6-CE1FF0884910}">
             <xm:f>AND((F7&lt;10),(F7&lt;&gt;solved!F7))</xm:f>
             <x14:dxf>
               <font>
@@ -8704,7 +8711,7 @@
           <xm:sqref>F7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="160" id="{468F7C76-30D9-46F2-9E8E-F69436BA2C70}">
+          <x14:cfRule type="expression" priority="160" id="{1F943D8A-A924-48BF-8630-732760BA9E20}">
             <xm:f>AND((F8&lt;10),(F8&lt;&gt;solved!F8))</xm:f>
             <x14:dxf>
               <font>
@@ -8715,7 +8722,7 @@
           <xm:sqref>F8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="161" id="{9220E981-D852-40C4-BFF8-3C94D0288D16}">
+          <x14:cfRule type="expression" priority="161" id="{739A7EED-13F7-4A4A-ABDC-756E969DD2B3}">
             <xm:f>AND((F9&lt;10),(F9&lt;&gt;solved!F9))</xm:f>
             <x14:dxf>
               <font>
@@ -8726,7 +8733,7 @@
           <xm:sqref>F9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="162" id="{63186030-B1D0-44D9-8C79-D7EBF014675E}">
+          <x14:cfRule type="expression" priority="162" id="{F829C7E9-C326-4B48-B41A-158F30A31880}">
             <xm:f>AND((G1&lt;10),(G1&lt;&gt;solved!G1))</xm:f>
             <x14:dxf>
               <font>
@@ -8737,7 +8744,7 @@
           <xm:sqref>G1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="163" id="{21BC1CD7-7D18-4014-AD5F-75DDA9B0FE75}">
+          <x14:cfRule type="expression" priority="163" id="{F92E228D-9D60-4E96-B888-6659DCDFB7FE}">
             <xm:f>AND((G2&lt;10),(G2&lt;&gt;solved!G2))</xm:f>
             <x14:dxf>
               <font>
@@ -8748,7 +8755,7 @@
           <xm:sqref>G2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="164" id="{90D19B8F-FBF4-4A4C-8875-1A54BACCF4D6}">
+          <x14:cfRule type="expression" priority="164" id="{163B2150-6CFF-4895-94FF-656EF3D72DA3}">
             <xm:f>AND((G3&lt;10),(G3&lt;&gt;solved!G3))</xm:f>
             <x14:dxf>
               <font>
@@ -8759,7 +8766,7 @@
           <xm:sqref>G3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="165" id="{18C0A8CB-16E4-45D8-9F20-39E8E1A99895}">
+          <x14:cfRule type="expression" priority="165" id="{C2EF90C0-74D7-404C-926F-8AEBE0D07362}">
             <xm:f>AND((G4&lt;10),(G4&lt;&gt;solved!G4))</xm:f>
             <x14:dxf>
               <font>
@@ -8770,7 +8777,7 @@
           <xm:sqref>G4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="166" id="{212C1642-3227-43FA-88D7-E16F91199E3E}">
+          <x14:cfRule type="expression" priority="166" id="{B552E148-C01D-4153-AB1E-8C7C6EC3A0AF}">
             <xm:f>AND((G5&lt;10),(G5&lt;&gt;solved!G5))</xm:f>
             <x14:dxf>
               <font>
@@ -8781,7 +8788,7 @@
           <xm:sqref>G5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="167" id="{AEB19DCA-2CA9-4A20-9B15-DA3DE56573D0}">
+          <x14:cfRule type="expression" priority="167" id="{2075BE97-9660-4220-8531-6071D4989542}">
             <xm:f>AND((G6&lt;10),(G6&lt;&gt;solved!G6))</xm:f>
             <x14:dxf>
               <font>
@@ -8792,7 +8799,7 @@
           <xm:sqref>G6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="168" id="{E7597ECC-9D54-4379-80B1-2B3FC628A2ED}">
+          <x14:cfRule type="expression" priority="168" id="{FCC491C5-32E0-44CC-A644-CCBD8410BAAE}">
             <xm:f>AND((G7&lt;10),(G7&lt;&gt;solved!G7))</xm:f>
             <x14:dxf>
               <font>
@@ -8803,7 +8810,7 @@
           <xm:sqref>G7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="169" id="{B9E64F3D-89A8-478A-A996-2038D6E360A7}">
+          <x14:cfRule type="expression" priority="169" id="{A47D6D50-AF93-4620-99E0-527594703B4C}">
             <xm:f>AND((G8&lt;10),(G8&lt;&gt;solved!G8))</xm:f>
             <x14:dxf>
               <font>
@@ -8814,7 +8821,7 @@
           <xm:sqref>G8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="170" id="{EE89A5FE-DAFB-4A5D-A22B-5471D4308A53}">
+          <x14:cfRule type="expression" priority="170" id="{C9F4D0EF-42EA-49E7-A838-374F3518F734}">
             <xm:f>AND((G9&lt;10),(G9&lt;&gt;solved!G9))</xm:f>
             <x14:dxf>
               <font>
@@ -8825,7 +8832,7 @@
           <xm:sqref>G9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="171" id="{27DDCB26-2195-4AC9-BB7F-3F7F3BB2F791}">
+          <x14:cfRule type="expression" priority="171" id="{777DDAA9-EB63-4441-9A2A-49153BF3D6BA}">
             <xm:f>AND((H1&lt;10),(H1&lt;&gt;solved!H1))</xm:f>
             <x14:dxf>
               <font>
@@ -8836,7 +8843,7 @@
           <xm:sqref>H1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="172" id="{68BBACEC-2744-4AC0-BCEC-BDE0E1E0EB20}">
+          <x14:cfRule type="expression" priority="172" id="{67B08E67-41BB-4FC2-8048-4597752756C4}">
             <xm:f>AND((H2&lt;10),(H2&lt;&gt;solved!H2))</xm:f>
             <x14:dxf>
               <font>
@@ -8847,7 +8854,7 @@
           <xm:sqref>H2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="173" id="{3FA8AEFD-C45A-40BF-BD50-114A6AF121E5}">
+          <x14:cfRule type="expression" priority="173" id="{3DB644EE-33D1-48A6-A3AE-E6A03394F334}">
             <xm:f>AND((H3&lt;10),(H3&lt;&gt;solved!H3))</xm:f>
             <x14:dxf>
               <font>
@@ -8858,7 +8865,7 @@
           <xm:sqref>H3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="174" id="{685EF828-F31A-46A5-94C5-1D34A84355D7}">
+          <x14:cfRule type="expression" priority="174" id="{1C1DE524-3F5A-40C5-BC4B-C27D8734EFE0}">
             <xm:f>AND((H4&lt;10),(H4&lt;&gt;solved!H4))</xm:f>
             <x14:dxf>
               <font>
@@ -8869,7 +8876,7 @@
           <xm:sqref>H4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="175" id="{DD606118-2F9B-438C-9D94-403C77122364}">
+          <x14:cfRule type="expression" priority="175" id="{73CE3B26-4154-403F-B1B4-A2AA52F05390}">
             <xm:f>AND((H5&lt;10),(H5&lt;&gt;solved!H5))</xm:f>
             <x14:dxf>
               <font>
@@ -8880,7 +8887,7 @@
           <xm:sqref>H5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="176" id="{CD2A1552-F0D5-4758-961B-A47BF160B340}">
+          <x14:cfRule type="expression" priority="176" id="{4D2C2E16-BAB7-40E2-9BB6-81C57E927D49}">
             <xm:f>AND((H6&lt;10),(H6&lt;&gt;solved!H6))</xm:f>
             <x14:dxf>
               <font>
@@ -8891,7 +8898,7 @@
           <xm:sqref>H6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="177" id="{8998A06D-F9FD-4E8C-8F73-94D879E8E192}">
+          <x14:cfRule type="expression" priority="177" id="{73FE6B1C-CF2A-4C65-9566-57CA1ED0362F}">
             <xm:f>AND((H7&lt;10),(H7&lt;&gt;solved!H7))</xm:f>
             <x14:dxf>
               <font>
@@ -8902,7 +8909,7 @@
           <xm:sqref>H7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="178" id="{811575BD-E86D-461E-B840-404FB04CEBA4}">
+          <x14:cfRule type="expression" priority="178" id="{51E4AAD5-9332-4CCF-A1F4-1C96D0388AF7}">
             <xm:f>AND((H8&lt;10),(H8&lt;&gt;solved!H8))</xm:f>
             <x14:dxf>
               <font>
@@ -8913,7 +8920,7 @@
           <xm:sqref>H8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="179" id="{21487049-2F6B-4C70-8385-27CCA6DAC249}">
+          <x14:cfRule type="expression" priority="179" id="{F243A6A4-2DBF-44DD-A152-5D2E6C60BA4E}">
             <xm:f>AND((H9&lt;10),(H9&lt;&gt;solved!H9))</xm:f>
             <x14:dxf>
               <font>
@@ -8924,7 +8931,7 @@
           <xm:sqref>H9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="180" id="{34981E72-2ADD-4B77-A845-E5B091F9BA9D}">
+          <x14:cfRule type="expression" priority="180" id="{F0ACA3A1-438D-4F97-8BE1-A712E55B39BE}">
             <xm:f>AND((I2&lt;10),(I2&lt;&gt;solved!I2))</xm:f>
             <x14:dxf>
               <font>
@@ -8935,7 +8942,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="181" id="{ADC88FD7-DD1A-4482-AF00-ED73268E39F9}">
+          <x14:cfRule type="expression" priority="181" id="{EF34AB3E-10C0-41AA-82DC-00A73690FCEE}">
             <xm:f>AND((I3&lt;10),(I3&lt;&gt;solved!I3))</xm:f>
             <x14:dxf>
               <font>
@@ -8946,7 +8953,7 @@
           <xm:sqref>I3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="182" id="{C9756028-82B2-4A48-A710-8DB0C0F5B975}">
+          <x14:cfRule type="expression" priority="182" id="{6470D84D-D89F-4433-834D-1FF0A7726DA3}">
             <xm:f>AND((I4&lt;10),(I4&lt;&gt;solved!I4))</xm:f>
             <x14:dxf>
               <font>
@@ -8957,7 +8964,7 @@
           <xm:sqref>I4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="183" id="{9976A5AB-E9A7-40D5-83AD-A0C2ED1BE9A0}">
+          <x14:cfRule type="expression" priority="183" id="{DD3B4F49-B990-42D3-968A-C04AB8816376}">
             <xm:f>AND((I5&lt;10),(I5&lt;&gt;solved!I5))</xm:f>
             <x14:dxf>
               <font>
@@ -8968,7 +8975,7 @@
           <xm:sqref>I5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="184" id="{FEE4598D-D8CC-44C0-8CAC-BBC1E9BF1DA5}">
+          <x14:cfRule type="expression" priority="184" id="{3B51BF84-E329-4FC3-A69B-EE2CEEE5A311}">
             <xm:f>AND((I6&lt;10),(I6&lt;&gt;solved!I6))</xm:f>
             <x14:dxf>
               <font>
@@ -8979,7 +8986,7 @@
           <xm:sqref>I6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="185" id="{202C607F-6952-4276-8C67-6867367F27C0}">
+          <x14:cfRule type="expression" priority="185" id="{7D566182-44C6-44D4-9E72-34693537A710}">
             <xm:f>AND((I7&lt;10),(I7&lt;&gt;solved!I7))</xm:f>
             <x14:dxf>
               <font>
@@ -8990,7 +8997,7 @@
           <xm:sqref>I7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="186" id="{226921BE-5956-4817-BCA9-AE3065DAC490}">
+          <x14:cfRule type="expression" priority="186" id="{4BBB27D9-76E0-44FB-BC3A-20ED46C682BE}">
             <xm:f>AND((I8&lt;10),(I8&lt;&gt;solved!I8))</xm:f>
             <x14:dxf>
               <font>
@@ -9001,7 +9008,7 @@
           <xm:sqref>I8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="187" id="{715BDA19-C616-432E-A3FD-AA83B85FFAAF}">
+          <x14:cfRule type="expression" priority="187" id="{3E9FFADB-607B-4483-987A-60824463CA94}">
             <xm:f>AND((I9&lt;10),(I9&lt;&gt;solved!I9))</xm:f>
             <x14:dxf>
               <font>
@@ -9012,7 +9019,7 @@
           <xm:sqref>I9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="188" id="{ADDAB711-1EC4-4EF1-B8F3-ABF5D2A9BFA7}">
+          <x14:cfRule type="expression" priority="188" id="{4F4155C0-7796-44A5-8B28-DE74F2BE5234}">
             <xm:f>AND(($A$1&lt;10),($A$1&lt;&gt;solved!$A$1))</xm:f>
             <x14:dxf>
               <font>
@@ -9023,7 +9030,7 @@
           <xm:sqref>A1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="189" id="{80B6D72E-13DA-4390-9E56-BFF022BE9984}">
+          <x14:cfRule type="expression" priority="189" id="{BFE02E46-A91D-4725-9B24-121ACD7FB0B6}">
             <xm:f>AND(($A$4&lt;10),($A$4&lt;&gt;solved!$A$4))</xm:f>
             <x14:dxf>
               <font>
@@ -9058,7 +9065,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -9066,22 +9073,22 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19"/>
+      <c r="A2" s="21"/>
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19"/>
+      <c r="A3" s="21"/>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="n">
+      <c r="A5" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="58" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -9089,10 +9096,10 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="19"/>
+      <c r="A6" s="21"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19" t="n">
+      <c r="A7" s="21" t="n">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -9103,10 +9110,10 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19"/>
+      <c r="A8" s="21"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19" t="n">
+      <c r="A9" s="21" t="n">
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -9117,10 +9124,10 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19"/>
+      <c r="A10" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19" t="n">
+      <c r="A11" s="21" t="n">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -9131,23 +9138,23 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="19"/>
+      <c r="A12" s="21"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="19"/>
+      <c r="A13" s="21"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19"/>
+      <c r="A14" s="21"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="19"/>
+      <c r="A15" s="21"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19"/>
-    </row>
-    <row r="17" s="19" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A16" s="21"/>
+    </row>
+    <row r="17" s="21" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="19"/>
+      <c r="A18" s="21"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -9453,133 +9460,133 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="D1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="G1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="n">
+      <c r="I1" s="1" t="n">
         <v>2</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="E2" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="n">
+      <c r="F2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="I2" s="1" t="n">
         <v>1</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>4</v>
-      </c>
       <c r="D3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H3" s="1" t="n">
+      <c r="I3" s="1" t="n">
         <v>5</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H4" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I4" s="1" t="n">
         <v>8</v>
-      </c>
-      <c r="I4" s="1" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>7</v>
@@ -9588,135 +9595,135 @@
         <v>8</v>
       </c>
       <c r="E5" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F5" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="G5" s="1" t="n">
+      <c r="H5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="I5" s="1" t="n">
         <v>3</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="F6" s="1" t="n">
+      <c r="I6" s="1" t="n">
         <v>7</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="H6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>7</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="E8" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="F8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" s="1" t="n">
         <v>9</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="I8" s="1" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="C9" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>6</v>
-      </c>
       <c r="E9" s="1" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>5</v>
       </c>
       <c r="H9" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -9753,7 +9760,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="3"/>
       <c r="I1" s="4"/>
-      <c r="K1" s="5" t="str">
+      <c r="K1" s="15" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "1")=9, 1, "")</f>
         <v/>
       </c>
@@ -9768,7 +9775,7 @@
       <c r="G2" s="7"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
-      <c r="K2" s="10" t="str">
+      <c r="K2" s="16" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "2")=9, 2, "")</f>
         <v/>
       </c>
@@ -9783,7 +9790,7 @@
       <c r="G3" s="11"/>
       <c r="H3" s="12"/>
       <c r="I3" s="13"/>
-      <c r="K3" s="10" t="str">
+      <c r="K3" s="16" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "3")=9, 3, "")</f>
         <v/>
       </c>
@@ -9798,7 +9805,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="3"/>
       <c r="I4" s="4"/>
-      <c r="K4" s="10" t="str">
+      <c r="K4" s="16" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "4")=9, 4, "")</f>
         <v/>
       </c>
@@ -9813,7 +9820,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="8"/>
       <c r="I5" s="9"/>
-      <c r="K5" s="10" t="str">
+      <c r="K5" s="16" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "5")=9, 5, "")</f>
         <v/>
       </c>
@@ -9828,7 +9835,7 @@
       <c r="G6" s="11"/>
       <c r="H6" s="12"/>
       <c r="I6" s="13"/>
-      <c r="K6" s="10" t="str">
+      <c r="K6" s="16" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "6")=9, 6, "")</f>
         <v/>
       </c>
@@ -9843,7 +9850,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="3"/>
       <c r="I7" s="4"/>
-      <c r="K7" s="10" t="str">
+      <c r="K7" s="16" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "7")=9, 7, "")</f>
         <v/>
       </c>
@@ -9858,7 +9865,7 @@
       <c r="G8" s="7"/>
       <c r="H8" s="8"/>
       <c r="I8" s="9"/>
-      <c r="K8" s="10" t="str">
+      <c r="K8" s="16" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "8")=9, 8, "")</f>
         <v/>
       </c>
@@ -9873,7 +9880,7 @@
       <c r="G9" s="11"/>
       <c r="H9" s="12"/>
       <c r="I9" s="13"/>
-      <c r="K9" s="15" t="str">
+      <c r="K9" s="17" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "9")=9, 9, "")</f>
         <v/>
       </c>
@@ -9971,7 +9978,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="29" id="{7539C153-2B20-49DE-A938-2327E2384D1C}">
+          <x14:cfRule type="expression" priority="29" id="{70258D44-405C-4BDA-8421-F04D96C91F91}">
             <xm:f>AND(($A$1&lt;10),($A$1&lt;&gt;solved!$A$1))</xm:f>
             <x14:dxf>
               <font>
@@ -9987,7 +9994,7 @@
           <xm:sqref>A1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="30" id="{46C81B7B-9031-4AD0-A8C5-3615804E80E0}">
+          <x14:cfRule type="expression" priority="30" id="{378CA49A-2CF7-4941-B92F-2472481CD46C}">
             <xm:f>AND((A2&lt;10),(A2&lt;&gt;solved!A2))</xm:f>
             <x14:dxf>
               <font>
@@ -9998,7 +10005,7 @@
           <xm:sqref>A2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="31" id="{B7449C79-9D88-4776-BEF9-C0BEE07455A1}">
+          <x14:cfRule type="expression" priority="31" id="{F1B0233F-A031-4528-8F7D-664AAE6B5A7A}">
             <xm:f>AND((A3&lt;10),(A3&lt;&gt;solved!A3))</xm:f>
             <x14:dxf>
               <font>
@@ -10009,7 +10016,7 @@
           <xm:sqref>A3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="32" id="{9F3A75D0-A4A0-4177-B538-BD6CB25FD485}">
+          <x14:cfRule type="expression" priority="32" id="{CB1B1EB2-2DF0-476A-A029-15D5DA8791A0}">
             <xm:f>AND((A4&lt;10),(A4&lt;&gt;solved!A4))</xm:f>
             <x14:dxf>
               <font>
@@ -10020,7 +10027,7 @@
           <xm:sqref>A4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="33" id="{E5BE80C4-DEF1-494B-89EB-F34636E34B4C}">
+          <x14:cfRule type="expression" priority="33" id="{582B3B72-32E1-43C0-AAE6-7E7BEB309CCF}">
             <xm:f>AND((A5&lt;10),(A5&lt;&gt;solved!A5))</xm:f>
             <x14:dxf>
               <font>
@@ -10031,7 +10038,7 @@
           <xm:sqref>A5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="34" id="{6D3EB4B1-C018-4772-AF8B-11DA4D33F1F9}">
+          <x14:cfRule type="expression" priority="34" id="{47E32134-F0AB-4372-B675-822D411DFF16}">
             <xm:f>AND((A6&lt;10),(A6&lt;&gt;solved!A6))</xm:f>
             <x14:dxf>
               <font>
@@ -10042,7 +10049,7 @@
           <xm:sqref>A6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="35" id="{79619EB2-E574-4437-AFE7-F9C367C23B2B}">
+          <x14:cfRule type="expression" priority="35" id="{13CF1BF8-41B9-4B19-BD30-36A2188DAD7E}">
             <xm:f>AND((A7&lt;10),(A7&lt;&gt;solved!A7))</xm:f>
             <x14:dxf>
               <font>
@@ -10053,7 +10060,7 @@
           <xm:sqref>A7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="36" id="{F064B4D2-545A-4291-8FC6-3AEA66FE69ED}">
+          <x14:cfRule type="expression" priority="36" id="{52DCA0A7-FD80-45C0-AB4D-F94542FD8798}">
             <xm:f>AND((A8&lt;10),(A8&lt;&gt;solved!A8))</xm:f>
             <x14:dxf>
               <font>
@@ -10064,7 +10071,7 @@
           <xm:sqref>A8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="37" id="{60EB2AE8-C420-4F25-A574-DAABC14579F9}">
+          <x14:cfRule type="expression" priority="37" id="{4060EC3A-FC9B-4BF1-83D0-41A9796A1A60}">
             <xm:f>AND((A9&lt;10),(A9&lt;&gt;solved!A9))</xm:f>
             <x14:dxf>
               <font>
@@ -10075,7 +10082,7 @@
           <xm:sqref>A9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="38" id="{14A0D927-DA93-4541-AD84-1E53C556B080}">
+          <x14:cfRule type="expression" priority="38" id="{1E9FC78E-7FD6-40C8-AE48-B14536139E53}">
             <xm:f>AND((B1&lt;10),(B1&lt;&gt;solved!B1))</xm:f>
             <x14:dxf>
               <font>
@@ -10086,7 +10093,7 @@
           <xm:sqref>B1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="39" id="{316C5A5A-DC39-44A0-BF7D-41BD7A82E075}">
+          <x14:cfRule type="expression" priority="39" id="{F4B14ED5-A0E7-4145-9579-2F967EBEDA4D}">
             <xm:f>AND((B2&lt;10),(B2&lt;&gt;solved!B2))</xm:f>
             <x14:dxf>
               <font>
@@ -10097,7 +10104,7 @@
           <xm:sqref>B2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="40" id="{EACECEA2-6DA1-4439-86CF-77A040F01A79}">
+          <x14:cfRule type="expression" priority="40" id="{F162609B-EB40-498D-80D1-849DC5F4C74D}">
             <xm:f>AND((B3&lt;10),(B3&lt;&gt;solved!B3))</xm:f>
             <x14:dxf>
               <font>
@@ -10108,7 +10115,7 @@
           <xm:sqref>B3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="41" id="{EA5015D0-1B4F-416A-9CA0-E47581CEB2A4}">
+          <x14:cfRule type="expression" priority="41" id="{6E85F1B7-60CE-408F-95B0-24532B73E078}">
             <xm:f>AND((B4&lt;10),(B4&lt;&gt;solved!B4))</xm:f>
             <x14:dxf>
               <font>
@@ -10119,7 +10126,7 @@
           <xm:sqref>B4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="42" id="{3D67F619-5228-44A3-B87C-DA41FBCC6AFA}">
+          <x14:cfRule type="expression" priority="42" id="{587420D8-4085-493F-B4F8-E58417A5CD11}">
             <xm:f>AND((B5&lt;10),(B5&lt;&gt;solved!B5))</xm:f>
             <x14:dxf>
               <font>
@@ -10130,7 +10137,7 @@
           <xm:sqref>B5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="43" id="{274DA53D-8184-4C8C-A6FC-F724BB3AAB48}">
+          <x14:cfRule type="expression" priority="43" id="{1CB0C380-9E9C-4CD4-93E4-CC91E68BB27B}">
             <xm:f>AND((B6&lt;10),(B6&lt;&gt;solved!B6))</xm:f>
             <x14:dxf>
               <font>
@@ -10141,7 +10148,7 @@
           <xm:sqref>B6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="44" id="{7182A52A-5FCB-4CDD-9441-623D854EE2CD}">
+          <x14:cfRule type="expression" priority="44" id="{7DF7B892-604D-4691-8690-18E54FF3FA52}">
             <xm:f>AND((B7&lt;10),(B7&lt;&gt;solved!B7))</xm:f>
             <x14:dxf>
               <font>
@@ -10152,7 +10159,7 @@
           <xm:sqref>B7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="45" id="{C5843042-49DA-4826-AFDA-47EAB6CD19FF}">
+          <x14:cfRule type="expression" priority="45" id="{D751DB3C-4B6B-4573-82D2-345D4E6ECC28}">
             <xm:f>AND((B8&lt;10),(B8&lt;&gt;solved!B8))</xm:f>
             <x14:dxf>
               <font>
@@ -10163,7 +10170,7 @@
           <xm:sqref>B8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="46" id="{E7605124-AD37-4D9A-A2E7-3B6177719474}">
+          <x14:cfRule type="expression" priority="46" id="{CD436595-73F5-4CB5-858B-66A81DABD676}">
             <xm:f>AND((B9&lt;10),(B9&lt;&gt;solved!B9))</xm:f>
             <x14:dxf>
               <font>
@@ -10174,7 +10181,7 @@
           <xm:sqref>B9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="47" id="{E2F3132C-81D5-4560-A580-C35B4E5E8184}">
+          <x14:cfRule type="expression" priority="47" id="{5E626A44-DEC1-457E-97C8-FDA380BB4523}">
             <xm:f>AND((C1&lt;10),(C1&lt;&gt;solved!C1))</xm:f>
             <x14:dxf>
               <font>
@@ -10185,7 +10192,7 @@
           <xm:sqref>C1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="48" id="{BF7389FB-2B75-4079-9C1D-4060FCD58629}">
+          <x14:cfRule type="expression" priority="48" id="{916626F0-3FAA-457E-B360-EA4B3C6CD417}">
             <xm:f>AND((C2&lt;10),(C2&lt;&gt;solved!C2))</xm:f>
             <x14:dxf>
               <font>
@@ -10196,7 +10203,7 @@
           <xm:sqref>C2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="49" id="{2D3873E0-5675-46B0-9D73-80791B4FA4DE}">
+          <x14:cfRule type="expression" priority="49" id="{C100E45E-8B18-42FA-BB15-87A11BB47BF6}">
             <xm:f>AND((C3&lt;10),(C3&lt;&gt;solved!C3))</xm:f>
             <x14:dxf>
               <font>
@@ -10207,7 +10214,7 @@
           <xm:sqref>C3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="50" id="{244CE7E0-7D4D-474A-A3ED-1491D7371DCA}">
+          <x14:cfRule type="expression" priority="50" id="{D852F8C3-B0AB-45DE-85F0-7E3920969067}">
             <xm:f>AND((C4&lt;10),(C4&lt;&gt;solved!C4))</xm:f>
             <x14:dxf>
               <font>
@@ -10218,7 +10225,7 @@
           <xm:sqref>C4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="51" id="{287CCF51-18A2-4111-A27C-ED7CCCB88112}">
+          <x14:cfRule type="expression" priority="51" id="{78666090-A494-452D-B674-E6196FB45EB7}">
             <xm:f>AND((C5&lt;10),(C5&lt;&gt;solved!C5))</xm:f>
             <x14:dxf>
               <font>
@@ -10229,7 +10236,7 @@
           <xm:sqref>C5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="52" id="{D57F4B52-539E-4DCA-B290-AE487CF69B6B}">
+          <x14:cfRule type="expression" priority="52" id="{F12923AD-CD3D-42A6-852B-1B40BAAE4799}">
             <xm:f>AND((C6&lt;10),(C6&lt;&gt;solved!C6))</xm:f>
             <x14:dxf>
               <font>
@@ -10240,7 +10247,7 @@
           <xm:sqref>C6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="53" id="{69E0ED97-4D7E-4F75-B1DC-701D13B3602F}">
+          <x14:cfRule type="expression" priority="53" id="{17A93497-4FF9-4F13-A9CF-5123A04C7414}">
             <xm:f>AND((C7&lt;10),(C7&lt;&gt;solved!C7))</xm:f>
             <x14:dxf>
               <font>
@@ -10251,7 +10258,7 @@
           <xm:sqref>C7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="54" id="{10A3C415-64C3-4889-A222-CDBC7F373897}">
+          <x14:cfRule type="expression" priority="54" id="{4495F46D-43AF-47DD-BA2D-A5C582441B53}">
             <xm:f>AND((C8&lt;10),(C8&lt;&gt;solved!C8))</xm:f>
             <x14:dxf>
               <font>
@@ -10262,7 +10269,7 @@
           <xm:sqref>C8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="55" id="{E9ABA69C-90F0-4CEC-A07C-152A5A40F1A7}">
+          <x14:cfRule type="expression" priority="55" id="{E52CFBB0-DB88-4980-96FA-1BFE66AB718C}">
             <xm:f>AND((C9&lt;10),(C9&lt;&gt;solved!C9))</xm:f>
             <x14:dxf>
               <font>
@@ -10273,7 +10280,7 @@
           <xm:sqref>C9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="56" id="{3D8F99B6-A622-4255-89E7-19D1E755DE36}">
+          <x14:cfRule type="expression" priority="56" id="{89F1EC50-F2B8-4D1B-A738-D37CA279A4F0}">
             <xm:f>AND((D1&lt;10),(D1&lt;&gt;solved!D1))</xm:f>
             <x14:dxf>
               <font>
@@ -10284,7 +10291,7 @@
           <xm:sqref>D1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="57" id="{F22FC078-9BF1-4ED1-A7F1-A0155A2FC49C}">
+          <x14:cfRule type="expression" priority="57" id="{261AEB8E-96EF-4B94-80CF-9E5FE879DA1E}">
             <xm:f>AND((D2&lt;10),(D2&lt;&gt;solved!D2))</xm:f>
             <x14:dxf>
               <font>
@@ -10295,7 +10302,7 @@
           <xm:sqref>D2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="58" id="{DB927BDC-4452-4C89-A13A-CA1DB22CAA1A}">
+          <x14:cfRule type="expression" priority="58" id="{52F38E1B-BF60-4874-B08C-741A86A0F09E}">
             <xm:f>AND((D3&lt;10),(D3&lt;&gt;solved!D3))</xm:f>
             <x14:dxf>
               <font>
@@ -10306,7 +10313,7 @@
           <xm:sqref>D3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="59" id="{90F07B63-90C0-4DD4-BA24-EDA4AFB64330}">
+          <x14:cfRule type="expression" priority="59" id="{0097DAC5-634C-4EB3-8CB2-88A140EF1E21}">
             <xm:f>AND((D4&lt;10),(D4&lt;&gt;solved!D4))</xm:f>
             <x14:dxf>
               <font>
@@ -10317,7 +10324,7 @@
           <xm:sqref>D4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="60" id="{A7A16DA0-4052-49DB-85A1-5FD8FEAE268B}">
+          <x14:cfRule type="expression" priority="60" id="{32C775D3-6CD7-41C1-B810-7CD346CC9AED}">
             <xm:f>AND((D5&lt;10),(D5&lt;&gt;solved!D5))</xm:f>
             <x14:dxf>
               <font>
@@ -10328,7 +10335,7 @@
           <xm:sqref>D5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="61" id="{ADD18667-5353-461F-ACEA-7F184056176B}">
+          <x14:cfRule type="expression" priority="61" id="{E0DBC7F7-7AB0-4FAF-B18C-80A6EA69ABDC}">
             <xm:f>AND((D6&lt;10),(D6&lt;&gt;solved!D6))</xm:f>
             <x14:dxf>
               <font>
@@ -10339,7 +10346,7 @@
           <xm:sqref>D6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="62" id="{5BCFBEF0-1D32-47D0-B991-DB851B8088CD}">
+          <x14:cfRule type="expression" priority="62" id="{E529C8B1-5293-4AE0-AEBE-9C51409DEB98}">
             <xm:f>AND((D7&lt;10),(D7&lt;&gt;solved!D7))</xm:f>
             <x14:dxf>
               <font>
@@ -10350,7 +10357,7 @@
           <xm:sqref>D7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="63" id="{D700D7EF-2827-4274-8115-CAE74CF9F67D}">
+          <x14:cfRule type="expression" priority="63" id="{3DBF36D6-4EAF-4570-9BCB-A07A5E646E23}">
             <xm:f>AND((D8&lt;10),(D8&lt;&gt;solved!D8))</xm:f>
             <x14:dxf>
               <font>
@@ -10361,7 +10368,7 @@
           <xm:sqref>D8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="64" id="{50D89F8B-EA92-4EBE-B245-E7906F458BD0}">
+          <x14:cfRule type="expression" priority="64" id="{B1E870E2-8FB1-45A4-AEFF-50597663D3DE}">
             <xm:f>AND((D9&lt;10),(D9&lt;&gt;solved!D9))</xm:f>
             <x14:dxf>
               <font>
@@ -10372,7 +10379,7 @@
           <xm:sqref>D9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="65" id="{5E14944E-9472-48D5-9BF0-13FE4B1288F1}">
+          <x14:cfRule type="expression" priority="65" id="{EFEAC81A-1134-4AA1-84B9-DB8D5A6E8C97}">
             <xm:f>AND((E1&lt;10),(E1&lt;&gt;solved!E1))</xm:f>
             <x14:dxf>
               <font>
@@ -10383,7 +10390,7 @@
           <xm:sqref>E1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="66" id="{A0F7F199-949A-407E-9B97-75244A4DC266}">
+          <x14:cfRule type="expression" priority="66" id="{E0DE81A8-81B2-4A2B-8CD0-43E2FF498E2D}">
             <xm:f>AND((E2&lt;10),(E2&lt;&gt;solved!E2))</xm:f>
             <x14:dxf>
               <font>
@@ -10394,7 +10401,7 @@
           <xm:sqref>E2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="67" id="{F7C494AD-C562-4668-9C7E-305E94959619}">
+          <x14:cfRule type="expression" priority="67" id="{21562687-C4F3-4128-BBB6-379AE711B619}">
             <xm:f>AND((E3&lt;10),(E3&lt;&gt;solved!E3))</xm:f>
             <x14:dxf>
               <font>
@@ -10405,7 +10412,7 @@
           <xm:sqref>E3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="68" id="{8E179444-16AB-4DE0-A1B6-8013BDC0FCE6}">
+          <x14:cfRule type="expression" priority="68" id="{27F5F2A4-712A-43BE-B368-7251E01C5DA0}">
             <xm:f>AND((E4&lt;10),(E4&lt;&gt;solved!E4))</xm:f>
             <x14:dxf>
               <font>
@@ -10416,7 +10423,7 @@
           <xm:sqref>E4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="69" id="{6D0025CE-95BB-4FE5-807C-D6B37DB4ABE3}">
+          <x14:cfRule type="expression" priority="69" id="{EEF46366-1FEB-492C-99AC-7D8FA2413150}">
             <xm:f>AND((E5&lt;10),(E5&lt;&gt;solved!E5))</xm:f>
             <x14:dxf>
               <font>
@@ -10427,7 +10434,7 @@
           <xm:sqref>E5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="70" id="{84761D51-7060-4548-BA33-CF35B774FAC8}">
+          <x14:cfRule type="expression" priority="70" id="{68EB4239-B2B6-4BFD-BFB6-BA00247F9FC1}">
             <xm:f>AND((E6&lt;10),(E6&lt;&gt;solved!E6))</xm:f>
             <x14:dxf>
               <font>
@@ -10438,7 +10445,7 @@
           <xm:sqref>E6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="71" id="{DD46A0CB-71A6-4B5F-B439-DF91D82F3451}">
+          <x14:cfRule type="expression" priority="71" id="{9CAFB015-EE7D-411E-913F-271EBF7C4FF5}">
             <xm:f>AND((E7&lt;10),(E7&lt;&gt;solved!E7))</xm:f>
             <x14:dxf>
               <font>
@@ -10449,7 +10456,7 @@
           <xm:sqref>E7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="72" id="{205CB6C0-9350-4766-A0C8-E0F024AA8739}">
+          <x14:cfRule type="expression" priority="72" id="{1CFAB5AE-6F3B-449B-8A7C-1AA0701D4C4B}">
             <xm:f>AND((E8&lt;10),(E8&lt;&gt;solved!E8))</xm:f>
             <x14:dxf>
               <font>
@@ -10460,7 +10467,7 @@
           <xm:sqref>E8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="73" id="{3050BD79-8CDD-4E38-BF7D-A9692315FFA0}">
+          <x14:cfRule type="expression" priority="73" id="{25FB66B9-1164-47E8-B38C-E46D8C9AAB8C}">
             <xm:f>AND((E9&lt;10),(E9&lt;&gt;solved!E9))</xm:f>
             <x14:dxf>
               <font>
@@ -10471,7 +10478,7 @@
           <xm:sqref>E9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="74" id="{B51DB8CB-D91E-46A7-9A43-CD39902FA8BA}">
+          <x14:cfRule type="expression" priority="74" id="{232117F8-BB70-428A-8AF0-30F3901AB9E2}">
             <xm:f>AND((F1&lt;10),(F1&lt;&gt;solved!F1))</xm:f>
             <x14:dxf>
               <font>
@@ -10482,7 +10489,7 @@
           <xm:sqref>F1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="75" id="{5670E0B6-9049-4550-818B-E940CCB067A9}">
+          <x14:cfRule type="expression" priority="75" id="{66B09495-6030-43CD-96BE-1620671845F8}">
             <xm:f>AND((F2&lt;10),(F2&lt;&gt;solved!F2))</xm:f>
             <x14:dxf>
               <font>
@@ -10493,7 +10500,7 @@
           <xm:sqref>F2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="76" id="{363C9EED-5952-4429-AE2A-3563723988D1}">
+          <x14:cfRule type="expression" priority="76" id="{5E11AB4D-E5F4-49D1-A2F0-FF7948F14080}">
             <xm:f>AND((F3&lt;10),(F3&lt;&gt;solved!F3))</xm:f>
             <x14:dxf>
               <font>
@@ -10504,7 +10511,7 @@
           <xm:sqref>F3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="77" id="{D5B59E65-E076-4A32-A87B-1FF5557E699C}">
+          <x14:cfRule type="expression" priority="77" id="{5F93C3D7-5BDA-49E0-9680-169A2AB819E8}">
             <xm:f>AND((F4&lt;10),(F4&lt;&gt;solved!F4))</xm:f>
             <x14:dxf>
               <font>
@@ -10515,7 +10522,7 @@
           <xm:sqref>F4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="78" id="{E3FA793C-22B6-44D0-9B11-8B34F190B720}">
+          <x14:cfRule type="expression" priority="78" id="{D077A170-1CF7-4033-B2AC-1532DAE3F3AC}">
             <xm:f>AND((F5&lt;10),(F5&lt;&gt;solved!F5))</xm:f>
             <x14:dxf>
               <font>
@@ -10526,7 +10533,7 @@
           <xm:sqref>F5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="79" id="{98FDAEBC-3844-4029-AFE5-DE8D452FE957}">
+          <x14:cfRule type="expression" priority="79" id="{30F63F22-61D4-4BDD-AC90-B593651717F1}">
             <xm:f>AND((F6&lt;10),(F6&lt;&gt;solved!F6))</xm:f>
             <x14:dxf>
               <font>
@@ -10537,7 +10544,7 @@
           <xm:sqref>F6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="80" id="{2C19D19D-E9F8-4810-8928-A2C0F940B267}">
+          <x14:cfRule type="expression" priority="80" id="{ABDD97E7-74F4-4111-9BE3-27A0A93252E5}">
             <xm:f>AND((F7&lt;10),(F7&lt;&gt;solved!F7))</xm:f>
             <x14:dxf>
               <font>
@@ -10548,7 +10555,7 @@
           <xm:sqref>F7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="81" id="{EB4D845F-2F4D-42A3-BB52-EB483E30ADF6}">
+          <x14:cfRule type="expression" priority="81" id="{12665854-BCE4-4294-9AA1-F186D4EC70AB}">
             <xm:f>AND((F8&lt;10),(F8&lt;&gt;solved!F8))</xm:f>
             <x14:dxf>
               <font>
@@ -10559,7 +10566,7 @@
           <xm:sqref>F8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="82" id="{795AF5F5-4374-4BA0-BE9D-17211AA4C0BE}">
+          <x14:cfRule type="expression" priority="82" id="{2A325E70-D589-4A3B-9765-5E4ACDE0BEB9}">
             <xm:f>AND((F9&lt;10),(F9&lt;&gt;solved!F9))</xm:f>
             <x14:dxf>
               <font>
@@ -10570,7 +10577,7 @@
           <xm:sqref>F9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="83" id="{C08AF1F2-5B99-4D40-8CF2-63E222103057}">
+          <x14:cfRule type="expression" priority="83" id="{6638C748-7ABB-4786-8033-E267DA86897B}">
             <xm:f>AND((G1&lt;10),(G1&lt;&gt;solved!G1))</xm:f>
             <x14:dxf>
               <font>
@@ -10581,7 +10588,7 @@
           <xm:sqref>G1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="84" id="{C0235744-AE27-4B1B-83EB-704F1B3767FD}">
+          <x14:cfRule type="expression" priority="84" id="{84139713-70CD-4110-9F6F-ADC65CEA49B4}">
             <xm:f>AND((G2&lt;10),(G2&lt;&gt;solved!G2))</xm:f>
             <x14:dxf>
               <font>
@@ -10592,7 +10599,7 @@
           <xm:sqref>G2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="85" id="{194E2B54-BE58-453B-8FFB-D667F54CEA7D}">
+          <x14:cfRule type="expression" priority="85" id="{21EF86D5-9765-4F2B-8073-4E4CE1CADCF0}">
             <xm:f>AND((G3&lt;10),(G3&lt;&gt;solved!G3))</xm:f>
             <x14:dxf>
               <font>
@@ -10603,7 +10610,7 @@
           <xm:sqref>G3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="86" id="{2B472846-2ECB-4EB7-8321-DCCB1D7F8CFE}">
+          <x14:cfRule type="expression" priority="86" id="{66E7FB6D-F8F0-44B6-8075-2B687076D15A}">
             <xm:f>AND((G4&lt;10),(G4&lt;&gt;solved!G4))</xm:f>
             <x14:dxf>
               <font>
@@ -10614,7 +10621,7 @@
           <xm:sqref>G4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="87" id="{B2AF7015-AE58-4A47-87D0-B860FDB8D952}">
+          <x14:cfRule type="expression" priority="87" id="{F0F36416-AB39-469D-8442-A841DC448D9E}">
             <xm:f>AND((G5&lt;10),(G5&lt;&gt;solved!G5))</xm:f>
             <x14:dxf>
               <font>
@@ -10625,7 +10632,7 @@
           <xm:sqref>G5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="88" id="{D0EDFDD7-68C2-4EC1-B49D-E89BA9FFC619}">
+          <x14:cfRule type="expression" priority="88" id="{1FEEB8E1-8D4F-4CC0-85EA-886735787D24}">
             <xm:f>AND((G6&lt;10),(G6&lt;&gt;solved!G6))</xm:f>
             <x14:dxf>
               <font>
@@ -10636,7 +10643,7 @@
           <xm:sqref>G6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="89" id="{5E1374C4-F06D-4177-89A6-5B107A63D8F9}">
+          <x14:cfRule type="expression" priority="89" id="{A618AFCA-DAAC-494E-BB2C-BBF457E26F4D}">
             <xm:f>AND((G7&lt;10),(G7&lt;&gt;solved!G7))</xm:f>
             <x14:dxf>
               <font>
@@ -10647,7 +10654,7 @@
           <xm:sqref>G7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="90" id="{F3F9BCF4-7878-481C-9D4A-179D208F32EA}">
+          <x14:cfRule type="expression" priority="90" id="{31FB9128-3B51-48B6-92F3-45E4A959D590}">
             <xm:f>AND((G8&lt;10),(G8&lt;&gt;solved!G8))</xm:f>
             <x14:dxf>
               <font>
@@ -10658,7 +10665,7 @@
           <xm:sqref>G8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="91" id="{CC9790C0-C14C-4C79-ABD8-A3C97050A7FC}">
+          <x14:cfRule type="expression" priority="91" id="{5FFC60F0-3C17-4096-8A34-C9574D14C7D8}">
             <xm:f>AND((G9&lt;10),(G9&lt;&gt;solved!G9))</xm:f>
             <x14:dxf>
               <font>
@@ -10669,7 +10676,7 @@
           <xm:sqref>G9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="92" id="{2C3071D0-6F35-4220-BADB-F190DDADC876}">
+          <x14:cfRule type="expression" priority="92" id="{19DE4864-6587-45F6-94A1-D0A55BFE8E12}">
             <xm:f>AND((H1&lt;10),(H1&lt;&gt;solved!H1))</xm:f>
             <x14:dxf>
               <font>
@@ -10680,7 +10687,7 @@
           <xm:sqref>H1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="93" id="{75FEA520-B8BF-44B6-8969-3EB2D056D517}">
+          <x14:cfRule type="expression" priority="93" id="{93904E80-78D0-4E29-B861-D1A829C63A5E}">
             <xm:f>AND((H2&lt;10),(H2&lt;&gt;solved!H2))</xm:f>
             <x14:dxf>
               <font>
@@ -10691,7 +10698,7 @@
           <xm:sqref>H2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="94" id="{56152ABE-4F7D-4BAB-B58F-F9AA103CE37D}">
+          <x14:cfRule type="expression" priority="94" id="{1FD38BD9-A7DA-4F95-8662-24EF60DD7A5D}">
             <xm:f>AND((H3&lt;10),(H3&lt;&gt;solved!H3))</xm:f>
             <x14:dxf>
               <font>
@@ -10702,7 +10709,7 @@
           <xm:sqref>H3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="95" id="{AF33FDBA-9400-4AAD-BC31-C860185EC31A}">
+          <x14:cfRule type="expression" priority="95" id="{25D7D0C5-62D8-47F8-B6F0-3A90888092AC}">
             <xm:f>AND((H4&lt;10),(H4&lt;&gt;solved!H4))</xm:f>
             <x14:dxf>
               <font>
@@ -10713,7 +10720,7 @@
           <xm:sqref>H4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="96" id="{CDC0A3AD-E060-4C36-B28C-5B1111C37FAC}">
+          <x14:cfRule type="expression" priority="96" id="{F4C3FEEC-B9B2-4E1F-A533-70F6F2AABFFB}">
             <xm:f>AND((H5&lt;10),(H5&lt;&gt;solved!H5))</xm:f>
             <x14:dxf>
               <font>
@@ -10724,7 +10731,7 @@
           <xm:sqref>H5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="97" id="{732018E5-F4F3-4866-8F2B-304415D7438F}">
+          <x14:cfRule type="expression" priority="97" id="{7521B46E-2045-49ED-85D7-39B9B84AF2FF}">
             <xm:f>AND((H6&lt;10),(H6&lt;&gt;solved!H6))</xm:f>
             <x14:dxf>
               <font>
@@ -10735,7 +10742,7 @@
           <xm:sqref>H6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="98" id="{5F616B5E-A91B-44D4-907B-5DDD5BA5C91E}">
+          <x14:cfRule type="expression" priority="98" id="{86E254F0-45DE-41A9-94D2-7E8E82BF866E}">
             <xm:f>AND((H7&lt;10),(H7&lt;&gt;solved!H7))</xm:f>
             <x14:dxf>
               <font>
@@ -10746,7 +10753,7 @@
           <xm:sqref>H7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="99" id="{73BC3FF3-80F4-4BAA-A7C1-F0ABE88F56E7}">
+          <x14:cfRule type="expression" priority="99" id="{32CF8610-8039-4E36-9077-56A3C53D8A86}">
             <xm:f>AND((H8&lt;10),(H8&lt;&gt;solved!H8))</xm:f>
             <x14:dxf>
               <font>
@@ -10757,7 +10764,7 @@
           <xm:sqref>H8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="100" id="{60BF6A20-A2FA-4B84-BD35-2D5960DE37D1}">
+          <x14:cfRule type="expression" priority="100" id="{462C1028-FE3E-4CBF-B2FF-B513AC742C39}">
             <xm:f>AND((H9&lt;10),(H9&lt;&gt;solved!H9))</xm:f>
             <x14:dxf>
               <font>
@@ -10768,7 +10775,7 @@
           <xm:sqref>H9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="101" id="{98E4C9A0-7BEB-4C68-86A3-84CC2D44E424}">
+          <x14:cfRule type="expression" priority="101" id="{2F70D053-B217-4CB7-8CAC-68C5CB9F10A9}">
             <xm:f>AND((I2&lt;10),(I2&lt;&gt;solved!I2))</xm:f>
             <x14:dxf>
               <font>
@@ -10779,7 +10786,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="102" id="{F5E02BEB-9564-475B-84C4-6E2040D1EF34}">
+          <x14:cfRule type="expression" priority="102" id="{F4F27232-5874-4F76-BB63-2D7B9686114F}">
             <xm:f>AND((I1&lt;10),(I1&lt;&gt;solved!I1))</xm:f>
             <x14:dxf>
               <font>
@@ -10790,7 +10797,7 @@
           <xm:sqref>I1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="103" id="{B717C49A-7A5D-47F7-8D18-5263C2C9692E}">
+          <x14:cfRule type="expression" priority="103" id="{F620DC8F-F89B-4D4F-9C54-D99947B01EF5}">
             <xm:f>AND((I3&lt;10),(I3&lt;&gt;solved!I3))</xm:f>
             <x14:dxf>
               <font>
@@ -10801,7 +10808,7 @@
           <xm:sqref>I3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="104" id="{D19ECBC3-1600-4FB6-8A20-2548473822AE}">
+          <x14:cfRule type="expression" priority="104" id="{F385A739-2D1A-4225-8EC1-977F20EDD08E}">
             <xm:f>AND((I4&lt;10),(I4&lt;&gt;solved!I4))</xm:f>
             <x14:dxf>
               <font>
@@ -10812,7 +10819,7 @@
           <xm:sqref>I4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="105" id="{7285EC32-8274-44D7-A01A-75B015EFD3D8}">
+          <x14:cfRule type="expression" priority="105" id="{97A6CEE3-7746-4569-89FE-2A6675E33E14}">
             <xm:f>AND((I5&lt;10),(I5&lt;&gt;solved!I5))</xm:f>
             <x14:dxf>
               <font>
@@ -10823,7 +10830,7 @@
           <xm:sqref>I5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="106" id="{3C7BE698-3628-43F7-A6D0-837E8A4531E2}">
+          <x14:cfRule type="expression" priority="106" id="{957520E9-2634-4BDA-A645-F080D0BA5AC5}">
             <xm:f>AND((I6&lt;10),(I6&lt;&gt;solved!I6))</xm:f>
             <x14:dxf>
               <font>
@@ -10834,7 +10841,7 @@
           <xm:sqref>I6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="107" id="{B6DBC365-F06B-40ED-B31F-502F13B62B76}">
+          <x14:cfRule type="expression" priority="107" id="{5CBD276C-5A89-49E6-A423-935B76FA5DBD}">
             <xm:f>AND((I7&lt;10),(I7&lt;&gt;solved!I7))</xm:f>
             <x14:dxf>
               <font>
@@ -10845,7 +10852,7 @@
           <xm:sqref>I7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="108" id="{64877415-8335-4143-A748-AD9296D05696}">
+          <x14:cfRule type="expression" priority="108" id="{3BA7F427-307E-4E52-AB6D-D7D79C22B720}">
             <xm:f>AND((I8&lt;10),(I8&lt;&gt;solved!I8))</xm:f>
             <x14:dxf>
               <font>
@@ -10856,7 +10863,7 @@
           <xm:sqref>I8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="109" id="{1842BE19-BDC2-47C0-8EE7-984388B94C99}">
+          <x14:cfRule type="expression" priority="109" id="{9BACD0C0-DAFB-4A4C-9140-7CCA6D4CDF70}">
             <xm:f>AND((I9&lt;10),(I9&lt;&gt;solved!I9))</xm:f>
             <x14:dxf>
               <font>
@@ -11254,9 +11261,9 @@
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="16"/>
+      <c r="E10" s="18"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="17"/>
+      <c r="G10" s="19"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -11362,108 +11369,108 @@
       <c r="J20" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="18" t="n">
+      <c r="C22" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="18" t="n">
+      <c r="D22" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="18" t="n">
+      <c r="E22" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="18" t="n">
+      <c r="F22" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="18" t="n">
+      <c r="G22" s="20" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="18" t="n">
+      <c r="B23" s="20" t="n">
         <v>15</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19" t="n">
+      <c r="C23" s="21"/>
+      <c r="D23" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19" t="n">
+      <c r="E23" s="21"/>
+      <c r="F23" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="G23" s="19" t="n">
+      <c r="G23" s="21" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="18" t="n">
+      <c r="B24" s="20" t="n">
         <v>35</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19" t="n">
+      <c r="C24" s="21"/>
+      <c r="D24" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19" t="n">
+      <c r="E24" s="21"/>
+      <c r="F24" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="G24" s="19" t="n">
+      <c r="G24" s="21" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="18" t="n">
+      <c r="B25" s="20" t="n">
         <v>45</v>
       </c>
-      <c r="C25" s="20" t="n">
+      <c r="C25" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="19" t="n">
+      <c r="D25" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19" t="n">
+      <c r="E25" s="21"/>
+      <c r="F25" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="G25" s="19" t="n">
+      <c r="G25" s="21" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="18" t="n">
+      <c r="B26" s="20" t="n">
         <v>75</v>
       </c>
-      <c r="C26" s="19" t="n">
+      <c r="C26" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19" t="n">
+      <c r="D26" s="21"/>
+      <c r="E26" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="20" t="n">
+      <c r="F26" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="G26" s="20" t="n">
+      <c r="G26" s="22" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="18" t="n">
+      <c r="B27" s="20" t="n">
         <v>95</v>
       </c>
-      <c r="C27" s="19" t="n">
+      <c r="C27" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19" t="n">
+      <c r="D27" s="21"/>
+      <c r="E27" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="F27" s="20" t="n">
+      <c r="F27" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="19"/>
+      <c r="G27" s="21"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B10">
@@ -12005,7 +12012,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="96" id="{A5F33DC4-18AC-458A-8643-DDAC8C3956CD}">
+          <x14:cfRule type="expression" priority="96" id="{3D7E83F3-7285-4533-A343-7EF270DD7169}">
             <xm:f>AND(($A$1&lt;10),($A$1&lt;&gt;solved!$A$1))</xm:f>
             <x14:dxf>
               <font>
@@ -12021,7 +12028,7 @@
           <xm:sqref>B1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="98" id="{DE3FEE18-855C-4857-81D6-10C6622F24D7}">
+          <x14:cfRule type="expression" priority="98" id="{BA666220-D9A7-4D57-B2AD-6F18C03AA67F}">
             <xm:f>AND((B2&lt;10),(B2&lt;&gt;solved!B2))</xm:f>
             <x14:dxf>
               <font>
@@ -12032,7 +12039,7 @@
           <xm:sqref>B2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="100" id="{72C3BC1F-AC98-49EB-A5F6-985749FCD444}">
+          <x14:cfRule type="expression" priority="100" id="{56902ACB-B68A-4B34-B6E4-94F5785F3D67}">
             <xm:f>AND((B3&lt;10),(B3&lt;&gt;solved!B3))</xm:f>
             <x14:dxf>
               <font>
@@ -12043,7 +12050,7 @@
           <xm:sqref>B3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="102" id="{6D2F4A23-9A3F-454D-92B2-BFD018991D7A}">
+          <x14:cfRule type="expression" priority="102" id="{54199E45-C3AE-4BC0-BCD1-41BCB0E62D5D}">
             <xm:f>AND(($A$4&lt;10),($A$4&lt;&gt;solved!$A$4))</xm:f>
             <x14:dxf>
               <font>
@@ -12054,7 +12061,7 @@
           <xm:sqref>B4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="104" id="{E0442AAF-EBB6-4184-8B16-7D33F449A069}">
+          <x14:cfRule type="expression" priority="104" id="{6E307C70-DE2C-43F5-8199-6D707E9D9A99}">
             <xm:f>AND((B5&lt;10),(B5&lt;&gt;solved!B5))</xm:f>
             <x14:dxf>
               <font>
@@ -12065,7 +12072,7 @@
           <xm:sqref>B5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="106" id="{3F6B69B0-3DAE-46AD-8C71-EC685EB0EBF4}">
+          <x14:cfRule type="expression" priority="106" id="{DD954D22-E08D-421B-B84C-BE3EF097E12B}">
             <xm:f>AND((B6&lt;10),(B6&lt;&gt;solved!B6))</xm:f>
             <x14:dxf>
               <font>
@@ -12076,7 +12083,7 @@
           <xm:sqref>B6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="108" id="{BA83C387-1E7A-487B-83F7-EFDCC0813D26}">
+          <x14:cfRule type="expression" priority="108" id="{8ED3251B-59B8-4823-ACA4-9538665A6A59}">
             <xm:f>AND((B7&lt;10),(B7&lt;&gt;solved!B7))</xm:f>
             <x14:dxf>
               <font>
@@ -12087,7 +12094,7 @@
           <xm:sqref>B7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="110" id="{C97C3439-5072-42D0-97DC-6FD5606A58C0}">
+          <x14:cfRule type="expression" priority="110" id="{FF41C37D-A881-4FAC-B9AF-4876B9871E16}">
             <xm:f>AND((B8&lt;10),(B8&lt;&gt;solved!B8))</xm:f>
             <x14:dxf>
               <font>
@@ -12098,7 +12105,7 @@
           <xm:sqref>B8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="112" id="{A1F07FF6-E030-4A60-96E2-DB82D626AA00}">
+          <x14:cfRule type="expression" priority="112" id="{47EFB529-A0A6-43C9-A0E1-4A8320D7206C}">
             <xm:f>AND((B9&lt;10),(B9&lt;&gt;solved!B9))</xm:f>
             <x14:dxf>
               <font>
@@ -12109,7 +12116,7 @@
           <xm:sqref>B9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="114" id="{F2D64F72-EF25-4D74-99B2-372D8A1729B0}">
+          <x14:cfRule type="expression" priority="114" id="{4AB04900-536E-4219-A057-DFDDD7B86C24}">
             <xm:f>AND((C1&lt;10),(C1&lt;&gt;solved!C1))</xm:f>
             <x14:dxf>
               <font>
@@ -12120,7 +12127,7 @@
           <xm:sqref>C1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="116" id="{B36DA600-2A60-48E7-9B50-37DDDB54485F}">
+          <x14:cfRule type="expression" priority="116" id="{57A06D35-E048-4051-8F19-5A8B116C19A7}">
             <xm:f>AND((C2&lt;10),(C2&lt;&gt;solved!C2))</xm:f>
             <x14:dxf>
               <font>
@@ -12131,7 +12138,7 @@
           <xm:sqref>C2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="118" id="{E768D9AD-8F1F-4EBD-B080-7FFF872D743C}">
+          <x14:cfRule type="expression" priority="118" id="{457F71D3-70C9-4A20-8416-404B68EC91A4}">
             <xm:f>AND((C3&lt;10),(C3&lt;&gt;solved!C3))</xm:f>
             <x14:dxf>
               <font>
@@ -12142,7 +12149,7 @@
           <xm:sqref>C3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="120" id="{15D9F02D-6A81-4D68-B320-C2F6E654D522}">
+          <x14:cfRule type="expression" priority="120" id="{863670F1-E05A-4160-84BA-891D3247CA67}">
             <xm:f>AND((C4&lt;10),(C4&lt;&gt;solved!C4))</xm:f>
             <x14:dxf>
               <font>
@@ -12153,7 +12160,7 @@
           <xm:sqref>C4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="122" id="{1A644C35-21C9-496F-AF6E-D24BDF40B03A}">
+          <x14:cfRule type="expression" priority="122" id="{6AC8A3CD-27D2-49D8-B05C-B26A2ABBE070}">
             <xm:f>AND((C5&lt;10),(C5&lt;&gt;solved!C5))</xm:f>
             <x14:dxf>
               <font>
@@ -12164,7 +12171,7 @@
           <xm:sqref>C5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="124" id="{EF1E1EAD-47E9-44F0-8049-7842236ACB44}">
+          <x14:cfRule type="expression" priority="124" id="{C09648BB-4361-40B3-B9D1-94B0B6ABE729}">
             <xm:f>AND((C6&lt;10),(C6&lt;&gt;solved!C6))</xm:f>
             <x14:dxf>
               <font>
@@ -12175,7 +12182,7 @@
           <xm:sqref>C6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="126" id="{4080516F-C26B-4C7C-81B3-204D7049D25B}">
+          <x14:cfRule type="expression" priority="126" id="{F5CBAA33-F65D-4BE5-9D61-A5AB2E3816A9}">
             <xm:f>AND((C7&lt;10),(C7&lt;&gt;solved!C7))</xm:f>
             <x14:dxf>
               <font>
@@ -12186,7 +12193,7 @@
           <xm:sqref>C7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="128" id="{948AA4C9-6B2B-4AAB-B6D5-C1B977690067}">
+          <x14:cfRule type="expression" priority="128" id="{B2CFE11C-5767-44A4-B87C-FF002FCEF53E}">
             <xm:f>AND((C8&lt;10),(C8&lt;&gt;solved!C8))</xm:f>
             <x14:dxf>
               <font>
@@ -12197,7 +12204,7 @@
           <xm:sqref>C8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="130" id="{65CB6F13-AB86-4BFC-8A57-D9AC4AED50F9}">
+          <x14:cfRule type="expression" priority="130" id="{865637FF-EACF-4D38-BA23-CA37AF32B19D}">
             <xm:f>AND((C9&lt;10),(C9&lt;&gt;solved!C9))</xm:f>
             <x14:dxf>
               <font>
@@ -12208,7 +12215,7 @@
           <xm:sqref>C9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="132" id="{7C4F41CE-70E0-4111-AEE9-926D2560F023}">
+          <x14:cfRule type="expression" priority="132" id="{194C80D3-D069-4675-B571-2A7070CD1A31}">
             <xm:f>AND((D1&lt;10),(D1&lt;&gt;solved!D1))</xm:f>
             <x14:dxf>
               <font>
@@ -12219,7 +12226,7 @@
           <xm:sqref>D1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="134" id="{DED4F0D2-8C70-4631-9B8D-6E3453C02350}">
+          <x14:cfRule type="expression" priority="134" id="{34F42F10-E0F5-42DE-A0F3-4FFAA1A57755}">
             <xm:f>AND((D2&lt;10),(D2&lt;&gt;solved!D2))</xm:f>
             <x14:dxf>
               <font>
@@ -12230,7 +12237,7 @@
           <xm:sqref>D2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="136" id="{73F287A5-5C3F-417B-9C16-F9CEDF85AAF3}">
+          <x14:cfRule type="expression" priority="136" id="{90A11F17-E483-4D76-90EE-15C657287354}">
             <xm:f>AND((D3&lt;10),(D3&lt;&gt;solved!D3))</xm:f>
             <x14:dxf>
               <font>
@@ -12241,7 +12248,7 @@
           <xm:sqref>D3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="138" id="{A9ACD475-4BA6-4228-A8F7-BB9B36C0B68D}">
+          <x14:cfRule type="expression" priority="138" id="{1ACD60DB-58DC-481E-A3F3-EBACE0F49D4E}">
             <xm:f>AND((D4&lt;10),(D4&lt;&gt;solved!D4))</xm:f>
             <x14:dxf>
               <font>
@@ -12252,7 +12259,7 @@
           <xm:sqref>D4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="140" id="{B683DC1D-4DB4-41E0-BC4D-41A67DB8C8A5}">
+          <x14:cfRule type="expression" priority="140" id="{CD4A5421-7241-406A-B028-E1B5E26465BD}">
             <xm:f>AND((D5&lt;10),(D5&lt;&gt;solved!D5))</xm:f>
             <x14:dxf>
               <font>
@@ -12263,7 +12270,7 @@
           <xm:sqref>D5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="142" id="{B5537281-E0AE-4B4D-87F8-5A58A3A7724F}">
+          <x14:cfRule type="expression" priority="142" id="{56B5787E-A620-4C29-9474-48BF5BE1A640}">
             <xm:f>AND((D6&lt;10),(D6&lt;&gt;solved!D6))</xm:f>
             <x14:dxf>
               <font>
@@ -12274,7 +12281,7 @@
           <xm:sqref>D6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="144" id="{44AB8440-A375-43BB-8B80-123B7955BDBA}">
+          <x14:cfRule type="expression" priority="144" id="{8684107F-FFB5-42B7-968F-9763B099BD57}">
             <xm:f>AND((D7&lt;10),(D7&lt;&gt;solved!D7))</xm:f>
             <x14:dxf>
               <font>
@@ -12285,7 +12292,7 @@
           <xm:sqref>D7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="146" id="{2CCF92F0-5FE6-431F-B3A0-2F7AC0B6F521}">
+          <x14:cfRule type="expression" priority="146" id="{5F10C036-C0C0-4154-877F-C8175FE0A324}">
             <xm:f>AND((D8&lt;10),(D8&lt;&gt;solved!D8))</xm:f>
             <x14:dxf>
               <font>
@@ -12296,7 +12303,7 @@
           <xm:sqref>D8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="148" id="{2F51354B-A3B8-43A0-A1E6-9827C9294DCF}">
+          <x14:cfRule type="expression" priority="148" id="{A52F47DA-A86D-4C78-B999-7146A4EF8F88}">
             <xm:f>AND((D9&lt;10),(D9&lt;&gt;solved!D9))</xm:f>
             <x14:dxf>
               <font>
@@ -12307,7 +12314,7 @@
           <xm:sqref>D9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="150" id="{9C26CED9-B9AA-4060-9C2A-D420C121F08E}">
+          <x14:cfRule type="expression" priority="150" id="{37FFF921-21B4-44B8-B9B6-BE7BD4688686}">
             <xm:f>AND((E1&lt;10),(E1&lt;&gt;solved!E1))</xm:f>
             <x14:dxf>
               <font>
@@ -12318,7 +12325,7 @@
           <xm:sqref>E1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="152" id="{10B85836-2943-454C-A2E2-89413AACB746}">
+          <x14:cfRule type="expression" priority="152" id="{35577575-6FC2-4F40-8550-D58645788A9D}">
             <xm:f>AND((E2&lt;10),(E2&lt;&gt;solved!E2))</xm:f>
             <x14:dxf>
               <font>
@@ -12329,7 +12336,7 @@
           <xm:sqref>E2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="154" id="{26131E92-ED5D-49E0-A9A0-10B2C0954ADA}">
+          <x14:cfRule type="expression" priority="154" id="{5220407C-86E3-4E7E-9A74-C9EF2F7B4232}">
             <xm:f>AND((E3&lt;10),(E3&lt;&gt;solved!E3))</xm:f>
             <x14:dxf>
               <font>
@@ -12340,7 +12347,7 @@
           <xm:sqref>E3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="156" id="{2627F490-D1FF-48FC-A12F-E5C3856174A8}">
+          <x14:cfRule type="expression" priority="156" id="{C0318241-D36D-43F7-BAC5-82EE6346FE4C}">
             <xm:f>AND((E4&lt;10),(E4&lt;&gt;solved!E4))</xm:f>
             <x14:dxf>
               <font>
@@ -12351,7 +12358,7 @@
           <xm:sqref>E4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="158" id="{E943E350-DDEE-42A8-9750-60BF88686530}">
+          <x14:cfRule type="expression" priority="158" id="{F7C73180-30C9-4EEF-879C-DBC795E26176}">
             <xm:f>AND((E5&lt;10),(E5&lt;&gt;solved!E5))</xm:f>
             <x14:dxf>
               <font>
@@ -12362,7 +12369,7 @@
           <xm:sqref>E5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="160" id="{C9812FF0-FB78-40EF-945D-B955DCDFEF12}">
+          <x14:cfRule type="expression" priority="160" id="{B3A9E112-A9C4-4B8B-87A2-CB7C2DEEFCB0}">
             <xm:f>AND((E6&lt;10),(E6&lt;&gt;solved!E6))</xm:f>
             <x14:dxf>
               <font>
@@ -12373,7 +12380,7 @@
           <xm:sqref>E6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="162" id="{5A1BEA4B-BDC3-41DA-9A6E-504F9BA0D1F6}">
+          <x14:cfRule type="expression" priority="162" id="{E7F4D690-9159-49F5-9719-3DCB1B772575}">
             <xm:f>AND((E7&lt;10),(E7&lt;&gt;solved!E7))</xm:f>
             <x14:dxf>
               <font>
@@ -12384,7 +12391,7 @@
           <xm:sqref>E7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="164" id="{60DECE9A-E593-47F0-A93E-CFEF3EF3D1F4}">
+          <x14:cfRule type="expression" priority="164" id="{74C21046-A21C-44E5-B7FB-784D167362C7}">
             <xm:f>AND((E8&lt;10),(E8&lt;&gt;solved!E8))</xm:f>
             <x14:dxf>
               <font>
@@ -12395,7 +12402,7 @@
           <xm:sqref>E8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="166" id="{DEEF8E83-DA5B-4B69-BA9D-5E77EAED2987}">
+          <x14:cfRule type="expression" priority="166" id="{30E9DCC3-718E-4767-B6A1-46E3A812CFFB}">
             <xm:f>AND((E9&lt;10),(E9&lt;&gt;solved!E9))</xm:f>
             <x14:dxf>
               <font>
@@ -12406,7 +12413,7 @@
           <xm:sqref>E9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="168" id="{DC4E9AB5-C482-4A93-92CB-3A1AAE9AFEAC}">
+          <x14:cfRule type="expression" priority="168" id="{368653A0-EF13-472D-956B-E8B14C462BFD}">
             <xm:f>AND((F1&lt;10),(F1&lt;&gt;solved!F1))</xm:f>
             <x14:dxf>
               <font>
@@ -12417,7 +12424,7 @@
           <xm:sqref>F1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="170" id="{E02D22D7-1F49-4BB2-86FB-DD352897B990}">
+          <x14:cfRule type="expression" priority="170" id="{92EE69BE-25EE-413D-AED5-D2EDDD815482}">
             <xm:f>AND((F2&lt;10),(F2&lt;&gt;solved!F2))</xm:f>
             <x14:dxf>
               <font>
@@ -12428,7 +12435,7 @@
           <xm:sqref>F2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="172" id="{402A3742-50A6-4055-9A13-865FCCE6486C}">
+          <x14:cfRule type="expression" priority="172" id="{D828C5B4-8360-4694-8759-28A4366B2C00}">
             <xm:f>AND((F3&lt;10),(F3&lt;&gt;solved!F3))</xm:f>
             <x14:dxf>
               <font>
@@ -12439,7 +12446,7 @@
           <xm:sqref>F3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="174" id="{40C85853-3353-4BB4-82C4-E09025BA8EB9}">
+          <x14:cfRule type="expression" priority="174" id="{F1D120BF-7AE0-4D7E-B380-5DB63181C1FE}">
             <xm:f>AND((F4&lt;10),(F4&lt;&gt;solved!F4))</xm:f>
             <x14:dxf>
               <font>
@@ -12450,7 +12457,7 @@
           <xm:sqref>F4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="176" id="{A094D0DB-E93B-4416-B740-521750CFF0D4}">
+          <x14:cfRule type="expression" priority="176" id="{F8F4AAF0-D2D0-4150-8CDD-2B69CB55CC38}">
             <xm:f>AND((F5&lt;10),(F5&lt;&gt;solved!F5))</xm:f>
             <x14:dxf>
               <font>
@@ -12461,7 +12468,7 @@
           <xm:sqref>F5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="178" id="{842B2540-F054-4B6A-A1A9-1CE3679E4195}">
+          <x14:cfRule type="expression" priority="178" id="{523059C1-2D92-4BEE-B64E-29D043E391A5}">
             <xm:f>AND((F6&lt;10),(F6&lt;&gt;solved!F6))</xm:f>
             <x14:dxf>
               <font>
@@ -12472,7 +12479,7 @@
           <xm:sqref>F6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="180" id="{27E07BB6-35E3-4F40-BA89-29E1F73843FB}">
+          <x14:cfRule type="expression" priority="180" id="{BE63BB70-E712-4320-AFA8-72102411B150}">
             <xm:f>AND((F7&lt;10),(F7&lt;&gt;solved!F7))</xm:f>
             <x14:dxf>
               <font>
@@ -12483,7 +12490,7 @@
           <xm:sqref>F7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="182" id="{3D815949-C5F0-4056-AA76-CF9BF51D84CA}">
+          <x14:cfRule type="expression" priority="182" id="{64ADCE41-67CD-4B87-9A33-662E1B6020DF}">
             <xm:f>AND((F8&lt;10),(F8&lt;&gt;solved!F8))</xm:f>
             <x14:dxf>
               <font>
@@ -12494,7 +12501,7 @@
           <xm:sqref>F8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="184" id="{59655A37-2349-4237-ABDF-8179C16C63F9}">
+          <x14:cfRule type="expression" priority="184" id="{CE719A57-852D-44D1-8D36-43DD8E6987CA}">
             <xm:f>AND((F9&lt;10),(F9&lt;&gt;solved!F9))</xm:f>
             <x14:dxf>
               <font>
@@ -12505,7 +12512,7 @@
           <xm:sqref>F9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="186" id="{C03DA796-9D55-4E1F-9BF9-2ADE3F57F24D}">
+          <x14:cfRule type="expression" priority="186" id="{4BFA1037-8630-4855-93EC-5B88D05628BA}">
             <xm:f>AND((G1&lt;10),(G1&lt;&gt;solved!G1))</xm:f>
             <x14:dxf>
               <font>
@@ -12516,7 +12523,7 @@
           <xm:sqref>G1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="188" id="{42442B2D-3D80-456B-BF74-A91AE6313462}">
+          <x14:cfRule type="expression" priority="188" id="{666922FE-15FD-4F2A-8696-E780A12E2842}">
             <xm:f>AND((G2&lt;10),(G2&lt;&gt;solved!G2))</xm:f>
             <x14:dxf>
               <font>
@@ -12527,7 +12534,7 @@
           <xm:sqref>G2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="190" id="{B0A420F0-E140-436F-BA54-BD8B57E04052}">
+          <x14:cfRule type="expression" priority="190" id="{F7FBD674-5FE9-427C-A77F-10C470EF2662}">
             <xm:f>AND((G3&lt;10),(G3&lt;&gt;solved!G3))</xm:f>
             <x14:dxf>
               <font>
@@ -12538,7 +12545,7 @@
           <xm:sqref>G3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="192" id="{C4143533-F5DB-4894-8870-8C20104A40B5}">
+          <x14:cfRule type="expression" priority="192" id="{EFBE7064-1E72-457F-A4C3-6430F255651F}">
             <xm:f>AND((G4&lt;10),(G4&lt;&gt;solved!G4))</xm:f>
             <x14:dxf>
               <font>
@@ -12549,7 +12556,7 @@
           <xm:sqref>G4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="194" id="{E3FFC3E8-547F-4258-96B6-D19C48801950}">
+          <x14:cfRule type="expression" priority="194" id="{19F6A1B5-F45E-4DA7-9D58-40EED63130CF}">
             <xm:f>AND((G5&lt;10),(G5&lt;&gt;solved!G5))</xm:f>
             <x14:dxf>
               <font>
@@ -12560,7 +12567,7 @@
           <xm:sqref>G5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="196" id="{F26C5C44-9175-4912-8A8D-CB692C723131}">
+          <x14:cfRule type="expression" priority="196" id="{56163F89-4161-4864-84EE-E77CF19F92F9}">
             <xm:f>AND((G6&lt;10),(G6&lt;&gt;solved!G6))</xm:f>
             <x14:dxf>
               <font>
@@ -12571,7 +12578,7 @@
           <xm:sqref>G6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="198" id="{C4FDC051-A7E3-4695-A29A-AECC22D5F97F}">
+          <x14:cfRule type="expression" priority="198" id="{AC50A389-C7E0-4AE4-99D5-6FC3C2B237A2}">
             <xm:f>AND((G7&lt;10),(G7&lt;&gt;solved!G7))</xm:f>
             <x14:dxf>
               <font>
@@ -12582,7 +12589,7 @@
           <xm:sqref>G7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="200" id="{40B63368-794F-4130-9077-6588CC71DF42}">
+          <x14:cfRule type="expression" priority="200" id="{5127763E-4549-44E0-9227-D41818FE8ACC}">
             <xm:f>AND((G8&lt;10),(G8&lt;&gt;solved!G8))</xm:f>
             <x14:dxf>
               <font>
@@ -12593,7 +12600,7 @@
           <xm:sqref>G8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="202" id="{4ED47FFC-DAA5-4F00-B3F1-C364A514B0EC}">
+          <x14:cfRule type="expression" priority="202" id="{13B9C070-A1B5-4267-8C30-2B7B93294630}">
             <xm:f>AND((G9&lt;10),(G9&lt;&gt;solved!G9))</xm:f>
             <x14:dxf>
               <font>
@@ -12604,7 +12611,7 @@
           <xm:sqref>G9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="204" id="{C7AA4172-5035-4BDC-A179-2980B1D8899D}">
+          <x14:cfRule type="expression" priority="204" id="{FC3620D7-86A0-4428-AA17-2688532D41BF}">
             <xm:f>AND((H1&lt;10),(H1&lt;&gt;solved!H1))</xm:f>
             <x14:dxf>
               <font>
@@ -12615,7 +12622,7 @@
           <xm:sqref>H1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="207" id="{6A92751A-B820-49E4-AA97-D0E988B4D0AA}">
+          <x14:cfRule type="expression" priority="207" id="{197FC64B-AE61-42D7-8750-CC1794BEB0ED}">
             <xm:f>AND((H2&lt;10),(H2&lt;&gt;solved!H2))</xm:f>
             <x14:dxf>
               <font>
@@ -12626,7 +12633,7 @@
           <xm:sqref>H2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="209" id="{FCAF241A-197E-4D45-B63A-4F5BC050EF35}">
+          <x14:cfRule type="expression" priority="209" id="{631F5198-6615-4F2E-A4E3-C14BD6FE5D69}">
             <xm:f>AND((H3&lt;10),(H3&lt;&gt;solved!H3))</xm:f>
             <x14:dxf>
               <font>
@@ -12637,7 +12644,7 @@
           <xm:sqref>H3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="211" id="{DAC5409A-A55A-4DCC-BF38-E8707D97732F}">
+          <x14:cfRule type="expression" priority="211" id="{5A6F8065-43D0-42AD-B677-9E218B12DC2D}">
             <xm:f>AND((H4&lt;10),(H4&lt;&gt;solved!H4))</xm:f>
             <x14:dxf>
               <font>
@@ -12648,7 +12655,7 @@
           <xm:sqref>H4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="213" id="{407933B1-7D55-4EBD-8B15-CB5CF078304C}">
+          <x14:cfRule type="expression" priority="213" id="{FCE39AEA-43D1-4AB2-B7ED-EDF3C4AD6CCF}">
             <xm:f>AND((H5&lt;10),(H5&lt;&gt;solved!H5))</xm:f>
             <x14:dxf>
               <font>
@@ -12659,7 +12666,7 @@
           <xm:sqref>H5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="215" id="{86FC9482-2BB1-4619-8F60-E0A2C69464D2}">
+          <x14:cfRule type="expression" priority="215" id="{179371DE-88FA-4790-B771-F7F3AD65F2F7}">
             <xm:f>AND((H6&lt;10),(H6&lt;&gt;solved!H6))</xm:f>
             <x14:dxf>
               <font>
@@ -12670,7 +12677,7 @@
           <xm:sqref>H6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="217" id="{403CDB2E-D3A0-4041-B05B-4A5CDCB17A62}">
+          <x14:cfRule type="expression" priority="217" id="{B5746C75-9394-43E8-AF72-E7BFA6122540}">
             <xm:f>AND((H7&lt;10),(H7&lt;&gt;solved!H7))</xm:f>
             <x14:dxf>
               <font>
@@ -12681,7 +12688,7 @@
           <xm:sqref>H7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="219" id="{EFB8A170-40ED-41AE-B53A-A0AD338C8781}">
+          <x14:cfRule type="expression" priority="219" id="{508BAEBB-4530-4936-BE6D-C110B2F0F68C}">
             <xm:f>AND((H8&lt;10),(H8&lt;&gt;solved!H8))</xm:f>
             <x14:dxf>
               <font>
@@ -12692,7 +12699,7 @@
           <xm:sqref>H8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="221" id="{EC3095E0-6633-4055-8871-E0FAB956EBEF}">
+          <x14:cfRule type="expression" priority="221" id="{BC94F243-816B-409C-A07F-88FC31BAEDAB}">
             <xm:f>AND((H9&lt;10),(H9&lt;&gt;solved!H9))</xm:f>
             <x14:dxf>
               <font>
@@ -12703,7 +12710,7 @@
           <xm:sqref>H9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="223" id="{8FC7EBAD-B428-4933-A520-D17627861E14}">
+          <x14:cfRule type="expression" priority="223" id="{2167D154-5D86-44DC-A04D-184787DCEF53}">
             <xm:f>AND((I1&lt;10),(I1&lt;&gt;solved!I1))</xm:f>
             <x14:dxf>
               <font>
@@ -12714,7 +12721,7 @@
           <xm:sqref>I1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="225" id="{BECCE285-568F-4927-8C1B-90B697D4C4E7}">
+          <x14:cfRule type="expression" priority="225" id="{F029EDC5-D01C-42D7-9CBF-A069449B282E}">
             <xm:f>AND((I2&lt;10),(I2&lt;&gt;solved!I2))</xm:f>
             <x14:dxf>
               <font>
@@ -12725,7 +12732,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="227" id="{C162B62C-30CC-46AB-A33A-28D5C95D36B7}">
+          <x14:cfRule type="expression" priority="227" id="{7499C2F7-C530-4879-956B-5560E783A0EF}">
             <xm:f>AND((I3&lt;10),(I3&lt;&gt;solved!I3))</xm:f>
             <x14:dxf>
               <font>
@@ -12736,7 +12743,7 @@
           <xm:sqref>I3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="229" id="{621A24C8-17F5-45D3-B32D-57293020CFC8}">
+          <x14:cfRule type="expression" priority="229" id="{9BDB1A65-EA80-4A74-94FC-88BC41151670}">
             <xm:f>AND((I4&lt;10),(I4&lt;&gt;solved!I4))</xm:f>
             <x14:dxf>
               <font>
@@ -12747,7 +12754,7 @@
           <xm:sqref>I4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="231" id="{6C14E1BA-3073-4C70-99D9-5A8B9B1358C3}">
+          <x14:cfRule type="expression" priority="231" id="{A6EE8BC4-38C2-42A0-964B-83D6CAD01F60}">
             <xm:f>AND((I5&lt;10),(I5&lt;&gt;solved!I5))</xm:f>
             <x14:dxf>
               <font>
@@ -12758,7 +12765,7 @@
           <xm:sqref>I5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="233" id="{F8DA2D40-8A31-4BD8-8A70-275EB5158B60}">
+          <x14:cfRule type="expression" priority="233" id="{A94AA036-E555-42F2-B33D-163CD575E53C}">
             <xm:f>AND((I6&lt;10),(I6&lt;&gt;solved!I6))</xm:f>
             <x14:dxf>
               <font>
@@ -12769,7 +12776,7 @@
           <xm:sqref>I6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="235" id="{61ACC6B7-97CB-4519-8A8B-FCBCD61BF6F2}">
+          <x14:cfRule type="expression" priority="235" id="{F0167AFC-1B34-4729-99EE-7EBCC4C28F26}">
             <xm:f>AND((I7&lt;10),(I7&lt;&gt;solved!I7))</xm:f>
             <x14:dxf>
               <font>
@@ -12780,7 +12787,7 @@
           <xm:sqref>I7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="237" id="{C9E1E2E7-8A9B-4AE5-8AD0-955E90AC1662}">
+          <x14:cfRule type="expression" priority="237" id="{635B1653-9B19-47EB-AA00-E730C51A8B20}">
             <xm:f>AND((I8&lt;10),(I8&lt;&gt;solved!I8))</xm:f>
             <x14:dxf>
               <font>
@@ -12791,7 +12798,7 @@
           <xm:sqref>I8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="239" id="{C8A6A08F-5D9D-4340-AF90-8FB4D31DAE53}">
+          <x14:cfRule type="expression" priority="239" id="{68B25FE2-20AE-48CC-AD36-CCA012189167}">
             <xm:f>AND((I9&lt;10),(I9&lt;&gt;solved!I9))</xm:f>
             <x14:dxf>
               <font>
@@ -12802,7 +12809,7 @@
           <xm:sqref>I9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="242" id="{A0CE263D-3B3F-40E0-BC40-6B5FD225AC51}">
+          <x14:cfRule type="expression" priority="242" id="{731A52F0-52F0-4940-B5FE-4037DA545442}">
             <xm:f>AND((J2&lt;10),(J2&lt;&gt;solved!J2))</xm:f>
             <x14:dxf>
               <font>
@@ -12813,7 +12820,7 @@
           <xm:sqref>J2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="244" id="{C75656C6-6D33-48A6-8167-D090DBFF56C9}">
+          <x14:cfRule type="expression" priority="244" id="{9FC1CA51-E1C2-4C1F-9B4E-F1A9DFE657D2}">
             <xm:f>AND((J3&lt;10),(J3&lt;&gt;solved!J3))</xm:f>
             <x14:dxf>
               <font>
@@ -12824,7 +12831,7 @@
           <xm:sqref>J3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="246" id="{A1C23B17-1713-4946-8E92-7937F24A9DBD}">
+          <x14:cfRule type="expression" priority="246" id="{DEA0A062-B7AA-443F-BCA2-4D2F202FFEA2}">
             <xm:f>AND((J4&lt;10),(J4&lt;&gt;solved!J4))</xm:f>
             <x14:dxf>
               <font>
@@ -12835,7 +12842,7 @@
           <xm:sqref>J4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="249" id="{E43F70CD-C6C2-4DDB-9CE3-F629474D4A34}">
+          <x14:cfRule type="expression" priority="249" id="{72E74AE8-8F50-4CDA-87A2-BF4230E01196}">
             <xm:f>AND((J5&lt;10),(J5&lt;&gt;solved!J5))</xm:f>
             <x14:dxf>
               <font>
@@ -12846,7 +12853,7 @@
           <xm:sqref>J5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="251" id="{4A16B8C8-D161-4F13-8A24-679D3AD23F00}">
+          <x14:cfRule type="expression" priority="251" id="{20ED7D67-F0F3-4CCC-8623-E7848AD09E12}">
             <xm:f>AND((J6&lt;10),(J6&lt;&gt;solved!J6))</xm:f>
             <x14:dxf>
               <font>
@@ -12857,7 +12864,7 @@
           <xm:sqref>J6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="253" id="{AA6C1B8F-4448-427F-85DD-5133E8551BC0}">
+          <x14:cfRule type="expression" priority="253" id="{5BE6F1BE-4440-4BE5-9FE7-E3C5BCA683CA}">
             <xm:f>AND((J7&lt;10),(J7&lt;&gt;solved!J7))</xm:f>
             <x14:dxf>
               <font>
@@ -12868,7 +12875,7 @@
           <xm:sqref>J7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="255" id="{F588F359-3C69-4375-8D94-264BBDE23540}">
+          <x14:cfRule type="expression" priority="255" id="{F09B3F47-74C7-4A50-9C9F-9B1043321CB3}">
             <xm:f>AND((J8&lt;10),(J8&lt;&gt;solved!J8))</xm:f>
             <x14:dxf>
               <font>
@@ -12879,7 +12886,7 @@
           <xm:sqref>J8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="257" id="{BDBDB1B5-FBC5-4097-A48F-343E901B901D}">
+          <x14:cfRule type="expression" priority="257" id="{793219EB-AFA2-4C2B-875B-80A2F49A2ED6}">
             <xm:f>AND((J9&lt;10),(J9&lt;&gt;solved!J9))</xm:f>
             <x14:dxf>
               <font>
@@ -13185,9 +13192,9 @@
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="16"/>
+      <c r="E10" s="18"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="17"/>
+      <c r="G10" s="19"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -13293,108 +13300,108 @@
       <c r="J20" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="18" t="n">
+      <c r="C22" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="18" t="n">
+      <c r="D22" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="18" t="n">
+      <c r="E22" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="18" t="n">
+      <c r="F22" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="18" t="n">
+      <c r="G22" s="20" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="18" t="n">
+      <c r="B23" s="20" t="n">
         <v>15</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19" t="n">
+      <c r="C23" s="21"/>
+      <c r="D23" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19" t="n">
+      <c r="E23" s="21"/>
+      <c r="F23" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="G23" s="19" t="n">
+      <c r="G23" s="21" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="18" t="n">
+      <c r="B24" s="20" t="n">
         <v>35</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19" t="n">
+      <c r="C24" s="21"/>
+      <c r="D24" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19" t="n">
+      <c r="E24" s="21"/>
+      <c r="F24" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="G24" s="19" t="n">
+      <c r="G24" s="21" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="18" t="n">
+      <c r="B25" s="20" t="n">
         <v>45</v>
       </c>
-      <c r="C25" s="20" t="n">
+      <c r="C25" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="19" t="n">
+      <c r="D25" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19" t="n">
+      <c r="E25" s="21"/>
+      <c r="F25" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="G25" s="19" t="n">
+      <c r="G25" s="21" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="18" t="n">
+      <c r="B26" s="20" t="n">
         <v>75</v>
       </c>
-      <c r="C26" s="19" t="n">
+      <c r="C26" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19" t="n">
+      <c r="D26" s="21"/>
+      <c r="E26" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="20" t="n">
+      <c r="F26" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="G26" s="20" t="n">
+      <c r="G26" s="22" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="18" t="n">
+      <c r="B27" s="20" t="n">
         <v>95</v>
       </c>
-      <c r="C27" s="19" t="n">
+      <c r="C27" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19" t="n">
+      <c r="D27" s="21"/>
+      <c r="E27" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="F27" s="20" t="n">
+      <c r="F27" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="19"/>
+      <c r="G27" s="21"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B10">
@@ -13894,9 +13901,9 @@
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="16"/>
+      <c r="E10" s="18"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="17"/>
+      <c r="G10" s="19"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -14002,108 +14009,108 @@
       <c r="J20" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="18" t="n">
+      <c r="C22" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="18" t="n">
+      <c r="D22" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="18" t="n">
+      <c r="E22" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="18" t="n">
+      <c r="F22" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="18" t="n">
+      <c r="G22" s="20" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="18" t="n">
+      <c r="B23" s="20" t="n">
         <v>15</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19" t="n">
+      <c r="C23" s="21"/>
+      <c r="D23" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19" t="n">
+      <c r="E23" s="21"/>
+      <c r="F23" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="G23" s="19" t="n">
+      <c r="G23" s="21" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="18" t="n">
+      <c r="B24" s="20" t="n">
         <v>35</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19" t="n">
+      <c r="C24" s="21"/>
+      <c r="D24" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19" t="n">
+      <c r="E24" s="21"/>
+      <c r="F24" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="G24" s="19" t="n">
+      <c r="G24" s="21" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="18" t="n">
+      <c r="B25" s="20" t="n">
         <v>45</v>
       </c>
-      <c r="C25" s="20" t="n">
+      <c r="C25" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="19" t="n">
+      <c r="D25" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19" t="n">
+      <c r="E25" s="21"/>
+      <c r="F25" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="G25" s="19" t="n">
+      <c r="G25" s="21" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="18" t="n">
+      <c r="B26" s="20" t="n">
         <v>75</v>
       </c>
-      <c r="C26" s="19" t="n">
+      <c r="C26" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19" t="n">
+      <c r="D26" s="21"/>
+      <c r="E26" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="20" t="n">
+      <c r="F26" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="G26" s="20" t="n">
+      <c r="G26" s="22" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="18" t="n">
+      <c r="B27" s="20" t="n">
         <v>95</v>
       </c>
-      <c r="C27" s="19" t="n">
+      <c r="C27" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19" t="n">
+      <c r="D27" s="21"/>
+      <c r="E27" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="F27" s="20" t="n">
+      <c r="F27" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="19"/>
+      <c r="G27" s="21"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B10">
@@ -14447,7 +14454,7 @@
       <c r="U1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21"/>
+      <c r="A2" s="23"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
       <c r="D2" s="9"/>
@@ -14473,7 +14480,7 @@
       <c r="U2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="21"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="11"/>
       <c r="C3" s="12"/>
       <c r="D3" s="13"/>
@@ -14495,7 +14502,7 @@
       <c r="U3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="21"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="n">
         <v>6</v>
@@ -14525,7 +14532,7 @@
       <c r="U4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="7"/>
@@ -14554,7 +14561,7 @@
       <c r="U5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="21"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
@@ -14576,7 +14583,7 @@
       <c r="U6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="21"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
@@ -14598,7 +14605,7 @@
       <c r="U7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8" t="n">
         <v>6</v>
@@ -14624,7 +14631,7 @@
       <c r="U8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="21"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="11"/>
       <c r="C9" s="12"/>
       <c r="D9" s="13" t="n">
@@ -14652,13 +14659,13 @@
       <c r="U9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="21"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="16"/>
+      <c r="E10" s="18"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="17"/>
+      <c r="G10" s="19"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -14764,113 +14771,113 @@
       <c r="J20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="23" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="18" t="n">
+      <c r="C22" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="18" t="n">
+      <c r="D22" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="18" t="n">
+      <c r="E22" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="18" t="n">
+      <c r="F22" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="18" t="n">
+      <c r="G22" s="20" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="18" t="n">
+      <c r="B23" s="20" t="n">
         <v>15</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19" t="n">
+      <c r="C23" s="21"/>
+      <c r="D23" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19" t="n">
+      <c r="E23" s="21"/>
+      <c r="F23" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="G23" s="19" t="n">
+      <c r="G23" s="21" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="18" t="n">
+      <c r="B24" s="20" t="n">
         <v>35</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19" t="n">
+      <c r="C24" s="21"/>
+      <c r="D24" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19" t="n">
+      <c r="E24" s="21"/>
+      <c r="F24" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="G24" s="19" t="n">
+      <c r="G24" s="21" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="18" t="n">
+      <c r="B25" s="20" t="n">
         <v>45</v>
       </c>
-      <c r="C25" s="20" t="n">
+      <c r="C25" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="19" t="n">
+      <c r="D25" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19" t="n">
+      <c r="E25" s="21"/>
+      <c r="F25" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="G25" s="19" t="n">
+      <c r="G25" s="21" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="18" t="n">
+      <c r="B26" s="20" t="n">
         <v>75</v>
       </c>
-      <c r="C26" s="19" t="n">
+      <c r="C26" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19" t="n">
+      <c r="D26" s="21"/>
+      <c r="E26" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="20" t="n">
+      <c r="F26" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="G26" s="20" t="n">
+      <c r="G26" s="22" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="18" t="n">
+      <c r="B27" s="20" t="n">
         <v>95</v>
       </c>
-      <c r="C27" s="19" t="n">
+      <c r="C27" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19" t="n">
+      <c r="D27" s="21"/>
+      <c r="E27" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="F27" s="20" t="n">
+      <c r="F27" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="19"/>
+      <c r="G27" s="21"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B10">
@@ -15200,22 +15207,22 @@
       <c r="R2" s="7"/>
       <c r="S2" s="8"/>
       <c r="T2" s="9"/>
-      <c r="U2" s="18" t="s">
+      <c r="U2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="V2" s="18" t="n">
+      <c r="V2" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="W2" s="18" t="n">
+      <c r="W2" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="X2" s="18" t="n">
+      <c r="X2" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="Y2" s="18" t="n">
+      <c r="Y2" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="Z2" s="18" t="n">
+      <c r="Z2" s="20" t="n">
         <v>9</v>
       </c>
     </row>
@@ -15244,18 +15251,18 @@
       <c r="R3" s="11"/>
       <c r="S3" s="12"/>
       <c r="T3" s="13"/>
-      <c r="U3" s="18" t="n">
+      <c r="U3" s="20" t="n">
         <v>15</v>
       </c>
-      <c r="V3" s="19"/>
-      <c r="W3" s="22" t="n">
+      <c r="V3" s="21"/>
+      <c r="W3" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="X3" s="19"/>
-      <c r="Y3" s="22" t="n">
+      <c r="X3" s="21"/>
+      <c r="Y3" s="24" t="n">
         <v>8</v>
       </c>
-      <c r="Z3" s="22" t="n">
+      <c r="Z3" s="24" t="n">
         <v>9</v>
       </c>
     </row>
@@ -15288,18 +15295,18 @@
       <c r="R4" s="2"/>
       <c r="S4" s="3"/>
       <c r="T4" s="4"/>
-      <c r="U4" s="18" t="n">
+      <c r="U4" s="20" t="n">
         <v>35</v>
       </c>
-      <c r="V4" s="19"/>
-      <c r="W4" s="22" t="n">
+      <c r="V4" s="21"/>
+      <c r="W4" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="X4" s="19"/>
-      <c r="Y4" s="22" t="n">
+      <c r="X4" s="21"/>
+      <c r="Y4" s="24" t="n">
         <v>8</v>
       </c>
-      <c r="Z4" s="22" t="n">
+      <c r="Z4" s="24" t="n">
         <v>9</v>
       </c>
     </row>
@@ -15344,20 +15351,20 @@
       <c r="R5" s="7"/>
       <c r="S5" s="8"/>
       <c r="T5" s="9"/>
-      <c r="U5" s="18" t="n">
+      <c r="U5" s="20" t="n">
         <v>45</v>
       </c>
-      <c r="V5" s="20" t="n">
+      <c r="V5" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="W5" s="22" t="n">
+      <c r="W5" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="X5" s="19"/>
-      <c r="Y5" s="22" t="n">
+      <c r="X5" s="21"/>
+      <c r="Y5" s="24" t="n">
         <v>8</v>
       </c>
-      <c r="Z5" s="22" t="n">
+      <c r="Z5" s="24" t="n">
         <v>9</v>
       </c>
     </row>
@@ -15392,20 +15399,20 @@
       <c r="R6" s="11"/>
       <c r="S6" s="12"/>
       <c r="T6" s="13"/>
-      <c r="U6" s="18" t="n">
+      <c r="U6" s="20" t="n">
         <v>75</v>
       </c>
-      <c r="V6" s="19" t="n">
+      <c r="V6" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="W6" s="19"/>
-      <c r="X6" s="19" t="n">
+      <c r="W6" s="21"/>
+      <c r="X6" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="Y6" s="20" t="n">
+      <c r="Y6" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="Z6" s="20" t="n">
+      <c r="Z6" s="22" t="n">
         <v>9</v>
       </c>
     </row>
@@ -15434,20 +15441,20 @@
       <c r="R7" s="2"/>
       <c r="S7" s="3"/>
       <c r="T7" s="4"/>
-      <c r="U7" s="18" t="n">
+      <c r="U7" s="20" t="n">
         <v>95</v>
       </c>
-      <c r="V7" s="19" t="n">
+      <c r="V7" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="W7" s="19"/>
-      <c r="X7" s="19" t="n">
+      <c r="W7" s="21"/>
+      <c r="X7" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="Y7" s="20" t="n">
+      <c r="Y7" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="Z7" s="19"/>
+      <c r="Z7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="7" t="s">
@@ -15509,7 +15516,7 @@
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="9"/>
-      <c r="E10" s="23"/>
+      <c r="E10" s="25"/>
       <c r="F10" s="8"/>
       <c r="H10" s="7"/>
       <c r="I10" s="8"/>
@@ -15898,45 +15905,45 @@
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="28"/>
       <c r="E2" s="8"/>
-      <c r="F2" s="27" t="n">
+      <c r="F2" s="29" t="n">
         <v>8</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="29" t="n">
+      <c r="G2" s="30"/>
+      <c r="H2" s="31" t="n">
         <v>3</v>
       </c>
       <c r="I2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="11"/>
-      <c r="B3" s="30"/>
+      <c r="B3" s="32"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="31" t="n">
+      <c r="D3" s="33" t="n">
         <v>5</v>
       </c>
       <c r="E3" s="12"/>
-      <c r="F3" s="32"/>
+      <c r="F3" s="34"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="33"/>
+      <c r="H3" s="35"/>
       <c r="I3" s="13" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="37" t="n">
+      <c r="F4" s="39" t="n">
         <v>4</v>
       </c>
-      <c r="G4" s="38"/>
-      <c r="H4" s="39" t="n">
+      <c r="G4" s="40"/>
+      <c r="H4" s="41" t="n">
         <v>1</v>
       </c>
       <c r="I4" s="4"/>
@@ -15954,47 +15961,47 @@
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="11"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="42" t="n">
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="44" t="n">
         <v>7</v>
       </c>
       <c r="E6" s="12"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="47"/>
       <c r="I6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
-      <c r="B7" s="46" t="n">
+      <c r="B7" s="48" t="n">
         <v>8</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="47"/>
+      <c r="D7" s="49"/>
       <c r="E7" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="F7" s="48"/>
+      <c r="F7" s="50"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="49"/>
+      <c r="H7" s="51"/>
       <c r="I7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="51" t="n">
+      <c r="B8" s="52"/>
+      <c r="C8" s="53" t="n">
         <v>9</v>
       </c>
-      <c r="D8" s="52"/>
+      <c r="D8" s="54"/>
       <c r="E8" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="53"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="55" t="n">
+      <c r="F8" s="55"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="57" t="n">
         <v>7</v>
       </c>
       <c r="I8" s="9"/>

</xml_diff>

<commit_message>
improved description and printing lines
</commit_message>
<xml_diff>
--- a/data/SDK.xlsx
+++ b/data/SDK.xlsx
@@ -96,10 +96,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
-    <numFmt numFmtId="166" formatCode="#,##0"/>
+    <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -565,15 +564,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -601,7 +600,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7503,7 +7502,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7514,30 +7513,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="3" t="n">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="C1" s="4" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D1" s="2" t="n">
-        <v>136</v>
+        <v>179</v>
       </c>
       <c r="E1" s="3" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F1" s="4" t="n">
-        <v>26</v>
+        <v>179</v>
       </c>
       <c r="G1" s="2" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="H1" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="I1" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="I1" s="4" t="n">
+        <v>17</v>
+      </c>
       <c r="K1" s="5" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "1")=9, 1, "")</f>
         <v/>
@@ -7548,31 +7549,31 @@
     </row>
     <row r="2" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B2" s="8" t="n">
+        <v>9</v>
+      </c>
+      <c r="C2" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <v>14</v>
+      </c>
+      <c r="E2" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="9" t="n">
+      <c r="G2" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2" s="8" t="n">
+      <c r="H2" s="8" t="n">
+        <v>14</v>
+      </c>
+      <c r="I2" s="9" t="n">
         <v>5</v>
-      </c>
-      <c r="F2" s="9" t="n">
-        <v>8</v>
-      </c>
-      <c r="G2" s="7" t="n">
-        <v>9</v>
-      </c>
-      <c r="H2" s="8" t="n">
-        <v>7</v>
-      </c>
-      <c r="I2" s="9" t="n">
-        <v>3</v>
       </c>
       <c r="K2" s="10" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "2")=9, 2, "")</f>
@@ -7581,31 +7582,31 @@
     </row>
     <row r="3" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3" s="12" t="n">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="C3" s="13" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="D3" s="11" t="n">
-        <v>13</v>
-      </c>
       <c r="E3" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="F3" s="13" t="n">
+        <v>47</v>
+      </c>
+      <c r="G3" s="11" t="n">
+        <v>47</v>
+      </c>
+      <c r="H3" s="12" t="n">
         <v>9</v>
       </c>
-      <c r="F3" s="13" t="n">
-        <v>7</v>
-      </c>
-      <c r="G3" s="11" t="n">
-        <v>18</v>
-      </c>
-      <c r="H3" s="12" t="n">
-        <v>6</v>
-      </c>
       <c r="I3" s="13" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K3" s="10" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "3")=9, 3, "")</f>
@@ -7614,97 +7615,97 @@
     </row>
     <row r="4" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E4" s="3" t="n">
+        <v>479</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>479</v>
+      </c>
+      <c r="H4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="F4" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="H4" s="3" t="n">
-        <v>5</v>
-      </c>
       <c r="I4" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="K4" s="14" t="n">
+        <v>1679</v>
+      </c>
+      <c r="K4" s="14" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "4")=9, 4, "")</f>
-        <v>4</v>
+        <v/>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="n">
-        <v>9</v>
+        <v>369</v>
       </c>
       <c r="B5" s="8" t="n">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="C5" s="9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="7" t="n">
-        <v>567</v>
+        <v>14789</v>
       </c>
       <c r="E5" s="8" t="n">
-        <v>78</v>
+        <v>479</v>
       </c>
       <c r="F5" s="9" t="n">
-        <v>56</v>
+        <v>14789</v>
       </c>
       <c r="G5" s="7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H5" s="8" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="I5" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="10" t="str">
+        <v>1679</v>
+      </c>
+      <c r="K5" s="14" t="n">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "5")=9, 5, "")</f>
-        <v/>
+        <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="C6" s="13" t="n">
+        <v>19</v>
+      </c>
+      <c r="D6" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" s="12" t="n">
+        <v>49</v>
+      </c>
+      <c r="F6" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="B6" s="12" t="n">
-        <v>25</v>
-      </c>
-      <c r="C6" s="13" t="n">
-        <v>7</v>
-      </c>
-      <c r="D6" s="11" t="n">
-        <v>15</v>
-      </c>
-      <c r="E6" s="12" t="n">
-        <v>18</v>
-      </c>
-      <c r="F6" s="13" t="n">
-        <v>4</v>
-      </c>
       <c r="G6" s="11" t="n">
-        <v>3</v>
+        <v>249</v>
       </c>
       <c r="H6" s="12" t="n">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="I6" s="13" t="n">
-        <v>9</v>
+        <v>129</v>
       </c>
       <c r="K6" s="10" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "6")=9, 6, "")</f>
@@ -7713,31 +7714,31 @@
     </row>
     <row r="7" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
+        <v>269</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>69</v>
+      </c>
+      <c r="E7" s="3" t="n">
         <v>5</v>
-      </c>
-      <c r="B7" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="C7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="E7" s="3" t="n">
-        <v>4</v>
       </c>
       <c r="F7" s="4" t="n">
         <v>3</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I7" s="4" t="n">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="K7" s="10" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "7")=9, 7, "")</f>
@@ -7746,28 +7747,28 @@
     </row>
     <row r="8" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="n">
+        <v>369</v>
+      </c>
+      <c r="B8" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="C8" s="9" t="n">
+        <v>169</v>
+      </c>
+      <c r="D8" s="7" t="n">
+        <v>679</v>
+      </c>
+      <c r="E8" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" s="9" t="n">
+        <v>79</v>
+      </c>
+      <c r="G8" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="B8" s="8" t="n">
-        <v>7</v>
-      </c>
-      <c r="C8" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="D8" s="7" t="n">
-        <v>9</v>
-      </c>
-      <c r="E8" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="F8" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="7" t="n">
+      <c r="H8" s="8" t="n">
         <v>5</v>
-      </c>
-      <c r="H8" s="8" t="n">
-        <v>3</v>
       </c>
       <c r="I8" s="9" t="n">
         <v>4</v>
@@ -7779,35 +7780,35 @@
     </row>
     <row r="9" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="n">
+        <v>29</v>
+      </c>
+      <c r="B9" s="12" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" s="13" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" s="11" t="n">
+        <v>489</v>
+      </c>
+      <c r="E9" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="13" t="n">
+        <v>489</v>
+      </c>
+      <c r="G9" s="11" t="n">
+        <v>29</v>
+      </c>
+      <c r="H9" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="I9" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="B9" s="12" t="n">
-        <v>9</v>
-      </c>
-      <c r="C9" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="D9" s="11" t="n">
-        <v>57</v>
-      </c>
-      <c r="E9" s="12" t="n">
-        <v>27</v>
-      </c>
-      <c r="F9" s="13" t="n">
-        <v>25</v>
-      </c>
-      <c r="G9" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="H9" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" s="13" t="n">
-        <v>8</v>
-      </c>
-      <c r="K9" s="15" t="n">
+      <c r="K9" s="15" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "9")=9, 9, "")</f>
-        <v>9</v>
+        <v/>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -8147,7 +8148,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="110" id="{80E2A98F-D03A-44D8-B4F6-5CB6E15F7073}">
+          <x14:cfRule type="expression" priority="110" id="{A0CE247A-BB30-4C32-94B0-64B4D770634B}">
             <xm:f>AND((A2&lt;10),(A2&lt;&gt;solved!A2))</xm:f>
             <x14:dxf>
               <font>
@@ -8163,7 +8164,7 @@
           <xm:sqref>A2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="111" id="{2E9C3026-3FB0-444C-88EA-DF88E03E8740}">
+          <x14:cfRule type="expression" priority="111" id="{6FD9797F-5D61-46BD-A417-2D2573F0DF1C}">
             <xm:f>AND((A3&lt;10),(A3&lt;&gt;solved!A3))</xm:f>
             <x14:dxf>
               <font>
@@ -8174,7 +8175,7 @@
           <xm:sqref>A3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="112" id="{FD14179C-C0C8-4EAC-88AE-FD3489DB1E39}">
+          <x14:cfRule type="expression" priority="112" id="{43B0E9C6-958B-4D61-A562-70BC1FEBEEE9}">
             <xm:f>AND((A5&lt;10),(A5&lt;&gt;solved!A5))</xm:f>
             <x14:dxf>
               <font>
@@ -8185,7 +8186,7 @@
           <xm:sqref>A5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="113" id="{612E4C6B-16F3-4CBD-887E-354E76966988}">
+          <x14:cfRule type="expression" priority="113" id="{9F15AC88-9AB6-40D2-B4F3-C0385EA27EB6}">
             <xm:f>AND((A6&lt;10),(A6&lt;&gt;solved!A6))</xm:f>
             <x14:dxf>
               <font>
@@ -8196,7 +8197,7 @@
           <xm:sqref>A6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="114" id="{99958045-6EB6-453A-95C8-3BE2204A1B80}">
+          <x14:cfRule type="expression" priority="114" id="{805B108C-F96E-46D3-8E7A-5E89C66AD6E6}">
             <xm:f>AND((A7&lt;10),(A7&lt;&gt;solved!A7))</xm:f>
             <x14:dxf>
               <font>
@@ -8207,7 +8208,7 @@
           <xm:sqref>A7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="115" id="{3270465F-7755-4018-B376-9392842A3FBD}">
+          <x14:cfRule type="expression" priority="115" id="{3443F93F-D7C6-456D-88B5-BE41C5D03481}">
             <xm:f>AND((A8&lt;10),(A8&lt;&gt;solved!A8))</xm:f>
             <x14:dxf>
               <font>
@@ -8218,7 +8219,7 @@
           <xm:sqref>A8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="116" id="{66ABF0FE-8583-47CA-8983-8DBDAE899EBF}">
+          <x14:cfRule type="expression" priority="116" id="{3E92E638-8C3C-4A20-9890-C88CF966F934}">
             <xm:f>AND((A9&lt;10),(A9&lt;&gt;solved!A9))</xm:f>
             <x14:dxf>
               <font>
@@ -8229,7 +8230,7 @@
           <xm:sqref>A9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="117" id="{6D95653D-9A27-487A-BB56-8285A0622CD4}">
+          <x14:cfRule type="expression" priority="117" id="{29F71C6E-9D70-4D3F-BC72-9C89C113FAC4}">
             <xm:f>AND((B1&lt;10),(B1&lt;&gt;solved!B1))</xm:f>
             <x14:dxf>
               <font>
@@ -8240,7 +8241,7 @@
           <xm:sqref>B1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="118" id="{62D6A893-AFEA-45E0-9CD5-E5D1585468C8}">
+          <x14:cfRule type="expression" priority="118" id="{B98D4C62-81A2-4860-8A21-64C024BEE684}">
             <xm:f>AND((B2&lt;10),(B2&lt;&gt;solved!B2))</xm:f>
             <x14:dxf>
               <font>
@@ -8251,7 +8252,7 @@
           <xm:sqref>B2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="119" id="{1834F5BD-BE86-4238-BC5A-E46F4459AD42}">
+          <x14:cfRule type="expression" priority="119" id="{6D5737D4-363F-40DF-8333-75242925AE60}">
             <xm:f>AND((B3&lt;10),(B3&lt;&gt;solved!B3))</xm:f>
             <x14:dxf>
               <font>
@@ -8262,7 +8263,7 @@
           <xm:sqref>B3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="120" id="{A06E54D9-373D-4C68-9473-8E6EE8EF413E}">
+          <x14:cfRule type="expression" priority="120" id="{9AE74043-B7F8-4AAC-9399-EA59A273BD94}">
             <xm:f>AND((B4&lt;10),(B4&lt;&gt;solved!B4))</xm:f>
             <x14:dxf>
               <font>
@@ -8273,7 +8274,7 @@
           <xm:sqref>B4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="121" id="{61D75D20-2333-4281-B1C7-00DE45BEDBF0}">
+          <x14:cfRule type="expression" priority="121" id="{331E745B-FAE4-478F-B964-2464E9645E74}">
             <xm:f>AND((B5&lt;10),(B5&lt;&gt;solved!B5))</xm:f>
             <x14:dxf>
               <font>
@@ -8284,7 +8285,7 @@
           <xm:sqref>B5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="122" id="{7F6A7331-8563-48EE-95B2-98C071A69DBD}">
+          <x14:cfRule type="expression" priority="122" id="{ABC847D7-7D87-4CF2-AFCD-3163D01D7612}">
             <xm:f>AND((B6&lt;10),(B6&lt;&gt;solved!B6))</xm:f>
             <x14:dxf>
               <font>
@@ -8295,7 +8296,7 @@
           <xm:sqref>B6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="123" id="{8BFC5EA4-CE53-4DC0-A163-ECFF815DC1F2}">
+          <x14:cfRule type="expression" priority="123" id="{90107C3A-BE23-42E2-BC86-2459349ACD6B}">
             <xm:f>AND((B7&lt;10),(B7&lt;&gt;solved!B7))</xm:f>
             <x14:dxf>
               <font>
@@ -8306,7 +8307,7 @@
           <xm:sqref>B7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="124" id="{1BC1CA52-9E5A-4383-A459-B9EB68237B26}">
+          <x14:cfRule type="expression" priority="124" id="{449257AB-9BFF-4D14-A485-C813C98D7DF0}">
             <xm:f>AND((B8&lt;10),(B8&lt;&gt;solved!B8))</xm:f>
             <x14:dxf>
               <font>
@@ -8317,7 +8318,7 @@
           <xm:sqref>B8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="125" id="{E0AB4312-203D-4053-AF46-1DD8EFA3E7BC}">
+          <x14:cfRule type="expression" priority="125" id="{4BF9B930-41C0-49BF-B53C-BD969D1288BF}">
             <xm:f>AND((B9&lt;10),(B9&lt;&gt;solved!B9))</xm:f>
             <x14:dxf>
               <font>
@@ -8328,7 +8329,7 @@
           <xm:sqref>B9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="126" id="{90D6328A-F0B8-4BAB-8CB6-146473404550}">
+          <x14:cfRule type="expression" priority="126" id="{DEF6E48F-1B2F-4338-B4AB-FC62F3ACE332}">
             <xm:f>AND((C1&lt;10),(C1&lt;&gt;solved!C1))</xm:f>
             <x14:dxf>
               <font>
@@ -8339,7 +8340,7 @@
           <xm:sqref>C1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="127" id="{8FD2449E-E01D-4DFD-9529-F05349F09ADC}">
+          <x14:cfRule type="expression" priority="127" id="{80BCBC30-FF99-485B-9CEC-66BB3B3E33E3}">
             <xm:f>AND((C2&lt;10),(C2&lt;&gt;solved!C2))</xm:f>
             <x14:dxf>
               <font>
@@ -8350,7 +8351,7 @@
           <xm:sqref>C2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="128" id="{25FFCA76-A7AD-48F4-A510-E2CF6A00CA24}">
+          <x14:cfRule type="expression" priority="128" id="{EB216865-F8C1-4C47-BD38-7F126FD7F329}">
             <xm:f>AND((C3&lt;10),(C3&lt;&gt;solved!C3))</xm:f>
             <x14:dxf>
               <font>
@@ -8361,7 +8362,7 @@
           <xm:sqref>C3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="129" id="{307486C2-36A0-46EF-B9E8-B7D3E71DBFD7}">
+          <x14:cfRule type="expression" priority="129" id="{DC5BE59C-B053-4323-B1B1-1D502F6145E9}">
             <xm:f>AND((C4&lt;10),(C4&lt;&gt;solved!C4))</xm:f>
             <x14:dxf>
               <font>
@@ -8372,7 +8373,7 @@
           <xm:sqref>C4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="130" id="{8CAEEE28-946D-4AB2-B1D8-50CAADCD7FD1}">
+          <x14:cfRule type="expression" priority="130" id="{53AA1046-8474-4E58-AF00-3E575880C6B0}">
             <xm:f>AND((C5&lt;10),(C5&lt;&gt;solved!C5))</xm:f>
             <x14:dxf>
               <font>
@@ -8383,7 +8384,7 @@
           <xm:sqref>C5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="131" id="{852417A6-7B94-4914-A415-FB117DFF7AEB}">
+          <x14:cfRule type="expression" priority="131" id="{A010DEEE-FC44-484F-ABA0-8FBACA867D57}">
             <xm:f>AND((C6&lt;10),(C6&lt;&gt;solved!C6))</xm:f>
             <x14:dxf>
               <font>
@@ -8394,7 +8395,7 @@
           <xm:sqref>C6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="132" id="{A3EB36EE-67F1-47AB-A2ED-C060D6E160F7}">
+          <x14:cfRule type="expression" priority="132" id="{E7BA7A20-6471-47AF-AD32-254929B62CC0}">
             <xm:f>AND((C7&lt;10),(C7&lt;&gt;solved!C7))</xm:f>
             <x14:dxf>
               <font>
@@ -8405,7 +8406,7 @@
           <xm:sqref>C7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="133" id="{7DA54074-3872-4657-83EF-F0EDCF6060AF}">
+          <x14:cfRule type="expression" priority="133" id="{FE703F6C-A994-40FB-B06A-E83070E0C44D}">
             <xm:f>AND((C8&lt;10),(C8&lt;&gt;solved!C8))</xm:f>
             <x14:dxf>
               <font>
@@ -8416,7 +8417,7 @@
           <xm:sqref>C8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="134" id="{87B625C1-61DE-4BE0-8D40-CCFC2495861A}">
+          <x14:cfRule type="expression" priority="134" id="{121A257F-E0AA-4EE0-B526-39B0A9B92FA2}">
             <xm:f>AND((C9&lt;10),(C9&lt;&gt;solved!C9))</xm:f>
             <x14:dxf>
               <font>
@@ -8427,7 +8428,7 @@
           <xm:sqref>C9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="135" id="{E1A62F1E-8696-415D-8433-165461147419}">
+          <x14:cfRule type="expression" priority="135" id="{E5338D6F-F600-4150-916B-11C0FB8EAF79}">
             <xm:f>AND((D1&lt;10),(D1&lt;&gt;solved!D1))</xm:f>
             <x14:dxf>
               <font>
@@ -8438,7 +8439,7 @@
           <xm:sqref>D1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="136" id="{85C115C4-F1DF-4E7B-A4B0-183BF064ABB8}">
+          <x14:cfRule type="expression" priority="136" id="{53D8F0C3-7A9C-4B73-A4AE-322037EB38AC}">
             <xm:f>AND((D2&lt;10),(D2&lt;&gt;solved!D2))</xm:f>
             <x14:dxf>
               <font>
@@ -8449,7 +8450,7 @@
           <xm:sqref>D2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="137" id="{641ACFB5-4684-4E50-84AC-1C31FCD8405C}">
+          <x14:cfRule type="expression" priority="137" id="{8058ACD1-9480-4D5C-A75B-4C74B1D34F1C}">
             <xm:f>AND((D3&lt;10),(D3&lt;&gt;solved!D3))</xm:f>
             <x14:dxf>
               <font>
@@ -8460,7 +8461,7 @@
           <xm:sqref>D3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="138" id="{2E17406A-C6C0-41AC-A1C5-F4D281204700}">
+          <x14:cfRule type="expression" priority="138" id="{C4355A7C-B4B8-42EC-9F1B-D5C93CC74DCC}">
             <xm:f>AND((D4&lt;10),(D4&lt;&gt;solved!D4))</xm:f>
             <x14:dxf>
               <font>
@@ -8471,7 +8472,7 @@
           <xm:sqref>D4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="139" id="{4020B088-B064-42E5-8FA4-98FE739E9329}">
+          <x14:cfRule type="expression" priority="139" id="{6533371F-9B13-4CA0-B9BB-9FC37CF0A117}">
             <xm:f>AND((D5&lt;10),(D5&lt;&gt;solved!D5))</xm:f>
             <x14:dxf>
               <font>
@@ -8482,7 +8483,7 @@
           <xm:sqref>D5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="140" id="{21BC7CA9-AAB8-4A48-B040-587948F96791}">
+          <x14:cfRule type="expression" priority="140" id="{9DF7EE55-E580-4A57-8252-D13D8820EFDD}">
             <xm:f>AND((D6&lt;10),(D6&lt;&gt;solved!D6))</xm:f>
             <x14:dxf>
               <font>
@@ -8493,7 +8494,7 @@
           <xm:sqref>D6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="141" id="{C59ECA25-688E-47BD-9F2A-48D0B374F120}">
+          <x14:cfRule type="expression" priority="141" id="{C93F7B85-18E9-4283-A194-157053D38680}">
             <xm:f>AND((D7&lt;10),(D7&lt;&gt;solved!D7))</xm:f>
             <x14:dxf>
               <font>
@@ -8504,7 +8505,7 @@
           <xm:sqref>D7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="142" id="{763EA1A3-D0FB-42F6-B988-32C432EB38EC}">
+          <x14:cfRule type="expression" priority="142" id="{1CDE3FE0-891E-48A3-B668-C24060E77D26}">
             <xm:f>AND((D8&lt;10),(D8&lt;&gt;solved!D8))</xm:f>
             <x14:dxf>
               <font>
@@ -8515,7 +8516,7 @@
           <xm:sqref>D8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="143" id="{71418EC9-20F2-434D-BC82-5454DDC0B2D1}">
+          <x14:cfRule type="expression" priority="143" id="{E1A7BCC5-48CD-4DD0-931F-52489B4EB64B}">
             <xm:f>AND((D9&lt;10),(D9&lt;&gt;solved!D9))</xm:f>
             <x14:dxf>
               <font>
@@ -8526,7 +8527,7 @@
           <xm:sqref>D9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="144" id="{487C1E8F-30E9-42F4-9C15-5D5C41EFB796}">
+          <x14:cfRule type="expression" priority="144" id="{FB401FE6-7B4F-47CA-A2D8-89FEAB173F51}">
             <xm:f>AND((E1&lt;10),(E1&lt;&gt;solved!E1))</xm:f>
             <x14:dxf>
               <font>
@@ -8537,7 +8538,7 @@
           <xm:sqref>E1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="145" id="{D4F06D1F-A09D-4C12-89CF-4A18CF80E355}">
+          <x14:cfRule type="expression" priority="145" id="{B03A5ACF-3845-4BE8-9EEA-533C5B9D59B4}">
             <xm:f>AND((E2&lt;10),(E2&lt;&gt;solved!E2))</xm:f>
             <x14:dxf>
               <font>
@@ -8548,7 +8549,7 @@
           <xm:sqref>E2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="146" id="{F3FA2EF2-BF26-4554-A4FD-F121C08E83E6}">
+          <x14:cfRule type="expression" priority="146" id="{572D6DA2-EC00-42CC-A03A-7C1ABF95DE37}">
             <xm:f>AND((E3&lt;10),(E3&lt;&gt;solved!E3))</xm:f>
             <x14:dxf>
               <font>
@@ -8559,7 +8560,7 @@
           <xm:sqref>E3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="147" id="{ADBD6BD0-2055-4E2D-B689-EEF06124907B}">
+          <x14:cfRule type="expression" priority="147" id="{5B728D68-CCD2-4AD3-A6DD-2236F695C15F}">
             <xm:f>AND((E4&lt;10),(E4&lt;&gt;solved!E4))</xm:f>
             <x14:dxf>
               <font>
@@ -8570,7 +8571,7 @@
           <xm:sqref>E4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="148" id="{1D5F2265-C05E-4489-A49E-92367C68263F}">
+          <x14:cfRule type="expression" priority="148" id="{807F6EFE-618C-4652-93B9-1938E66EC2C0}">
             <xm:f>AND((E5&lt;10),(E5&lt;&gt;solved!E5))</xm:f>
             <x14:dxf>
               <font>
@@ -8581,7 +8582,7 @@
           <xm:sqref>E5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="149" id="{773715E0-E178-44D0-9767-74CB8F2480E1}">
+          <x14:cfRule type="expression" priority="149" id="{76DCAE1B-AD5A-44D8-BBCA-724E836DA357}">
             <xm:f>AND((E6&lt;10),(E6&lt;&gt;solved!E6))</xm:f>
             <x14:dxf>
               <font>
@@ -8592,7 +8593,7 @@
           <xm:sqref>E6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="150" id="{8FEC18B0-34A1-46A3-BE58-4E6F8EE68B4B}">
+          <x14:cfRule type="expression" priority="150" id="{74F5849E-EB15-4567-B4CA-FBFB88F65E2F}">
             <xm:f>AND((E7&lt;10),(E7&lt;&gt;solved!E7))</xm:f>
             <x14:dxf>
               <font>
@@ -8603,7 +8604,7 @@
           <xm:sqref>E7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="151" id="{F06F7260-C037-402A-B5AB-D6AE223823DC}">
+          <x14:cfRule type="expression" priority="151" id="{DF37593D-77A0-4688-B670-B7FBF786FBA5}">
             <xm:f>AND((E8&lt;10),(E8&lt;&gt;solved!E8))</xm:f>
             <x14:dxf>
               <font>
@@ -8614,7 +8615,7 @@
           <xm:sqref>E8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="152" id="{60E72A6A-9DA0-4BA2-9317-CD23F9221142}">
+          <x14:cfRule type="expression" priority="152" id="{FF78685A-E8A6-4AEC-BD37-8BE5ECBB3966}">
             <xm:f>AND((E9&lt;10),(E9&lt;&gt;solved!E9))</xm:f>
             <x14:dxf>
               <font>
@@ -8625,7 +8626,7 @@
           <xm:sqref>E9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="153" id="{CAED19A7-3A6A-472D-B927-F134C0C94FE3}">
+          <x14:cfRule type="expression" priority="153" id="{1D4D4AD0-CCEF-43D8-A61B-308DB15F8A12}">
             <xm:f>AND((F1&lt;10),(F1&lt;&gt;solved!F1))</xm:f>
             <x14:dxf>
               <font>
@@ -8636,7 +8637,7 @@
           <xm:sqref>F1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="154" id="{2AFA60E3-624E-4EA3-9372-935739549076}">
+          <x14:cfRule type="expression" priority="154" id="{F0A78A99-4350-4BAA-A55A-E6CCEA156B4B}">
             <xm:f>AND((F2&lt;10),(F2&lt;&gt;solved!F2))</xm:f>
             <x14:dxf>
               <font>
@@ -8647,7 +8648,7 @@
           <xm:sqref>F2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="155" id="{309ACB79-50E7-4143-9B8A-70FB797AED6F}">
+          <x14:cfRule type="expression" priority="155" id="{564AE776-B4D0-4EDD-BE72-9C98FC6E5A7E}">
             <xm:f>AND((F3&lt;10),(F3&lt;&gt;solved!F3))</xm:f>
             <x14:dxf>
               <font>
@@ -8658,7 +8659,7 @@
           <xm:sqref>F3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="156" id="{AC285335-99EA-46E0-9DBD-9D4EC34F5AF1}">
+          <x14:cfRule type="expression" priority="156" id="{509DFC8B-8EB2-41AD-8550-A0AB633C8D3A}">
             <xm:f>AND((F4&lt;10),(F4&lt;&gt;solved!F4))</xm:f>
             <x14:dxf>
               <font>
@@ -8669,7 +8670,7 @@
           <xm:sqref>F4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="157" id="{2483E799-2968-4FF2-986B-55C71161E83B}">
+          <x14:cfRule type="expression" priority="157" id="{EE3A6B78-50E0-4359-A2EC-B2754BC7263C}">
             <xm:f>AND((F5&lt;10),(F5&lt;&gt;solved!F5))</xm:f>
             <x14:dxf>
               <font>
@@ -8680,7 +8681,7 @@
           <xm:sqref>F5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="158" id="{E7E51B45-E94F-4D5E-ABB2-BF8C2B1B8916}">
+          <x14:cfRule type="expression" priority="158" id="{339F5D54-2DAE-4513-8272-8BEDA26CE0A1}">
             <xm:f>AND((F6&lt;10),(F6&lt;&gt;solved!F6))</xm:f>
             <x14:dxf>
               <font>
@@ -8691,7 +8692,7 @@
           <xm:sqref>F6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="159" id="{314AA7D8-A96C-497B-ADC0-5D2CD27F2014}">
+          <x14:cfRule type="expression" priority="159" id="{F0A42E8D-4813-4DE3-BD79-61478E904DC0}">
             <xm:f>AND((F7&lt;10),(F7&lt;&gt;solved!F7))</xm:f>
             <x14:dxf>
               <font>
@@ -8702,7 +8703,7 @@
           <xm:sqref>F7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="160" id="{91958431-A09C-42D8-B839-8E84433F5D22}">
+          <x14:cfRule type="expression" priority="160" id="{6220C06B-B2F9-4870-B5A5-A082FB4331EC}">
             <xm:f>AND((F8&lt;10),(F8&lt;&gt;solved!F8))</xm:f>
             <x14:dxf>
               <font>
@@ -8713,7 +8714,7 @@
           <xm:sqref>F8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="161" id="{15C05690-E049-4E84-9233-2966DD67A0C6}">
+          <x14:cfRule type="expression" priority="161" id="{A6502F99-80F1-4A99-B07D-49F6ECC63F5E}">
             <xm:f>AND((F9&lt;10),(F9&lt;&gt;solved!F9))</xm:f>
             <x14:dxf>
               <font>
@@ -8724,7 +8725,7 @@
           <xm:sqref>F9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="162" id="{91998588-B02A-4DF0-8AE4-80FE2B6EF674}">
+          <x14:cfRule type="expression" priority="162" id="{35898035-C8A4-4BB6-BA21-89464C3A2425}">
             <xm:f>AND((G1&lt;10),(G1&lt;&gt;solved!G1))</xm:f>
             <x14:dxf>
               <font>
@@ -8735,7 +8736,7 @@
           <xm:sqref>G1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="163" id="{544DA176-4C70-452B-B766-BAA85AA93AB7}">
+          <x14:cfRule type="expression" priority="163" id="{2CB38A60-407A-4ED5-ADCB-DD54FDA1F83A}">
             <xm:f>AND((G2&lt;10),(G2&lt;&gt;solved!G2))</xm:f>
             <x14:dxf>
               <font>
@@ -8746,7 +8747,7 @@
           <xm:sqref>G2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="164" id="{6092EAC0-A093-4762-8FF0-A089633141E1}">
+          <x14:cfRule type="expression" priority="164" id="{31F4F683-7FC0-43B4-9B6A-F7122F2C779A}">
             <xm:f>AND((G3&lt;10),(G3&lt;&gt;solved!G3))</xm:f>
             <x14:dxf>
               <font>
@@ -8757,7 +8758,7 @@
           <xm:sqref>G3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="165" id="{65BC2E20-8E88-4021-BFA5-CBA0311B142B}">
+          <x14:cfRule type="expression" priority="165" id="{60DDF956-EB6C-41D3-B572-B2D18EAC77D0}">
             <xm:f>AND((G4&lt;10),(G4&lt;&gt;solved!G4))</xm:f>
             <x14:dxf>
               <font>
@@ -8768,7 +8769,7 @@
           <xm:sqref>G4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="166" id="{757F9EB7-408B-4CB0-98D8-E81262BE1D80}">
+          <x14:cfRule type="expression" priority="166" id="{84482C00-B276-4D23-989E-D1A2A3F0BA14}">
             <xm:f>AND((G5&lt;10),(G5&lt;&gt;solved!G5))</xm:f>
             <x14:dxf>
               <font>
@@ -8779,7 +8780,7 @@
           <xm:sqref>G5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="167" id="{382F31B6-4610-448E-BC30-7782C5DC94A8}">
+          <x14:cfRule type="expression" priority="167" id="{41F4DFAA-528B-4181-83C4-503FF0C47910}">
             <xm:f>AND((G6&lt;10),(G6&lt;&gt;solved!G6))</xm:f>
             <x14:dxf>
               <font>
@@ -8790,7 +8791,7 @@
           <xm:sqref>G6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="168" id="{8158195A-3FC2-4BF3-88C9-BAEAFA30F814}">
+          <x14:cfRule type="expression" priority="168" id="{2C70924E-90F6-4A36-9646-BD599D1235C0}">
             <xm:f>AND((G7&lt;10),(G7&lt;&gt;solved!G7))</xm:f>
             <x14:dxf>
               <font>
@@ -8801,7 +8802,7 @@
           <xm:sqref>G7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="169" id="{9E5DE6D9-F3E9-4264-BE65-68A992606BF8}">
+          <x14:cfRule type="expression" priority="169" id="{99A7587D-C756-4300-8BAA-9D814F3E2039}">
             <xm:f>AND((G8&lt;10),(G8&lt;&gt;solved!G8))</xm:f>
             <x14:dxf>
               <font>
@@ -8812,7 +8813,7 @@
           <xm:sqref>G8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="170" id="{2BAF85A0-356B-43C1-BACA-EEBA7F4F4635}">
+          <x14:cfRule type="expression" priority="170" id="{957C65FA-954D-4825-8271-E18A6FDA78A3}">
             <xm:f>AND((G9&lt;10),(G9&lt;&gt;solved!G9))</xm:f>
             <x14:dxf>
               <font>
@@ -8823,7 +8824,7 @@
           <xm:sqref>G9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="171" id="{77F7E07A-A4DA-4CC3-8066-63D46E46C76C}">
+          <x14:cfRule type="expression" priority="171" id="{7BD99E4B-2671-4E61-9CE2-7C361D2EFAA4}">
             <xm:f>AND((H1&lt;10),(H1&lt;&gt;solved!H1))</xm:f>
             <x14:dxf>
               <font>
@@ -8834,7 +8835,7 @@
           <xm:sqref>H1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="172" id="{2F685D73-AD86-4AA2-AB8E-1028879EFBB3}">
+          <x14:cfRule type="expression" priority="172" id="{D72AF9C0-1CA0-424B-9F5D-7490F35E837E}">
             <xm:f>AND((H2&lt;10),(H2&lt;&gt;solved!H2))</xm:f>
             <x14:dxf>
               <font>
@@ -8845,7 +8846,7 @@
           <xm:sqref>H2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="173" id="{102C304E-2C23-43CD-BFC5-B0CE236788C6}">
+          <x14:cfRule type="expression" priority="173" id="{2AA88670-D813-42D0-95E5-ED17743069B9}">
             <xm:f>AND((H3&lt;10),(H3&lt;&gt;solved!H3))</xm:f>
             <x14:dxf>
               <font>
@@ -8856,7 +8857,7 @@
           <xm:sqref>H3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="174" id="{A46E39FE-88A8-4432-9795-E42D70D85E26}">
+          <x14:cfRule type="expression" priority="174" id="{6E9CD250-97C6-4234-B6D7-8A2D4F8BC0F4}">
             <xm:f>AND((H4&lt;10),(H4&lt;&gt;solved!H4))</xm:f>
             <x14:dxf>
               <font>
@@ -8867,7 +8868,7 @@
           <xm:sqref>H4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="175" id="{B3A026D2-5FE0-4634-9761-286B19DFD813}">
+          <x14:cfRule type="expression" priority="175" id="{BEA55CA0-E3BC-4E18-B1D4-EE7BF4B51DD8}">
             <xm:f>AND((H5&lt;10),(H5&lt;&gt;solved!H5))</xm:f>
             <x14:dxf>
               <font>
@@ -8878,7 +8879,7 @@
           <xm:sqref>H5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="176" id="{649127E3-9234-413A-9DF0-302D14A226C0}">
+          <x14:cfRule type="expression" priority="176" id="{3D77F8BD-F76B-4232-AC84-72F4CBE817E9}">
             <xm:f>AND((H6&lt;10),(H6&lt;&gt;solved!H6))</xm:f>
             <x14:dxf>
               <font>
@@ -8889,7 +8890,7 @@
           <xm:sqref>H6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="177" id="{CEDFE3A7-8EE4-4B2A-9631-D94218D9BA81}">
+          <x14:cfRule type="expression" priority="177" id="{A4688E2E-23C7-4FAE-8EB7-539D7A308E20}">
             <xm:f>AND((H7&lt;10),(H7&lt;&gt;solved!H7))</xm:f>
             <x14:dxf>
               <font>
@@ -8900,7 +8901,7 @@
           <xm:sqref>H7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="178" id="{E0A065F4-B0E3-4B68-B0C5-25B511ED6A2E}">
+          <x14:cfRule type="expression" priority="178" id="{63464515-64DE-4BFE-A34D-5C669B50862D}">
             <xm:f>AND((H8&lt;10),(H8&lt;&gt;solved!H8))</xm:f>
             <x14:dxf>
               <font>
@@ -8911,7 +8912,7 @@
           <xm:sqref>H8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="179" id="{3EE232F6-2728-4F6D-B1C0-2431892DE016}">
+          <x14:cfRule type="expression" priority="179" id="{465D004D-3F2B-4560-AB31-7E74962D1DF3}">
             <xm:f>AND((H9&lt;10),(H9&lt;&gt;solved!H9))</xm:f>
             <x14:dxf>
               <font>
@@ -8922,7 +8923,7 @@
           <xm:sqref>H9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="180" id="{32B967FB-F636-4100-9B70-8A38EB63B2F6}">
+          <x14:cfRule type="expression" priority="180" id="{E0B5F21C-CDA6-4038-B2BC-A650F7FFB4A0}">
             <xm:f>AND((I2&lt;10),(I2&lt;&gt;solved!I2))</xm:f>
             <x14:dxf>
               <font>
@@ -8933,7 +8934,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="181" id="{464370C2-D6E6-421F-8F1F-80D7E0B180D3}">
+          <x14:cfRule type="expression" priority="181" id="{1256B28E-B011-40AB-BBC0-10F988A71870}">
             <xm:f>AND((I3&lt;10),(I3&lt;&gt;solved!I3))</xm:f>
             <x14:dxf>
               <font>
@@ -8944,7 +8945,7 @@
           <xm:sqref>I3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="182" id="{25D9D940-358A-4867-80CF-0099609AEF72}">
+          <x14:cfRule type="expression" priority="182" id="{72AF4DF8-20BC-45A6-A3D9-DA4D6B7D1F4B}">
             <xm:f>AND((I4&lt;10),(I4&lt;&gt;solved!I4))</xm:f>
             <x14:dxf>
               <font>
@@ -8955,7 +8956,7 @@
           <xm:sqref>I4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="183" id="{FE409F4C-583B-4F3B-9232-2D8EEA33E18F}">
+          <x14:cfRule type="expression" priority="183" id="{63F7C96F-6CCF-4D99-BE30-C18B751CFA5E}">
             <xm:f>AND((I5&lt;10),(I5&lt;&gt;solved!I5))</xm:f>
             <x14:dxf>
               <font>
@@ -8966,7 +8967,7 @@
           <xm:sqref>I5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="184" id="{87B4B456-5086-4A96-9070-F79AC032C4D3}">
+          <x14:cfRule type="expression" priority="184" id="{AF5AF43B-A757-4CAE-8766-B3DF27AE4F8A}">
             <xm:f>AND((I6&lt;10),(I6&lt;&gt;solved!I6))</xm:f>
             <x14:dxf>
               <font>
@@ -8977,7 +8978,7 @@
           <xm:sqref>I6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="185" id="{F28CC930-1B1C-49D6-A597-C3F0EC676A81}">
+          <x14:cfRule type="expression" priority="185" id="{DBBEB256-3350-424B-AEDF-D36E2090CE44}">
             <xm:f>AND((I7&lt;10),(I7&lt;&gt;solved!I7))</xm:f>
             <x14:dxf>
               <font>
@@ -8988,7 +8989,7 @@
           <xm:sqref>I7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="186" id="{45F97C60-5357-43C6-A1F1-6A5591B04720}">
+          <x14:cfRule type="expression" priority="186" id="{FE2FD8BE-35D5-4ECF-99BC-C74A3A1CA6CA}">
             <xm:f>AND((I8&lt;10),(I8&lt;&gt;solved!I8))</xm:f>
             <x14:dxf>
               <font>
@@ -8999,7 +9000,7 @@
           <xm:sqref>I8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="187" id="{47DDF46B-A828-4025-9728-EB305BC06D6E}">
+          <x14:cfRule type="expression" priority="187" id="{71B4A1BF-68A0-4F61-9D23-225C8E6A5981}">
             <xm:f>AND((I9&lt;10),(I9&lt;&gt;solved!I9))</xm:f>
             <x14:dxf>
               <font>
@@ -9010,7 +9011,7 @@
           <xm:sqref>I9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="188" id="{99E6A9A4-30B0-415F-8359-15A874471A6C}">
+          <x14:cfRule type="expression" priority="188" id="{9657BA12-76EC-4159-91E0-6836532F5093}">
             <xm:f>AND(($A$1&lt;10),($A$1&lt;&gt;solved!$A$1))</xm:f>
             <x14:dxf>
               <font>
@@ -9021,7 +9022,7 @@
           <xm:sqref>A1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="189" id="{BEE874EA-92F8-4227-A534-682132A062D0}">
+          <x14:cfRule type="expression" priority="189" id="{F6A244F4-514B-41DE-BD7C-5E3121EA3A83}">
             <xm:f>AND(($A$4&lt;10),($A$4&lt;&gt;solved!$A$4))</xm:f>
             <x14:dxf>
               <font>
@@ -9969,7 +9970,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="29" id="{BD8324A4-6AB1-40DE-A49D-ED27AFA96754}">
+          <x14:cfRule type="expression" priority="29" id="{D26CDA51-C321-4D2C-9A88-B598268C8171}">
             <xm:f>AND(($A$1&lt;10),($A$1&lt;&gt;solved!$A$1))</xm:f>
             <x14:dxf>
               <font>
@@ -9985,7 +9986,7 @@
           <xm:sqref>A1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="30" id="{DA17F052-2880-4454-A0C0-F91E65F8CB3A}">
+          <x14:cfRule type="expression" priority="30" id="{C26BEC53-AA13-4627-AAD0-5A9F204EEE21}">
             <xm:f>AND((A2&lt;10),(A2&lt;&gt;solved!A2))</xm:f>
             <x14:dxf>
               <font>
@@ -9996,7 +9997,7 @@
           <xm:sqref>A2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="31" id="{D3F87F92-25DB-47A9-9594-8272E25AE7AB}">
+          <x14:cfRule type="expression" priority="31" id="{A52BC9C3-54AC-43E9-AB8C-87F76F7027EB}">
             <xm:f>AND((A3&lt;10),(A3&lt;&gt;solved!A3))</xm:f>
             <x14:dxf>
               <font>
@@ -10007,7 +10008,7 @@
           <xm:sqref>A3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="32" id="{4647B5B0-DDC2-4321-A886-651B92D8C41C}">
+          <x14:cfRule type="expression" priority="32" id="{7933836D-9030-4C52-97F6-4C8B4CAF89D2}">
             <xm:f>AND((A4&lt;10),(A4&lt;&gt;solved!A4))</xm:f>
             <x14:dxf>
               <font>
@@ -10018,7 +10019,7 @@
           <xm:sqref>A4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="33" id="{406F6617-97A4-4AB4-9D50-69BE83AB67E2}">
+          <x14:cfRule type="expression" priority="33" id="{DC58A28F-8DFD-4141-B8BB-2C2CA96868A0}">
             <xm:f>AND((A5&lt;10),(A5&lt;&gt;solved!A5))</xm:f>
             <x14:dxf>
               <font>
@@ -10029,7 +10030,7 @@
           <xm:sqref>A5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="34" id="{9129C151-DDA1-4CA3-AC7F-265A92FDB0C1}">
+          <x14:cfRule type="expression" priority="34" id="{FBA3D8EC-4B10-433C-98B6-A0B0E51CB12F}">
             <xm:f>AND((A6&lt;10),(A6&lt;&gt;solved!A6))</xm:f>
             <x14:dxf>
               <font>
@@ -10040,7 +10041,7 @@
           <xm:sqref>A6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="35" id="{4C873986-38E2-4D6C-AE74-CBB392379B55}">
+          <x14:cfRule type="expression" priority="35" id="{E0872E7D-7EAD-402A-BB3D-DA355CFD7677}">
             <xm:f>AND((A7&lt;10),(A7&lt;&gt;solved!A7))</xm:f>
             <x14:dxf>
               <font>
@@ -10051,7 +10052,7 @@
           <xm:sqref>A7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="36" id="{5E20464C-7C7A-4EEA-8474-E6575400CB8E}">
+          <x14:cfRule type="expression" priority="36" id="{17948EE3-B975-4930-8C4B-B2F952429252}">
             <xm:f>AND((A8&lt;10),(A8&lt;&gt;solved!A8))</xm:f>
             <x14:dxf>
               <font>
@@ -10062,7 +10063,7 @@
           <xm:sqref>A8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="37" id="{2AC5B265-E12E-4510-801D-8DC344E650E3}">
+          <x14:cfRule type="expression" priority="37" id="{69F7FB20-24B4-431C-AB4E-FCE8A151F66F}">
             <xm:f>AND((A9&lt;10),(A9&lt;&gt;solved!A9))</xm:f>
             <x14:dxf>
               <font>
@@ -10073,7 +10074,7 @@
           <xm:sqref>A9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="38" id="{409A77D7-842A-4A2F-9710-D031E315948B}">
+          <x14:cfRule type="expression" priority="38" id="{2F51CB4A-B2BC-46B2-A7F9-0046D8C8C613}">
             <xm:f>AND((B1&lt;10),(B1&lt;&gt;solved!B1))</xm:f>
             <x14:dxf>
               <font>
@@ -10084,7 +10085,7 @@
           <xm:sqref>B1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="39" id="{3D77CCE0-1F66-41E5-AFBC-8C45D7C8BC20}">
+          <x14:cfRule type="expression" priority="39" id="{834630C0-CB7A-4154-8469-6A62BFB693C7}">
             <xm:f>AND((B2&lt;10),(B2&lt;&gt;solved!B2))</xm:f>
             <x14:dxf>
               <font>
@@ -10095,7 +10096,7 @@
           <xm:sqref>B2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="40" id="{F396E0DD-919F-44AB-B500-F1B3A9F02B35}">
+          <x14:cfRule type="expression" priority="40" id="{60464039-D092-4EA1-8240-EC3A27428658}">
             <xm:f>AND((B3&lt;10),(B3&lt;&gt;solved!B3))</xm:f>
             <x14:dxf>
               <font>
@@ -10106,7 +10107,7 @@
           <xm:sqref>B3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="41" id="{F881761F-9982-40A4-90F5-7E60F856768A}">
+          <x14:cfRule type="expression" priority="41" id="{7C15CEF4-C4B7-44DD-9368-905C3AD6B4BB}">
             <xm:f>AND((B4&lt;10),(B4&lt;&gt;solved!B4))</xm:f>
             <x14:dxf>
               <font>
@@ -10117,7 +10118,7 @@
           <xm:sqref>B4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="42" id="{4897639F-D15F-4BBF-A0E9-CA97D8C93010}">
+          <x14:cfRule type="expression" priority="42" id="{2D922414-D0B0-43E4-83E5-C02FDEF8EF3F}">
             <xm:f>AND((B5&lt;10),(B5&lt;&gt;solved!B5))</xm:f>
             <x14:dxf>
               <font>
@@ -10128,7 +10129,7 @@
           <xm:sqref>B5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="43" id="{70A02BFC-8A94-4BDF-A299-CA7F6B4C9890}">
+          <x14:cfRule type="expression" priority="43" id="{53D0F27A-7319-4347-A49F-307C1DAAF777}">
             <xm:f>AND((B6&lt;10),(B6&lt;&gt;solved!B6))</xm:f>
             <x14:dxf>
               <font>
@@ -10139,7 +10140,7 @@
           <xm:sqref>B6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="44" id="{742266DB-534F-4374-BD29-E1D030A9D068}">
+          <x14:cfRule type="expression" priority="44" id="{3A2ED2B0-FC91-47F9-8225-B839D3DB8D51}">
             <xm:f>AND((B7&lt;10),(B7&lt;&gt;solved!B7))</xm:f>
             <x14:dxf>
               <font>
@@ -10150,7 +10151,7 @@
           <xm:sqref>B7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="45" id="{AE75659A-9017-4871-8765-6BABDB35D973}">
+          <x14:cfRule type="expression" priority="45" id="{C03B74EC-1A94-4837-8716-53BA3E71E471}">
             <xm:f>AND((B8&lt;10),(B8&lt;&gt;solved!B8))</xm:f>
             <x14:dxf>
               <font>
@@ -10161,7 +10162,7 @@
           <xm:sqref>B8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="46" id="{C3215F17-4EB0-4DF0-B722-2062746DD755}">
+          <x14:cfRule type="expression" priority="46" id="{F0ACB048-AB98-4AEC-B7A1-565BEA879CFE}">
             <xm:f>AND((B9&lt;10),(B9&lt;&gt;solved!B9))</xm:f>
             <x14:dxf>
               <font>
@@ -10172,7 +10173,7 @@
           <xm:sqref>B9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="47" id="{F3B0DEC7-7568-41FC-9C79-261A38CB1058}">
+          <x14:cfRule type="expression" priority="47" id="{7B75C762-C2CA-4CD2-B653-546049D2238A}">
             <xm:f>AND((C1&lt;10),(C1&lt;&gt;solved!C1))</xm:f>
             <x14:dxf>
               <font>
@@ -10183,7 +10184,7 @@
           <xm:sqref>C1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="48" id="{6E4156AF-3C85-489B-B03A-D3894F798B9F}">
+          <x14:cfRule type="expression" priority="48" id="{5B1ECA6C-1757-4CB6-9674-64DB4CF87AEA}">
             <xm:f>AND((C2&lt;10),(C2&lt;&gt;solved!C2))</xm:f>
             <x14:dxf>
               <font>
@@ -10194,7 +10195,7 @@
           <xm:sqref>C2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="49" id="{E8725580-BE98-4599-8525-44E57B448EA4}">
+          <x14:cfRule type="expression" priority="49" id="{85AF278A-6AFC-4AD1-BEED-54762526B51D}">
             <xm:f>AND((C3&lt;10),(C3&lt;&gt;solved!C3))</xm:f>
             <x14:dxf>
               <font>
@@ -10205,7 +10206,7 @@
           <xm:sqref>C3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="50" id="{51D6D3C7-43BD-4756-8F20-A2205F2647F0}">
+          <x14:cfRule type="expression" priority="50" id="{88E69A62-F0B4-48A5-ABAE-7D859A8641D6}">
             <xm:f>AND((C4&lt;10),(C4&lt;&gt;solved!C4))</xm:f>
             <x14:dxf>
               <font>
@@ -10216,7 +10217,7 @@
           <xm:sqref>C4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="51" id="{44A5FE26-6BEC-4054-AA3C-5FE428207675}">
+          <x14:cfRule type="expression" priority="51" id="{B7388966-5558-45E6-BE44-E8D555577428}">
             <xm:f>AND((C5&lt;10),(C5&lt;&gt;solved!C5))</xm:f>
             <x14:dxf>
               <font>
@@ -10227,7 +10228,7 @@
           <xm:sqref>C5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="52" id="{DC5454EB-9EAA-401B-B3CA-EA3E90ECBE80}">
+          <x14:cfRule type="expression" priority="52" id="{4E909320-F5FB-4BEA-AF28-709E95A31535}">
             <xm:f>AND((C6&lt;10),(C6&lt;&gt;solved!C6))</xm:f>
             <x14:dxf>
               <font>
@@ -10238,7 +10239,7 @@
           <xm:sqref>C6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="53" id="{CBF822EA-4BBA-43FE-BFA4-2815202A48B7}">
+          <x14:cfRule type="expression" priority="53" id="{5AF8E03C-9C94-4CFD-B3E3-2D9D8AC88812}">
             <xm:f>AND((C7&lt;10),(C7&lt;&gt;solved!C7))</xm:f>
             <x14:dxf>
               <font>
@@ -10249,7 +10250,7 @@
           <xm:sqref>C7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="54" id="{10B4207E-B52F-4934-A965-E26FF73828AE}">
+          <x14:cfRule type="expression" priority="54" id="{5CDC7D68-FC83-41B4-B27C-14FBD51F4960}">
             <xm:f>AND((C8&lt;10),(C8&lt;&gt;solved!C8))</xm:f>
             <x14:dxf>
               <font>
@@ -10260,7 +10261,7 @@
           <xm:sqref>C8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="55" id="{4BE012BE-40DA-4480-8771-D77551902761}">
+          <x14:cfRule type="expression" priority="55" id="{C6EBFC2E-00EE-4740-ADA5-5D3C95502068}">
             <xm:f>AND((C9&lt;10),(C9&lt;&gt;solved!C9))</xm:f>
             <x14:dxf>
               <font>
@@ -10271,7 +10272,7 @@
           <xm:sqref>C9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="56" id="{6DA53019-4367-43BB-86C3-F680745F4E32}">
+          <x14:cfRule type="expression" priority="56" id="{255A1DD6-B5B0-42F7-9693-DADC6173807E}">
             <xm:f>AND((D1&lt;10),(D1&lt;&gt;solved!D1))</xm:f>
             <x14:dxf>
               <font>
@@ -10282,7 +10283,7 @@
           <xm:sqref>D1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="57" id="{BBED9DA0-9A2A-48DC-BE1E-4C8C387FA477}">
+          <x14:cfRule type="expression" priority="57" id="{BE1CE893-5E20-4B3F-8C31-DF3E1A722ADB}">
             <xm:f>AND((D2&lt;10),(D2&lt;&gt;solved!D2))</xm:f>
             <x14:dxf>
               <font>
@@ -10293,7 +10294,7 @@
           <xm:sqref>D2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="58" id="{99C04FC2-7077-4B31-9A3E-3FA6533FBF9E}">
+          <x14:cfRule type="expression" priority="58" id="{50BD9499-F4AE-4F58-B7BC-DB7F775BCAEA}">
             <xm:f>AND((D3&lt;10),(D3&lt;&gt;solved!D3))</xm:f>
             <x14:dxf>
               <font>
@@ -10304,7 +10305,7 @@
           <xm:sqref>D3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="59" id="{721EF08E-49E9-4A98-9160-3F84702F359C}">
+          <x14:cfRule type="expression" priority="59" id="{E9F36B10-E3B8-46CE-9378-264B30EC7C47}">
             <xm:f>AND((D4&lt;10),(D4&lt;&gt;solved!D4))</xm:f>
             <x14:dxf>
               <font>
@@ -10315,7 +10316,7 @@
           <xm:sqref>D4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="60" id="{9A6E6A45-FBD9-4920-9BAA-B09547E930DB}">
+          <x14:cfRule type="expression" priority="60" id="{578A8CE1-2664-4720-AAE8-C872D6145044}">
             <xm:f>AND((D5&lt;10),(D5&lt;&gt;solved!D5))</xm:f>
             <x14:dxf>
               <font>
@@ -10326,7 +10327,7 @@
           <xm:sqref>D5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="61" id="{452E1A42-1CC6-46CA-A180-A28DDCD63295}">
+          <x14:cfRule type="expression" priority="61" id="{5150A0AE-C390-4680-AC3B-A0F07A7C4A9C}">
             <xm:f>AND((D6&lt;10),(D6&lt;&gt;solved!D6))</xm:f>
             <x14:dxf>
               <font>
@@ -10337,7 +10338,7 @@
           <xm:sqref>D6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="62" id="{D6A2195B-6137-4F84-8D6C-4A41ECC0C396}">
+          <x14:cfRule type="expression" priority="62" id="{A9A6AC54-549B-43CB-8EC8-F830D9F7F090}">
             <xm:f>AND((D7&lt;10),(D7&lt;&gt;solved!D7))</xm:f>
             <x14:dxf>
               <font>
@@ -10348,7 +10349,7 @@
           <xm:sqref>D7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="63" id="{30BE1165-7892-43D0-A081-7E6CEE87F284}">
+          <x14:cfRule type="expression" priority="63" id="{84858D2B-F84B-48AB-927C-E547A760BE43}">
             <xm:f>AND((D8&lt;10),(D8&lt;&gt;solved!D8))</xm:f>
             <x14:dxf>
               <font>
@@ -10359,7 +10360,7 @@
           <xm:sqref>D8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="64" id="{3583FF39-938F-4627-8AB3-4660169E804E}">
+          <x14:cfRule type="expression" priority="64" id="{68A859CD-898B-4E15-AB81-7FF1FFAB4BDE}">
             <xm:f>AND((D9&lt;10),(D9&lt;&gt;solved!D9))</xm:f>
             <x14:dxf>
               <font>
@@ -10370,7 +10371,7 @@
           <xm:sqref>D9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="65" id="{51A63070-B121-42E7-A493-2CB48F2FF885}">
+          <x14:cfRule type="expression" priority="65" id="{DB568072-8BDC-4FDE-A937-61A729CBE3AA}">
             <xm:f>AND((E1&lt;10),(E1&lt;&gt;solved!E1))</xm:f>
             <x14:dxf>
               <font>
@@ -10381,7 +10382,7 @@
           <xm:sqref>E1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="66" id="{8CBB4FE6-F88D-4F97-9AF2-64F0F01B604D}">
+          <x14:cfRule type="expression" priority="66" id="{ECF3CE9F-6441-4D4C-BFA6-EC855FA29073}">
             <xm:f>AND((E2&lt;10),(E2&lt;&gt;solved!E2))</xm:f>
             <x14:dxf>
               <font>
@@ -10392,7 +10393,7 @@
           <xm:sqref>E2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="67" id="{6522B5AD-2680-42F4-8DCE-D082B5647B59}">
+          <x14:cfRule type="expression" priority="67" id="{75FADF1C-57B6-47F4-8C60-60E0A079E445}">
             <xm:f>AND((E3&lt;10),(E3&lt;&gt;solved!E3))</xm:f>
             <x14:dxf>
               <font>
@@ -10403,7 +10404,7 @@
           <xm:sqref>E3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="68" id="{CD954243-957B-4AE5-B5E9-5D167BA6B9E2}">
+          <x14:cfRule type="expression" priority="68" id="{1A5CEFC3-BA96-4314-A214-9C4AB04A3A85}">
             <xm:f>AND((E4&lt;10),(E4&lt;&gt;solved!E4))</xm:f>
             <x14:dxf>
               <font>
@@ -10414,7 +10415,7 @@
           <xm:sqref>E4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="69" id="{3A7C428C-36BD-4B5A-931D-BFB0FF45A9E4}">
+          <x14:cfRule type="expression" priority="69" id="{333B80CC-E976-4250-8D4B-1780DABA8327}">
             <xm:f>AND((E5&lt;10),(E5&lt;&gt;solved!E5))</xm:f>
             <x14:dxf>
               <font>
@@ -10425,7 +10426,7 @@
           <xm:sqref>E5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="70" id="{AD8AB945-F3EF-4ABE-BD70-6EA09BDEC3B9}">
+          <x14:cfRule type="expression" priority="70" id="{11E54038-E7D0-4556-BCFA-9386B4FED6C4}">
             <xm:f>AND((E6&lt;10),(E6&lt;&gt;solved!E6))</xm:f>
             <x14:dxf>
               <font>
@@ -10436,7 +10437,7 @@
           <xm:sqref>E6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="71" id="{7430C5BC-D4A6-4DC9-9C9F-A9B9FA19C88F}">
+          <x14:cfRule type="expression" priority="71" id="{A4757080-EE19-4C36-9210-BBF897658311}">
             <xm:f>AND((E7&lt;10),(E7&lt;&gt;solved!E7))</xm:f>
             <x14:dxf>
               <font>
@@ -10447,7 +10448,7 @@
           <xm:sqref>E7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="72" id="{EA9B2C43-554F-4EE4-B1F6-AB36D2E69E6C}">
+          <x14:cfRule type="expression" priority="72" id="{EAA65891-7087-4694-882A-10C0312F36DF}">
             <xm:f>AND((E8&lt;10),(E8&lt;&gt;solved!E8))</xm:f>
             <x14:dxf>
               <font>
@@ -10458,7 +10459,7 @@
           <xm:sqref>E8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="73" id="{B08F7184-34CF-4E14-8C66-46103310E785}">
+          <x14:cfRule type="expression" priority="73" id="{604CEE5D-D2DD-4AFD-8746-DF60D9E5601B}">
             <xm:f>AND((E9&lt;10),(E9&lt;&gt;solved!E9))</xm:f>
             <x14:dxf>
               <font>
@@ -10469,7 +10470,7 @@
           <xm:sqref>E9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="74" id="{7950FA34-9EE0-412E-8912-463CFCDC4D83}">
+          <x14:cfRule type="expression" priority="74" id="{5B82436D-1857-42AB-94CA-82502960B466}">
             <xm:f>AND((F1&lt;10),(F1&lt;&gt;solved!F1))</xm:f>
             <x14:dxf>
               <font>
@@ -10480,7 +10481,7 @@
           <xm:sqref>F1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="75" id="{1E15C890-3F57-4274-BACE-72623359C255}">
+          <x14:cfRule type="expression" priority="75" id="{B2DD56E3-2821-426D-96A5-22663BE9A0FD}">
             <xm:f>AND((F2&lt;10),(F2&lt;&gt;solved!F2))</xm:f>
             <x14:dxf>
               <font>
@@ -10491,7 +10492,7 @@
           <xm:sqref>F2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="76" id="{9BF39D5A-7BAC-4820-93CB-D43F7FD0499D}">
+          <x14:cfRule type="expression" priority="76" id="{F4D1DE3B-8BAA-46CE-931E-AAF8F11CC7D8}">
             <xm:f>AND((F3&lt;10),(F3&lt;&gt;solved!F3))</xm:f>
             <x14:dxf>
               <font>
@@ -10502,7 +10503,7 @@
           <xm:sqref>F3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="77" id="{91866A19-4350-40BF-9456-F07BC4C253AC}">
+          <x14:cfRule type="expression" priority="77" id="{7D3DB3B8-2447-422A-B96A-A54CCEF4C29A}">
             <xm:f>AND((F4&lt;10),(F4&lt;&gt;solved!F4))</xm:f>
             <x14:dxf>
               <font>
@@ -10513,7 +10514,7 @@
           <xm:sqref>F4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="78" id="{6A9B761B-B800-4294-B589-2A49F9632420}">
+          <x14:cfRule type="expression" priority="78" id="{1E4E93E6-80A8-4D6F-BD9E-15A4187D20C0}">
             <xm:f>AND((F5&lt;10),(F5&lt;&gt;solved!F5))</xm:f>
             <x14:dxf>
               <font>
@@ -10524,7 +10525,7 @@
           <xm:sqref>F5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="79" id="{49A81053-D2C5-42D0-8A7D-F5D1D438F88B}">
+          <x14:cfRule type="expression" priority="79" id="{E93B90D0-472C-4EF8-9DB8-31CA8DABDBDD}">
             <xm:f>AND((F6&lt;10),(F6&lt;&gt;solved!F6))</xm:f>
             <x14:dxf>
               <font>
@@ -10535,7 +10536,7 @@
           <xm:sqref>F6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="80" id="{692AF893-3443-4ACC-AD4A-EC3793D0EF39}">
+          <x14:cfRule type="expression" priority="80" id="{FD1268F6-675A-407E-9325-1B37E3177B7F}">
             <xm:f>AND((F7&lt;10),(F7&lt;&gt;solved!F7))</xm:f>
             <x14:dxf>
               <font>
@@ -10546,7 +10547,7 @@
           <xm:sqref>F7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="81" id="{C988823D-4229-4079-A48E-9C7C696E9F6D}">
+          <x14:cfRule type="expression" priority="81" id="{1C8FA47C-48F2-4C96-938A-E0DC40A81E86}">
             <xm:f>AND((F8&lt;10),(F8&lt;&gt;solved!F8))</xm:f>
             <x14:dxf>
               <font>
@@ -10557,7 +10558,7 @@
           <xm:sqref>F8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="82" id="{8EA397AD-724E-40D0-8350-BC396CA71A88}">
+          <x14:cfRule type="expression" priority="82" id="{65A1EBFE-8782-4E70-BF34-2F161FD9E357}">
             <xm:f>AND((F9&lt;10),(F9&lt;&gt;solved!F9))</xm:f>
             <x14:dxf>
               <font>
@@ -10568,7 +10569,7 @@
           <xm:sqref>F9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="83" id="{E2902A75-7880-4D52-B94D-7549D4FD33C7}">
+          <x14:cfRule type="expression" priority="83" id="{274539B3-1E2E-401C-8631-381EF52D2355}">
             <xm:f>AND((G1&lt;10),(G1&lt;&gt;solved!G1))</xm:f>
             <x14:dxf>
               <font>
@@ -10579,7 +10580,7 @@
           <xm:sqref>G1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="84" id="{F8BFA7DB-CEDC-4E97-86E1-25DEAB5368CC}">
+          <x14:cfRule type="expression" priority="84" id="{D4DB707C-E940-4E3C-9369-BE6DCF2FED29}">
             <xm:f>AND((G2&lt;10),(G2&lt;&gt;solved!G2))</xm:f>
             <x14:dxf>
               <font>
@@ -10590,7 +10591,7 @@
           <xm:sqref>G2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="85" id="{4EF0A442-7940-4562-9B1A-E0D192C03C26}">
+          <x14:cfRule type="expression" priority="85" id="{B397CB97-AEDF-4C82-B138-90DD9AC3A346}">
             <xm:f>AND((G3&lt;10),(G3&lt;&gt;solved!G3))</xm:f>
             <x14:dxf>
               <font>
@@ -10601,7 +10602,7 @@
           <xm:sqref>G3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="86" id="{188050CB-1010-4A8D-AAAE-ECF07EDED2A0}">
+          <x14:cfRule type="expression" priority="86" id="{F56AED37-54A7-41FA-8512-63C36893B365}">
             <xm:f>AND((G4&lt;10),(G4&lt;&gt;solved!G4))</xm:f>
             <x14:dxf>
               <font>
@@ -10612,7 +10613,7 @@
           <xm:sqref>G4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="87" id="{8CA82143-4A8C-40A2-BB8F-E560AA6F4BE0}">
+          <x14:cfRule type="expression" priority="87" id="{9D5FF2B6-264C-4BD9-81FF-BAE98E367855}">
             <xm:f>AND((G5&lt;10),(G5&lt;&gt;solved!G5))</xm:f>
             <x14:dxf>
               <font>
@@ -10623,7 +10624,7 @@
           <xm:sqref>G5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="88" id="{70C0D558-3060-4B38-8248-C377715FA51B}">
+          <x14:cfRule type="expression" priority="88" id="{BA9192A3-B65D-4B6C-8AF9-297C581090FB}">
             <xm:f>AND((G6&lt;10),(G6&lt;&gt;solved!G6))</xm:f>
             <x14:dxf>
               <font>
@@ -10634,7 +10635,7 @@
           <xm:sqref>G6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="89" id="{96D73633-C9BA-49FB-8CC3-5A54F0ABCA62}">
+          <x14:cfRule type="expression" priority="89" id="{43119556-A655-423A-8C62-6F8090A3401B}">
             <xm:f>AND((G7&lt;10),(G7&lt;&gt;solved!G7))</xm:f>
             <x14:dxf>
               <font>
@@ -10645,7 +10646,7 @@
           <xm:sqref>G7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="90" id="{19C0CB24-391A-4F49-94D5-815F2DCB689A}">
+          <x14:cfRule type="expression" priority="90" id="{FDAF2ADF-E241-44DC-9477-AFD77BCC5FD9}">
             <xm:f>AND((G8&lt;10),(G8&lt;&gt;solved!G8))</xm:f>
             <x14:dxf>
               <font>
@@ -10656,7 +10657,7 @@
           <xm:sqref>G8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="91" id="{7ACAD170-677D-4AE8-A89F-595E1D33487D}">
+          <x14:cfRule type="expression" priority="91" id="{D6F3D3B0-E920-40C4-9535-1BD7D8798D90}">
             <xm:f>AND((G9&lt;10),(G9&lt;&gt;solved!G9))</xm:f>
             <x14:dxf>
               <font>
@@ -10667,7 +10668,7 @@
           <xm:sqref>G9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="92" id="{A300108C-A32D-4B7D-AEB0-479BF3A89044}">
+          <x14:cfRule type="expression" priority="92" id="{2B8AFE2D-B918-433D-909B-16573F7EC483}">
             <xm:f>AND((H1&lt;10),(H1&lt;&gt;solved!H1))</xm:f>
             <x14:dxf>
               <font>
@@ -10678,7 +10679,7 @@
           <xm:sqref>H1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="93" id="{D3FF1EB6-3450-41BB-BF81-471DFE94FB6A}">
+          <x14:cfRule type="expression" priority="93" id="{749643BC-D537-4FD2-B9F3-A5AE77F3F8E9}">
             <xm:f>AND((H2&lt;10),(H2&lt;&gt;solved!H2))</xm:f>
             <x14:dxf>
               <font>
@@ -10689,7 +10690,7 @@
           <xm:sqref>H2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="94" id="{62D6CB6E-606A-4DC0-88F1-98909874D4E4}">
+          <x14:cfRule type="expression" priority="94" id="{E9C48F58-C3C0-4429-98B3-3B6D1C766087}">
             <xm:f>AND((H3&lt;10),(H3&lt;&gt;solved!H3))</xm:f>
             <x14:dxf>
               <font>
@@ -10700,7 +10701,7 @@
           <xm:sqref>H3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="95" id="{36A63C9A-5FD7-4FA6-B193-CE9BC097288B}">
+          <x14:cfRule type="expression" priority="95" id="{3DFC82B2-86BD-4AC6-903A-BC80373AE759}">
             <xm:f>AND((H4&lt;10),(H4&lt;&gt;solved!H4))</xm:f>
             <x14:dxf>
               <font>
@@ -10711,7 +10712,7 @@
           <xm:sqref>H4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="96" id="{E4F81E73-A472-4A7D-8842-8A76D5573444}">
+          <x14:cfRule type="expression" priority="96" id="{484DDBA0-9411-4B17-86E8-3B11FDC78035}">
             <xm:f>AND((H5&lt;10),(H5&lt;&gt;solved!H5))</xm:f>
             <x14:dxf>
               <font>
@@ -10722,7 +10723,7 @@
           <xm:sqref>H5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="97" id="{FA7FBD7B-BBDC-4958-A7BC-FA3692ED5C30}">
+          <x14:cfRule type="expression" priority="97" id="{D2EBA43F-28D3-4320-854C-A55BCC505FCF}">
             <xm:f>AND((H6&lt;10),(H6&lt;&gt;solved!H6))</xm:f>
             <x14:dxf>
               <font>
@@ -10733,7 +10734,7 @@
           <xm:sqref>H6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="98" id="{5A8AA823-433E-40A5-B848-684DA050127A}">
+          <x14:cfRule type="expression" priority="98" id="{40DDAE18-A02F-4F21-BDDC-18EF54B36930}">
             <xm:f>AND((H7&lt;10),(H7&lt;&gt;solved!H7))</xm:f>
             <x14:dxf>
               <font>
@@ -10744,7 +10745,7 @@
           <xm:sqref>H7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="99" id="{20C6FE41-3A48-4FA4-8375-CA52CD30A785}">
+          <x14:cfRule type="expression" priority="99" id="{F5A660FE-F86D-45B4-92F2-F55FDA9EE7D4}">
             <xm:f>AND((H8&lt;10),(H8&lt;&gt;solved!H8))</xm:f>
             <x14:dxf>
               <font>
@@ -10755,7 +10756,7 @@
           <xm:sqref>H8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="100" id="{19FF17E4-99CB-4421-BD4E-B97AC67CBC40}">
+          <x14:cfRule type="expression" priority="100" id="{802088F9-9858-4651-9D97-BBDF816B76EB}">
             <xm:f>AND((H9&lt;10),(H9&lt;&gt;solved!H9))</xm:f>
             <x14:dxf>
               <font>
@@ -10766,7 +10767,7 @@
           <xm:sqref>H9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="101" id="{60EFF9FF-5D20-4296-9329-6DD2D98F3A24}">
+          <x14:cfRule type="expression" priority="101" id="{5E138CFF-D6DD-42BB-BEE2-8EE659109EB2}">
             <xm:f>AND((I2&lt;10),(I2&lt;&gt;solved!I2))</xm:f>
             <x14:dxf>
               <font>
@@ -10777,7 +10778,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="102" id="{29DF7462-F522-4CC9-96A4-724495488DAF}">
+          <x14:cfRule type="expression" priority="102" id="{BA848AB0-2E6F-46D0-97EE-C2CDBBF8B65B}">
             <xm:f>AND((I1&lt;10),(I1&lt;&gt;solved!I1))</xm:f>
             <x14:dxf>
               <font>
@@ -10788,7 +10789,7 @@
           <xm:sqref>I1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="103" id="{343640A3-3B10-4A50-9098-6E6F41FCEEB2}">
+          <x14:cfRule type="expression" priority="103" id="{E0B11CB5-7C9A-40A3-95A3-FC9326F343A2}">
             <xm:f>AND((I3&lt;10),(I3&lt;&gt;solved!I3))</xm:f>
             <x14:dxf>
               <font>
@@ -10799,7 +10800,7 @@
           <xm:sqref>I3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="104" id="{AB27EC2F-0084-4D2E-8FAB-F2ECFDB495B7}">
+          <x14:cfRule type="expression" priority="104" id="{E07928E8-BEBB-496F-BE48-B6486EB112EF}">
             <xm:f>AND((I4&lt;10),(I4&lt;&gt;solved!I4))</xm:f>
             <x14:dxf>
               <font>
@@ -10810,7 +10811,7 @@
           <xm:sqref>I4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="105" id="{9081344C-40D1-4A60-B6D7-A810A22147E5}">
+          <x14:cfRule type="expression" priority="105" id="{F1ECC023-5831-44BC-AABC-537CB3C41082}">
             <xm:f>AND((I5&lt;10),(I5&lt;&gt;solved!I5))</xm:f>
             <x14:dxf>
               <font>
@@ -10821,7 +10822,7 @@
           <xm:sqref>I5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="106" id="{ACB170F2-CBE0-4BFE-9163-B9D54F45CAC5}">
+          <x14:cfRule type="expression" priority="106" id="{4B3BB01A-9BE4-42B9-94A2-B752BB93C2A0}">
             <xm:f>AND((I6&lt;10),(I6&lt;&gt;solved!I6))</xm:f>
             <x14:dxf>
               <font>
@@ -10832,7 +10833,7 @@
           <xm:sqref>I6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="107" id="{37B1AA70-762B-408F-AF38-BF5DDBE786FD}">
+          <x14:cfRule type="expression" priority="107" id="{4FE3C057-B0BB-4959-9344-BC3DAB58F55F}">
             <xm:f>AND((I7&lt;10),(I7&lt;&gt;solved!I7))</xm:f>
             <x14:dxf>
               <font>
@@ -10843,7 +10844,7 @@
           <xm:sqref>I7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="108" id="{659485AD-48D7-4923-B500-FDC4B0CD40B3}">
+          <x14:cfRule type="expression" priority="108" id="{7A32AD70-E6C0-4F84-9B9D-B16C60FE3077}">
             <xm:f>AND((I8&lt;10),(I8&lt;&gt;solved!I8))</xm:f>
             <x14:dxf>
               <font>
@@ -10854,7 +10855,7 @@
           <xm:sqref>I8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="109" id="{C2CCF0F9-A85C-44DE-9399-B5D0CA51C030}">
+          <x14:cfRule type="expression" priority="109" id="{573428B7-676C-4C61-A327-481350AE8081}">
             <xm:f>AND((I9&lt;10),(I9&lt;&gt;solved!I9))</xm:f>
             <x14:dxf>
               <font>
@@ -12003,7 +12004,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="96" id="{58B75BBF-CB18-4AF2-9B33-DB90713F7760}">
+          <x14:cfRule type="expression" priority="96" id="{C8FCB08B-F366-4A34-9F30-D791D3502C9B}">
             <xm:f>AND(($A$1&lt;10),($A$1&lt;&gt;solved!$A$1))</xm:f>
             <x14:dxf>
               <font>
@@ -12019,7 +12020,7 @@
           <xm:sqref>B1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="98" id="{CD6AAFE9-744E-4AC0-A887-C8CD5A278082}">
+          <x14:cfRule type="expression" priority="98" id="{CC5B5D40-D43D-4EA2-8D5E-A7DD97E5D715}">
             <xm:f>AND((B2&lt;10),(B2&lt;&gt;solved!B2))</xm:f>
             <x14:dxf>
               <font>
@@ -12030,7 +12031,7 @@
           <xm:sqref>B2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="100" id="{44235417-5070-4A98-AA66-72C45A935B00}">
+          <x14:cfRule type="expression" priority="100" id="{32D4A086-1533-4B8F-9A3C-A4B7C99A9161}">
             <xm:f>AND((B3&lt;10),(B3&lt;&gt;solved!B3))</xm:f>
             <x14:dxf>
               <font>
@@ -12041,7 +12042,7 @@
           <xm:sqref>B3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="102" id="{10CB4025-34C7-4E55-BA8C-C3C4ABA9382E}">
+          <x14:cfRule type="expression" priority="102" id="{BB945611-C5B4-4C57-B04A-AE8CC4D42467}">
             <xm:f>AND(($A$4&lt;10),($A$4&lt;&gt;solved!$A$4))</xm:f>
             <x14:dxf>
               <font>
@@ -12052,7 +12053,7 @@
           <xm:sqref>B4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="104" id="{32407932-C2FB-463E-A629-1A504F6E2441}">
+          <x14:cfRule type="expression" priority="104" id="{20BD6D2A-1DE0-4384-8878-596B62DEDB2B}">
             <xm:f>AND((B5&lt;10),(B5&lt;&gt;solved!B5))</xm:f>
             <x14:dxf>
               <font>
@@ -12063,7 +12064,7 @@
           <xm:sqref>B5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="106" id="{97F11DEF-3758-4D65-9A3D-A6D0EC5B992B}">
+          <x14:cfRule type="expression" priority="106" id="{26BEFA6C-29CA-434D-ABB9-3E20A99441F3}">
             <xm:f>AND((B6&lt;10),(B6&lt;&gt;solved!B6))</xm:f>
             <x14:dxf>
               <font>
@@ -12074,7 +12075,7 @@
           <xm:sqref>B6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="108" id="{F0F5A868-4CEE-4994-9526-F077779D10FE}">
+          <x14:cfRule type="expression" priority="108" id="{49F6A62E-98F5-4FDC-8945-CCEE4975933D}">
             <xm:f>AND((B7&lt;10),(B7&lt;&gt;solved!B7))</xm:f>
             <x14:dxf>
               <font>
@@ -12085,7 +12086,7 @@
           <xm:sqref>B7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="110" id="{1B37F54E-C952-4F12-954B-9A794A6B706A}">
+          <x14:cfRule type="expression" priority="110" id="{20AD471C-1886-4A6D-A58F-A5235111A2B4}">
             <xm:f>AND((B8&lt;10),(B8&lt;&gt;solved!B8))</xm:f>
             <x14:dxf>
               <font>
@@ -12096,7 +12097,7 @@
           <xm:sqref>B8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="112" id="{F94C3FAF-95A1-43F3-A57C-943F91C53288}">
+          <x14:cfRule type="expression" priority="112" id="{F0C66083-DE90-471B-A0E1-79639344695C}">
             <xm:f>AND((B9&lt;10),(B9&lt;&gt;solved!B9))</xm:f>
             <x14:dxf>
               <font>
@@ -12107,7 +12108,7 @@
           <xm:sqref>B9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="114" id="{3111D59D-2286-4F6E-B979-7F31BAA8EE5D}">
+          <x14:cfRule type="expression" priority="114" id="{5F2B1C5D-EB8C-4B2B-87F9-EB724E11BF1C}">
             <xm:f>AND((C1&lt;10),(C1&lt;&gt;solved!C1))</xm:f>
             <x14:dxf>
               <font>
@@ -12118,7 +12119,7 @@
           <xm:sqref>C1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="116" id="{A44AFC51-2173-4A84-80E2-BFFA711C5000}">
+          <x14:cfRule type="expression" priority="116" id="{956AF1DA-8076-4BED-8B73-DCEAE050F713}">
             <xm:f>AND((C2&lt;10),(C2&lt;&gt;solved!C2))</xm:f>
             <x14:dxf>
               <font>
@@ -12129,7 +12130,7 @@
           <xm:sqref>C2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="118" id="{BF70CCC5-A46B-495C-AF4C-8460CF2BE300}">
+          <x14:cfRule type="expression" priority="118" id="{B023341F-13D6-4AC7-A4DD-2817EE2ECFA4}">
             <xm:f>AND((C3&lt;10),(C3&lt;&gt;solved!C3))</xm:f>
             <x14:dxf>
               <font>
@@ -12140,7 +12141,7 @@
           <xm:sqref>C3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="120" id="{D383E4FF-A626-49B0-8FD1-72C973CB6F69}">
+          <x14:cfRule type="expression" priority="120" id="{20687173-6E3A-4250-B92E-46AD5D2ED4DE}">
             <xm:f>AND((C4&lt;10),(C4&lt;&gt;solved!C4))</xm:f>
             <x14:dxf>
               <font>
@@ -12151,7 +12152,7 @@
           <xm:sqref>C4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="122" id="{A7B3FE3D-FDDC-402F-B240-C25EAE803AAC}">
+          <x14:cfRule type="expression" priority="122" id="{547C48A8-B2E4-463D-BD3D-89F3911D317D}">
             <xm:f>AND((C5&lt;10),(C5&lt;&gt;solved!C5))</xm:f>
             <x14:dxf>
               <font>
@@ -12162,7 +12163,7 @@
           <xm:sqref>C5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="124" id="{71B939B4-7DD4-46C9-8492-814E116D5321}">
+          <x14:cfRule type="expression" priority="124" id="{ED46BF75-608E-4343-98FB-769B51ADC1C3}">
             <xm:f>AND((C6&lt;10),(C6&lt;&gt;solved!C6))</xm:f>
             <x14:dxf>
               <font>
@@ -12173,7 +12174,7 @@
           <xm:sqref>C6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="126" id="{AAE33C73-2F61-423C-968F-54F54AECCD38}">
+          <x14:cfRule type="expression" priority="126" id="{92889E53-C2F0-4720-8841-80F9549460BA}">
             <xm:f>AND((C7&lt;10),(C7&lt;&gt;solved!C7))</xm:f>
             <x14:dxf>
               <font>
@@ -12184,7 +12185,7 @@
           <xm:sqref>C7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="128" id="{761A21C3-7B3D-42D8-9A3B-23AA128940DC}">
+          <x14:cfRule type="expression" priority="128" id="{B4E7B849-D15A-4562-A5F5-C0A7E8B648A7}">
             <xm:f>AND((C8&lt;10),(C8&lt;&gt;solved!C8))</xm:f>
             <x14:dxf>
               <font>
@@ -12195,7 +12196,7 @@
           <xm:sqref>C8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="130" id="{8DD0B8EF-50C0-41C2-A748-904D60D466D4}">
+          <x14:cfRule type="expression" priority="130" id="{FB7E1620-F7FD-482A-91D9-B64F52DAEF90}">
             <xm:f>AND((C9&lt;10),(C9&lt;&gt;solved!C9))</xm:f>
             <x14:dxf>
               <font>
@@ -12206,7 +12207,7 @@
           <xm:sqref>C9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="132" id="{B019AC57-23C6-489B-A0E1-5B83CD2DA4A7}">
+          <x14:cfRule type="expression" priority="132" id="{1880E02C-895F-46CB-8339-679BAF1B37ED}">
             <xm:f>AND((D1&lt;10),(D1&lt;&gt;solved!D1))</xm:f>
             <x14:dxf>
               <font>
@@ -12217,7 +12218,7 @@
           <xm:sqref>D1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="134" id="{90ED5C76-F660-4854-97C1-B0C0F88BD4D9}">
+          <x14:cfRule type="expression" priority="134" id="{E4C03223-36F2-4279-B6CE-645FEAECC0AF}">
             <xm:f>AND((D2&lt;10),(D2&lt;&gt;solved!D2))</xm:f>
             <x14:dxf>
               <font>
@@ -12228,7 +12229,7 @@
           <xm:sqref>D2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="136" id="{24578284-8310-4AC3-9E52-4C2047B96AD8}">
+          <x14:cfRule type="expression" priority="136" id="{109C3586-6D33-49CB-85CD-BA5071A050F8}">
             <xm:f>AND((D3&lt;10),(D3&lt;&gt;solved!D3))</xm:f>
             <x14:dxf>
               <font>
@@ -12239,7 +12240,7 @@
           <xm:sqref>D3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="138" id="{BF76561B-BDE0-40EA-A7C1-7F2EF62132B5}">
+          <x14:cfRule type="expression" priority="138" id="{60B4F1AA-4624-4771-AFC5-AE4094581389}">
             <xm:f>AND((D4&lt;10),(D4&lt;&gt;solved!D4))</xm:f>
             <x14:dxf>
               <font>
@@ -12250,7 +12251,7 @@
           <xm:sqref>D4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="140" id="{9BF61AC8-AE53-4036-BBE0-504BE317F5A0}">
+          <x14:cfRule type="expression" priority="140" id="{5346E0D0-2AAD-4240-86CC-8BB09055579B}">
             <xm:f>AND((D5&lt;10),(D5&lt;&gt;solved!D5))</xm:f>
             <x14:dxf>
               <font>
@@ -12261,7 +12262,7 @@
           <xm:sqref>D5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="142" id="{945945BA-F07A-4ACF-AD15-60F6DB8E90A8}">
+          <x14:cfRule type="expression" priority="142" id="{AA9FA547-6BAC-4FCD-AFDA-3F6FDBB7DE8D}">
             <xm:f>AND((D6&lt;10),(D6&lt;&gt;solved!D6))</xm:f>
             <x14:dxf>
               <font>
@@ -12272,7 +12273,7 @@
           <xm:sqref>D6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="144" id="{32E7E0F9-4B20-46CB-B170-57575C70BAC0}">
+          <x14:cfRule type="expression" priority="144" id="{4AD79C54-C3C8-4C50-A0DF-60E9DE4E87BD}">
             <xm:f>AND((D7&lt;10),(D7&lt;&gt;solved!D7))</xm:f>
             <x14:dxf>
               <font>
@@ -12283,7 +12284,7 @@
           <xm:sqref>D7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="146" id="{53BC5B87-92C6-4F40-805B-F22CFEC275C5}">
+          <x14:cfRule type="expression" priority="146" id="{5837CDD0-D9CA-498E-B6EE-98776E51661F}">
             <xm:f>AND((D8&lt;10),(D8&lt;&gt;solved!D8))</xm:f>
             <x14:dxf>
               <font>
@@ -12294,7 +12295,7 @@
           <xm:sqref>D8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="148" id="{72999C86-C5A4-4F63-B8F4-F129A641B924}">
+          <x14:cfRule type="expression" priority="148" id="{267A719D-B09A-4E69-B630-ABA21AC83CE1}">
             <xm:f>AND((D9&lt;10),(D9&lt;&gt;solved!D9))</xm:f>
             <x14:dxf>
               <font>
@@ -12305,7 +12306,7 @@
           <xm:sqref>D9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="150" id="{A72DD875-B710-4379-AFFE-4B626E75CF9F}">
+          <x14:cfRule type="expression" priority="150" id="{DD479286-1D54-4894-A298-DEC35C5BE03E}">
             <xm:f>AND((E1&lt;10),(E1&lt;&gt;solved!E1))</xm:f>
             <x14:dxf>
               <font>
@@ -12316,7 +12317,7 @@
           <xm:sqref>E1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="152" id="{4DB1ED46-FA4E-4BC3-85EF-D525A263B0C0}">
+          <x14:cfRule type="expression" priority="152" id="{173EA43F-7AEA-4984-8AEE-5E50D173865C}">
             <xm:f>AND((E2&lt;10),(E2&lt;&gt;solved!E2))</xm:f>
             <x14:dxf>
               <font>
@@ -12327,7 +12328,7 @@
           <xm:sqref>E2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="154" id="{10F611FA-F978-4252-AFFD-E065EF301CB0}">
+          <x14:cfRule type="expression" priority="154" id="{2078BF2B-BE7B-442E-BE4D-76414F31C07B}">
             <xm:f>AND((E3&lt;10),(E3&lt;&gt;solved!E3))</xm:f>
             <x14:dxf>
               <font>
@@ -12338,7 +12339,7 @@
           <xm:sqref>E3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="156" id="{A753F9EC-D02F-40B0-871A-BE89DCD91EC6}">
+          <x14:cfRule type="expression" priority="156" id="{8DACDCAE-A3CD-498D-A857-C46B809ABB2A}">
             <xm:f>AND((E4&lt;10),(E4&lt;&gt;solved!E4))</xm:f>
             <x14:dxf>
               <font>
@@ -12349,7 +12350,7 @@
           <xm:sqref>E4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="158" id="{CE8D3F5E-12A5-4143-BAA4-BEA82F74E611}">
+          <x14:cfRule type="expression" priority="158" id="{1C44BD7A-97D3-4D7A-99B5-CE194BDD433B}">
             <xm:f>AND((E5&lt;10),(E5&lt;&gt;solved!E5))</xm:f>
             <x14:dxf>
               <font>
@@ -12360,7 +12361,7 @@
           <xm:sqref>E5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="160" id="{523794FC-3350-4653-8A52-D875C08C20C7}">
+          <x14:cfRule type="expression" priority="160" id="{1A705AA1-9255-422F-B6C9-22E1E96D79A4}">
             <xm:f>AND((E6&lt;10),(E6&lt;&gt;solved!E6))</xm:f>
             <x14:dxf>
               <font>
@@ -12371,7 +12372,7 @@
           <xm:sqref>E6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="162" id="{F2464A99-C397-4910-BBE2-A5329680A5FA}">
+          <x14:cfRule type="expression" priority="162" id="{82F0EE33-8F42-46BA-ADE1-66F22B4E12DF}">
             <xm:f>AND((E7&lt;10),(E7&lt;&gt;solved!E7))</xm:f>
             <x14:dxf>
               <font>
@@ -12382,7 +12383,7 @@
           <xm:sqref>E7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="164" id="{CA694B65-B35E-4050-A3A9-80F7F84D1BB5}">
+          <x14:cfRule type="expression" priority="164" id="{12FA87AD-001E-4520-80F5-B0F28079C5B0}">
             <xm:f>AND((E8&lt;10),(E8&lt;&gt;solved!E8))</xm:f>
             <x14:dxf>
               <font>
@@ -12393,7 +12394,7 @@
           <xm:sqref>E8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="166" id="{2248B05D-3AAE-4154-80DD-42352F49DD27}">
+          <x14:cfRule type="expression" priority="166" id="{17358746-664B-49A6-B87A-4E2C3AB815FA}">
             <xm:f>AND((E9&lt;10),(E9&lt;&gt;solved!E9))</xm:f>
             <x14:dxf>
               <font>
@@ -12404,7 +12405,7 @@
           <xm:sqref>E9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="168" id="{4D794068-B0F1-42A5-86CD-32FE1B5B2AD1}">
+          <x14:cfRule type="expression" priority="168" id="{7A5F8620-36DB-4280-BBE0-88E67D4F2CB3}">
             <xm:f>AND((F1&lt;10),(F1&lt;&gt;solved!F1))</xm:f>
             <x14:dxf>
               <font>
@@ -12415,7 +12416,7 @@
           <xm:sqref>F1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="170" id="{87A1FAF3-1D3D-4BE1-AD60-3DA71B9995C0}">
+          <x14:cfRule type="expression" priority="170" id="{404D987C-8C72-4FD5-B7DF-837B63CDEF21}">
             <xm:f>AND((F2&lt;10),(F2&lt;&gt;solved!F2))</xm:f>
             <x14:dxf>
               <font>
@@ -12426,7 +12427,7 @@
           <xm:sqref>F2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="172" id="{F82D5059-E0FD-48D0-94D8-9A12DE6CB182}">
+          <x14:cfRule type="expression" priority="172" id="{3226A694-B079-4E47-B7BA-7CAD86F98C23}">
             <xm:f>AND((F3&lt;10),(F3&lt;&gt;solved!F3))</xm:f>
             <x14:dxf>
               <font>
@@ -12437,7 +12438,7 @@
           <xm:sqref>F3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="174" id="{3EBB9D52-D2DA-4561-9D74-8D296DD1491D}">
+          <x14:cfRule type="expression" priority="174" id="{883920F6-2821-4FE9-801D-8BD067BA404F}">
             <xm:f>AND((F4&lt;10),(F4&lt;&gt;solved!F4))</xm:f>
             <x14:dxf>
               <font>
@@ -12448,7 +12449,7 @@
           <xm:sqref>F4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="176" id="{F6CF9A23-B110-4244-B977-B096DC86F2D0}">
+          <x14:cfRule type="expression" priority="176" id="{9F761F4A-96DC-4355-9720-1F2F84D61C98}">
             <xm:f>AND((F5&lt;10),(F5&lt;&gt;solved!F5))</xm:f>
             <x14:dxf>
               <font>
@@ -12459,7 +12460,7 @@
           <xm:sqref>F5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="178" id="{C2B1CBE5-8EA8-4A62-9F37-CE1149D136FB}">
+          <x14:cfRule type="expression" priority="178" id="{51B2E093-DA47-4FE0-A080-44F2E25361DC}">
             <xm:f>AND((F6&lt;10),(F6&lt;&gt;solved!F6))</xm:f>
             <x14:dxf>
               <font>
@@ -12470,7 +12471,7 @@
           <xm:sqref>F6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="180" id="{15603643-4BA5-4BFC-B968-A07B19DBD3F1}">
+          <x14:cfRule type="expression" priority="180" id="{F91BEBEE-D93E-47FF-A01E-FA94CD289F66}">
             <xm:f>AND((F7&lt;10),(F7&lt;&gt;solved!F7))</xm:f>
             <x14:dxf>
               <font>
@@ -12481,7 +12482,7 @@
           <xm:sqref>F7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="182" id="{CE72ADA4-30A8-44B0-947F-3000FD6D49E8}">
+          <x14:cfRule type="expression" priority="182" id="{CF13C5F4-F3AE-4158-9F1D-448CCB29AECB}">
             <xm:f>AND((F8&lt;10),(F8&lt;&gt;solved!F8))</xm:f>
             <x14:dxf>
               <font>
@@ -12492,7 +12493,7 @@
           <xm:sqref>F8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="184" id="{39E7B9B2-2014-4E5F-92C7-6E6B73E779FA}">
+          <x14:cfRule type="expression" priority="184" id="{DD6451A1-F8C5-44FA-95BF-F4322ECFCD70}">
             <xm:f>AND((F9&lt;10),(F9&lt;&gt;solved!F9))</xm:f>
             <x14:dxf>
               <font>
@@ -12503,7 +12504,7 @@
           <xm:sqref>F9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="186" id="{4620637D-1AC4-46C7-8C2D-22A668FF299A}">
+          <x14:cfRule type="expression" priority="186" id="{6CEE8B3F-5C5A-4A1E-9EA1-3930C1007EA9}">
             <xm:f>AND((G1&lt;10),(G1&lt;&gt;solved!G1))</xm:f>
             <x14:dxf>
               <font>
@@ -12514,7 +12515,7 @@
           <xm:sqref>G1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="188" id="{4CF95AEF-D3EE-4948-A2B4-647F448091F3}">
+          <x14:cfRule type="expression" priority="188" id="{C1DDF1F8-776B-46FA-B5A8-FF5960311B3D}">
             <xm:f>AND((G2&lt;10),(G2&lt;&gt;solved!G2))</xm:f>
             <x14:dxf>
               <font>
@@ -12525,7 +12526,7 @@
           <xm:sqref>G2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="190" id="{1AA5D211-3F3B-4D5B-86EC-1664D1E2F9EC}">
+          <x14:cfRule type="expression" priority="190" id="{C99CEAEE-CAB5-4CF0-9457-779E6A4E9D80}">
             <xm:f>AND((G3&lt;10),(G3&lt;&gt;solved!G3))</xm:f>
             <x14:dxf>
               <font>
@@ -12536,7 +12537,7 @@
           <xm:sqref>G3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="192" id="{B442BD61-97C1-4AD4-AEB9-10F9127E3449}">
+          <x14:cfRule type="expression" priority="192" id="{8DC46618-B81B-426A-9A5E-9C4593B91A6E}">
             <xm:f>AND((G4&lt;10),(G4&lt;&gt;solved!G4))</xm:f>
             <x14:dxf>
               <font>
@@ -12547,7 +12548,7 @@
           <xm:sqref>G4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="194" id="{491A62BE-B370-49CF-93E3-D5E182356FEE}">
+          <x14:cfRule type="expression" priority="194" id="{A083107B-407E-48D9-8098-AC19E074DF40}">
             <xm:f>AND((G5&lt;10),(G5&lt;&gt;solved!G5))</xm:f>
             <x14:dxf>
               <font>
@@ -12558,7 +12559,7 @@
           <xm:sqref>G5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="196" id="{CF4BCC86-34E1-4DBF-BD4D-31AB57B79722}">
+          <x14:cfRule type="expression" priority="196" id="{DBCACFD2-EC92-41F6-BF53-E3A754D563FB}">
             <xm:f>AND((G6&lt;10),(G6&lt;&gt;solved!G6))</xm:f>
             <x14:dxf>
               <font>
@@ -12569,7 +12570,7 @@
           <xm:sqref>G6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="198" id="{39EDDFF8-197F-4FEC-831B-6E3831882015}">
+          <x14:cfRule type="expression" priority="198" id="{6D8750D8-5F50-4FAE-BAD4-88D78A333BA1}">
             <xm:f>AND((G7&lt;10),(G7&lt;&gt;solved!G7))</xm:f>
             <x14:dxf>
               <font>
@@ -12580,7 +12581,7 @@
           <xm:sqref>G7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="200" id="{D33FD062-209F-4650-BBC3-9641556DF07C}">
+          <x14:cfRule type="expression" priority="200" id="{4266A4F3-FF4B-49E9-A514-523D33D39216}">
             <xm:f>AND((G8&lt;10),(G8&lt;&gt;solved!G8))</xm:f>
             <x14:dxf>
               <font>
@@ -12591,7 +12592,7 @@
           <xm:sqref>G8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="202" id="{ECC35D4F-FA90-4B42-A099-5C8CB5CFDF4B}">
+          <x14:cfRule type="expression" priority="202" id="{6514DCAD-1267-4B20-B31F-D13BE261A8D3}">
             <xm:f>AND((G9&lt;10),(G9&lt;&gt;solved!G9))</xm:f>
             <x14:dxf>
               <font>
@@ -12602,7 +12603,7 @@
           <xm:sqref>G9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="204" id="{F1E856B3-95B3-4A8D-8FFC-2CEDC1B65176}">
+          <x14:cfRule type="expression" priority="204" id="{BB451DCC-7F63-4BB5-86BE-BCBEAD493C19}">
             <xm:f>AND((H1&lt;10),(H1&lt;&gt;solved!H1))</xm:f>
             <x14:dxf>
               <font>
@@ -12613,7 +12614,7 @@
           <xm:sqref>H1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="207" id="{62161D73-DDB2-437C-87C4-72DBECE19F7B}">
+          <x14:cfRule type="expression" priority="207" id="{409C6EA0-B7B6-409F-9897-1F14D21FC623}">
             <xm:f>AND((H2&lt;10),(H2&lt;&gt;solved!H2))</xm:f>
             <x14:dxf>
               <font>
@@ -12624,7 +12625,7 @@
           <xm:sqref>H2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="209" id="{3C302BA6-2F19-49AB-8D17-C0D17D468092}">
+          <x14:cfRule type="expression" priority="209" id="{90514C2A-A73C-4793-A979-A0648495E0EF}">
             <xm:f>AND((H3&lt;10),(H3&lt;&gt;solved!H3))</xm:f>
             <x14:dxf>
               <font>
@@ -12635,7 +12636,7 @@
           <xm:sqref>H3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="211" id="{6A4BFC44-7BCB-46CE-B366-CFFC4027FDBD}">
+          <x14:cfRule type="expression" priority="211" id="{18722978-BAEE-4363-A22D-4AA0DAE7B68A}">
             <xm:f>AND((H4&lt;10),(H4&lt;&gt;solved!H4))</xm:f>
             <x14:dxf>
               <font>
@@ -12646,7 +12647,7 @@
           <xm:sqref>H4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="213" id="{97F14E3A-2165-4142-8FFF-CEAAE8B33D8E}">
+          <x14:cfRule type="expression" priority="213" id="{2FE76AD4-9C40-415F-BF9D-FC4CA3FD94DA}">
             <xm:f>AND((H5&lt;10),(H5&lt;&gt;solved!H5))</xm:f>
             <x14:dxf>
               <font>
@@ -12657,7 +12658,7 @@
           <xm:sqref>H5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="215" id="{B02BFD37-7FCC-4775-A0A8-80C4627DCA80}">
+          <x14:cfRule type="expression" priority="215" id="{94AE39AB-1600-44D0-9ACF-9E1282F3324D}">
             <xm:f>AND((H6&lt;10),(H6&lt;&gt;solved!H6))</xm:f>
             <x14:dxf>
               <font>
@@ -12668,7 +12669,7 @@
           <xm:sqref>H6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="217" id="{8D93F2F5-9276-4B89-B3A6-CC9D50365326}">
+          <x14:cfRule type="expression" priority="217" id="{A4E44F26-84B5-4FC2-8656-3272D0AE2038}">
             <xm:f>AND((H7&lt;10),(H7&lt;&gt;solved!H7))</xm:f>
             <x14:dxf>
               <font>
@@ -12679,7 +12680,7 @@
           <xm:sqref>H7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="219" id="{F9C1F8A6-76B3-4CCC-AB3D-F3F8DA67D0B2}">
+          <x14:cfRule type="expression" priority="219" id="{4FCBBA80-2758-4A5E-A6D8-C0BD9B8575E7}">
             <xm:f>AND((H8&lt;10),(H8&lt;&gt;solved!H8))</xm:f>
             <x14:dxf>
               <font>
@@ -12690,7 +12691,7 @@
           <xm:sqref>H8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="221" id="{C9704885-4B39-46E1-8DA8-21FEBC4C47AD}">
+          <x14:cfRule type="expression" priority="221" id="{1258E6EE-9430-41E9-98EE-8E67B6FA59E2}">
             <xm:f>AND((H9&lt;10),(H9&lt;&gt;solved!H9))</xm:f>
             <x14:dxf>
               <font>
@@ -12701,7 +12702,7 @@
           <xm:sqref>H9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="223" id="{5433F562-D187-4013-AE6D-5DB1CAB6FEAE}">
+          <x14:cfRule type="expression" priority="223" id="{56937055-F280-4565-8EE2-A020F753D63A}">
             <xm:f>AND((I1&lt;10),(I1&lt;&gt;solved!I1))</xm:f>
             <x14:dxf>
               <font>
@@ -12712,7 +12713,7 @@
           <xm:sqref>I1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="225" id="{E637885A-FD80-4220-8360-D1F33E1074BF}">
+          <x14:cfRule type="expression" priority="225" id="{4D5AF941-F4D0-46C0-8AF1-DC292AAC8A7B}">
             <xm:f>AND((I2&lt;10),(I2&lt;&gt;solved!I2))</xm:f>
             <x14:dxf>
               <font>
@@ -12723,7 +12724,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="227" id="{187996FB-2E82-41C9-A582-832CA618F038}">
+          <x14:cfRule type="expression" priority="227" id="{C611D2CB-F7ED-4539-AB5B-909CD6DAD060}">
             <xm:f>AND((I3&lt;10),(I3&lt;&gt;solved!I3))</xm:f>
             <x14:dxf>
               <font>
@@ -12734,7 +12735,7 @@
           <xm:sqref>I3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="229" id="{40CA637A-4A53-4A70-BCAD-4CD035DEB580}">
+          <x14:cfRule type="expression" priority="229" id="{BB1CF9C2-9DF6-477C-A773-66BB96E89D1A}">
             <xm:f>AND((I4&lt;10),(I4&lt;&gt;solved!I4))</xm:f>
             <x14:dxf>
               <font>
@@ -12745,7 +12746,7 @@
           <xm:sqref>I4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="231" id="{8540278C-84DE-4089-A595-E9F7D95317FC}">
+          <x14:cfRule type="expression" priority="231" id="{7785C215-94BE-4BAA-9669-E69FA663A512}">
             <xm:f>AND((I5&lt;10),(I5&lt;&gt;solved!I5))</xm:f>
             <x14:dxf>
               <font>
@@ -12756,7 +12757,7 @@
           <xm:sqref>I5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="233" id="{DEF3B065-5DA2-42F8-80F4-C6D05F64EFEE}">
+          <x14:cfRule type="expression" priority="233" id="{417100B5-8FBD-4D6E-A1C1-8FB07E247B38}">
             <xm:f>AND((I6&lt;10),(I6&lt;&gt;solved!I6))</xm:f>
             <x14:dxf>
               <font>
@@ -12767,7 +12768,7 @@
           <xm:sqref>I6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="235" id="{40C02030-7F72-47AF-86E0-C21996BD2FAC}">
+          <x14:cfRule type="expression" priority="235" id="{427A9C42-5C74-45D7-AAB4-B33A5394946C}">
             <xm:f>AND((I7&lt;10),(I7&lt;&gt;solved!I7))</xm:f>
             <x14:dxf>
               <font>
@@ -12778,7 +12779,7 @@
           <xm:sqref>I7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="237" id="{8E99379F-DF46-41B1-B0E3-F0694CBF80E1}">
+          <x14:cfRule type="expression" priority="237" id="{83D82741-65ED-4C90-96A6-43A3E7CEBCA4}">
             <xm:f>AND((I8&lt;10),(I8&lt;&gt;solved!I8))</xm:f>
             <x14:dxf>
               <font>
@@ -12789,7 +12790,7 @@
           <xm:sqref>I8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="239" id="{40C36C56-2BF6-48CA-8133-4EB19AE02C5C}">
+          <x14:cfRule type="expression" priority="239" id="{72956B3D-8ADF-45E9-9AB5-A2EC91817DAD}">
             <xm:f>AND((I9&lt;10),(I9&lt;&gt;solved!I9))</xm:f>
             <x14:dxf>
               <font>
@@ -12800,7 +12801,7 @@
           <xm:sqref>I9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="242" id="{CF689E70-1B25-4C86-B6A0-F4E0306B9479}">
+          <x14:cfRule type="expression" priority="242" id="{EAEFDC3C-CA87-47FB-B9CB-3010BBD67BE0}">
             <xm:f>AND((J2&lt;10),(J2&lt;&gt;solved!J2))</xm:f>
             <x14:dxf>
               <font>
@@ -12811,7 +12812,7 @@
           <xm:sqref>J2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="244" id="{2B9AD841-85CF-41B5-8B75-3028C0E3FC45}">
+          <x14:cfRule type="expression" priority="244" id="{A3CF4D90-AB62-4780-B996-1A10B8ED1ED0}">
             <xm:f>AND((J3&lt;10),(J3&lt;&gt;solved!J3))</xm:f>
             <x14:dxf>
               <font>
@@ -12822,7 +12823,7 @@
           <xm:sqref>J3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="246" id="{F6ECB163-5C6B-4E50-A4FB-5525CFC151EE}">
+          <x14:cfRule type="expression" priority="246" id="{75E2B5B7-F918-4C70-98A7-1A38BF6E67C8}">
             <xm:f>AND((J4&lt;10),(J4&lt;&gt;solved!J4))</xm:f>
             <x14:dxf>
               <font>
@@ -12833,7 +12834,7 @@
           <xm:sqref>J4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="249" id="{6C76E348-2DCC-467B-9060-B7E092AE3D5C}">
+          <x14:cfRule type="expression" priority="249" id="{E9F8C930-BD8C-49A5-81F4-7DBC3BBCBFF0}">
             <xm:f>AND((J5&lt;10),(J5&lt;&gt;solved!J5))</xm:f>
             <x14:dxf>
               <font>
@@ -12844,7 +12845,7 @@
           <xm:sqref>J5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="251" id="{684C2558-F4C6-4622-88C7-16121F2EB550}">
+          <x14:cfRule type="expression" priority="251" id="{F42D6C83-2220-48B4-9829-ECBFDC363F8D}">
             <xm:f>AND((J6&lt;10),(J6&lt;&gt;solved!J6))</xm:f>
             <x14:dxf>
               <font>
@@ -12855,7 +12856,7 @@
           <xm:sqref>J6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="253" id="{DA9DBFD6-C41C-417B-9384-10EC18D63B94}">
+          <x14:cfRule type="expression" priority="253" id="{7C7A7AEB-A4DD-4DBF-9511-C6BA151CEA95}">
             <xm:f>AND((J7&lt;10),(J7&lt;&gt;solved!J7))</xm:f>
             <x14:dxf>
               <font>
@@ -12866,7 +12867,7 @@
           <xm:sqref>J7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="255" id="{4A4851E0-1A45-4ECA-B65F-DBA0E9904A36}">
+          <x14:cfRule type="expression" priority="255" id="{91BBB635-1650-4142-8DA3-8F35B4A62578}">
             <xm:f>AND((J8&lt;10),(J8&lt;&gt;solved!J8))</xm:f>
             <x14:dxf>
               <font>
@@ -12877,7 +12878,7 @@
           <xm:sqref>J8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="257" id="{58D089A9-BF46-4691-BCAD-F9EA823C58CD}">
+          <x14:cfRule type="expression" priority="257" id="{B02C6959-38A1-42C1-A392-B850127883BF}">
             <xm:f>AND((J9&lt;10),(J9&lt;&gt;solved!J9))</xm:f>
             <x14:dxf>
               <font>

</xml_diff>

<commit_message>
Interaction added, via branch
</commit_message>
<xml_diff>
--- a/data/SDK.xlsx
+++ b/data/SDK.xlsx
@@ -96,9 +96,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="#,##0"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -507,7 +508,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -528,7 +529,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -564,7 +565,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -572,7 +573,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -600,7 +605,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7502,7 +7507,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7516,32 +7521,32 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="n">
-        <v>6</v>
+        <v>257</v>
       </c>
       <c r="C1" s="4" t="n">
-        <v>5</v>
+        <v>2567</v>
       </c>
       <c r="D1" s="2" t="n">
-        <v>179</v>
+        <v>1</v>
       </c>
       <c r="E1" s="3" t="n">
         <v>8</v>
       </c>
       <c r="F1" s="4" t="n">
-        <v>179</v>
+        <v>279</v>
       </c>
       <c r="G1" s="2" t="n">
+        <v>259</v>
+      </c>
+      <c r="H1" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H1" s="3" t="n">
-        <v>2</v>
-      </c>
       <c r="I1" s="4" t="n">
-        <v>17</v>
-      </c>
-      <c r="K1" s="5" t="str">
+        <v>5679</v>
+      </c>
+      <c r="K1" s="5" t="n">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "1")=9, 1, "")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="L1" s="6" t="n">
         <v>0</v>
@@ -7549,31 +7554,31 @@
     </row>
     <row r="2" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
-        <v>7</v>
+        <v>579</v>
       </c>
       <c r="B2" s="8" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C2" s="9" t="n">
+        <v>257</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" s="8" t="n">
+        <v>25</v>
+      </c>
+      <c r="F2" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="8" t="n">
+        <v>259</v>
+      </c>
+      <c r="I2" s="9" t="n">
         <v>8</v>
-      </c>
-      <c r="D2" s="7" t="n">
-        <v>14</v>
-      </c>
-      <c r="E2" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="F2" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="H2" s="8" t="n">
-        <v>14</v>
-      </c>
-      <c r="I2" s="9" t="n">
-        <v>5</v>
       </c>
       <c r="K2" s="10" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "2")=9, 2, "")</f>
@@ -7582,31 +7587,31 @@
     </row>
     <row r="3" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="n">
+        <v>5679</v>
+      </c>
+      <c r="B3" s="12" t="n">
+        <v>8</v>
+      </c>
+      <c r="C3" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="13" t="n">
+      <c r="D3" s="11" t="n">
+        <v>57</v>
+      </c>
+      <c r="E3" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="D3" s="11" t="n">
-        <v>5</v>
-      </c>
-      <c r="E3" s="12" t="n">
-        <v>6</v>
-      </c>
       <c r="F3" s="13" t="n">
-        <v>47</v>
+        <v>279</v>
       </c>
       <c r="G3" s="11" t="n">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="H3" s="12" t="n">
-        <v>9</v>
+        <v>259</v>
       </c>
       <c r="I3" s="13" t="n">
-        <v>8</v>
+        <v>5679</v>
       </c>
       <c r="K3" s="10" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "3")=9, 3, "")</f>
@@ -7615,97 +7620,97 @@
     </row>
     <row r="4" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>169</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>479</v>
+        <v>4</v>
       </c>
       <c r="F4" s="4" t="n">
         <v>5</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>479</v>
+        <v>7</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I4" s="4" t="n">
-        <v>1679</v>
-      </c>
-      <c r="K4" s="14" t="str">
+        <v>1</v>
+      </c>
+      <c r="K4" s="14" t="n">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "4")=9, 4, "")</f>
-        <v/>
+        <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="n">
-        <v>369</v>
+        <v>1</v>
       </c>
       <c r="B5" s="8" t="n">
-        <v>134</v>
+        <v>4</v>
       </c>
       <c r="C5" s="9" t="n">
+        <v>35</v>
+      </c>
+      <c r="D5" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="D5" s="7" t="n">
-        <v>14789</v>
-      </c>
       <c r="E5" s="8" t="n">
-        <v>479</v>
+        <v>7</v>
       </c>
       <c r="F5" s="9" t="n">
-        <v>14789</v>
+        <v>8</v>
       </c>
       <c r="G5" s="7" t="n">
-        <v>5</v>
+        <v>359</v>
       </c>
       <c r="H5" s="8" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I5" s="9" t="n">
-        <v>1679</v>
-      </c>
-      <c r="K5" s="14" t="n">
+        <v>59</v>
+      </c>
+      <c r="K5" s="14" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "5")=9, 5, "")</f>
-        <v>5</v>
+        <v/>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="n">
-        <v>5</v>
+        <v>357</v>
       </c>
       <c r="B6" s="12" t="n">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="C6" s="13" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D6" s="11" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E6" s="12" t="n">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="F6" s="13" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G6" s="11" t="n">
-        <v>249</v>
+        <v>35</v>
       </c>
       <c r="H6" s="12" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I6" s="13" t="n">
-        <v>129</v>
+        <v>2</v>
       </c>
       <c r="K6" s="10" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "6")=9, 6, "")</f>
@@ -7714,31 +7719,31 @@
     </row>
     <row r="7" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
-        <v>269</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>4</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F7" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4" t="n">
         <v>3</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="I7" s="4" t="n">
-        <v>29</v>
       </c>
       <c r="K7" s="10" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "7")=9, 7, "")</f>
@@ -7747,64 +7752,64 @@
     </row>
     <row r="8" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="n">
-        <v>369</v>
+        <v>579</v>
       </c>
       <c r="B8" s="8" t="n">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C8" s="9" t="n">
-        <v>169</v>
+        <v>257</v>
       </c>
       <c r="D8" s="7" t="n">
-        <v>679</v>
+        <v>8</v>
       </c>
       <c r="E8" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="G8" s="7" t="n">
+        <v>259</v>
+      </c>
+      <c r="H8" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="F8" s="9" t="n">
-        <v>79</v>
-      </c>
-      <c r="G8" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="H8" s="8" t="n">
-        <v>5</v>
-      </c>
       <c r="I8" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="K8" s="10" t="str">
+        <v>59</v>
+      </c>
+      <c r="K8" s="14" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "8")=9, 8, "")</f>
         <v/>
       </c>
     </row>
     <row r="9" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="n">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="B9" s="12" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C9" s="13" t="n">
+        <v>257</v>
+      </c>
+      <c r="D9" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="E9" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="F9" s="13" t="n">
+        <v>3</v>
+      </c>
+      <c r="G9" s="11" t="n">
         <v>7</v>
       </c>
-      <c r="D9" s="11" t="n">
-        <v>489</v>
-      </c>
-      <c r="E9" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="13" t="n">
-        <v>489</v>
-      </c>
-      <c r="G9" s="11" t="n">
-        <v>29</v>
-      </c>
       <c r="H9" s="12" t="n">
+        <v>25</v>
+      </c>
+      <c r="I9" s="13" t="n">
         <v>4</v>
-      </c>
-      <c r="I9" s="13" t="n">
-        <v>3</v>
       </c>
       <c r="K9" s="15" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "9")=9, 9, "")</f>
@@ -8148,7 +8153,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="110" id="{A0CE247A-BB30-4C32-94B0-64B4D770634B}">
+          <x14:cfRule type="expression" priority="110" id="{B7106014-F5AD-4D6F-90E7-C0D67022F82E}">
             <xm:f>AND((A2&lt;10),(A2&lt;&gt;solved!A2))</xm:f>
             <x14:dxf>
               <font>
@@ -8164,7 +8169,7 @@
           <xm:sqref>A2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="111" id="{6FD9797F-5D61-46BD-A417-2D2573F0DF1C}">
+          <x14:cfRule type="expression" priority="111" id="{3028AF82-7560-4084-A7B8-382DD3329432}">
             <xm:f>AND((A3&lt;10),(A3&lt;&gt;solved!A3))</xm:f>
             <x14:dxf>
               <font>
@@ -8175,7 +8180,7 @@
           <xm:sqref>A3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="112" id="{43B0E9C6-958B-4D61-A562-70BC1FEBEEE9}">
+          <x14:cfRule type="expression" priority="112" id="{CDD7F4F1-28AB-4C4A-ABFA-1BEEA2169213}">
             <xm:f>AND((A5&lt;10),(A5&lt;&gt;solved!A5))</xm:f>
             <x14:dxf>
               <font>
@@ -8186,7 +8191,7 @@
           <xm:sqref>A5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="113" id="{9F15AC88-9AB6-40D2-B4F3-C0385EA27EB6}">
+          <x14:cfRule type="expression" priority="113" id="{F024F395-3B60-4282-AFF5-F2F2D9BCE3D5}">
             <xm:f>AND((A6&lt;10),(A6&lt;&gt;solved!A6))</xm:f>
             <x14:dxf>
               <font>
@@ -8197,7 +8202,7 @@
           <xm:sqref>A6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="114" id="{805B108C-F96E-46D3-8E7A-5E89C66AD6E6}">
+          <x14:cfRule type="expression" priority="114" id="{A3DC5899-687B-42CF-ACA1-B8E98133C277}">
             <xm:f>AND((A7&lt;10),(A7&lt;&gt;solved!A7))</xm:f>
             <x14:dxf>
               <font>
@@ -8208,7 +8213,7 @@
           <xm:sqref>A7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="115" id="{3443F93F-D7C6-456D-88B5-BE41C5D03481}">
+          <x14:cfRule type="expression" priority="115" id="{8BBED9C2-9D5B-423F-A3F4-7C7EC8E5F4A9}">
             <xm:f>AND((A8&lt;10),(A8&lt;&gt;solved!A8))</xm:f>
             <x14:dxf>
               <font>
@@ -8219,7 +8224,7 @@
           <xm:sqref>A8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="116" id="{3E92E638-8C3C-4A20-9890-C88CF966F934}">
+          <x14:cfRule type="expression" priority="116" id="{B9FE30BD-3A43-4C91-A932-878480918037}">
             <xm:f>AND((A9&lt;10),(A9&lt;&gt;solved!A9))</xm:f>
             <x14:dxf>
               <font>
@@ -8230,7 +8235,7 @@
           <xm:sqref>A9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="117" id="{29F71C6E-9D70-4D3F-BC72-9C89C113FAC4}">
+          <x14:cfRule type="expression" priority="117" id="{73ECBD50-CD43-496B-8F42-B08292B05EA0}">
             <xm:f>AND((B1&lt;10),(B1&lt;&gt;solved!B1))</xm:f>
             <x14:dxf>
               <font>
@@ -8241,7 +8246,7 @@
           <xm:sqref>B1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="118" id="{B98D4C62-81A2-4860-8A21-64C024BEE684}">
+          <x14:cfRule type="expression" priority="118" id="{E69E6AA3-AEF7-47F3-A681-91ABAC6C7C90}">
             <xm:f>AND((B2&lt;10),(B2&lt;&gt;solved!B2))</xm:f>
             <x14:dxf>
               <font>
@@ -8252,7 +8257,7 @@
           <xm:sqref>B2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="119" id="{6D5737D4-363F-40DF-8333-75242925AE60}">
+          <x14:cfRule type="expression" priority="119" id="{E1B4F82E-D75F-418F-9D8A-46DAB6EE66D7}">
             <xm:f>AND((B3&lt;10),(B3&lt;&gt;solved!B3))</xm:f>
             <x14:dxf>
               <font>
@@ -8263,7 +8268,7 @@
           <xm:sqref>B3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="120" id="{9AE74043-B7F8-4AAC-9399-EA59A273BD94}">
+          <x14:cfRule type="expression" priority="120" id="{9250AC86-A3E0-4710-AE60-D150F0EA6DBE}">
             <xm:f>AND((B4&lt;10),(B4&lt;&gt;solved!B4))</xm:f>
             <x14:dxf>
               <font>
@@ -8274,7 +8279,7 @@
           <xm:sqref>B4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="121" id="{331E745B-FAE4-478F-B964-2464E9645E74}">
+          <x14:cfRule type="expression" priority="121" id="{CC2EB332-AA69-4E2B-8FBD-27ADE3EBC79A}">
             <xm:f>AND((B5&lt;10),(B5&lt;&gt;solved!B5))</xm:f>
             <x14:dxf>
               <font>
@@ -8285,7 +8290,7 @@
           <xm:sqref>B5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="122" id="{ABC847D7-7D87-4CF2-AFCD-3163D01D7612}">
+          <x14:cfRule type="expression" priority="122" id="{956CA7E0-F376-43B4-B987-9647EA543765}">
             <xm:f>AND((B6&lt;10),(B6&lt;&gt;solved!B6))</xm:f>
             <x14:dxf>
               <font>
@@ -8296,7 +8301,7 @@
           <xm:sqref>B6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="123" id="{90107C3A-BE23-42E2-BC86-2459349ACD6B}">
+          <x14:cfRule type="expression" priority="123" id="{97BABA72-20B0-4C68-8597-AB2FC0597E43}">
             <xm:f>AND((B7&lt;10),(B7&lt;&gt;solved!B7))</xm:f>
             <x14:dxf>
               <font>
@@ -8307,7 +8312,7 @@
           <xm:sqref>B7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="124" id="{449257AB-9BFF-4D14-A485-C813C98D7DF0}">
+          <x14:cfRule type="expression" priority="124" id="{404C3450-F960-4AF2-B53A-85218EA66D96}">
             <xm:f>AND((B8&lt;10),(B8&lt;&gt;solved!B8))</xm:f>
             <x14:dxf>
               <font>
@@ -8318,7 +8323,7 @@
           <xm:sqref>B8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="125" id="{4BF9B930-41C0-49BF-B53C-BD969D1288BF}">
+          <x14:cfRule type="expression" priority="125" id="{7685B0AF-B6D8-46D4-BB73-74265C719F73}">
             <xm:f>AND((B9&lt;10),(B9&lt;&gt;solved!B9))</xm:f>
             <x14:dxf>
               <font>
@@ -8329,7 +8334,7 @@
           <xm:sqref>B9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="126" id="{DEF6E48F-1B2F-4338-B4AB-FC62F3ACE332}">
+          <x14:cfRule type="expression" priority="126" id="{BE27EBD0-E14E-4CA6-BEB3-B7BEAA888BBB}">
             <xm:f>AND((C1&lt;10),(C1&lt;&gt;solved!C1))</xm:f>
             <x14:dxf>
               <font>
@@ -8340,7 +8345,7 @@
           <xm:sqref>C1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="127" id="{80BCBC30-FF99-485B-9CEC-66BB3B3E33E3}">
+          <x14:cfRule type="expression" priority="127" id="{C3BF4536-EA36-4DB4-BD50-F073EFE86566}">
             <xm:f>AND((C2&lt;10),(C2&lt;&gt;solved!C2))</xm:f>
             <x14:dxf>
               <font>
@@ -8351,7 +8356,7 @@
           <xm:sqref>C2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="128" id="{EB216865-F8C1-4C47-BD38-7F126FD7F329}">
+          <x14:cfRule type="expression" priority="128" id="{F4766224-A2A3-42E0-BCF6-8C8C9A7A68AA}">
             <xm:f>AND((C3&lt;10),(C3&lt;&gt;solved!C3))</xm:f>
             <x14:dxf>
               <font>
@@ -8362,7 +8367,7 @@
           <xm:sqref>C3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="129" id="{DC5BE59C-B053-4323-B1B1-1D502F6145E9}">
+          <x14:cfRule type="expression" priority="129" id="{9E7AFB72-30D8-4175-BCFE-F7537F855AA4}">
             <xm:f>AND((C4&lt;10),(C4&lt;&gt;solved!C4))</xm:f>
             <x14:dxf>
               <font>
@@ -8373,7 +8378,7 @@
           <xm:sqref>C4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="130" id="{53AA1046-8474-4E58-AF00-3E575880C6B0}">
+          <x14:cfRule type="expression" priority="130" id="{3E3BC063-C5BF-4BC4-BF54-7742A86B1259}">
             <xm:f>AND((C5&lt;10),(C5&lt;&gt;solved!C5))</xm:f>
             <x14:dxf>
               <font>
@@ -8384,7 +8389,7 @@
           <xm:sqref>C5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="131" id="{A010DEEE-FC44-484F-ABA0-8FBACA867D57}">
+          <x14:cfRule type="expression" priority="131" id="{3C3AF2F2-EEAC-406D-8A3B-58FF77154B14}">
             <xm:f>AND((C6&lt;10),(C6&lt;&gt;solved!C6))</xm:f>
             <x14:dxf>
               <font>
@@ -8395,7 +8400,7 @@
           <xm:sqref>C6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="132" id="{E7BA7A20-6471-47AF-AD32-254929B62CC0}">
+          <x14:cfRule type="expression" priority="132" id="{6113C899-C09F-4ACE-9A1C-89D838D041CC}">
             <xm:f>AND((C7&lt;10),(C7&lt;&gt;solved!C7))</xm:f>
             <x14:dxf>
               <font>
@@ -8406,7 +8411,7 @@
           <xm:sqref>C7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="133" id="{FE703F6C-A994-40FB-B06A-E83070E0C44D}">
+          <x14:cfRule type="expression" priority="133" id="{315E1A62-9C8B-4AAF-B3AA-5B6E9BE144DF}">
             <xm:f>AND((C8&lt;10),(C8&lt;&gt;solved!C8))</xm:f>
             <x14:dxf>
               <font>
@@ -8417,7 +8422,7 @@
           <xm:sqref>C8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="134" id="{121A257F-E0AA-4EE0-B526-39B0A9B92FA2}">
+          <x14:cfRule type="expression" priority="134" id="{EF5849E1-BB94-4F5E-A78E-ED105D2CDFF3}">
             <xm:f>AND((C9&lt;10),(C9&lt;&gt;solved!C9))</xm:f>
             <x14:dxf>
               <font>
@@ -8428,7 +8433,7 @@
           <xm:sqref>C9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="135" id="{E5338D6F-F600-4150-916B-11C0FB8EAF79}">
+          <x14:cfRule type="expression" priority="135" id="{A670A0D8-5419-4A78-B610-6C9C63D1D311}">
             <xm:f>AND((D1&lt;10),(D1&lt;&gt;solved!D1))</xm:f>
             <x14:dxf>
               <font>
@@ -8439,7 +8444,7 @@
           <xm:sqref>D1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="136" id="{53D8F0C3-7A9C-4B73-A4AE-322037EB38AC}">
+          <x14:cfRule type="expression" priority="136" id="{C7C1AA3E-562C-4554-9948-95A4C1D2B130}">
             <xm:f>AND((D2&lt;10),(D2&lt;&gt;solved!D2))</xm:f>
             <x14:dxf>
               <font>
@@ -8450,7 +8455,7 @@
           <xm:sqref>D2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="137" id="{8058ACD1-9480-4D5C-A75B-4C74B1D34F1C}">
+          <x14:cfRule type="expression" priority="137" id="{CEDF7A6D-AEF5-4537-B48C-8F20A0E6E59E}">
             <xm:f>AND((D3&lt;10),(D3&lt;&gt;solved!D3))</xm:f>
             <x14:dxf>
               <font>
@@ -8461,7 +8466,7 @@
           <xm:sqref>D3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="138" id="{C4355A7C-B4B8-42EC-9F1B-D5C93CC74DCC}">
+          <x14:cfRule type="expression" priority="138" id="{907F38C1-1C24-4972-9244-60CE4A3C8DE1}">
             <xm:f>AND((D4&lt;10),(D4&lt;&gt;solved!D4))</xm:f>
             <x14:dxf>
               <font>
@@ -8472,7 +8477,7 @@
           <xm:sqref>D4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="139" id="{6533371F-9B13-4CA0-B9BB-9FC37CF0A117}">
+          <x14:cfRule type="expression" priority="139" id="{1792222D-61FF-41C5-801F-2E8E47F9814E}">
             <xm:f>AND((D5&lt;10),(D5&lt;&gt;solved!D5))</xm:f>
             <x14:dxf>
               <font>
@@ -8483,7 +8488,7 @@
           <xm:sqref>D5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="140" id="{9DF7EE55-E580-4A57-8252-D13D8820EFDD}">
+          <x14:cfRule type="expression" priority="140" id="{25594678-EEFA-4298-8BA3-D0A04F79A8CE}">
             <xm:f>AND((D6&lt;10),(D6&lt;&gt;solved!D6))</xm:f>
             <x14:dxf>
               <font>
@@ -8494,7 +8499,7 @@
           <xm:sqref>D6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="141" id="{C93F7B85-18E9-4283-A194-157053D38680}">
+          <x14:cfRule type="expression" priority="141" id="{C7DC9C5F-257A-4D20-8CCE-C46913C65327}">
             <xm:f>AND((D7&lt;10),(D7&lt;&gt;solved!D7))</xm:f>
             <x14:dxf>
               <font>
@@ -8505,7 +8510,7 @@
           <xm:sqref>D7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="142" id="{1CDE3FE0-891E-48A3-B668-C24060E77D26}">
+          <x14:cfRule type="expression" priority="142" id="{762794B8-E6A3-4BB6-95C4-DAA9308E20C6}">
             <xm:f>AND((D8&lt;10),(D8&lt;&gt;solved!D8))</xm:f>
             <x14:dxf>
               <font>
@@ -8516,7 +8521,7 @@
           <xm:sqref>D8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="143" id="{E1A7BCC5-48CD-4DD0-931F-52489B4EB64B}">
+          <x14:cfRule type="expression" priority="143" id="{5BE47A79-3199-4EBD-8F28-608CFF2181FA}">
             <xm:f>AND((D9&lt;10),(D9&lt;&gt;solved!D9))</xm:f>
             <x14:dxf>
               <font>
@@ -8527,7 +8532,7 @@
           <xm:sqref>D9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="144" id="{FB401FE6-7B4F-47CA-A2D8-89FEAB173F51}">
+          <x14:cfRule type="expression" priority="144" id="{21AB3070-88B2-488E-9F6F-4D9FD615B941}">
             <xm:f>AND((E1&lt;10),(E1&lt;&gt;solved!E1))</xm:f>
             <x14:dxf>
               <font>
@@ -8538,7 +8543,7 @@
           <xm:sqref>E1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="145" id="{B03A5ACF-3845-4BE8-9EEA-533C5B9D59B4}">
+          <x14:cfRule type="expression" priority="145" id="{326C20DB-268E-4F41-BE4D-6CC65EA91B5B}">
             <xm:f>AND((E2&lt;10),(E2&lt;&gt;solved!E2))</xm:f>
             <x14:dxf>
               <font>
@@ -8549,7 +8554,7 @@
           <xm:sqref>E2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="146" id="{572D6DA2-EC00-42CC-A03A-7C1ABF95DE37}">
+          <x14:cfRule type="expression" priority="146" id="{ECCAC280-FEA9-4350-ACDF-2EAB91FCF7B2}">
             <xm:f>AND((E3&lt;10),(E3&lt;&gt;solved!E3))</xm:f>
             <x14:dxf>
               <font>
@@ -8560,7 +8565,7 @@
           <xm:sqref>E3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="147" id="{5B728D68-CCD2-4AD3-A6DD-2236F695C15F}">
+          <x14:cfRule type="expression" priority="147" id="{7C778EBA-2DF0-41F3-87EE-6AB641EE40E0}">
             <xm:f>AND((E4&lt;10),(E4&lt;&gt;solved!E4))</xm:f>
             <x14:dxf>
               <font>
@@ -8571,7 +8576,7 @@
           <xm:sqref>E4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="148" id="{807F6EFE-618C-4652-93B9-1938E66EC2C0}">
+          <x14:cfRule type="expression" priority="148" id="{53917090-1BC3-4BAC-81C0-28FC6051F223}">
             <xm:f>AND((E5&lt;10),(E5&lt;&gt;solved!E5))</xm:f>
             <x14:dxf>
               <font>
@@ -8582,7 +8587,7 @@
           <xm:sqref>E5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="149" id="{76DCAE1B-AD5A-44D8-BBCA-724E836DA357}">
+          <x14:cfRule type="expression" priority="149" id="{7EEAD3C4-E898-4D67-9DCE-6DF12FAC8B72}">
             <xm:f>AND((E6&lt;10),(E6&lt;&gt;solved!E6))</xm:f>
             <x14:dxf>
               <font>
@@ -8593,7 +8598,7 @@
           <xm:sqref>E6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="150" id="{74F5849E-EB15-4567-B4CA-FBFB88F65E2F}">
+          <x14:cfRule type="expression" priority="150" id="{AA97D0A3-44C6-4015-9C26-7DBFD65E4772}">
             <xm:f>AND((E7&lt;10),(E7&lt;&gt;solved!E7))</xm:f>
             <x14:dxf>
               <font>
@@ -8604,7 +8609,7 @@
           <xm:sqref>E7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="151" id="{DF37593D-77A0-4688-B670-B7FBF786FBA5}">
+          <x14:cfRule type="expression" priority="151" id="{5A685E95-61DA-4C89-A84D-5B297864C340}">
             <xm:f>AND((E8&lt;10),(E8&lt;&gt;solved!E8))</xm:f>
             <x14:dxf>
               <font>
@@ -8615,7 +8620,7 @@
           <xm:sqref>E8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="152" id="{FF78685A-E8A6-4AEC-BD37-8BE5ECBB3966}">
+          <x14:cfRule type="expression" priority="152" id="{1A712A5F-8E00-4F88-9932-6D3EDC9B145B}">
             <xm:f>AND((E9&lt;10),(E9&lt;&gt;solved!E9))</xm:f>
             <x14:dxf>
               <font>
@@ -8626,7 +8631,7 @@
           <xm:sqref>E9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="153" id="{1D4D4AD0-CCEF-43D8-A61B-308DB15F8A12}">
+          <x14:cfRule type="expression" priority="153" id="{C186CA8B-3CBF-4ABD-9238-00CDCA21803E}">
             <xm:f>AND((F1&lt;10),(F1&lt;&gt;solved!F1))</xm:f>
             <x14:dxf>
               <font>
@@ -8637,7 +8642,7 @@
           <xm:sqref>F1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="154" id="{F0A78A99-4350-4BAA-A55A-E6CCEA156B4B}">
+          <x14:cfRule type="expression" priority="154" id="{DFEDECA5-E3A1-4BF4-ACF9-BAADA96FC715}">
             <xm:f>AND((F2&lt;10),(F2&lt;&gt;solved!F2))</xm:f>
             <x14:dxf>
               <font>
@@ -8648,7 +8653,7 @@
           <xm:sqref>F2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="155" id="{564AE776-B4D0-4EDD-BE72-9C98FC6E5A7E}">
+          <x14:cfRule type="expression" priority="155" id="{D9575A5F-E7DB-4945-862F-296FBF11E8B4}">
             <xm:f>AND((F3&lt;10),(F3&lt;&gt;solved!F3))</xm:f>
             <x14:dxf>
               <font>
@@ -8659,7 +8664,7 @@
           <xm:sqref>F3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="156" id="{509DFC8B-8EB2-41AD-8550-A0AB633C8D3A}">
+          <x14:cfRule type="expression" priority="156" id="{88F63BCD-21ED-416E-BCD1-B51F7EC8F8FB}">
             <xm:f>AND((F4&lt;10),(F4&lt;&gt;solved!F4))</xm:f>
             <x14:dxf>
               <font>
@@ -8670,7 +8675,7 @@
           <xm:sqref>F4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="157" id="{EE3A6B78-50E0-4359-A2EC-B2754BC7263C}">
+          <x14:cfRule type="expression" priority="157" id="{6B3BCEEE-E057-4BE0-A91B-45C7C672203A}">
             <xm:f>AND((F5&lt;10),(F5&lt;&gt;solved!F5))</xm:f>
             <x14:dxf>
               <font>
@@ -8681,7 +8686,7 @@
           <xm:sqref>F5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="158" id="{339F5D54-2DAE-4513-8272-8BEDA26CE0A1}">
+          <x14:cfRule type="expression" priority="158" id="{3D33FD76-6B4C-447F-B66B-1434BFBC2434}">
             <xm:f>AND((F6&lt;10),(F6&lt;&gt;solved!F6))</xm:f>
             <x14:dxf>
               <font>
@@ -8692,7 +8697,7 @@
           <xm:sqref>F6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="159" id="{F0A42E8D-4813-4DE3-BD79-61478E904DC0}">
+          <x14:cfRule type="expression" priority="159" id="{101CB0DE-CDE6-4638-853B-6A59CE925FED}">
             <xm:f>AND((F7&lt;10),(F7&lt;&gt;solved!F7))</xm:f>
             <x14:dxf>
               <font>
@@ -8703,7 +8708,7 @@
           <xm:sqref>F7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="160" id="{6220C06B-B2F9-4870-B5A5-A082FB4331EC}">
+          <x14:cfRule type="expression" priority="160" id="{7C64A36A-3D30-4B58-8C3A-BB3CC69E9739}">
             <xm:f>AND((F8&lt;10),(F8&lt;&gt;solved!F8))</xm:f>
             <x14:dxf>
               <font>
@@ -8714,7 +8719,7 @@
           <xm:sqref>F8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="161" id="{A6502F99-80F1-4A99-B07D-49F6ECC63F5E}">
+          <x14:cfRule type="expression" priority="161" id="{E8A06391-FDE9-444B-9140-DB4C4EE8334F}">
             <xm:f>AND((F9&lt;10),(F9&lt;&gt;solved!F9))</xm:f>
             <x14:dxf>
               <font>
@@ -8725,7 +8730,7 @@
           <xm:sqref>F9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="162" id="{35898035-C8A4-4BB6-BA21-89464C3A2425}">
+          <x14:cfRule type="expression" priority="162" id="{54C58140-601D-4927-8BD9-82DD1E30C988}">
             <xm:f>AND((G1&lt;10),(G1&lt;&gt;solved!G1))</xm:f>
             <x14:dxf>
               <font>
@@ -8736,7 +8741,7 @@
           <xm:sqref>G1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="163" id="{2CB38A60-407A-4ED5-ADCB-DD54FDA1F83A}">
+          <x14:cfRule type="expression" priority="163" id="{D0B249F4-8FEF-49A8-829D-A71C88D87A82}">
             <xm:f>AND((G2&lt;10),(G2&lt;&gt;solved!G2))</xm:f>
             <x14:dxf>
               <font>
@@ -8747,7 +8752,7 @@
           <xm:sqref>G2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="164" id="{31F4F683-7FC0-43B4-9B6A-F7122F2C779A}">
+          <x14:cfRule type="expression" priority="164" id="{C33D97B6-3D98-4CBF-AEBA-B55374A15882}">
             <xm:f>AND((G3&lt;10),(G3&lt;&gt;solved!G3))</xm:f>
             <x14:dxf>
               <font>
@@ -8758,7 +8763,7 @@
           <xm:sqref>G3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="165" id="{60DDF956-EB6C-41D3-B572-B2D18EAC77D0}">
+          <x14:cfRule type="expression" priority="165" id="{1A11563F-C019-4A99-8C2B-6EBACF6FFA3F}">
             <xm:f>AND((G4&lt;10),(G4&lt;&gt;solved!G4))</xm:f>
             <x14:dxf>
               <font>
@@ -8769,7 +8774,7 @@
           <xm:sqref>G4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="166" id="{84482C00-B276-4D23-989E-D1A2A3F0BA14}">
+          <x14:cfRule type="expression" priority="166" id="{2799E854-A9A1-4680-88C4-FAF9DAD6E5D5}">
             <xm:f>AND((G5&lt;10),(G5&lt;&gt;solved!G5))</xm:f>
             <x14:dxf>
               <font>
@@ -8780,7 +8785,7 @@
           <xm:sqref>G5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="167" id="{41F4DFAA-528B-4181-83C4-503FF0C47910}">
+          <x14:cfRule type="expression" priority="167" id="{58B94A9D-3F41-4C4C-AC90-691DB0778E2C}">
             <xm:f>AND((G6&lt;10),(G6&lt;&gt;solved!G6))</xm:f>
             <x14:dxf>
               <font>
@@ -8791,7 +8796,7 @@
           <xm:sqref>G6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="168" id="{2C70924E-90F6-4A36-9646-BD599D1235C0}">
+          <x14:cfRule type="expression" priority="168" id="{F2DA3125-DCFB-4990-8ACF-BA8D7FF24293}">
             <xm:f>AND((G7&lt;10),(G7&lt;&gt;solved!G7))</xm:f>
             <x14:dxf>
               <font>
@@ -8802,7 +8807,7 @@
           <xm:sqref>G7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="169" id="{99A7587D-C756-4300-8BAA-9D814F3E2039}">
+          <x14:cfRule type="expression" priority="169" id="{1778A6D0-5E29-43A6-A051-8E6A6963BBE9}">
             <xm:f>AND((G8&lt;10),(G8&lt;&gt;solved!G8))</xm:f>
             <x14:dxf>
               <font>
@@ -8813,7 +8818,7 @@
           <xm:sqref>G8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="170" id="{957C65FA-954D-4825-8271-E18A6FDA78A3}">
+          <x14:cfRule type="expression" priority="170" id="{A182C3E4-3EAD-4647-994A-86F9ECCEC7EA}">
             <xm:f>AND((G9&lt;10),(G9&lt;&gt;solved!G9))</xm:f>
             <x14:dxf>
               <font>
@@ -8824,7 +8829,7 @@
           <xm:sqref>G9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="171" id="{7BD99E4B-2671-4E61-9CE2-7C361D2EFAA4}">
+          <x14:cfRule type="expression" priority="171" id="{A3BAD98B-4CE0-4AC0-82E2-2130A63969B8}">
             <xm:f>AND((H1&lt;10),(H1&lt;&gt;solved!H1))</xm:f>
             <x14:dxf>
               <font>
@@ -8835,7 +8840,7 @@
           <xm:sqref>H1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="172" id="{D72AF9C0-1CA0-424B-9F5D-7490F35E837E}">
+          <x14:cfRule type="expression" priority="172" id="{1660CDA8-6FCA-44EF-B549-1ADF744FCC96}">
             <xm:f>AND((H2&lt;10),(H2&lt;&gt;solved!H2))</xm:f>
             <x14:dxf>
               <font>
@@ -8846,7 +8851,7 @@
           <xm:sqref>H2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="173" id="{2AA88670-D813-42D0-95E5-ED17743069B9}">
+          <x14:cfRule type="expression" priority="173" id="{7AD096BA-FBDB-4D3B-B56B-56254A109B4C}">
             <xm:f>AND((H3&lt;10),(H3&lt;&gt;solved!H3))</xm:f>
             <x14:dxf>
               <font>
@@ -8857,7 +8862,7 @@
           <xm:sqref>H3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="174" id="{6E9CD250-97C6-4234-B6D7-8A2D4F8BC0F4}">
+          <x14:cfRule type="expression" priority="174" id="{55F4EF75-81DF-4065-AEBB-878FD060305F}">
             <xm:f>AND((H4&lt;10),(H4&lt;&gt;solved!H4))</xm:f>
             <x14:dxf>
               <font>
@@ -8868,7 +8873,7 @@
           <xm:sqref>H4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="175" id="{BEA55CA0-E3BC-4E18-B1D4-EE7BF4B51DD8}">
+          <x14:cfRule type="expression" priority="175" id="{73B855E4-1DBA-4EDE-A0E4-72314EF0FC1F}">
             <xm:f>AND((H5&lt;10),(H5&lt;&gt;solved!H5))</xm:f>
             <x14:dxf>
               <font>
@@ -8879,7 +8884,7 @@
           <xm:sqref>H5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="176" id="{3D77F8BD-F76B-4232-AC84-72F4CBE817E9}">
+          <x14:cfRule type="expression" priority="176" id="{788A4052-4DEE-4930-A941-77FAF7351B8B}">
             <xm:f>AND((H6&lt;10),(H6&lt;&gt;solved!H6))</xm:f>
             <x14:dxf>
               <font>
@@ -8890,7 +8895,7 @@
           <xm:sqref>H6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="177" id="{A4688E2E-23C7-4FAE-8EB7-539D7A308E20}">
+          <x14:cfRule type="expression" priority="177" id="{EE512738-C2D6-409E-A63D-FD937E5517E0}">
             <xm:f>AND((H7&lt;10),(H7&lt;&gt;solved!H7))</xm:f>
             <x14:dxf>
               <font>
@@ -8901,7 +8906,7 @@
           <xm:sqref>H7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="178" id="{63464515-64DE-4BFE-A34D-5C669B50862D}">
+          <x14:cfRule type="expression" priority="178" id="{D9901FB6-101E-45DB-BBD4-D7ACE643FD1E}">
             <xm:f>AND((H8&lt;10),(H8&lt;&gt;solved!H8))</xm:f>
             <x14:dxf>
               <font>
@@ -8912,7 +8917,7 @@
           <xm:sqref>H8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="179" id="{465D004D-3F2B-4560-AB31-7E74962D1DF3}">
+          <x14:cfRule type="expression" priority="179" id="{F6733076-B8A2-4115-B36E-BEAFB5834C77}">
             <xm:f>AND((H9&lt;10),(H9&lt;&gt;solved!H9))</xm:f>
             <x14:dxf>
               <font>
@@ -8923,7 +8928,7 @@
           <xm:sqref>H9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="180" id="{E0B5F21C-CDA6-4038-B2BC-A650F7FFB4A0}">
+          <x14:cfRule type="expression" priority="180" id="{D5AA404F-65A1-49CE-B1CC-3876C06DDA6C}">
             <xm:f>AND((I2&lt;10),(I2&lt;&gt;solved!I2))</xm:f>
             <x14:dxf>
               <font>
@@ -8934,7 +8939,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="181" id="{1256B28E-B011-40AB-BBC0-10F988A71870}">
+          <x14:cfRule type="expression" priority="181" id="{C7D91E84-ED3C-4E47-8130-C5A16C89B824}">
             <xm:f>AND((I3&lt;10),(I3&lt;&gt;solved!I3))</xm:f>
             <x14:dxf>
               <font>
@@ -8945,7 +8950,7 @@
           <xm:sqref>I3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="182" id="{72AF4DF8-20BC-45A6-A3D9-DA4D6B7D1F4B}">
+          <x14:cfRule type="expression" priority="182" id="{CAF194ED-66F0-4337-AB91-2C7A58DF2AA2}">
             <xm:f>AND((I4&lt;10),(I4&lt;&gt;solved!I4))</xm:f>
             <x14:dxf>
               <font>
@@ -8956,7 +8961,7 @@
           <xm:sqref>I4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="183" id="{63F7C96F-6CCF-4D99-BE30-C18B751CFA5E}">
+          <x14:cfRule type="expression" priority="183" id="{762F1F78-CAC1-45B8-ADE6-B0C57D3B6A5B}">
             <xm:f>AND((I5&lt;10),(I5&lt;&gt;solved!I5))</xm:f>
             <x14:dxf>
               <font>
@@ -8967,7 +8972,7 @@
           <xm:sqref>I5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="184" id="{AF5AF43B-A757-4CAE-8766-B3DF27AE4F8A}">
+          <x14:cfRule type="expression" priority="184" id="{102D9451-4CAE-4A94-ADAE-BA91709D8136}">
             <xm:f>AND((I6&lt;10),(I6&lt;&gt;solved!I6))</xm:f>
             <x14:dxf>
               <font>
@@ -8978,7 +8983,7 @@
           <xm:sqref>I6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="185" id="{DBBEB256-3350-424B-AEDF-D36E2090CE44}">
+          <x14:cfRule type="expression" priority="185" id="{3D356F47-6522-406B-8645-A72D58A040DB}">
             <xm:f>AND((I7&lt;10),(I7&lt;&gt;solved!I7))</xm:f>
             <x14:dxf>
               <font>
@@ -8989,7 +8994,7 @@
           <xm:sqref>I7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="186" id="{FE2FD8BE-35D5-4ECF-99BC-C74A3A1CA6CA}">
+          <x14:cfRule type="expression" priority="186" id="{76ADC081-7377-4C7C-BE19-C5DEDB71B927}">
             <xm:f>AND((I8&lt;10),(I8&lt;&gt;solved!I8))</xm:f>
             <x14:dxf>
               <font>
@@ -9000,7 +9005,7 @@
           <xm:sqref>I8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="187" id="{71B4A1BF-68A0-4F61-9D23-225C8E6A5981}">
+          <x14:cfRule type="expression" priority="187" id="{15C096E0-2517-49A5-A2FB-DCAB33E168DE}">
             <xm:f>AND((I9&lt;10),(I9&lt;&gt;solved!I9))</xm:f>
             <x14:dxf>
               <font>
@@ -9011,7 +9016,7 @@
           <xm:sqref>I9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="188" id="{9657BA12-76EC-4159-91E0-6836532F5093}">
+          <x14:cfRule type="expression" priority="188" id="{949AD213-526E-4920-82E8-FD1C4910A964}">
             <xm:f>AND(($A$1&lt;10),($A$1&lt;&gt;solved!$A$1))</xm:f>
             <x14:dxf>
               <font>
@@ -9022,7 +9027,7 @@
           <xm:sqref>A1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="189" id="{F6A244F4-514B-41DE-BD7C-5E3121EA3A83}">
+          <x14:cfRule type="expression" priority="189" id="{797A7CFC-59B5-4C38-90C9-10E74D117D40}">
             <xm:f>AND(($A$4&lt;10),($A$4&lt;&gt;solved!$A$4))</xm:f>
             <x14:dxf>
               <font>
@@ -9057,7 +9062,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -9065,22 +9070,22 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19"/>
+      <c r="A2" s="20"/>
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19"/>
+      <c r="A3" s="20"/>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="n">
+      <c r="A5" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="57" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -9088,10 +9093,10 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="19"/>
+      <c r="A6" s="20"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19" t="n">
+      <c r="A7" s="20" t="n">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -9102,10 +9107,10 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19"/>
+      <c r="A8" s="20"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19" t="n">
+      <c r="A9" s="20" t="n">
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -9116,10 +9121,10 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19"/>
+      <c r="A10" s="20"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19" t="n">
+      <c r="A11" s="20" t="n">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -9130,23 +9135,23 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="19"/>
+      <c r="A12" s="20"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="19"/>
+      <c r="A13" s="20"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19"/>
+      <c r="A14" s="20"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="19"/>
+      <c r="A15" s="20"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19"/>
-    </row>
-    <row r="17" s="19" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A16" s="20"/>
+    </row>
+    <row r="17" s="20" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="19"/>
+      <c r="A18" s="20"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -9752,7 +9757,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="3"/>
       <c r="I1" s="4"/>
-      <c r="K1" s="5" t="str">
+      <c r="K1" s="16" t="str">
         <f aca="false">IF(COUNTIF($A$1:$I$9, "1")=9, 1, "")</f>
         <v/>
       </c>
@@ -9970,7 +9975,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="29" id="{D26CDA51-C321-4D2C-9A88-B598268C8171}">
+          <x14:cfRule type="expression" priority="29" id="{7ACB586B-7C91-42ED-B750-501F1CE429CA}">
             <xm:f>AND(($A$1&lt;10),($A$1&lt;&gt;solved!$A$1))</xm:f>
             <x14:dxf>
               <font>
@@ -9986,7 +9991,7 @@
           <xm:sqref>A1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="30" id="{C26BEC53-AA13-4627-AAD0-5A9F204EEE21}">
+          <x14:cfRule type="expression" priority="30" id="{37936E16-4AF0-41DA-8C85-86959010A675}">
             <xm:f>AND((A2&lt;10),(A2&lt;&gt;solved!A2))</xm:f>
             <x14:dxf>
               <font>
@@ -9997,7 +10002,7 @@
           <xm:sqref>A2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="31" id="{A52BC9C3-54AC-43E9-AB8C-87F76F7027EB}">
+          <x14:cfRule type="expression" priority="31" id="{75D7E819-CE60-4E3A-8A7C-955D4FE856A6}">
             <xm:f>AND((A3&lt;10),(A3&lt;&gt;solved!A3))</xm:f>
             <x14:dxf>
               <font>
@@ -10008,7 +10013,7 @@
           <xm:sqref>A3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="32" id="{7933836D-9030-4C52-97F6-4C8B4CAF89D2}">
+          <x14:cfRule type="expression" priority="32" id="{A0D81311-2FE2-4550-9BB0-4F9EBED51A70}">
             <xm:f>AND((A4&lt;10),(A4&lt;&gt;solved!A4))</xm:f>
             <x14:dxf>
               <font>
@@ -10019,7 +10024,7 @@
           <xm:sqref>A4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="33" id="{DC58A28F-8DFD-4141-B8BB-2C2CA96868A0}">
+          <x14:cfRule type="expression" priority="33" id="{CF2378C3-A08D-4AB3-AF2B-801D904DF73A}">
             <xm:f>AND((A5&lt;10),(A5&lt;&gt;solved!A5))</xm:f>
             <x14:dxf>
               <font>
@@ -10030,7 +10035,7 @@
           <xm:sqref>A5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="34" id="{FBA3D8EC-4B10-433C-98B6-A0B0E51CB12F}">
+          <x14:cfRule type="expression" priority="34" id="{373EBA61-B4A2-4D58-8E38-A2701D75FCD7}">
             <xm:f>AND((A6&lt;10),(A6&lt;&gt;solved!A6))</xm:f>
             <x14:dxf>
               <font>
@@ -10041,7 +10046,7 @@
           <xm:sqref>A6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="35" id="{E0872E7D-7EAD-402A-BB3D-DA355CFD7677}">
+          <x14:cfRule type="expression" priority="35" id="{88838728-F7BB-48A3-8E4C-653BA28A797A}">
             <xm:f>AND((A7&lt;10),(A7&lt;&gt;solved!A7))</xm:f>
             <x14:dxf>
               <font>
@@ -10052,7 +10057,7 @@
           <xm:sqref>A7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="36" id="{17948EE3-B975-4930-8C4B-B2F952429252}">
+          <x14:cfRule type="expression" priority="36" id="{8AC6E000-2041-42C7-9C2B-3BBC39E51CF1}">
             <xm:f>AND((A8&lt;10),(A8&lt;&gt;solved!A8))</xm:f>
             <x14:dxf>
               <font>
@@ -10063,7 +10068,7 @@
           <xm:sqref>A8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="37" id="{69F7FB20-24B4-431C-AB4E-FCE8A151F66F}">
+          <x14:cfRule type="expression" priority="37" id="{5052FB9C-3476-4275-B418-419A86354749}">
             <xm:f>AND((A9&lt;10),(A9&lt;&gt;solved!A9))</xm:f>
             <x14:dxf>
               <font>
@@ -10074,7 +10079,7 @@
           <xm:sqref>A9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="38" id="{2F51CB4A-B2BC-46B2-A7F9-0046D8C8C613}">
+          <x14:cfRule type="expression" priority="38" id="{26EFD817-70C1-4E4E-A04A-56B96D8EC066}">
             <xm:f>AND((B1&lt;10),(B1&lt;&gt;solved!B1))</xm:f>
             <x14:dxf>
               <font>
@@ -10085,7 +10090,7 @@
           <xm:sqref>B1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="39" id="{834630C0-CB7A-4154-8469-6A62BFB693C7}">
+          <x14:cfRule type="expression" priority="39" id="{FA74117F-1327-4340-9F16-A697106A4A8B}">
             <xm:f>AND((B2&lt;10),(B2&lt;&gt;solved!B2))</xm:f>
             <x14:dxf>
               <font>
@@ -10096,7 +10101,7 @@
           <xm:sqref>B2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="40" id="{60464039-D092-4EA1-8240-EC3A27428658}">
+          <x14:cfRule type="expression" priority="40" id="{A5591135-FDD0-4D20-8A96-969ACDD63EBB}">
             <xm:f>AND((B3&lt;10),(B3&lt;&gt;solved!B3))</xm:f>
             <x14:dxf>
               <font>
@@ -10107,7 +10112,7 @@
           <xm:sqref>B3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="41" id="{7C15CEF4-C4B7-44DD-9368-905C3AD6B4BB}">
+          <x14:cfRule type="expression" priority="41" id="{E66A8B94-7FC9-4774-B759-8E84608DA0EF}">
             <xm:f>AND((B4&lt;10),(B4&lt;&gt;solved!B4))</xm:f>
             <x14:dxf>
               <font>
@@ -10118,7 +10123,7 @@
           <xm:sqref>B4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="42" id="{2D922414-D0B0-43E4-83E5-C02FDEF8EF3F}">
+          <x14:cfRule type="expression" priority="42" id="{84179036-6F13-4F55-81A1-5FDC77A0D470}">
             <xm:f>AND((B5&lt;10),(B5&lt;&gt;solved!B5))</xm:f>
             <x14:dxf>
               <font>
@@ -10129,7 +10134,7 @@
           <xm:sqref>B5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="43" id="{53D0F27A-7319-4347-A49F-307C1DAAF777}">
+          <x14:cfRule type="expression" priority="43" id="{3757C071-2B6F-464B-9393-DA38C6395D4E}">
             <xm:f>AND((B6&lt;10),(B6&lt;&gt;solved!B6))</xm:f>
             <x14:dxf>
               <font>
@@ -10140,7 +10145,7 @@
           <xm:sqref>B6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="44" id="{3A2ED2B0-FC91-47F9-8225-B839D3DB8D51}">
+          <x14:cfRule type="expression" priority="44" id="{D5BF20D5-A34F-4D16-857A-2E311010AEDE}">
             <xm:f>AND((B7&lt;10),(B7&lt;&gt;solved!B7))</xm:f>
             <x14:dxf>
               <font>
@@ -10151,7 +10156,7 @@
           <xm:sqref>B7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="45" id="{C03B74EC-1A94-4837-8716-53BA3E71E471}">
+          <x14:cfRule type="expression" priority="45" id="{BFF0A614-20AC-4712-9655-E06B6CD22CDE}">
             <xm:f>AND((B8&lt;10),(B8&lt;&gt;solved!B8))</xm:f>
             <x14:dxf>
               <font>
@@ -10162,7 +10167,7 @@
           <xm:sqref>B8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="46" id="{F0ACB048-AB98-4AEC-B7A1-565BEA879CFE}">
+          <x14:cfRule type="expression" priority="46" id="{E357CEAA-4367-4F76-A858-D08630163916}">
             <xm:f>AND((B9&lt;10),(B9&lt;&gt;solved!B9))</xm:f>
             <x14:dxf>
               <font>
@@ -10173,7 +10178,7 @@
           <xm:sqref>B9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="47" id="{7B75C762-C2CA-4CD2-B653-546049D2238A}">
+          <x14:cfRule type="expression" priority="47" id="{3C61829B-6620-49B7-9459-EB1F69201BC3}">
             <xm:f>AND((C1&lt;10),(C1&lt;&gt;solved!C1))</xm:f>
             <x14:dxf>
               <font>
@@ -10184,7 +10189,7 @@
           <xm:sqref>C1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="48" id="{5B1ECA6C-1757-4CB6-9674-64DB4CF87AEA}">
+          <x14:cfRule type="expression" priority="48" id="{8B80D4E5-DF72-4EA1-A0D2-6CAF35657F15}">
             <xm:f>AND((C2&lt;10),(C2&lt;&gt;solved!C2))</xm:f>
             <x14:dxf>
               <font>
@@ -10195,7 +10200,7 @@
           <xm:sqref>C2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="49" id="{85AF278A-6AFC-4AD1-BEED-54762526B51D}">
+          <x14:cfRule type="expression" priority="49" id="{863893E0-F46D-4EFE-B864-63202336A433}">
             <xm:f>AND((C3&lt;10),(C3&lt;&gt;solved!C3))</xm:f>
             <x14:dxf>
               <font>
@@ -10206,7 +10211,7 @@
           <xm:sqref>C3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="50" id="{88E69A62-F0B4-48A5-ABAE-7D859A8641D6}">
+          <x14:cfRule type="expression" priority="50" id="{DCB6CBC2-8A64-4825-96E4-26A57D7BDDFE}">
             <xm:f>AND((C4&lt;10),(C4&lt;&gt;solved!C4))</xm:f>
             <x14:dxf>
               <font>
@@ -10217,7 +10222,7 @@
           <xm:sqref>C4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="51" id="{B7388966-5558-45E6-BE44-E8D555577428}">
+          <x14:cfRule type="expression" priority="51" id="{8F8DC63B-C528-4AAA-AF2A-67D03DFFE580}">
             <xm:f>AND((C5&lt;10),(C5&lt;&gt;solved!C5))</xm:f>
             <x14:dxf>
               <font>
@@ -10228,7 +10233,7 @@
           <xm:sqref>C5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="52" id="{4E909320-F5FB-4BEA-AF28-709E95A31535}">
+          <x14:cfRule type="expression" priority="52" id="{C3B076DC-A72C-4767-9AF3-1092EB62389B}">
             <xm:f>AND((C6&lt;10),(C6&lt;&gt;solved!C6))</xm:f>
             <x14:dxf>
               <font>
@@ -10239,7 +10244,7 @@
           <xm:sqref>C6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="53" id="{5AF8E03C-9C94-4CFD-B3E3-2D9D8AC88812}">
+          <x14:cfRule type="expression" priority="53" id="{CA96CD57-90B1-46DF-9278-50F3CB14256B}">
             <xm:f>AND((C7&lt;10),(C7&lt;&gt;solved!C7))</xm:f>
             <x14:dxf>
               <font>
@@ -10250,7 +10255,7 @@
           <xm:sqref>C7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="54" id="{5CDC7D68-FC83-41B4-B27C-14FBD51F4960}">
+          <x14:cfRule type="expression" priority="54" id="{DA58D481-BD98-4583-9855-D78ADE8D87A3}">
             <xm:f>AND((C8&lt;10),(C8&lt;&gt;solved!C8))</xm:f>
             <x14:dxf>
               <font>
@@ -10261,7 +10266,7 @@
           <xm:sqref>C8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="55" id="{C6EBFC2E-00EE-4740-ADA5-5D3C95502068}">
+          <x14:cfRule type="expression" priority="55" id="{2891B8FA-8C58-4382-936C-A8BF49BBC841}">
             <xm:f>AND((C9&lt;10),(C9&lt;&gt;solved!C9))</xm:f>
             <x14:dxf>
               <font>
@@ -10272,7 +10277,7 @@
           <xm:sqref>C9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="56" id="{255A1DD6-B5B0-42F7-9693-DADC6173807E}">
+          <x14:cfRule type="expression" priority="56" id="{52C5BCA5-959E-4366-B747-47F9EEB4D027}">
             <xm:f>AND((D1&lt;10),(D1&lt;&gt;solved!D1))</xm:f>
             <x14:dxf>
               <font>
@@ -10283,7 +10288,7 @@
           <xm:sqref>D1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="57" id="{BE1CE893-5E20-4B3F-8C31-DF3E1A722ADB}">
+          <x14:cfRule type="expression" priority="57" id="{B4705BA5-7FCD-40A0-883F-75F458ADCC47}">
             <xm:f>AND((D2&lt;10),(D2&lt;&gt;solved!D2))</xm:f>
             <x14:dxf>
               <font>
@@ -10294,7 +10299,7 @@
           <xm:sqref>D2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="58" id="{50BD9499-F4AE-4F58-B7BC-DB7F775BCAEA}">
+          <x14:cfRule type="expression" priority="58" id="{8E90F3B9-5E5B-4A79-BB10-61A090589F51}">
             <xm:f>AND((D3&lt;10),(D3&lt;&gt;solved!D3))</xm:f>
             <x14:dxf>
               <font>
@@ -10305,7 +10310,7 @@
           <xm:sqref>D3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="59" id="{E9F36B10-E3B8-46CE-9378-264B30EC7C47}">
+          <x14:cfRule type="expression" priority="59" id="{FFF34DB1-DA15-419D-8284-5EA77DAD14D8}">
             <xm:f>AND((D4&lt;10),(D4&lt;&gt;solved!D4))</xm:f>
             <x14:dxf>
               <font>
@@ -10316,7 +10321,7 @@
           <xm:sqref>D4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="60" id="{578A8CE1-2664-4720-AAE8-C872D6145044}">
+          <x14:cfRule type="expression" priority="60" id="{D9291492-E25F-474D-AEDE-28B7E65A4043}">
             <xm:f>AND((D5&lt;10),(D5&lt;&gt;solved!D5))</xm:f>
             <x14:dxf>
               <font>
@@ -10327,7 +10332,7 @@
           <xm:sqref>D5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="61" id="{5150A0AE-C390-4680-AC3B-A0F07A7C4A9C}">
+          <x14:cfRule type="expression" priority="61" id="{204A27D8-7550-4D2A-955A-B722B087A330}">
             <xm:f>AND((D6&lt;10),(D6&lt;&gt;solved!D6))</xm:f>
             <x14:dxf>
               <font>
@@ -10338,7 +10343,7 @@
           <xm:sqref>D6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="62" id="{A9A6AC54-549B-43CB-8EC8-F830D9F7F090}">
+          <x14:cfRule type="expression" priority="62" id="{A37E4195-7B9D-4AAC-8AB0-BF61AFC8E891}">
             <xm:f>AND((D7&lt;10),(D7&lt;&gt;solved!D7))</xm:f>
             <x14:dxf>
               <font>
@@ -10349,7 +10354,7 @@
           <xm:sqref>D7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="63" id="{84858D2B-F84B-48AB-927C-E547A760BE43}">
+          <x14:cfRule type="expression" priority="63" id="{62269B1B-2623-4B69-9C8F-D93EC729E019}">
             <xm:f>AND((D8&lt;10),(D8&lt;&gt;solved!D8))</xm:f>
             <x14:dxf>
               <font>
@@ -10360,7 +10365,7 @@
           <xm:sqref>D8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="64" id="{68A859CD-898B-4E15-AB81-7FF1FFAB4BDE}">
+          <x14:cfRule type="expression" priority="64" id="{E6E08D39-F813-47E5-8A7B-FEED7D7DE123}">
             <xm:f>AND((D9&lt;10),(D9&lt;&gt;solved!D9))</xm:f>
             <x14:dxf>
               <font>
@@ -10371,7 +10376,7 @@
           <xm:sqref>D9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="65" id="{DB568072-8BDC-4FDE-A937-61A729CBE3AA}">
+          <x14:cfRule type="expression" priority="65" id="{46D33919-1939-4E95-AFD5-BC24DD2815CD}">
             <xm:f>AND((E1&lt;10),(E1&lt;&gt;solved!E1))</xm:f>
             <x14:dxf>
               <font>
@@ -10382,7 +10387,7 @@
           <xm:sqref>E1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="66" id="{ECF3CE9F-6441-4D4C-BFA6-EC855FA29073}">
+          <x14:cfRule type="expression" priority="66" id="{5BE8D761-8CB3-4180-A189-7BE4E5E250ED}">
             <xm:f>AND((E2&lt;10),(E2&lt;&gt;solved!E2))</xm:f>
             <x14:dxf>
               <font>
@@ -10393,7 +10398,7 @@
           <xm:sqref>E2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="67" id="{75FADF1C-57B6-47F4-8C60-60E0A079E445}">
+          <x14:cfRule type="expression" priority="67" id="{80D08F00-A73C-4553-9F16-5799188150F2}">
             <xm:f>AND((E3&lt;10),(E3&lt;&gt;solved!E3))</xm:f>
             <x14:dxf>
               <font>
@@ -10404,7 +10409,7 @@
           <xm:sqref>E3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="68" id="{1A5CEFC3-BA96-4314-A214-9C4AB04A3A85}">
+          <x14:cfRule type="expression" priority="68" id="{C055E178-72D7-4787-AE6D-26F0FDF3C872}">
             <xm:f>AND((E4&lt;10),(E4&lt;&gt;solved!E4))</xm:f>
             <x14:dxf>
               <font>
@@ -10415,7 +10420,7 @@
           <xm:sqref>E4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="69" id="{333B80CC-E976-4250-8D4B-1780DABA8327}">
+          <x14:cfRule type="expression" priority="69" id="{C021E0F5-6A47-4CCA-BB5D-83CF90742AFC}">
             <xm:f>AND((E5&lt;10),(E5&lt;&gt;solved!E5))</xm:f>
             <x14:dxf>
               <font>
@@ -10426,7 +10431,7 @@
           <xm:sqref>E5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="70" id="{11E54038-E7D0-4556-BCFA-9386B4FED6C4}">
+          <x14:cfRule type="expression" priority="70" id="{A6E12716-8FBF-42C8-93B8-752394AF3976}">
             <xm:f>AND((E6&lt;10),(E6&lt;&gt;solved!E6))</xm:f>
             <x14:dxf>
               <font>
@@ -10437,7 +10442,7 @@
           <xm:sqref>E6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="71" id="{A4757080-EE19-4C36-9210-BBF897658311}">
+          <x14:cfRule type="expression" priority="71" id="{20B0C15B-28D0-4572-9098-85B83E922957}">
             <xm:f>AND((E7&lt;10),(E7&lt;&gt;solved!E7))</xm:f>
             <x14:dxf>
               <font>
@@ -10448,7 +10453,7 @@
           <xm:sqref>E7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="72" id="{EAA65891-7087-4694-882A-10C0312F36DF}">
+          <x14:cfRule type="expression" priority="72" id="{80439C72-D88D-499F-A6C4-BF37CA77DC68}">
             <xm:f>AND((E8&lt;10),(E8&lt;&gt;solved!E8))</xm:f>
             <x14:dxf>
               <font>
@@ -10459,7 +10464,7 @@
           <xm:sqref>E8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="73" id="{604CEE5D-D2DD-4AFD-8746-DF60D9E5601B}">
+          <x14:cfRule type="expression" priority="73" id="{C0D6D9F4-BA39-45D7-95D2-4BA5D0834CC9}">
             <xm:f>AND((E9&lt;10),(E9&lt;&gt;solved!E9))</xm:f>
             <x14:dxf>
               <font>
@@ -10470,7 +10475,7 @@
           <xm:sqref>E9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="74" id="{5B82436D-1857-42AB-94CA-82502960B466}">
+          <x14:cfRule type="expression" priority="74" id="{10B5B9C0-AAA4-41D6-9D3D-98A4F792307D}">
             <xm:f>AND((F1&lt;10),(F1&lt;&gt;solved!F1))</xm:f>
             <x14:dxf>
               <font>
@@ -10481,7 +10486,7 @@
           <xm:sqref>F1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="75" id="{B2DD56E3-2821-426D-96A5-22663BE9A0FD}">
+          <x14:cfRule type="expression" priority="75" id="{ABD53DC2-A495-439B-A820-6564906669E9}">
             <xm:f>AND((F2&lt;10),(F2&lt;&gt;solved!F2))</xm:f>
             <x14:dxf>
               <font>
@@ -10492,7 +10497,7 @@
           <xm:sqref>F2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="76" id="{F4D1DE3B-8BAA-46CE-931E-AAF8F11CC7D8}">
+          <x14:cfRule type="expression" priority="76" id="{E7953C2D-3964-4924-947A-D3409BB258CA}">
             <xm:f>AND((F3&lt;10),(F3&lt;&gt;solved!F3))</xm:f>
             <x14:dxf>
               <font>
@@ -10503,7 +10508,7 @@
           <xm:sqref>F3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="77" id="{7D3DB3B8-2447-422A-B96A-A54CCEF4C29A}">
+          <x14:cfRule type="expression" priority="77" id="{70979321-53C0-467E-A2B3-11C0D98E9063}">
             <xm:f>AND((F4&lt;10),(F4&lt;&gt;solved!F4))</xm:f>
             <x14:dxf>
               <font>
@@ -10514,7 +10519,7 @@
           <xm:sqref>F4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="78" id="{1E4E93E6-80A8-4D6F-BD9E-15A4187D20C0}">
+          <x14:cfRule type="expression" priority="78" id="{AEF0BBF1-A4F3-4B65-A26F-E0DC4A8CEB89}">
             <xm:f>AND((F5&lt;10),(F5&lt;&gt;solved!F5))</xm:f>
             <x14:dxf>
               <font>
@@ -10525,7 +10530,7 @@
           <xm:sqref>F5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="79" id="{E93B90D0-472C-4EF8-9DB8-31CA8DABDBDD}">
+          <x14:cfRule type="expression" priority="79" id="{D55CECC8-ACF5-4095-9051-B7219558B69A}">
             <xm:f>AND((F6&lt;10),(F6&lt;&gt;solved!F6))</xm:f>
             <x14:dxf>
               <font>
@@ -10536,7 +10541,7 @@
           <xm:sqref>F6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="80" id="{FD1268F6-675A-407E-9325-1B37E3177B7F}">
+          <x14:cfRule type="expression" priority="80" id="{31FAE327-88DA-4A4D-A798-71C03A2FCFFB}">
             <xm:f>AND((F7&lt;10),(F7&lt;&gt;solved!F7))</xm:f>
             <x14:dxf>
               <font>
@@ -10547,7 +10552,7 @@
           <xm:sqref>F7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="81" id="{1C8FA47C-48F2-4C96-938A-E0DC40A81E86}">
+          <x14:cfRule type="expression" priority="81" id="{1B46F4F2-8B14-4C4B-AF23-D4399D30B1AE}">
             <xm:f>AND((F8&lt;10),(F8&lt;&gt;solved!F8))</xm:f>
             <x14:dxf>
               <font>
@@ -10558,7 +10563,7 @@
           <xm:sqref>F8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="82" id="{65A1EBFE-8782-4E70-BF34-2F161FD9E357}">
+          <x14:cfRule type="expression" priority="82" id="{928F26E9-88E9-4D11-92EF-70593E57FDE6}">
             <xm:f>AND((F9&lt;10),(F9&lt;&gt;solved!F9))</xm:f>
             <x14:dxf>
               <font>
@@ -10569,7 +10574,7 @@
           <xm:sqref>F9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="83" id="{274539B3-1E2E-401C-8631-381EF52D2355}">
+          <x14:cfRule type="expression" priority="83" id="{9F4E54BB-EFF5-40C3-9C2F-897CFB57404E}">
             <xm:f>AND((G1&lt;10),(G1&lt;&gt;solved!G1))</xm:f>
             <x14:dxf>
               <font>
@@ -10580,7 +10585,7 @@
           <xm:sqref>G1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="84" id="{D4DB707C-E940-4E3C-9369-BE6DCF2FED29}">
+          <x14:cfRule type="expression" priority="84" id="{A22CB461-6254-4CC3-AF33-B28E9BBAF93C}">
             <xm:f>AND((G2&lt;10),(G2&lt;&gt;solved!G2))</xm:f>
             <x14:dxf>
               <font>
@@ -10591,7 +10596,7 @@
           <xm:sqref>G2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="85" id="{B397CB97-AEDF-4C82-B138-90DD9AC3A346}">
+          <x14:cfRule type="expression" priority="85" id="{355868DB-2210-4220-8923-E77F6D1022E7}">
             <xm:f>AND((G3&lt;10),(G3&lt;&gt;solved!G3))</xm:f>
             <x14:dxf>
               <font>
@@ -10602,7 +10607,7 @@
           <xm:sqref>G3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="86" id="{F56AED37-54A7-41FA-8512-63C36893B365}">
+          <x14:cfRule type="expression" priority="86" id="{BFA1298F-A5F2-401C-845A-5421BB1F3A4E}">
             <xm:f>AND((G4&lt;10),(G4&lt;&gt;solved!G4))</xm:f>
             <x14:dxf>
               <font>
@@ -10613,7 +10618,7 @@
           <xm:sqref>G4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="87" id="{9D5FF2B6-264C-4BD9-81FF-BAE98E367855}">
+          <x14:cfRule type="expression" priority="87" id="{8AF46C9D-D9B3-437A-97DE-6D77868E4780}">
             <xm:f>AND((G5&lt;10),(G5&lt;&gt;solved!G5))</xm:f>
             <x14:dxf>
               <font>
@@ -10624,7 +10629,7 @@
           <xm:sqref>G5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="88" id="{BA9192A3-B65D-4B6C-8AF9-297C581090FB}">
+          <x14:cfRule type="expression" priority="88" id="{434B34AC-9132-40CB-BAB1-ABC170D05017}">
             <xm:f>AND((G6&lt;10),(G6&lt;&gt;solved!G6))</xm:f>
             <x14:dxf>
               <font>
@@ -10635,7 +10640,7 @@
           <xm:sqref>G6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="89" id="{43119556-A655-423A-8C62-6F8090A3401B}">
+          <x14:cfRule type="expression" priority="89" id="{117A145A-5FCE-4F3C-89DA-8A951922CD70}">
             <xm:f>AND((G7&lt;10),(G7&lt;&gt;solved!G7))</xm:f>
             <x14:dxf>
               <font>
@@ -10646,7 +10651,7 @@
           <xm:sqref>G7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="90" id="{FDAF2ADF-E241-44DC-9477-AFD77BCC5FD9}">
+          <x14:cfRule type="expression" priority="90" id="{875F2D16-CCBD-4D2F-9FA9-BF196755163E}">
             <xm:f>AND((G8&lt;10),(G8&lt;&gt;solved!G8))</xm:f>
             <x14:dxf>
               <font>
@@ -10657,7 +10662,7 @@
           <xm:sqref>G8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="91" id="{D6F3D3B0-E920-40C4-9535-1BD7D8798D90}">
+          <x14:cfRule type="expression" priority="91" id="{A8F9AD99-5377-4629-91B4-E08BF0265564}">
             <xm:f>AND((G9&lt;10),(G9&lt;&gt;solved!G9))</xm:f>
             <x14:dxf>
               <font>
@@ -10668,7 +10673,7 @@
           <xm:sqref>G9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="92" id="{2B8AFE2D-B918-433D-909B-16573F7EC483}">
+          <x14:cfRule type="expression" priority="92" id="{2BFB5D82-AF90-49BC-A06B-5EC5A3CD35B6}">
             <xm:f>AND((H1&lt;10),(H1&lt;&gt;solved!H1))</xm:f>
             <x14:dxf>
               <font>
@@ -10679,7 +10684,7 @@
           <xm:sqref>H1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="93" id="{749643BC-D537-4FD2-B9F3-A5AE77F3F8E9}">
+          <x14:cfRule type="expression" priority="93" id="{9C45EFBD-7E4E-4A3F-BBEB-FECA5E3B11BF}">
             <xm:f>AND((H2&lt;10),(H2&lt;&gt;solved!H2))</xm:f>
             <x14:dxf>
               <font>
@@ -10690,7 +10695,7 @@
           <xm:sqref>H2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="94" id="{E9C48F58-C3C0-4429-98B3-3B6D1C766087}">
+          <x14:cfRule type="expression" priority="94" id="{144DD6E1-BA8A-4E8C-95A2-744550F9DBE2}">
             <xm:f>AND((H3&lt;10),(H3&lt;&gt;solved!H3))</xm:f>
             <x14:dxf>
               <font>
@@ -10701,7 +10706,7 @@
           <xm:sqref>H3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="95" id="{3DFC82B2-86BD-4AC6-903A-BC80373AE759}">
+          <x14:cfRule type="expression" priority="95" id="{7DDFF0A5-97F7-40B6-A3A7-1DCA93186EA2}">
             <xm:f>AND((H4&lt;10),(H4&lt;&gt;solved!H4))</xm:f>
             <x14:dxf>
               <font>
@@ -10712,7 +10717,7 @@
           <xm:sqref>H4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="96" id="{484DDBA0-9411-4B17-86E8-3B11FDC78035}">
+          <x14:cfRule type="expression" priority="96" id="{C8CC13AC-43E7-4E36-B332-70AFA78D6CBF}">
             <xm:f>AND((H5&lt;10),(H5&lt;&gt;solved!H5))</xm:f>
             <x14:dxf>
               <font>
@@ -10723,7 +10728,7 @@
           <xm:sqref>H5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="97" id="{D2EBA43F-28D3-4320-854C-A55BCC505FCF}">
+          <x14:cfRule type="expression" priority="97" id="{3BBDA8B7-7C21-403B-B733-87742C2192CC}">
             <xm:f>AND((H6&lt;10),(H6&lt;&gt;solved!H6))</xm:f>
             <x14:dxf>
               <font>
@@ -10734,7 +10739,7 @@
           <xm:sqref>H6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="98" id="{40DDAE18-A02F-4F21-BDDC-18EF54B36930}">
+          <x14:cfRule type="expression" priority="98" id="{261BDFD0-20F0-4BE2-A1ED-B33422E152C5}">
             <xm:f>AND((H7&lt;10),(H7&lt;&gt;solved!H7))</xm:f>
             <x14:dxf>
               <font>
@@ -10745,7 +10750,7 @@
           <xm:sqref>H7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="99" id="{F5A660FE-F86D-45B4-92F2-F55FDA9EE7D4}">
+          <x14:cfRule type="expression" priority="99" id="{35584813-2B2B-4859-8E22-249A3FC8C011}">
             <xm:f>AND((H8&lt;10),(H8&lt;&gt;solved!H8))</xm:f>
             <x14:dxf>
               <font>
@@ -10756,7 +10761,7 @@
           <xm:sqref>H8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="100" id="{802088F9-9858-4651-9D97-BBDF816B76EB}">
+          <x14:cfRule type="expression" priority="100" id="{F5E32E51-386A-4D4A-B847-18DCCDE569C4}">
             <xm:f>AND((H9&lt;10),(H9&lt;&gt;solved!H9))</xm:f>
             <x14:dxf>
               <font>
@@ -10767,7 +10772,7 @@
           <xm:sqref>H9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="101" id="{5E138CFF-D6DD-42BB-BEE2-8EE659109EB2}">
+          <x14:cfRule type="expression" priority="101" id="{F956DC3E-2626-4A8A-8474-6F16975B9399}">
             <xm:f>AND((I2&lt;10),(I2&lt;&gt;solved!I2))</xm:f>
             <x14:dxf>
               <font>
@@ -10778,7 +10783,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="102" id="{BA848AB0-2E6F-46D0-97EE-C2CDBBF8B65B}">
+          <x14:cfRule type="expression" priority="102" id="{573FFE19-6A77-46A8-AB88-866050973059}">
             <xm:f>AND((I1&lt;10),(I1&lt;&gt;solved!I1))</xm:f>
             <x14:dxf>
               <font>
@@ -10789,7 +10794,7 @@
           <xm:sqref>I1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="103" id="{E0B11CB5-7C9A-40A3-95A3-FC9326F343A2}">
+          <x14:cfRule type="expression" priority="103" id="{96B5673D-9C2D-49B0-BA9E-F371EBDE5C48}">
             <xm:f>AND((I3&lt;10),(I3&lt;&gt;solved!I3))</xm:f>
             <x14:dxf>
               <font>
@@ -10800,7 +10805,7 @@
           <xm:sqref>I3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="104" id="{E07928E8-BEBB-496F-BE48-B6486EB112EF}">
+          <x14:cfRule type="expression" priority="104" id="{CB9B9350-DF74-467C-9130-9E51ED2F6BB7}">
             <xm:f>AND((I4&lt;10),(I4&lt;&gt;solved!I4))</xm:f>
             <x14:dxf>
               <font>
@@ -10811,7 +10816,7 @@
           <xm:sqref>I4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="105" id="{F1ECC023-5831-44BC-AABC-537CB3C41082}">
+          <x14:cfRule type="expression" priority="105" id="{36A5DDDF-3064-4252-BCFE-A9CA31F4D1B8}">
             <xm:f>AND((I5&lt;10),(I5&lt;&gt;solved!I5))</xm:f>
             <x14:dxf>
               <font>
@@ -10822,7 +10827,7 @@
           <xm:sqref>I5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="106" id="{4B3BB01A-9BE4-42B9-94A2-B752BB93C2A0}">
+          <x14:cfRule type="expression" priority="106" id="{C0DEA249-514F-488E-A1B0-61DE42601BBE}">
             <xm:f>AND((I6&lt;10),(I6&lt;&gt;solved!I6))</xm:f>
             <x14:dxf>
               <font>
@@ -10833,7 +10838,7 @@
           <xm:sqref>I6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="107" id="{4FE3C057-B0BB-4959-9344-BC3DAB58F55F}">
+          <x14:cfRule type="expression" priority="107" id="{2A49F132-18A8-40C5-8755-84276DFE1B9D}">
             <xm:f>AND((I7&lt;10),(I7&lt;&gt;solved!I7))</xm:f>
             <x14:dxf>
               <font>
@@ -10844,7 +10849,7 @@
           <xm:sqref>I7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="108" id="{7A32AD70-E6C0-4F84-9B9D-B16C60FE3077}">
+          <x14:cfRule type="expression" priority="108" id="{9F401556-4430-4013-8620-2D436A31F024}">
             <xm:f>AND((I8&lt;10),(I8&lt;&gt;solved!I8))</xm:f>
             <x14:dxf>
               <font>
@@ -10855,7 +10860,7 @@
           <xm:sqref>I8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="109" id="{573428B7-676C-4C61-A327-481350AE8081}">
+          <x14:cfRule type="expression" priority="109" id="{49EFF389-809D-4F43-B115-E4A64332644B}">
             <xm:f>AND((I9&lt;10),(I9&lt;&gt;solved!I9))</xm:f>
             <x14:dxf>
               <font>
@@ -11253,9 +11258,9 @@
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="16"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="17"/>
+      <c r="G10" s="18"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -11361,108 +11366,108 @@
       <c r="J20" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="18" t="n">
+      <c r="C22" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="18" t="n">
+      <c r="D22" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="18" t="n">
+      <c r="E22" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="18" t="n">
+      <c r="F22" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="18" t="n">
+      <c r="G22" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="18" t="n">
+      <c r="B23" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19" t="n">
+      <c r="C23" s="20"/>
+      <c r="D23" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19" t="n">
+      <c r="E23" s="20"/>
+      <c r="F23" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G23" s="19" t="n">
+      <c r="G23" s="20" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="18" t="n">
+      <c r="B24" s="19" t="n">
         <v>35</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19" t="n">
+      <c r="C24" s="20"/>
+      <c r="D24" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19" t="n">
+      <c r="E24" s="20"/>
+      <c r="F24" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G24" s="19" t="n">
+      <c r="G24" s="20" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="18" t="n">
+      <c r="B25" s="19" t="n">
         <v>45</v>
       </c>
-      <c r="C25" s="20" t="n">
+      <c r="C25" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="19" t="n">
+      <c r="D25" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19" t="n">
+      <c r="E25" s="20"/>
+      <c r="F25" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G25" s="19" t="n">
+      <c r="G25" s="20" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="18" t="n">
+      <c r="B26" s="19" t="n">
         <v>75</v>
       </c>
-      <c r="C26" s="19" t="n">
+      <c r="C26" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19" t="n">
+      <c r="D26" s="20"/>
+      <c r="E26" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="20" t="n">
+      <c r="F26" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="G26" s="20" t="n">
+      <c r="G26" s="21" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="18" t="n">
+      <c r="B27" s="19" t="n">
         <v>95</v>
       </c>
-      <c r="C27" s="19" t="n">
+      <c r="C27" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19" t="n">
+      <c r="D27" s="20"/>
+      <c r="E27" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="F27" s="20" t="n">
+      <c r="F27" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="19"/>
+      <c r="G27" s="20"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B10">
@@ -12004,7 +12009,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="96" id="{C8FCB08B-F366-4A34-9F30-D791D3502C9B}">
+          <x14:cfRule type="expression" priority="96" id="{F6F5C373-1148-4710-A3B0-F58B2C402F31}">
             <xm:f>AND(($A$1&lt;10),($A$1&lt;&gt;solved!$A$1))</xm:f>
             <x14:dxf>
               <font>
@@ -12020,7 +12025,7 @@
           <xm:sqref>B1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="98" id="{CC5B5D40-D43D-4EA2-8D5E-A7DD97E5D715}">
+          <x14:cfRule type="expression" priority="98" id="{73CBAF9D-D3F4-427D-8292-713A94E7BCB6}">
             <xm:f>AND((B2&lt;10),(B2&lt;&gt;solved!B2))</xm:f>
             <x14:dxf>
               <font>
@@ -12031,7 +12036,7 @@
           <xm:sqref>B2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="100" id="{32D4A086-1533-4B8F-9A3C-A4B7C99A9161}">
+          <x14:cfRule type="expression" priority="100" id="{7AAA49C8-ED76-48E1-96E2-6D3C74D1CA1C}">
             <xm:f>AND((B3&lt;10),(B3&lt;&gt;solved!B3))</xm:f>
             <x14:dxf>
               <font>
@@ -12042,7 +12047,7 @@
           <xm:sqref>B3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="102" id="{BB945611-C5B4-4C57-B04A-AE8CC4D42467}">
+          <x14:cfRule type="expression" priority="102" id="{886E2856-A0F8-4819-B8CF-1269AE77E9A5}">
             <xm:f>AND(($A$4&lt;10),($A$4&lt;&gt;solved!$A$4))</xm:f>
             <x14:dxf>
               <font>
@@ -12053,7 +12058,7 @@
           <xm:sqref>B4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="104" id="{20BD6D2A-1DE0-4384-8878-596B62DEDB2B}">
+          <x14:cfRule type="expression" priority="104" id="{A8756FCA-2093-4B51-B768-C129009BCE64}">
             <xm:f>AND((B5&lt;10),(B5&lt;&gt;solved!B5))</xm:f>
             <x14:dxf>
               <font>
@@ -12064,7 +12069,7 @@
           <xm:sqref>B5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="106" id="{26BEFA6C-29CA-434D-ABB9-3E20A99441F3}">
+          <x14:cfRule type="expression" priority="106" id="{31C0DBAA-47C7-4C90-9839-4C3731CAEFA2}">
             <xm:f>AND((B6&lt;10),(B6&lt;&gt;solved!B6))</xm:f>
             <x14:dxf>
               <font>
@@ -12075,7 +12080,7 @@
           <xm:sqref>B6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="108" id="{49F6A62E-98F5-4FDC-8945-CCEE4975933D}">
+          <x14:cfRule type="expression" priority="108" id="{444D4834-B1E6-43F5-8636-13EF2F7C3DCC}">
             <xm:f>AND((B7&lt;10),(B7&lt;&gt;solved!B7))</xm:f>
             <x14:dxf>
               <font>
@@ -12086,7 +12091,7 @@
           <xm:sqref>B7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="110" id="{20AD471C-1886-4A6D-A58F-A5235111A2B4}">
+          <x14:cfRule type="expression" priority="110" id="{1C39F0D6-DF2D-45F0-8059-1047AAF0703C}">
             <xm:f>AND((B8&lt;10),(B8&lt;&gt;solved!B8))</xm:f>
             <x14:dxf>
               <font>
@@ -12097,7 +12102,7 @@
           <xm:sqref>B8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="112" id="{F0C66083-DE90-471B-A0E1-79639344695C}">
+          <x14:cfRule type="expression" priority="112" id="{5113C28E-6930-449F-A3AF-965FDC1DA0E0}">
             <xm:f>AND((B9&lt;10),(B9&lt;&gt;solved!B9))</xm:f>
             <x14:dxf>
               <font>
@@ -12108,7 +12113,7 @@
           <xm:sqref>B9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="114" id="{5F2B1C5D-EB8C-4B2B-87F9-EB724E11BF1C}">
+          <x14:cfRule type="expression" priority="114" id="{2FD2F3CE-27F1-4C51-B87B-CE80E0BA1DE2}">
             <xm:f>AND((C1&lt;10),(C1&lt;&gt;solved!C1))</xm:f>
             <x14:dxf>
               <font>
@@ -12119,7 +12124,7 @@
           <xm:sqref>C1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="116" id="{956AF1DA-8076-4BED-8B73-DCEAE050F713}">
+          <x14:cfRule type="expression" priority="116" id="{3AB26A11-ADBF-4F18-A41E-B8A51AE07478}">
             <xm:f>AND((C2&lt;10),(C2&lt;&gt;solved!C2))</xm:f>
             <x14:dxf>
               <font>
@@ -12130,7 +12135,7 @@
           <xm:sqref>C2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="118" id="{B023341F-13D6-4AC7-A4DD-2817EE2ECFA4}">
+          <x14:cfRule type="expression" priority="118" id="{2EBD68D4-1B90-4C5D-A82F-A658703F8F2E}">
             <xm:f>AND((C3&lt;10),(C3&lt;&gt;solved!C3))</xm:f>
             <x14:dxf>
               <font>
@@ -12141,7 +12146,7 @@
           <xm:sqref>C3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="120" id="{20687173-6E3A-4250-B92E-46AD5D2ED4DE}">
+          <x14:cfRule type="expression" priority="120" id="{B8D2A961-7613-4EBA-8CBE-78FEC0A5108D}">
             <xm:f>AND((C4&lt;10),(C4&lt;&gt;solved!C4))</xm:f>
             <x14:dxf>
               <font>
@@ -12152,7 +12157,7 @@
           <xm:sqref>C4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="122" id="{547C48A8-B2E4-463D-BD3D-89F3911D317D}">
+          <x14:cfRule type="expression" priority="122" id="{C667C436-E976-43E7-B0ED-CD806680F92F}">
             <xm:f>AND((C5&lt;10),(C5&lt;&gt;solved!C5))</xm:f>
             <x14:dxf>
               <font>
@@ -12163,7 +12168,7 @@
           <xm:sqref>C5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="124" id="{ED46BF75-608E-4343-98FB-769B51ADC1C3}">
+          <x14:cfRule type="expression" priority="124" id="{4E978AF4-3E3E-4C80-A42D-22B489333DA3}">
             <xm:f>AND((C6&lt;10),(C6&lt;&gt;solved!C6))</xm:f>
             <x14:dxf>
               <font>
@@ -12174,7 +12179,7 @@
           <xm:sqref>C6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="126" id="{92889E53-C2F0-4720-8841-80F9549460BA}">
+          <x14:cfRule type="expression" priority="126" id="{C7A0525B-526D-458B-BD59-A2C262BE1C91}">
             <xm:f>AND((C7&lt;10),(C7&lt;&gt;solved!C7))</xm:f>
             <x14:dxf>
               <font>
@@ -12185,7 +12190,7 @@
           <xm:sqref>C7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="128" id="{B4E7B849-D15A-4562-A5F5-C0A7E8B648A7}">
+          <x14:cfRule type="expression" priority="128" id="{3480FC1A-7B68-499B-B2AE-E0442275C3E2}">
             <xm:f>AND((C8&lt;10),(C8&lt;&gt;solved!C8))</xm:f>
             <x14:dxf>
               <font>
@@ -12196,7 +12201,7 @@
           <xm:sqref>C8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="130" id="{FB7E1620-F7FD-482A-91D9-B64F52DAEF90}">
+          <x14:cfRule type="expression" priority="130" id="{6D688B90-6018-41CA-B7CB-F0AC7FCCD395}">
             <xm:f>AND((C9&lt;10),(C9&lt;&gt;solved!C9))</xm:f>
             <x14:dxf>
               <font>
@@ -12207,7 +12212,7 @@
           <xm:sqref>C9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="132" id="{1880E02C-895F-46CB-8339-679BAF1B37ED}">
+          <x14:cfRule type="expression" priority="132" id="{98D6DDB1-FFE4-4370-B176-24D640A5D33A}">
             <xm:f>AND((D1&lt;10),(D1&lt;&gt;solved!D1))</xm:f>
             <x14:dxf>
               <font>
@@ -12218,7 +12223,7 @@
           <xm:sqref>D1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="134" id="{E4C03223-36F2-4279-B6CE-645FEAECC0AF}">
+          <x14:cfRule type="expression" priority="134" id="{A6AC433A-64D0-4450-94CF-2639A07315E9}">
             <xm:f>AND((D2&lt;10),(D2&lt;&gt;solved!D2))</xm:f>
             <x14:dxf>
               <font>
@@ -12229,7 +12234,7 @@
           <xm:sqref>D2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="136" id="{109C3586-6D33-49CB-85CD-BA5071A050F8}">
+          <x14:cfRule type="expression" priority="136" id="{FE73CDCA-7B67-4B88-AEA2-1CE98AA294DE}">
             <xm:f>AND((D3&lt;10),(D3&lt;&gt;solved!D3))</xm:f>
             <x14:dxf>
               <font>
@@ -12240,7 +12245,7 @@
           <xm:sqref>D3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="138" id="{60B4F1AA-4624-4771-AFC5-AE4094581389}">
+          <x14:cfRule type="expression" priority="138" id="{A7945069-839C-4AF0-914A-9032CD43B06D}">
             <xm:f>AND((D4&lt;10),(D4&lt;&gt;solved!D4))</xm:f>
             <x14:dxf>
               <font>
@@ -12251,7 +12256,7 @@
           <xm:sqref>D4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="140" id="{5346E0D0-2AAD-4240-86CC-8BB09055579B}">
+          <x14:cfRule type="expression" priority="140" id="{7F3A1674-501A-4A17-8E98-D57BE32A6912}">
             <xm:f>AND((D5&lt;10),(D5&lt;&gt;solved!D5))</xm:f>
             <x14:dxf>
               <font>
@@ -12262,7 +12267,7 @@
           <xm:sqref>D5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="142" id="{AA9FA547-6BAC-4FCD-AFDA-3F6FDBB7DE8D}">
+          <x14:cfRule type="expression" priority="142" id="{903FEB86-E178-4260-9F84-A659C0D0C49D}">
             <xm:f>AND((D6&lt;10),(D6&lt;&gt;solved!D6))</xm:f>
             <x14:dxf>
               <font>
@@ -12273,7 +12278,7 @@
           <xm:sqref>D6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="144" id="{4AD79C54-C3C8-4C50-A0DF-60E9DE4E87BD}">
+          <x14:cfRule type="expression" priority="144" id="{9A333975-7889-4FB3-9BF0-7EB9BB67BD30}">
             <xm:f>AND((D7&lt;10),(D7&lt;&gt;solved!D7))</xm:f>
             <x14:dxf>
               <font>
@@ -12284,7 +12289,7 @@
           <xm:sqref>D7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="146" id="{5837CDD0-D9CA-498E-B6EE-98776E51661F}">
+          <x14:cfRule type="expression" priority="146" id="{8AC09C1C-466D-48DF-9B86-62E1112E21FD}">
             <xm:f>AND((D8&lt;10),(D8&lt;&gt;solved!D8))</xm:f>
             <x14:dxf>
               <font>
@@ -12295,7 +12300,7 @@
           <xm:sqref>D8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="148" id="{267A719D-B09A-4E69-B630-ABA21AC83CE1}">
+          <x14:cfRule type="expression" priority="148" id="{3736D1CC-6D23-4D2B-A86F-B67626652E11}">
             <xm:f>AND((D9&lt;10),(D9&lt;&gt;solved!D9))</xm:f>
             <x14:dxf>
               <font>
@@ -12306,7 +12311,7 @@
           <xm:sqref>D9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="150" id="{DD479286-1D54-4894-A298-DEC35C5BE03E}">
+          <x14:cfRule type="expression" priority="150" id="{8BC1BF64-64D8-4989-AFA8-F5F0C76EB82D}">
             <xm:f>AND((E1&lt;10),(E1&lt;&gt;solved!E1))</xm:f>
             <x14:dxf>
               <font>
@@ -12317,7 +12322,7 @@
           <xm:sqref>E1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="152" id="{173EA43F-7AEA-4984-8AEE-5E50D173865C}">
+          <x14:cfRule type="expression" priority="152" id="{9E36F2ED-44E4-4950-A35D-2D9622A53396}">
             <xm:f>AND((E2&lt;10),(E2&lt;&gt;solved!E2))</xm:f>
             <x14:dxf>
               <font>
@@ -12328,7 +12333,7 @@
           <xm:sqref>E2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="154" id="{2078BF2B-BE7B-442E-BE4D-76414F31C07B}">
+          <x14:cfRule type="expression" priority="154" id="{2D97B670-965F-4929-AD58-1C3B2743A41C}">
             <xm:f>AND((E3&lt;10),(E3&lt;&gt;solved!E3))</xm:f>
             <x14:dxf>
               <font>
@@ -12339,7 +12344,7 @@
           <xm:sqref>E3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="156" id="{8DACDCAE-A3CD-498D-A857-C46B809ABB2A}">
+          <x14:cfRule type="expression" priority="156" id="{FE80D98B-EBF3-40B0-AF98-FC1581298E48}">
             <xm:f>AND((E4&lt;10),(E4&lt;&gt;solved!E4))</xm:f>
             <x14:dxf>
               <font>
@@ -12350,7 +12355,7 @@
           <xm:sqref>E4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="158" id="{1C44BD7A-97D3-4D7A-99B5-CE194BDD433B}">
+          <x14:cfRule type="expression" priority="158" id="{A0E6EDF0-177E-4DA8-B165-C3A063485720}">
             <xm:f>AND((E5&lt;10),(E5&lt;&gt;solved!E5))</xm:f>
             <x14:dxf>
               <font>
@@ -12361,7 +12366,7 @@
           <xm:sqref>E5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="160" id="{1A705AA1-9255-422F-B6C9-22E1E96D79A4}">
+          <x14:cfRule type="expression" priority="160" id="{639A7BCD-D9C0-4A5F-8882-9A98B670347F}">
             <xm:f>AND((E6&lt;10),(E6&lt;&gt;solved!E6))</xm:f>
             <x14:dxf>
               <font>
@@ -12372,7 +12377,7 @@
           <xm:sqref>E6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="162" id="{82F0EE33-8F42-46BA-ADE1-66F22B4E12DF}">
+          <x14:cfRule type="expression" priority="162" id="{1DE044CD-B435-4DC7-8770-4F76AF87CB7E}">
             <xm:f>AND((E7&lt;10),(E7&lt;&gt;solved!E7))</xm:f>
             <x14:dxf>
               <font>
@@ -12383,7 +12388,7 @@
           <xm:sqref>E7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="164" id="{12FA87AD-001E-4520-80F5-B0F28079C5B0}">
+          <x14:cfRule type="expression" priority="164" id="{5ECED4A1-6010-4C6C-82DA-C067E54880D0}">
             <xm:f>AND((E8&lt;10),(E8&lt;&gt;solved!E8))</xm:f>
             <x14:dxf>
               <font>
@@ -12394,7 +12399,7 @@
           <xm:sqref>E8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="166" id="{17358746-664B-49A6-B87A-4E2C3AB815FA}">
+          <x14:cfRule type="expression" priority="166" id="{4F96416B-36A8-4D38-8754-581BB0832CC3}">
             <xm:f>AND((E9&lt;10),(E9&lt;&gt;solved!E9))</xm:f>
             <x14:dxf>
               <font>
@@ -12405,7 +12410,7 @@
           <xm:sqref>E9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="168" id="{7A5F8620-36DB-4280-BBE0-88E67D4F2CB3}">
+          <x14:cfRule type="expression" priority="168" id="{EDD0498D-80E3-4EF3-A730-E56F6B306F51}">
             <xm:f>AND((F1&lt;10),(F1&lt;&gt;solved!F1))</xm:f>
             <x14:dxf>
               <font>
@@ -12416,7 +12421,7 @@
           <xm:sqref>F1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="170" id="{404D987C-8C72-4FD5-B7DF-837B63CDEF21}">
+          <x14:cfRule type="expression" priority="170" id="{54C88E6B-51F0-4E2A-A772-39BBF58610FC}">
             <xm:f>AND((F2&lt;10),(F2&lt;&gt;solved!F2))</xm:f>
             <x14:dxf>
               <font>
@@ -12427,7 +12432,7 @@
           <xm:sqref>F2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="172" id="{3226A694-B079-4E47-B7BA-7CAD86F98C23}">
+          <x14:cfRule type="expression" priority="172" id="{B0F6B088-EA5E-439A-8E90-B984B3575483}">
             <xm:f>AND((F3&lt;10),(F3&lt;&gt;solved!F3))</xm:f>
             <x14:dxf>
               <font>
@@ -12438,7 +12443,7 @@
           <xm:sqref>F3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="174" id="{883920F6-2821-4FE9-801D-8BD067BA404F}">
+          <x14:cfRule type="expression" priority="174" id="{4785BDC0-92E5-4C34-9654-C0104B1CDE50}">
             <xm:f>AND((F4&lt;10),(F4&lt;&gt;solved!F4))</xm:f>
             <x14:dxf>
               <font>
@@ -12449,7 +12454,7 @@
           <xm:sqref>F4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="176" id="{9F761F4A-96DC-4355-9720-1F2F84D61C98}">
+          <x14:cfRule type="expression" priority="176" id="{72804594-BEA2-4B3F-BF7D-6EAA6D92255B}">
             <xm:f>AND((F5&lt;10),(F5&lt;&gt;solved!F5))</xm:f>
             <x14:dxf>
               <font>
@@ -12460,7 +12465,7 @@
           <xm:sqref>F5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="178" id="{51B2E093-DA47-4FE0-A080-44F2E25361DC}">
+          <x14:cfRule type="expression" priority="178" id="{F3BCBFA8-DDB8-4066-A0D5-392BC017FAB7}">
             <xm:f>AND((F6&lt;10),(F6&lt;&gt;solved!F6))</xm:f>
             <x14:dxf>
               <font>
@@ -12471,7 +12476,7 @@
           <xm:sqref>F6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="180" id="{F91BEBEE-D93E-47FF-A01E-FA94CD289F66}">
+          <x14:cfRule type="expression" priority="180" id="{DE2D288F-5189-4135-B3C4-54A532F5C091}">
             <xm:f>AND((F7&lt;10),(F7&lt;&gt;solved!F7))</xm:f>
             <x14:dxf>
               <font>
@@ -12482,7 +12487,7 @@
           <xm:sqref>F7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="182" id="{CF13C5F4-F3AE-4158-9F1D-448CCB29AECB}">
+          <x14:cfRule type="expression" priority="182" id="{39D86A3D-47F1-4599-9DBC-84F05187B49C}">
             <xm:f>AND((F8&lt;10),(F8&lt;&gt;solved!F8))</xm:f>
             <x14:dxf>
               <font>
@@ -12493,7 +12498,7 @@
           <xm:sqref>F8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="184" id="{DD6451A1-F8C5-44FA-95BF-F4322ECFCD70}">
+          <x14:cfRule type="expression" priority="184" id="{387F6E60-8EF4-456F-89BA-F619656F7E14}">
             <xm:f>AND((F9&lt;10),(F9&lt;&gt;solved!F9))</xm:f>
             <x14:dxf>
               <font>
@@ -12504,7 +12509,7 @@
           <xm:sqref>F9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="186" id="{6CEE8B3F-5C5A-4A1E-9EA1-3930C1007EA9}">
+          <x14:cfRule type="expression" priority="186" id="{8FA7937A-36E4-4E44-80A0-9468B33BC14E}">
             <xm:f>AND((G1&lt;10),(G1&lt;&gt;solved!G1))</xm:f>
             <x14:dxf>
               <font>
@@ -12515,7 +12520,7 @@
           <xm:sqref>G1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="188" id="{C1DDF1F8-776B-46FA-B5A8-FF5960311B3D}">
+          <x14:cfRule type="expression" priority="188" id="{CF8EBE73-643E-4EFC-93E4-727160878330}">
             <xm:f>AND((G2&lt;10),(G2&lt;&gt;solved!G2))</xm:f>
             <x14:dxf>
               <font>
@@ -12526,7 +12531,7 @@
           <xm:sqref>G2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="190" id="{C99CEAEE-CAB5-4CF0-9457-779E6A4E9D80}">
+          <x14:cfRule type="expression" priority="190" id="{F294FC51-47CE-49B4-94AA-FD7478486D7F}">
             <xm:f>AND((G3&lt;10),(G3&lt;&gt;solved!G3))</xm:f>
             <x14:dxf>
               <font>
@@ -12537,7 +12542,7 @@
           <xm:sqref>G3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="192" id="{8DC46618-B81B-426A-9A5E-9C4593B91A6E}">
+          <x14:cfRule type="expression" priority="192" id="{AAAFAB80-D08B-4AD7-8871-E3619D1E7C5A}">
             <xm:f>AND((G4&lt;10),(G4&lt;&gt;solved!G4))</xm:f>
             <x14:dxf>
               <font>
@@ -12548,7 +12553,7 @@
           <xm:sqref>G4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="194" id="{A083107B-407E-48D9-8098-AC19E074DF40}">
+          <x14:cfRule type="expression" priority="194" id="{79F77056-4C1F-4294-A43C-E065A84698EC}">
             <xm:f>AND((G5&lt;10),(G5&lt;&gt;solved!G5))</xm:f>
             <x14:dxf>
               <font>
@@ -12559,7 +12564,7 @@
           <xm:sqref>G5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="196" id="{DBCACFD2-EC92-41F6-BF53-E3A754D563FB}">
+          <x14:cfRule type="expression" priority="196" id="{9E4F67BE-58CA-4C30-9C66-50E1CB2D7046}">
             <xm:f>AND((G6&lt;10),(G6&lt;&gt;solved!G6))</xm:f>
             <x14:dxf>
               <font>
@@ -12570,7 +12575,7 @@
           <xm:sqref>G6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="198" id="{6D8750D8-5F50-4FAE-BAD4-88D78A333BA1}">
+          <x14:cfRule type="expression" priority="198" id="{E870A043-F98A-42BD-9300-356C3A2537ED}">
             <xm:f>AND((G7&lt;10),(G7&lt;&gt;solved!G7))</xm:f>
             <x14:dxf>
               <font>
@@ -12581,7 +12586,7 @@
           <xm:sqref>G7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="200" id="{4266A4F3-FF4B-49E9-A514-523D33D39216}">
+          <x14:cfRule type="expression" priority="200" id="{23F74B17-B759-441B-B787-F5556C8FB3D7}">
             <xm:f>AND((G8&lt;10),(G8&lt;&gt;solved!G8))</xm:f>
             <x14:dxf>
               <font>
@@ -12592,7 +12597,7 @@
           <xm:sqref>G8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="202" id="{6514DCAD-1267-4B20-B31F-D13BE261A8D3}">
+          <x14:cfRule type="expression" priority="202" id="{ACB21763-AA56-4C3C-A22A-191DB8FA9499}">
             <xm:f>AND((G9&lt;10),(G9&lt;&gt;solved!G9))</xm:f>
             <x14:dxf>
               <font>
@@ -12603,7 +12608,7 @@
           <xm:sqref>G9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="204" id="{BB451DCC-7F63-4BB5-86BE-BCBEAD493C19}">
+          <x14:cfRule type="expression" priority="204" id="{1D629310-21A6-4C64-8849-50C028F034C1}">
             <xm:f>AND((H1&lt;10),(H1&lt;&gt;solved!H1))</xm:f>
             <x14:dxf>
               <font>
@@ -12614,7 +12619,7 @@
           <xm:sqref>H1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="207" id="{409C6EA0-B7B6-409F-9897-1F14D21FC623}">
+          <x14:cfRule type="expression" priority="207" id="{72F02C1E-4B1F-4BEF-A347-B299D15FEABF}">
             <xm:f>AND((H2&lt;10),(H2&lt;&gt;solved!H2))</xm:f>
             <x14:dxf>
               <font>
@@ -12625,7 +12630,7 @@
           <xm:sqref>H2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="209" id="{90514C2A-A73C-4793-A979-A0648495E0EF}">
+          <x14:cfRule type="expression" priority="209" id="{C96E22C2-4790-4AFF-B8B7-3A7B4433A3C1}">
             <xm:f>AND((H3&lt;10),(H3&lt;&gt;solved!H3))</xm:f>
             <x14:dxf>
               <font>
@@ -12636,7 +12641,7 @@
           <xm:sqref>H3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="211" id="{18722978-BAEE-4363-A22D-4AA0DAE7B68A}">
+          <x14:cfRule type="expression" priority="211" id="{C975DC3E-7FCE-45B4-B848-20BD32E42BED}">
             <xm:f>AND((H4&lt;10),(H4&lt;&gt;solved!H4))</xm:f>
             <x14:dxf>
               <font>
@@ -12647,7 +12652,7 @@
           <xm:sqref>H4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="213" id="{2FE76AD4-9C40-415F-BF9D-FC4CA3FD94DA}">
+          <x14:cfRule type="expression" priority="213" id="{11C0A114-6939-494E-B297-CB997D30FB53}">
             <xm:f>AND((H5&lt;10),(H5&lt;&gt;solved!H5))</xm:f>
             <x14:dxf>
               <font>
@@ -12658,7 +12663,7 @@
           <xm:sqref>H5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="215" id="{94AE39AB-1600-44D0-9ACF-9E1282F3324D}">
+          <x14:cfRule type="expression" priority="215" id="{9AEF2BC1-BF60-49E4-9DD7-15CEFBE0B05F}">
             <xm:f>AND((H6&lt;10),(H6&lt;&gt;solved!H6))</xm:f>
             <x14:dxf>
               <font>
@@ -12669,7 +12674,7 @@
           <xm:sqref>H6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="217" id="{A4E44F26-84B5-4FC2-8656-3272D0AE2038}">
+          <x14:cfRule type="expression" priority="217" id="{1C193390-25B1-43EE-ACE6-EF99F485F57C}">
             <xm:f>AND((H7&lt;10),(H7&lt;&gt;solved!H7))</xm:f>
             <x14:dxf>
               <font>
@@ -12680,7 +12685,7 @@
           <xm:sqref>H7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="219" id="{4FCBBA80-2758-4A5E-A6D8-C0BD9B8575E7}">
+          <x14:cfRule type="expression" priority="219" id="{3F19E6DE-8FE9-45E4-BBDF-D0607C48F192}">
             <xm:f>AND((H8&lt;10),(H8&lt;&gt;solved!H8))</xm:f>
             <x14:dxf>
               <font>
@@ -12691,7 +12696,7 @@
           <xm:sqref>H8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="221" id="{1258E6EE-9430-41E9-98EE-8E67B6FA59E2}">
+          <x14:cfRule type="expression" priority="221" id="{44185668-59B5-46C6-9D70-741439821D83}">
             <xm:f>AND((H9&lt;10),(H9&lt;&gt;solved!H9))</xm:f>
             <x14:dxf>
               <font>
@@ -12702,7 +12707,7 @@
           <xm:sqref>H9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="223" id="{56937055-F280-4565-8EE2-A020F753D63A}">
+          <x14:cfRule type="expression" priority="223" id="{3E2033D3-81BB-4F5E-A75D-A7CE39E320A1}">
             <xm:f>AND((I1&lt;10),(I1&lt;&gt;solved!I1))</xm:f>
             <x14:dxf>
               <font>
@@ -12713,7 +12718,7 @@
           <xm:sqref>I1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="225" id="{4D5AF941-F4D0-46C0-8AF1-DC292AAC8A7B}">
+          <x14:cfRule type="expression" priority="225" id="{FFB0EA99-4219-4D63-8CDC-B2EC4516CAE0}">
             <xm:f>AND((I2&lt;10),(I2&lt;&gt;solved!I2))</xm:f>
             <x14:dxf>
               <font>
@@ -12724,7 +12729,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="227" id="{C611D2CB-F7ED-4539-AB5B-909CD6DAD060}">
+          <x14:cfRule type="expression" priority="227" id="{C0804C92-CEED-4A44-BBC8-A829AA698481}">
             <xm:f>AND((I3&lt;10),(I3&lt;&gt;solved!I3))</xm:f>
             <x14:dxf>
               <font>
@@ -12735,7 +12740,7 @@
           <xm:sqref>I3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="229" id="{BB1CF9C2-9DF6-477C-A773-66BB96E89D1A}">
+          <x14:cfRule type="expression" priority="229" id="{E1F9E37C-98BA-4AE8-8A61-CFAC79709255}">
             <xm:f>AND((I4&lt;10),(I4&lt;&gt;solved!I4))</xm:f>
             <x14:dxf>
               <font>
@@ -12746,7 +12751,7 @@
           <xm:sqref>I4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="231" id="{7785C215-94BE-4BAA-9669-E69FA663A512}">
+          <x14:cfRule type="expression" priority="231" id="{5BBE8B90-E0D1-4914-BF1C-856B80E69B77}">
             <xm:f>AND((I5&lt;10),(I5&lt;&gt;solved!I5))</xm:f>
             <x14:dxf>
               <font>
@@ -12757,7 +12762,7 @@
           <xm:sqref>I5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="233" id="{417100B5-8FBD-4D6E-A1C1-8FB07E247B38}">
+          <x14:cfRule type="expression" priority="233" id="{43A7E6E2-1766-44F6-B072-C0CDCFDF2DE7}">
             <xm:f>AND((I6&lt;10),(I6&lt;&gt;solved!I6))</xm:f>
             <x14:dxf>
               <font>
@@ -12768,7 +12773,7 @@
           <xm:sqref>I6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="235" id="{427A9C42-5C74-45D7-AAB4-B33A5394946C}">
+          <x14:cfRule type="expression" priority="235" id="{966DBEF4-6111-4D8D-85AB-C675272C3F28}">
             <xm:f>AND((I7&lt;10),(I7&lt;&gt;solved!I7))</xm:f>
             <x14:dxf>
               <font>
@@ -12779,7 +12784,7 @@
           <xm:sqref>I7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="237" id="{83D82741-65ED-4C90-96A6-43A3E7CEBCA4}">
+          <x14:cfRule type="expression" priority="237" id="{1F40F087-F879-4FDC-AEDF-43147D4BA380}">
             <xm:f>AND((I8&lt;10),(I8&lt;&gt;solved!I8))</xm:f>
             <x14:dxf>
               <font>
@@ -12790,7 +12795,7 @@
           <xm:sqref>I8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="239" id="{72956B3D-8ADF-45E9-9AB5-A2EC91817DAD}">
+          <x14:cfRule type="expression" priority="239" id="{B98FC2A4-8625-4450-943B-407A87786961}">
             <xm:f>AND((I9&lt;10),(I9&lt;&gt;solved!I9))</xm:f>
             <x14:dxf>
               <font>
@@ -12801,7 +12806,7 @@
           <xm:sqref>I9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="242" id="{EAEFDC3C-CA87-47FB-B9CB-3010BBD67BE0}">
+          <x14:cfRule type="expression" priority="242" id="{4E80E4CC-CB4E-43EA-A08A-20557222F94E}">
             <xm:f>AND((J2&lt;10),(J2&lt;&gt;solved!J2))</xm:f>
             <x14:dxf>
               <font>
@@ -12812,7 +12817,7 @@
           <xm:sqref>J2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="244" id="{A3CF4D90-AB62-4780-B996-1A10B8ED1ED0}">
+          <x14:cfRule type="expression" priority="244" id="{9DB6F090-91FC-48A3-A46B-E6D4B471B05D}">
             <xm:f>AND((J3&lt;10),(J3&lt;&gt;solved!J3))</xm:f>
             <x14:dxf>
               <font>
@@ -12823,7 +12828,7 @@
           <xm:sqref>J3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="246" id="{75E2B5B7-F918-4C70-98A7-1A38BF6E67C8}">
+          <x14:cfRule type="expression" priority="246" id="{205130FD-C0F5-4DE5-A496-925D9852CEB4}">
             <xm:f>AND((J4&lt;10),(J4&lt;&gt;solved!J4))</xm:f>
             <x14:dxf>
               <font>
@@ -12834,7 +12839,7 @@
           <xm:sqref>J4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="249" id="{E9F8C930-BD8C-49A5-81F4-7DBC3BBCBFF0}">
+          <x14:cfRule type="expression" priority="249" id="{109737C0-54D3-4987-B3F0-00A31013B070}">
             <xm:f>AND((J5&lt;10),(J5&lt;&gt;solved!J5))</xm:f>
             <x14:dxf>
               <font>
@@ -12845,7 +12850,7 @@
           <xm:sqref>J5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="251" id="{F42D6C83-2220-48B4-9829-ECBFDC363F8D}">
+          <x14:cfRule type="expression" priority="251" id="{45326C5B-8DBE-407F-B47A-2493F848E969}">
             <xm:f>AND((J6&lt;10),(J6&lt;&gt;solved!J6))</xm:f>
             <x14:dxf>
               <font>
@@ -12856,7 +12861,7 @@
           <xm:sqref>J6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="253" id="{7C7A7AEB-A4DD-4DBF-9511-C6BA151CEA95}">
+          <x14:cfRule type="expression" priority="253" id="{9B486974-E379-4D9F-AC20-D4D3E726F100}">
             <xm:f>AND((J7&lt;10),(J7&lt;&gt;solved!J7))</xm:f>
             <x14:dxf>
               <font>
@@ -12867,7 +12872,7 @@
           <xm:sqref>J7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="255" id="{91BBB635-1650-4142-8DA3-8F35B4A62578}">
+          <x14:cfRule type="expression" priority="255" id="{E0EDB36B-58F6-4F11-91A7-764196E76FD1}">
             <xm:f>AND((J8&lt;10),(J8&lt;&gt;solved!J8))</xm:f>
             <x14:dxf>
               <font>
@@ -12878,7 +12883,7 @@
           <xm:sqref>J8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="257" id="{B02C6959-38A1-42C1-A392-B850127883BF}">
+          <x14:cfRule type="expression" priority="257" id="{6870744A-2977-4777-8B98-683B467BA810}">
             <xm:f>AND((J9&lt;10),(J9&lt;&gt;solved!J9))</xm:f>
             <x14:dxf>
               <font>
@@ -13184,9 +13189,9 @@
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="16"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="17"/>
+      <c r="G10" s="18"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -13292,108 +13297,108 @@
       <c r="J20" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="18" t="n">
+      <c r="C22" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="18" t="n">
+      <c r="D22" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="18" t="n">
+      <c r="E22" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="18" t="n">
+      <c r="F22" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="18" t="n">
+      <c r="G22" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="18" t="n">
+      <c r="B23" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19" t="n">
+      <c r="C23" s="20"/>
+      <c r="D23" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19" t="n">
+      <c r="E23" s="20"/>
+      <c r="F23" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G23" s="19" t="n">
+      <c r="G23" s="20" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="18" t="n">
+      <c r="B24" s="19" t="n">
         <v>35</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19" t="n">
+      <c r="C24" s="20"/>
+      <c r="D24" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19" t="n">
+      <c r="E24" s="20"/>
+      <c r="F24" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G24" s="19" t="n">
+      <c r="G24" s="20" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="18" t="n">
+      <c r="B25" s="19" t="n">
         <v>45</v>
       </c>
-      <c r="C25" s="20" t="n">
+      <c r="C25" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="19" t="n">
+      <c r="D25" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19" t="n">
+      <c r="E25" s="20"/>
+      <c r="F25" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G25" s="19" t="n">
+      <c r="G25" s="20" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="18" t="n">
+      <c r="B26" s="19" t="n">
         <v>75</v>
       </c>
-      <c r="C26" s="19" t="n">
+      <c r="C26" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19" t="n">
+      <c r="D26" s="20"/>
+      <c r="E26" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="20" t="n">
+      <c r="F26" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="G26" s="20" t="n">
+      <c r="G26" s="21" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="18" t="n">
+      <c r="B27" s="19" t="n">
         <v>95</v>
       </c>
-      <c r="C27" s="19" t="n">
+      <c r="C27" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19" t="n">
+      <c r="D27" s="20"/>
+      <c r="E27" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="F27" s="20" t="n">
+      <c r="F27" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="19"/>
+      <c r="G27" s="20"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B10">
@@ -13893,9 +13898,9 @@
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="16"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="17"/>
+      <c r="G10" s="18"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -14001,108 +14006,108 @@
       <c r="J20" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="18" t="n">
+      <c r="C22" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="18" t="n">
+      <c r="D22" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="18" t="n">
+      <c r="E22" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="18" t="n">
+      <c r="F22" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="18" t="n">
+      <c r="G22" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="18" t="n">
+      <c r="B23" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19" t="n">
+      <c r="C23" s="20"/>
+      <c r="D23" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19" t="n">
+      <c r="E23" s="20"/>
+      <c r="F23" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G23" s="19" t="n">
+      <c r="G23" s="20" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="18" t="n">
+      <c r="B24" s="19" t="n">
         <v>35</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19" t="n">
+      <c r="C24" s="20"/>
+      <c r="D24" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19" t="n">
+      <c r="E24" s="20"/>
+      <c r="F24" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G24" s="19" t="n">
+      <c r="G24" s="20" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="18" t="n">
+      <c r="B25" s="19" t="n">
         <v>45</v>
       </c>
-      <c r="C25" s="20" t="n">
+      <c r="C25" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="19" t="n">
+      <c r="D25" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19" t="n">
+      <c r="E25" s="20"/>
+      <c r="F25" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G25" s="19" t="n">
+      <c r="G25" s="20" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="18" t="n">
+      <c r="B26" s="19" t="n">
         <v>75</v>
       </c>
-      <c r="C26" s="19" t="n">
+      <c r="C26" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19" t="n">
+      <c r="D26" s="20"/>
+      <c r="E26" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="20" t="n">
+      <c r="F26" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="G26" s="20" t="n">
+      <c r="G26" s="21" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="18" t="n">
+      <c r="B27" s="19" t="n">
         <v>95</v>
       </c>
-      <c r="C27" s="19" t="n">
+      <c r="C27" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19" t="n">
+      <c r="D27" s="20"/>
+      <c r="E27" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="F27" s="20" t="n">
+      <c r="F27" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="19"/>
+      <c r="G27" s="20"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B10">
@@ -14446,7 +14451,7 @@
       <c r="U1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21"/>
+      <c r="A2" s="22"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
       <c r="D2" s="9"/>
@@ -14472,7 +14477,7 @@
       <c r="U2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="21"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="11"/>
       <c r="C3" s="12"/>
       <c r="D3" s="13"/>
@@ -14494,7 +14499,7 @@
       <c r="U3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="21"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="n">
         <v>6</v>
@@ -14524,7 +14529,7 @@
       <c r="U4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="22" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="7"/>
@@ -14553,7 +14558,7 @@
       <c r="U5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="21"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
@@ -14575,7 +14580,7 @@
       <c r="U6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="21"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
@@ -14597,7 +14602,7 @@
       <c r="U7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8" t="n">
         <v>6</v>
@@ -14623,7 +14628,7 @@
       <c r="U8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="21"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="11"/>
       <c r="C9" s="12"/>
       <c r="D9" s="13" t="n">
@@ -14651,13 +14656,13 @@
       <c r="U9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="21"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="16"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="17"/>
+      <c r="G10" s="18"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -14763,113 +14768,113 @@
       <c r="J20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="22" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="18" t="n">
+      <c r="C22" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="18" t="n">
+      <c r="D22" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="18" t="n">
+      <c r="E22" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="18" t="n">
+      <c r="F22" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="18" t="n">
+      <c r="G22" s="19" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="18" t="n">
+      <c r="B23" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19" t="n">
+      <c r="C23" s="20"/>
+      <c r="D23" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19" t="n">
+      <c r="E23" s="20"/>
+      <c r="F23" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G23" s="19" t="n">
+      <c r="G23" s="20" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="18" t="n">
+      <c r="B24" s="19" t="n">
         <v>35</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19" t="n">
+      <c r="C24" s="20"/>
+      <c r="D24" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19" t="n">
+      <c r="E24" s="20"/>
+      <c r="F24" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G24" s="19" t="n">
+      <c r="G24" s="20" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="18" t="n">
+      <c r="B25" s="19" t="n">
         <v>45</v>
       </c>
-      <c r="C25" s="20" t="n">
+      <c r="C25" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="19" t="n">
+      <c r="D25" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19" t="n">
+      <c r="E25" s="20"/>
+      <c r="F25" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="G25" s="19" t="n">
+      <c r="G25" s="20" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="18" t="n">
+      <c r="B26" s="19" t="n">
         <v>75</v>
       </c>
-      <c r="C26" s="19" t="n">
+      <c r="C26" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19" t="n">
+      <c r="D26" s="20"/>
+      <c r="E26" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="F26" s="20" t="n">
+      <c r="F26" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="G26" s="20" t="n">
+      <c r="G26" s="21" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="18" t="n">
+      <c r="B27" s="19" t="n">
         <v>95</v>
       </c>
-      <c r="C27" s="19" t="n">
+      <c r="C27" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19" t="n">
+      <c r="D27" s="20"/>
+      <c r="E27" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="F27" s="20" t="n">
+      <c r="F27" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="G27" s="19"/>
+      <c r="G27" s="20"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B10">
@@ -15199,22 +15204,22 @@
       <c r="R2" s="7"/>
       <c r="S2" s="8"/>
       <c r="T2" s="9"/>
-      <c r="U2" s="18" t="s">
+      <c r="U2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="V2" s="18" t="n">
+      <c r="V2" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="W2" s="18" t="n">
+      <c r="W2" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="X2" s="18" t="n">
+      <c r="X2" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="Y2" s="18" t="n">
+      <c r="Y2" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="Z2" s="18" t="n">
+      <c r="Z2" s="19" t="n">
         <v>9</v>
       </c>
     </row>
@@ -15243,18 +15248,18 @@
       <c r="R3" s="11"/>
       <c r="S3" s="12"/>
       <c r="T3" s="13"/>
-      <c r="U3" s="18" t="n">
+      <c r="U3" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="V3" s="19"/>
-      <c r="W3" s="22" t="n">
+      <c r="V3" s="20"/>
+      <c r="W3" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="X3" s="19"/>
-      <c r="Y3" s="22" t="n">
+      <c r="X3" s="20"/>
+      <c r="Y3" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="Z3" s="22" t="n">
+      <c r="Z3" s="23" t="n">
         <v>9</v>
       </c>
     </row>
@@ -15287,18 +15292,18 @@
       <c r="R4" s="2"/>
       <c r="S4" s="3"/>
       <c r="T4" s="4"/>
-      <c r="U4" s="18" t="n">
+      <c r="U4" s="19" t="n">
         <v>35</v>
       </c>
-      <c r="V4" s="19"/>
-      <c r="W4" s="22" t="n">
+      <c r="V4" s="20"/>
+      <c r="W4" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="X4" s="19"/>
-      <c r="Y4" s="22" t="n">
+      <c r="X4" s="20"/>
+      <c r="Y4" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="Z4" s="22" t="n">
+      <c r="Z4" s="23" t="n">
         <v>9</v>
       </c>
     </row>
@@ -15343,20 +15348,20 @@
       <c r="R5" s="7"/>
       <c r="S5" s="8"/>
       <c r="T5" s="9"/>
-      <c r="U5" s="18" t="n">
+      <c r="U5" s="19" t="n">
         <v>45</v>
       </c>
-      <c r="V5" s="20" t="n">
+      <c r="V5" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="W5" s="22" t="n">
+      <c r="W5" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="X5" s="19"/>
-      <c r="Y5" s="22" t="n">
+      <c r="X5" s="20"/>
+      <c r="Y5" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="Z5" s="22" t="n">
+      <c r="Z5" s="23" t="n">
         <v>9</v>
       </c>
     </row>
@@ -15391,20 +15396,20 @@
       <c r="R6" s="11"/>
       <c r="S6" s="12"/>
       <c r="T6" s="13"/>
-      <c r="U6" s="18" t="n">
+      <c r="U6" s="19" t="n">
         <v>75</v>
       </c>
-      <c r="V6" s="19" t="n">
+      <c r="V6" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="W6" s="19"/>
-      <c r="X6" s="19" t="n">
+      <c r="W6" s="20"/>
+      <c r="X6" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="Y6" s="20" t="n">
+      <c r="Y6" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="Z6" s="20" t="n">
+      <c r="Z6" s="21" t="n">
         <v>9</v>
       </c>
     </row>
@@ -15433,20 +15438,20 @@
       <c r="R7" s="2"/>
       <c r="S7" s="3"/>
       <c r="T7" s="4"/>
-      <c r="U7" s="18" t="n">
+      <c r="U7" s="19" t="n">
         <v>95</v>
       </c>
-      <c r="V7" s="19" t="n">
+      <c r="V7" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="W7" s="19"/>
-      <c r="X7" s="19" t="n">
+      <c r="W7" s="20"/>
+      <c r="X7" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="Y7" s="20" t="n">
+      <c r="Y7" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="Z7" s="19"/>
+      <c r="Z7" s="20"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="7" t="s">
@@ -15508,7 +15513,7 @@
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="9"/>
-      <c r="E10" s="23"/>
+      <c r="E10" s="24"/>
       <c r="F10" s="8"/>
       <c r="H10" s="7"/>
       <c r="I10" s="8"/>
@@ -15897,45 +15902,45 @@
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="26"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="27"/>
       <c r="E2" s="8"/>
-      <c r="F2" s="27" t="n">
+      <c r="F2" s="28" t="n">
         <v>8</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="29" t="n">
+      <c r="G2" s="29"/>
+      <c r="H2" s="30" t="n">
         <v>3</v>
       </c>
       <c r="I2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="11"/>
-      <c r="B3" s="30"/>
+      <c r="B3" s="31"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="31" t="n">
+      <c r="D3" s="32" t="n">
         <v>5</v>
       </c>
       <c r="E3" s="12"/>
-      <c r="F3" s="32"/>
+      <c r="F3" s="33"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="33"/>
+      <c r="H3" s="34"/>
       <c r="I3" s="13" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="37"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="37" t="n">
+      <c r="F4" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="G4" s="38"/>
-      <c r="H4" s="39" t="n">
+      <c r="G4" s="39"/>
+      <c r="H4" s="40" t="n">
         <v>1</v>
       </c>
       <c r="I4" s="4"/>
@@ -15953,47 +15958,47 @@
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="11"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="42" t="n">
+      <c r="B6" s="41"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="43" t="n">
         <v>7</v>
       </c>
       <c r="E6" s="12"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="45"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="46"/>
       <c r="I6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
-      <c r="B7" s="46" t="n">
+      <c r="B7" s="47" t="n">
         <v>8</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="47"/>
+      <c r="D7" s="48"/>
       <c r="E7" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="F7" s="48"/>
+      <c r="F7" s="49"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="49"/>
+      <c r="H7" s="50"/>
       <c r="I7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="51" t="n">
+      <c r="B8" s="51"/>
+      <c r="C8" s="52" t="n">
         <v>9</v>
       </c>
-      <c r="D8" s="52"/>
+      <c r="D8" s="53"/>
       <c r="E8" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="53"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="55" t="n">
+      <c r="F8" s="54"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="56" t="n">
         <v>7</v>
       </c>
       <c r="I8" s="9"/>

</xml_diff>